<commit_message>
Add "990" prefix to all all-lane tolling classes
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/TOLLCLASS_Designations.xlsx
+++ b/utilities/NextGenFwys/TOLLCLASS_Designations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Downloads\All Aboard VO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natchison\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5D1FA314-FD0B-49F3-951B-8E1FB23A6983}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1AE4534-12C2-431C-9C13-D820AB2D9957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{0F0A9957-56E7-4C48-967B-2AB2A1965C2F}"/>
+    <workbookView xWindow="1905" yWindow="2100" windowWidth="22245" windowHeight="11715" xr2:uid="{0F0A9957-56E7-4C48-967B-2AB2A1965C2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs_for_tollcalib" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="276">
   <si>
     <t>SR92 SM - I-280 Interchange to US101 Interchange - WB</t>
   </si>
@@ -509,6 +509,366 @@
   </si>
   <si>
     <t>facility_name</t>
+  </si>
+  <si>
+    <t>SR4 CC - SR160 Interchange to Vasco Rd  (Per Mile Tolling) - WB</t>
+  </si>
+  <si>
+    <t>SR4 CC - SR160 Interchange to Vasco Rd  (Per Mile Tolling) - EB</t>
+  </si>
+  <si>
+    <t>SR24 - SR13 Interchange to I-680 Interchange  (Per Mile Tolling) - EB</t>
+  </si>
+  <si>
+    <t>I-680 CC - Livorna (Alamo) to Marina Vista   (Per Mile Tolling) - SB</t>
+  </si>
+  <si>
+    <t>SR242 CC - I680 to SR4  (Per Mile Tolling) - EB</t>
+  </si>
+  <si>
+    <t>SR242 CC - I680 to SR4  (Per Mile Tolling) - WB</t>
+  </si>
+  <si>
+    <t>I-680 CC - Livorna (Alamo) to Marina Vista   (Per Mile Tolling) - NB</t>
+  </si>
+  <si>
+    <t>SR4 - Port Chicago to Hillcrest Ave  (Per Mile Tolling) - WB</t>
+  </si>
+  <si>
+    <t>SR4 - Port Chicago to Hillcrest Ave  (Per Mile Tolling) - EB</t>
+  </si>
+  <si>
+    <t>SR24 - I-580 Interchange to SR13 Interchange  (Per Mile Tolling) - WB</t>
+  </si>
+  <si>
+    <t>I-580 - SFOBB toll plaza to SR24 Interchange  (Per Mile Tolling) - EB</t>
+  </si>
+  <si>
+    <t>I-980 ALA  (Per Mile Tolling) - NB</t>
+  </si>
+  <si>
+    <t>I-80 ALA - SFOBB Toll Plaza to University Ave (Berkeley)  (Per Mile Tolling) - WB</t>
+  </si>
+  <si>
+    <t>I-80 Bay Bridge - SF Transbay Terminal to SFOBB Toll Plaza  (Per Mile Tolling) - EB</t>
+  </si>
+  <si>
+    <t>I-580 - SFOBB toll plaza to SR24 Interchange  (Per Mile Tolling) - WB</t>
+  </si>
+  <si>
+    <t>I-238 - I-880 Interchange to I-580 Interchange  (Per Mile Tolling) - WB</t>
+  </si>
+  <si>
+    <t>I-880 ALA - SM Bridge to Hegenberger  (Per Mile Tolling) - SB</t>
+  </si>
+  <si>
+    <t>US101 SCL - SR85 to I-880  (Per Mile Tolling) - SB</t>
+  </si>
+  <si>
+    <t>SR85 - SR87 to US101 Interchange  (Per Mile Tolling) - EB</t>
+  </si>
+  <si>
+    <t>SR85 - SR87 to US101 Interchange  (Per Mile Tolling) - WB</t>
+  </si>
+  <si>
+    <t>SR87 - US101 Interchange to SR85  (Per Mile Tolling) - SB</t>
+  </si>
+  <si>
+    <t>I-280 SCL - US101 to Magdalena Ave (Loyola)  (Per Mile Tolling) - NB</t>
+  </si>
+  <si>
+    <t>SR17 - I-280 Interchange to SR85  (Per Mile Tolling) - NB</t>
+  </si>
+  <si>
+    <t>SR17 - I-280 Interchange to SR85  (Per Mile Tolling) - SB</t>
+  </si>
+  <si>
+    <t>I-280 SCL - US101 to Magdalena Ave (Loyola)  (Per Mile Tolling) - SB</t>
+  </si>
+  <si>
+    <t>I-880 SCL - I-280 Interchange to US101 Interchange  (Per Mile Tolling) - SB</t>
+  </si>
+  <si>
+    <t>SR87 - US101 Interchange to SR85  (Per Mile Tolling) - NB</t>
+  </si>
+  <si>
+    <t>US101 SCL - SR85 to I-880  (Per Mile Tolling) - NB</t>
+  </si>
+  <si>
+    <t>I-880 SCL - I-280 Interchange to US101 Interchange  (Per Mile Tolling) - NB</t>
+  </si>
+  <si>
+    <t>I-680 SCL - US101 to Alameda County Line  (Per Mile Tolling) - SB</t>
+  </si>
+  <si>
+    <t>US101 SCL - I-880 to SR237  (Per Mile Tolling) - SB</t>
+  </si>
+  <si>
+    <t>US101 SCL - SR237 to SM County Line  (Per Mile Tolling) - SB</t>
+  </si>
+  <si>
+    <t>I-880 SCL - US101 Interchange to SR237  (Per Mile Tolling) - SB</t>
+  </si>
+  <si>
+    <t>SR237 - US101 Interchange to I-880 Interchange  (Per Mile Tolling) - EB</t>
+  </si>
+  <si>
+    <t>SR237 - US101 Interchange to I-880 Interchange  (Per Mile Tolling) - WB</t>
+  </si>
+  <si>
+    <t>SR237 - SR85 to US101 Interchange  (Per Mile Tolling) - WB</t>
+  </si>
+  <si>
+    <t>I-280 SM - Millbrae Ave to SM County Line  (Per Mile Tolling) - WB</t>
+  </si>
+  <si>
+    <t>I-280 SM - Millbrae Ave to SM County Line  (Per Mile Tolling) - EB</t>
+  </si>
+  <si>
+    <t>SR92 SM - I-280 Interchange to US101 Interchange  (Per Mile Tolling) - EB</t>
+  </si>
+  <si>
+    <t>SR92 SM - I-280 Interchange to US101 Interchange  (Per Mile Tolling) - WB</t>
+  </si>
+  <si>
+    <t>US101 SM - SM Bridge (SR92) to I-380 Interchange  (Per Mile Tolling) - SB</t>
+  </si>
+  <si>
+    <t>SR92 - San Mateo Bridge  (Per Mile Tolling) - WB</t>
+  </si>
+  <si>
+    <t>US101 SM - Whipple Ave to SM Bridge (SR92)  (Per Mile Tolling) - NB</t>
+  </si>
+  <si>
+    <t>I-380 SM - I-280 Interchange to US101 Interchange  (Per Mile Tolling) - WB</t>
+  </si>
+  <si>
+    <t>I-380 SM - I-280 Interchange to US101 Interchange  (Per Mile Tolling) - EB</t>
+  </si>
+  <si>
+    <t>I-280 SF - I-380 Interchange to US101 Interchange  (Per Mile Tolling) - NB</t>
+  </si>
+  <si>
+    <t>US101 SM - I-380 Interchange to SF county line  (Per Mile Tolling) - SB</t>
+  </si>
+  <si>
+    <t>I-280 SF - US101 Interchange to 4th and King  (Per Mile Tolling) - NB</t>
+  </si>
+  <si>
+    <t>I-280 SF - US101 Interchange to 4th and King  (Per Mile Tolling) - SB</t>
+  </si>
+  <si>
+    <t>US101 SF - Golden Gate Bridge to Richardson Ave  (Per Mile Tolling) - SB</t>
+  </si>
+  <si>
+    <t>US101 SF - Golden Gate Bridge to Richardson Ave  (Per Mile Tolling) - NB</t>
+  </si>
+  <si>
+    <t>US101 MN - I-580 Interchange to SR116  (Per Mile Tolling) - NB</t>
+  </si>
+  <si>
+    <t>US101 MN - I-580 Interchange to SR116  (Per Mile Tolling) - SB</t>
+  </si>
+  <si>
+    <t>I-80 SOL - SR12/I-680 Interchange (Red Top Road) to I-505 Interchange  (Per Mile Tolling) - WB</t>
+  </si>
+  <si>
+    <t>I-80 SOL - SR12/I-680 Interchange (Red Top Road) to I-505 Interchange  (Per Mile Tolling) - EB</t>
+  </si>
+  <si>
+    <t>SR24 - SR13 Interchange to I-680 Interchange  (Per Mile Tolling) - WB</t>
+  </si>
+  <si>
+    <t>I-80 ALA - University Ave (Berkeley) to Cutting Blvd (Richmond)  (Per Mile Tolling) - EB</t>
+  </si>
+  <si>
+    <t>I-80 ALA - University Ave (Berkeley) to Cutting Blvd (Richmond)  (Per Mile Tolling) - WB</t>
+  </si>
+  <si>
+    <t>I-80 CC - Cutting Blvd (Richmond) to Carquinez Bridge Toll Plaza  (Per Mile Tolling) - EB</t>
+  </si>
+  <si>
+    <t>I-80 CC - Cutting Blvd (Richmond) to Carquinez Bridge Toll Plaza  (Per Mile Tolling) - WB</t>
+  </si>
+  <si>
+    <t>I-880 ALA - Hegenberger to SFOBB Toll Plaza  (Per Mile Tolling) - NB</t>
+  </si>
+  <si>
+    <t>I-880 ALA - Hegenberger to SFOBB Toll Plaza  (Per Mile Tolling) - SB</t>
+  </si>
+  <si>
+    <t>I-80 ALA - SFOBB Toll Plaza to University Ave (Berkeley)  (Per Mile Tolling) - EB</t>
+  </si>
+  <si>
+    <t>I-880 ALA - Dumbarton Bridge to SM Bridge  (Per Mile Tolling) - SB</t>
+  </si>
+  <si>
+    <t>I-880 ALA - Dumbarton Bridge to SM Bridge  (Per Mile Tolling) - NB</t>
+  </si>
+  <si>
+    <t>SR24 - I-580 Interchange to SR13 Interchange  (Per Mile Tolling) - EB</t>
+  </si>
+  <si>
+    <t>I-580 - SR24 Interchange to I-238 Interchange  (Per Mile Tolling) - EB</t>
+  </si>
+  <si>
+    <t>I-980 ALA  (Per Mile Tolling) - SB</t>
+  </si>
+  <si>
+    <t>I-580 - I-238 Interchange to I-680 Interchange  (Per Mile Tolling) - EB</t>
+  </si>
+  <si>
+    <t>I-580 - I-238 Interchange to I-680 Interchange  (Per Mile Tolling) - WB</t>
+  </si>
+  <si>
+    <t>I-580 - I-680 Interchange to Greenville  (Per Mile Tolling) - WB</t>
+  </si>
+  <si>
+    <t>I-580 - I-680 Interchange to Greenville  (Per Mile Tolling) - EB</t>
+  </si>
+  <si>
+    <t>I-580 - Greenville to SJ County Line  (Per Mile Tolling) - EB</t>
+  </si>
+  <si>
+    <t>I-580 - SR24 Interchange to I-238 Interchange  (Per Mile Tolling) - WB</t>
+  </si>
+  <si>
+    <t>I-580 - Greenville to SJ County Line  (Per Mile Tolling) - WB</t>
+  </si>
+  <si>
+    <t>I-880 ALA - SM Bridge to Hegenberger  (Per Mile Tolling) - NB</t>
+  </si>
+  <si>
+    <t>I-238 - I-880 Interchange to I-580 Interchange  (Per Mile Tolling) - EB</t>
+  </si>
+  <si>
+    <t>I-680 ALA - SCL County Line to SR84  (Per Mile Tolling) - SB</t>
+  </si>
+  <si>
+    <t>I-880 ALA - SR262 Mission Blvd to Dumbarton Bridge  (Per Mile Tolling) - NB</t>
+  </si>
+  <si>
+    <t>I-880 SCL - SR237 to SR262 Mission Blvd  (Per Mile Tolling) - SB</t>
+  </si>
+  <si>
+    <t>I-880 ALA - SR262 Mission Blvd to Dumbarton Bridge  (Per Mile Tolling) - SB</t>
+  </si>
+  <si>
+    <t>I-680 ALA - SCL County Line to SR84  (Per Mile Tolling) - NB</t>
+  </si>
+  <si>
+    <t>US101 SCL - San Benito County Line to Morgan Hill  (Per Mile Tolling) - NB</t>
+  </si>
+  <si>
+    <t>US101 SCL - San Benito County Line to Morgan Hill  (Per Mile Tolling) - SB</t>
+  </si>
+  <si>
+    <t>I-880 SCL - SR237 to SR262 Mission Blvd  (Per Mile Tolling) - NB</t>
+  </si>
+  <si>
+    <t>US101 SCL - Morgan Hill to SR85  (Per Mile Tolling) - NB</t>
+  </si>
+  <si>
+    <t>US101 SCL - Morgan Hill to SR85  (Per Mile Tolling) - SB</t>
+  </si>
+  <si>
+    <t>SR85 - I-280 Interchange to SR87  (Per Mile Tolling) - WB</t>
+  </si>
+  <si>
+    <t>SR85 - I-280 Interchange to SR87  (Per Mile Tolling) - EB</t>
+  </si>
+  <si>
+    <t>I-680 SCL - US101 to Alameda County Line  (Per Mile Tolling) - NB</t>
+  </si>
+  <si>
+    <t>I-280 SCL - Magdalena Ave (Loyola) to SM County Line  (Per Mile Tolling) - NB</t>
+  </si>
+  <si>
+    <t>I-280 SCL - Magdalena Ave (Loyola) to SM County Line  (Per Mile Tolling) - SB</t>
+  </si>
+  <si>
+    <t>I-880 SCL - US101 Interchange to SR237  (Per Mile Tolling) - NB</t>
+  </si>
+  <si>
+    <t>SR237 - SR85 to US101 Interchange  (Per Mile Tolling) - EB</t>
+  </si>
+  <si>
+    <t>US101 SCL - I-880 to SR237  (Per Mile Tolling) - NB</t>
+  </si>
+  <si>
+    <t>US101 SCL - SR237 to SM County Line  (Per Mile Tolling) - NB</t>
+  </si>
+  <si>
+    <t>US101 SM - Dumbarton Bridge (Willow Road) to Whipple Ave  (Per Mile Tolling) - NB</t>
+  </si>
+  <si>
+    <t>US101 SM - Dumbarton Bridge (Willow Road) to Whipple Ave  (Per Mile Tolling) - SB</t>
+  </si>
+  <si>
+    <t>US101 SM - SCL County Line to Dumbarton Bridge (Willow Road)  (Per Mile Tolling) - NB</t>
+  </si>
+  <si>
+    <t>US101 SM - I-380 Interchange to SF county line  (Per Mile Tolling) - NB</t>
+  </si>
+  <si>
+    <t>US101 SM - SCL County Line to Dumbarton Bridge (Willow Road)  (Per Mile Tolling) - SB</t>
+  </si>
+  <si>
+    <t>US101 SM - SM Bridge (SR92) to I-380 Interchange  (Per Mile Tolling) - NB</t>
+  </si>
+  <si>
+    <t>I-280 SF - I-380 Interchange to US101 Interchange  (Per Mile Tolling) - SB</t>
+  </si>
+  <si>
+    <t>US101 SM - Whipple Ave to SM Bridge (SR92)  (Per Mile Tolling) - SB</t>
+  </si>
+  <si>
+    <t>SR92 - San Mateo Bridge  (Per Mile Tolling) - EB</t>
+  </si>
+  <si>
+    <t>US101 SF - SF County Line to I-280 Interchange  (Per Mile Tolling) - SB</t>
+  </si>
+  <si>
+    <t>US101 SF - SF County Line to I-280 Interchange  (Per Mile Tolling) - NB</t>
+  </si>
+  <si>
+    <t>US101 SF - I-280 Interchange to SFOBB entrance  (Per Mile Tolling) - NB</t>
+  </si>
+  <si>
+    <t>US101 SF - I-280 Interchange to SFOBB entrance  (Per Mile Tolling) - SB</t>
+  </si>
+  <si>
+    <t>I-80 Bay Bridge - Civic Center to SF Transbay Terminal  (Per Mile Tolling) - WB</t>
+  </si>
+  <si>
+    <t>I-80 Bay Bridge - Civic Center to SF Transbay Terminal  (Per Mile Tolling) - EB</t>
+  </si>
+  <si>
+    <t>I-80 Bay Bridge - US101 to Civic Center  (Per Mile Tolling) - WB</t>
+  </si>
+  <si>
+    <t>I-80 Bay Bridge - US101 to Civic Center  (Per Mile Tolling) - EB</t>
+  </si>
+  <si>
+    <t>US101 MN - I-580 Interchange to GGB entrance  (Per Mile Tolling) - NB</t>
+  </si>
+  <si>
+    <t>US101 MN - I-580 Interchange to GGB entrance  (Per Mile Tolling) - SB</t>
+  </si>
+  <si>
+    <t>I-80 SOL - SR37 Interchange to SR12/I-680 Interchange (Red Top Road)  (Per Mile Tolling) - EB</t>
+  </si>
+  <si>
+    <t>I-80 SOL - SR37 Interchange to SR12/I-680 Interchange (Red Top Road)  (Per Mile Tolling) - WB</t>
+  </si>
+  <si>
+    <t>SR4 - I-680 (Grayson Creek) to Port Chicago  (Per Mile Tolling) - EB</t>
+  </si>
+  <si>
+    <t>I-80 SOL - Carquinez Bridge Toll Plaza to SR37 Interchange  (Per Mile Tolling) - EB</t>
+  </si>
+  <si>
+    <t>I-80 SOL - Carquinez Bridge Toll Plaza to SR37 Interchange  (Per Mile Tolling) - WB</t>
   </si>
 </sst>
 </file>
@@ -2953,22 +3313,22 @@
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
-  <dimension ref="A1:F151"/>
+  <dimension ref="A1:F292"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A185" sqref="A185"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="68.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.1796875" customWidth="1"/>
+    <col min="1" max="1" width="68.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>155</v>
       </c>
@@ -2986,12 +3346,12 @@
       </c>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>150</v>
       </c>
       <c r="B2">
-        <f>C2*1000+4</f>
+        <f t="shared" ref="B2:B33" si="0">C2*1000+4</f>
         <v>75004</v>
       </c>
       <c r="C2">
@@ -3004,12 +3364,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>149</v>
       </c>
       <c r="B3">
-        <f>C3*1000+4</f>
+        <f t="shared" si="0"/>
         <v>76004</v>
       </c>
       <c r="C3">
@@ -3022,12 +3382,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>148</v>
       </c>
       <c r="B4">
-        <f>C4*1000+4</f>
+        <f t="shared" si="0"/>
         <v>77004</v>
       </c>
       <c r="C4">
@@ -3040,12 +3400,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>147</v>
       </c>
       <c r="B5">
-        <f>C5*1000+4</f>
+        <f t="shared" si="0"/>
         <v>78004</v>
       </c>
       <c r="C5">
@@ -3058,12 +3418,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>146</v>
       </c>
       <c r="B6">
-        <f>C6*1000+4</f>
+        <f t="shared" si="0"/>
         <v>79004</v>
       </c>
       <c r="C6">
@@ -3076,12 +3436,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>145</v>
       </c>
       <c r="B7">
-        <f>C7*1000+4</f>
+        <f t="shared" si="0"/>
         <v>80004</v>
       </c>
       <c r="C7">
@@ -3094,12 +3454,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>144</v>
       </c>
       <c r="B8">
-        <f>C8*1000+4</f>
+        <f t="shared" si="0"/>
         <v>81004</v>
       </c>
       <c r="C8">
@@ -3113,12 +3473,12 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>143</v>
       </c>
       <c r="B9">
-        <f>C9*1000+4</f>
+        <f t="shared" si="0"/>
         <v>82004</v>
       </c>
       <c r="C9">
@@ -3132,12 +3492,12 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>142</v>
       </c>
       <c r="B10">
-        <f>C10*1000+4</f>
+        <f t="shared" si="0"/>
         <v>83004</v>
       </c>
       <c r="C10">
@@ -3151,12 +3511,12 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>141</v>
       </c>
       <c r="B11">
-        <f>C11*1000+4</f>
+        <f t="shared" si="0"/>
         <v>84004</v>
       </c>
       <c r="C11">
@@ -3170,12 +3530,12 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>140</v>
       </c>
       <c r="B12">
-        <f>C12*1000+4</f>
+        <f t="shared" si="0"/>
         <v>85004</v>
       </c>
       <c r="C12">
@@ -3189,12 +3549,12 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>139</v>
       </c>
       <c r="B13">
-        <f>C13*1000+4</f>
+        <f t="shared" si="0"/>
         <v>86004</v>
       </c>
       <c r="C13">
@@ -3208,12 +3568,12 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>138</v>
       </c>
       <c r="B14">
-        <f>C14*1000+4</f>
+        <f t="shared" si="0"/>
         <v>87004</v>
       </c>
       <c r="C14">
@@ -3227,12 +3587,12 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>137</v>
       </c>
       <c r="B15">
-        <f>C15*1000+4</f>
+        <f t="shared" si="0"/>
         <v>88004</v>
       </c>
       <c r="C15">
@@ -3246,12 +3606,12 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>136</v>
       </c>
       <c r="B16">
-        <f>C16*1000+4</f>
+        <f t="shared" si="0"/>
         <v>89004</v>
       </c>
       <c r="C16">
@@ -3265,12 +3625,12 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>135</v>
       </c>
       <c r="B17">
-        <f>C17*1000+4</f>
+        <f t="shared" si="0"/>
         <v>90004</v>
       </c>
       <c r="C17">
@@ -3284,12 +3644,12 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>134</v>
       </c>
       <c r="B18">
-        <f>C18*1000+4</f>
+        <f t="shared" si="0"/>
         <v>91004</v>
       </c>
       <c r="C18">
@@ -3303,12 +3663,12 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>133</v>
       </c>
       <c r="B19">
-        <f>C19*1000+4</f>
+        <f t="shared" si="0"/>
         <v>92004</v>
       </c>
       <c r="C19">
@@ -3322,12 +3682,12 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>132</v>
       </c>
       <c r="B20">
-        <f>C20*1000+4</f>
+        <f t="shared" si="0"/>
         <v>93004</v>
       </c>
       <c r="C20">
@@ -3341,12 +3701,12 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>131</v>
       </c>
       <c r="B21">
-        <f>C21*1000+4</f>
+        <f t="shared" si="0"/>
         <v>94004</v>
       </c>
       <c r="C21">
@@ -3360,12 +3720,12 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>130</v>
       </c>
       <c r="B22">
-        <f>C22*1000+4</f>
+        <f t="shared" si="0"/>
         <v>101004</v>
       </c>
       <c r="C22">
@@ -3379,12 +3739,12 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>129</v>
       </c>
       <c r="B23">
-        <f>C23*1000+4</f>
+        <f t="shared" si="0"/>
         <v>102004</v>
       </c>
       <c r="C23">
@@ -3398,12 +3758,12 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>128</v>
       </c>
       <c r="B24">
-        <f>C24*1000+4</f>
+        <f t="shared" si="0"/>
         <v>103004</v>
       </c>
       <c r="C24">
@@ -3417,12 +3777,12 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>127</v>
       </c>
       <c r="B25">
-        <f>C25*1000+4</f>
+        <f t="shared" si="0"/>
         <v>104004</v>
       </c>
       <c r="C25">
@@ -3436,12 +3796,12 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>126</v>
       </c>
       <c r="B26">
-        <f>C26*1000+4</f>
+        <f t="shared" si="0"/>
         <v>105004</v>
       </c>
       <c r="C26">
@@ -3455,12 +3815,12 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>125</v>
       </c>
       <c r="B27">
-        <f>C27*1000+4</f>
+        <f t="shared" si="0"/>
         <v>106004</v>
       </c>
       <c r="C27">
@@ -3474,12 +3834,12 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>124</v>
       </c>
       <c r="B28">
-        <f>C28*1000+4</f>
+        <f t="shared" si="0"/>
         <v>107004</v>
       </c>
       <c r="C28">
@@ -3493,12 +3853,12 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>123</v>
       </c>
       <c r="B29">
-        <f>C29*1000+4</f>
+        <f t="shared" si="0"/>
         <v>108004</v>
       </c>
       <c r="C29">
@@ -3512,12 +3872,12 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>122</v>
       </c>
       <c r="B30">
-        <f>C30*1000+4</f>
+        <f t="shared" si="0"/>
         <v>109004</v>
       </c>
       <c r="C30">
@@ -3531,12 +3891,12 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>121</v>
       </c>
       <c r="B31">
-        <f>C31*1000+4</f>
+        <f t="shared" si="0"/>
         <v>110004</v>
       </c>
       <c r="C31">
@@ -3550,12 +3910,12 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>120</v>
       </c>
       <c r="B32">
-        <f>C32*1000+4</f>
+        <f t="shared" si="0"/>
         <v>111004</v>
       </c>
       <c r="C32">
@@ -3569,12 +3929,12 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>119</v>
       </c>
       <c r="B33">
-        <f>C33*1000+4</f>
+        <f t="shared" si="0"/>
         <v>112004</v>
       </c>
       <c r="C33">
@@ -3588,12 +3948,12 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>118</v>
       </c>
       <c r="B34">
-        <f>C34*1000+4</f>
+        <f t="shared" ref="B34:B65" si="1">C34*1000+4</f>
         <v>113004</v>
       </c>
       <c r="C34">
@@ -3607,12 +3967,12 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>117</v>
       </c>
       <c r="B35">
-        <f>C35*1000+4</f>
+        <f t="shared" si="1"/>
         <v>114004</v>
       </c>
       <c r="C35">
@@ -3626,12 +3986,12 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>116</v>
       </c>
       <c r="B36">
-        <f>C36*1000+4</f>
+        <f t="shared" si="1"/>
         <v>115004</v>
       </c>
       <c r="C36">
@@ -3645,12 +4005,12 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>115</v>
       </c>
       <c r="B37">
-        <f>C37*1000+4</f>
+        <f t="shared" si="1"/>
         <v>116004</v>
       </c>
       <c r="C37">
@@ -3664,12 +4024,12 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>114</v>
       </c>
       <c r="B38">
-        <f>C38*1000+4</f>
+        <f t="shared" si="1"/>
         <v>117004</v>
       </c>
       <c r="C38">
@@ -3683,12 +4043,12 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>113</v>
       </c>
       <c r="B39">
-        <f>C39*1000+4</f>
+        <f t="shared" si="1"/>
         <v>118004</v>
       </c>
       <c r="C39">
@@ -3702,12 +4062,12 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>112</v>
       </c>
       <c r="B40">
-        <f>C40*1000+4</f>
+        <f t="shared" si="1"/>
         <v>119004</v>
       </c>
       <c r="C40">
@@ -3721,12 +4081,12 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>111</v>
       </c>
       <c r="B41">
-        <f>C41*1000+4</f>
+        <f t="shared" si="1"/>
         <v>120004</v>
       </c>
       <c r="C41">
@@ -3740,12 +4100,12 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>110</v>
       </c>
       <c r="B42">
-        <f>C42*1000+4</f>
+        <f t="shared" si="1"/>
         <v>121004</v>
       </c>
       <c r="C42">
@@ -3759,12 +4119,12 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>109</v>
       </c>
       <c r="B43">
-        <f>C43*1000+4</f>
+        <f t="shared" si="1"/>
         <v>122004</v>
       </c>
       <c r="C43">
@@ -3778,12 +4138,12 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>108</v>
       </c>
       <c r="B44">
-        <f>C44*1000+4</f>
+        <f t="shared" si="1"/>
         <v>123004</v>
       </c>
       <c r="C44">
@@ -3797,12 +4157,12 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>107</v>
       </c>
       <c r="B45">
-        <f>C45*1000+4</f>
+        <f t="shared" si="1"/>
         <v>124004</v>
       </c>
       <c r="C45">
@@ -3816,12 +4176,12 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>106</v>
       </c>
       <c r="B46">
-        <f>C46*1000+4</f>
+        <f t="shared" si="1"/>
         <v>131004</v>
       </c>
       <c r="C46">
@@ -3834,12 +4194,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>105</v>
       </c>
       <c r="B47">
-        <f>C47*1000+4</f>
+        <f t="shared" si="1"/>
         <v>132004</v>
       </c>
       <c r="C47">
@@ -3852,12 +4212,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>104</v>
       </c>
       <c r="B48">
-        <f>C48*1000+4</f>
+        <f t="shared" si="1"/>
         <v>133004</v>
       </c>
       <c r="C48">
@@ -3870,12 +4230,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>103</v>
       </c>
       <c r="B49">
-        <f>C49*1000+4</f>
+        <f t="shared" si="1"/>
         <v>134004</v>
       </c>
       <c r="C49">
@@ -3888,12 +4248,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>102</v>
       </c>
       <c r="B50">
-        <f>C50*1000+4</f>
+        <f t="shared" si="1"/>
         <v>171004</v>
       </c>
       <c r="C50">
@@ -3907,12 +4267,12 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>101</v>
       </c>
       <c r="B51">
-        <f>C51*1000+4</f>
+        <f t="shared" si="1"/>
         <v>172004</v>
       </c>
       <c r="C51">
@@ -3926,12 +4286,12 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>100</v>
       </c>
       <c r="B52">
-        <f>C52*1000+4</f>
+        <f t="shared" si="1"/>
         <v>231004</v>
       </c>
       <c r="C52">
@@ -3945,12 +4305,12 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>99</v>
       </c>
       <c r="B53">
-        <f>C53*1000+4</f>
+        <f t="shared" si="1"/>
         <v>232004</v>
       </c>
       <c r="C53">
@@ -3964,12 +4324,12 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>98</v>
       </c>
       <c r="B54">
-        <f>C54*1000+4</f>
+        <f t="shared" si="1"/>
         <v>233004</v>
       </c>
       <c r="C54">
@@ -3983,12 +4343,12 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>97</v>
       </c>
       <c r="B55">
-        <f>C55*1000+4</f>
+        <f t="shared" si="1"/>
         <v>234004</v>
       </c>
       <c r="C55">
@@ -4002,12 +4362,12 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>96</v>
       </c>
       <c r="B56">
-        <f>C56*1000+4</f>
+        <f t="shared" si="1"/>
         <v>239004</v>
       </c>
       <c r="C56">
@@ -4020,12 +4380,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>95</v>
       </c>
       <c r="B57">
-        <f>C57*1000+4</f>
+        <f t="shared" si="1"/>
         <v>240004</v>
       </c>
       <c r="C57">
@@ -4038,12 +4398,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>94</v>
       </c>
       <c r="B58">
-        <f>C58*1000+4</f>
+        <f t="shared" si="1"/>
         <v>241004</v>
       </c>
       <c r="C58">
@@ -4056,12 +4416,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>93</v>
       </c>
       <c r="B59">
-        <f>C59*1000+4</f>
+        <f t="shared" si="1"/>
         <v>242004</v>
       </c>
       <c r="C59">
@@ -4074,12 +4434,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>92</v>
       </c>
       <c r="B60">
-        <f>C60*1000+4</f>
+        <f t="shared" si="1"/>
         <v>243004</v>
       </c>
       <c r="C60">
@@ -4092,12 +4452,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>91</v>
       </c>
       <c r="B61">
-        <f>C61*1000+4</f>
+        <f t="shared" si="1"/>
         <v>244004</v>
       </c>
       <c r="C61">
@@ -4110,12 +4470,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>90</v>
       </c>
       <c r="B62">
-        <f>C62*1000+4</f>
+        <f t="shared" si="1"/>
         <v>281004</v>
       </c>
       <c r="C62">
@@ -4129,12 +4489,12 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>89</v>
       </c>
       <c r="B63">
-        <f>C63*1000+4</f>
+        <f t="shared" si="1"/>
         <v>282004</v>
       </c>
       <c r="C63">
@@ -4148,12 +4508,12 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>88</v>
       </c>
       <c r="B64">
-        <f>C64*1000+4</f>
+        <f t="shared" si="1"/>
         <v>283004</v>
       </c>
       <c r="C64">
@@ -4167,12 +4527,12 @@
         <v/>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>87</v>
       </c>
       <c r="B65">
-        <f>C65*1000+4</f>
+        <f t="shared" si="1"/>
         <v>284004</v>
       </c>
       <c r="C65">
@@ -4186,12 +4546,12 @@
         <v/>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>86</v>
       </c>
       <c r="B66">
-        <f>C66*1000+4</f>
+        <f t="shared" ref="B66:B97" si="2">C66*1000+4</f>
         <v>285004</v>
       </c>
       <c r="C66">
@@ -4205,12 +4565,12 @@
         <v/>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>85</v>
       </c>
       <c r="B67">
-        <f>C67*1000+4</f>
+        <f t="shared" si="2"/>
         <v>286004</v>
       </c>
       <c r="C67">
@@ -4224,12 +4584,12 @@
         <v/>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>84</v>
       </c>
       <c r="B68">
-        <f>C68*1000+4</f>
+        <f t="shared" si="2"/>
         <v>287004</v>
       </c>
       <c r="C68">
@@ -4242,12 +4602,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>83</v>
       </c>
       <c r="B69">
-        <f>C69*1000+4</f>
+        <f t="shared" si="2"/>
         <v>288004</v>
       </c>
       <c r="C69">
@@ -4260,12 +4620,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>82</v>
       </c>
       <c r="B70">
-        <f>C70*1000+4</f>
+        <f t="shared" si="2"/>
         <v>381004</v>
       </c>
       <c r="C70">
@@ -4278,12 +4638,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>81</v>
       </c>
       <c r="B71">
-        <f>C71*1000+4</f>
+        <f t="shared" si="2"/>
         <v>382004</v>
       </c>
       <c r="C71">
@@ -4296,12 +4656,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>80</v>
       </c>
       <c r="B72">
-        <f>C72*1000+4</f>
+        <f t="shared" si="2"/>
         <v>401004</v>
       </c>
       <c r="C72">
@@ -4315,12 +4675,12 @@
         <v/>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>79</v>
       </c>
       <c r="B73">
-        <f>C73*1000+4</f>
+        <f t="shared" si="2"/>
         <v>402004</v>
       </c>
       <c r="C73">
@@ -4334,12 +4694,12 @@
         <v/>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B74">
-        <f>C74*1000+4</f>
+        <f t="shared" si="2"/>
         <v>403004</v>
       </c>
       <c r="C74">
@@ -4349,12 +4709,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>77</v>
       </c>
       <c r="B75">
-        <f>C75*1000+4</f>
+        <f t="shared" si="2"/>
         <v>404004</v>
       </c>
       <c r="C75">
@@ -4364,12 +4724,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B76">
-        <f>C76*1000+4</f>
+        <f t="shared" si="2"/>
         <v>405004</v>
       </c>
       <c r="C76">
@@ -4379,12 +4739,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>75</v>
       </c>
       <c r="B77">
-        <f>C77*1000+4</f>
+        <f t="shared" si="2"/>
         <v>406004</v>
       </c>
       <c r="C77">
@@ -4394,12 +4754,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>74</v>
       </c>
       <c r="B78">
-        <f>C78*1000+4</f>
+        <f t="shared" si="2"/>
         <v>581004</v>
       </c>
       <c r="C78">
@@ -4413,12 +4773,12 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>73</v>
       </c>
       <c r="B79">
-        <f>C79*1000+4</f>
+        <f t="shared" si="2"/>
         <v>582004</v>
       </c>
       <c r="C79">
@@ -4432,12 +4792,12 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>72</v>
       </c>
       <c r="B80">
-        <f>C80*1000+4</f>
+        <f t="shared" si="2"/>
         <v>583004</v>
       </c>
       <c r="C80">
@@ -4451,12 +4811,12 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>71</v>
       </c>
       <c r="B81">
-        <f>C81*1000+4</f>
+        <f t="shared" si="2"/>
         <v>584004</v>
       </c>
       <c r="C81">
@@ -4470,12 +4830,12 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>70</v>
       </c>
       <c r="B82">
-        <f>C82*1000+4</f>
+        <f t="shared" si="2"/>
         <v>585004</v>
       </c>
       <c r="C82">
@@ -4489,12 +4849,12 @@
         <v/>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>69</v>
       </c>
       <c r="B83">
-        <f>C83*1000+4</f>
+        <f t="shared" si="2"/>
         <v>586004</v>
       </c>
       <c r="C83">
@@ -4508,12 +4868,12 @@
         <v/>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>68</v>
       </c>
       <c r="B84">
-        <f>C84*1000+4</f>
+        <f t="shared" si="2"/>
         <v>587004</v>
       </c>
       <c r="C84">
@@ -4527,12 +4887,12 @@
         <v/>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>67</v>
       </c>
       <c r="B85">
-        <f>C85*1000+4</f>
+        <f t="shared" si="2"/>
         <v>588004</v>
       </c>
       <c r="C85">
@@ -4546,12 +4906,12 @@
         <v/>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>66</v>
       </c>
       <c r="B86">
-        <f>C86*1000+4</f>
+        <f t="shared" si="2"/>
         <v>589004</v>
       </c>
       <c r="C86">
@@ -4565,12 +4925,12 @@
         <v/>
       </c>
     </row>
-    <row r="87" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>65</v>
       </c>
       <c r="B87">
-        <f>C87*1000+4</f>
+        <f t="shared" si="2"/>
         <v>590004</v>
       </c>
       <c r="C87">
@@ -4584,12 +4944,12 @@
         <v/>
       </c>
     </row>
-    <row r="88" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>64</v>
       </c>
       <c r="B88">
-        <f>C88*1000+4</f>
+        <f t="shared" si="2"/>
         <v>591004</v>
       </c>
       <c r="C88">
@@ -4602,12 +4962,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="89" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>63</v>
       </c>
       <c r="B89">
-        <f>C89*1000+4</f>
+        <f t="shared" si="2"/>
         <v>592004</v>
       </c>
       <c r="C89">
@@ -4620,12 +4980,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>62</v>
       </c>
       <c r="B90">
-        <f>C90*1000+4</f>
+        <f t="shared" si="2"/>
         <v>593004</v>
       </c>
       <c r="C90">
@@ -4638,12 +4998,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>61</v>
       </c>
       <c r="B91">
-        <f>C91*1000+4</f>
+        <f t="shared" si="2"/>
         <v>594004</v>
       </c>
       <c r="C91">
@@ -4656,12 +5016,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>60</v>
       </c>
       <c r="B92">
-        <f>C92*1000+4</f>
+        <f t="shared" si="2"/>
         <v>595004</v>
       </c>
       <c r="C92">
@@ -4674,12 +5034,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>59</v>
       </c>
       <c r="B93">
-        <f>C93*1000+4</f>
+        <f t="shared" si="2"/>
         <v>596004</v>
       </c>
       <c r="C93">
@@ -4692,12 +5052,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="94" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>58</v>
       </c>
       <c r="B94">
-        <f>C94*1000+4</f>
+        <f t="shared" si="2"/>
         <v>681004</v>
       </c>
       <c r="C94">
@@ -4711,12 +5071,12 @@
         <v/>
       </c>
     </row>
-    <row r="95" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>57</v>
       </c>
       <c r="B95">
-        <f>C95*1000+4</f>
+        <f t="shared" si="2"/>
         <v>682004</v>
       </c>
       <c r="C95">
@@ -4730,12 +5090,12 @@
         <v/>
       </c>
     </row>
-    <row r="96" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>56</v>
       </c>
       <c r="B96">
-        <f>C96*1000+4</f>
+        <f t="shared" si="2"/>
         <v>683004</v>
       </c>
       <c r="C96">
@@ -4749,12 +5109,12 @@
         <v/>
       </c>
     </row>
-    <row r="97" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>55</v>
       </c>
       <c r="B97">
-        <f>C97*1000+4</f>
+        <f t="shared" si="2"/>
         <v>684004</v>
       </c>
       <c r="C97">
@@ -4768,12 +5128,12 @@
         <v/>
       </c>
     </row>
-    <row r="98" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>54</v>
       </c>
       <c r="B98">
-        <f>C98*1000+4</f>
+        <f t="shared" ref="B98:B129" si="3">C98*1000+4</f>
         <v>685004</v>
       </c>
       <c r="C98">
@@ -4787,12 +5147,12 @@
         <v/>
       </c>
     </row>
-    <row r="99" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>53</v>
       </c>
       <c r="B99">
-        <f>C99*1000+4</f>
+        <f t="shared" si="3"/>
         <v>686004</v>
       </c>
       <c r="C99">
@@ -4806,12 +5166,12 @@
         <v/>
       </c>
     </row>
-    <row r="100" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>52</v>
       </c>
       <c r="B100">
-        <f>C100*1000+4</f>
+        <f t="shared" si="3"/>
         <v>687004</v>
       </c>
       <c r="C100">
@@ -4825,12 +5185,12 @@
         <v/>
       </c>
     </row>
-    <row r="101" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>51</v>
       </c>
       <c r="B101">
-        <f>C101*1000+4</f>
+        <f t="shared" si="3"/>
         <v>688004</v>
       </c>
       <c r="C101">
@@ -4844,12 +5204,12 @@
         <v/>
       </c>
     </row>
-    <row r="102" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>50</v>
       </c>
       <c r="B102">
-        <f>C102*1000+4</f>
+        <f t="shared" si="3"/>
         <v>689004</v>
       </c>
       <c r="C102">
@@ -4863,12 +5223,12 @@
         <v/>
       </c>
     </row>
-    <row r="103" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>49</v>
       </c>
       <c r="B103">
-        <f>C103*1000+4</f>
+        <f t="shared" si="3"/>
         <v>690004</v>
       </c>
       <c r="C103">
@@ -4882,12 +5242,12 @@
         <v/>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>48</v>
       </c>
       <c r="B104">
-        <f>C104*1000+4</f>
+        <f t="shared" si="3"/>
         <v>691004</v>
       </c>
       <c r="C104">
@@ -4901,12 +5261,12 @@
         <v/>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>47</v>
       </c>
       <c r="B105">
-        <f>C105*1000+4</f>
+        <f t="shared" si="3"/>
         <v>692004</v>
       </c>
       <c r="C105">
@@ -4920,12 +5280,12 @@
         <v/>
       </c>
     </row>
-    <row r="106" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>46</v>
       </c>
       <c r="B106">
-        <f>C106*1000+4</f>
+        <f t="shared" si="3"/>
         <v>841004</v>
       </c>
       <c r="C106">
@@ -4939,12 +5299,12 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="107" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>45</v>
       </c>
       <c r="B107">
-        <f>C107*1000+4</f>
+        <f t="shared" si="3"/>
         <v>842004</v>
       </c>
       <c r="C107">
@@ -4958,12 +5318,12 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="108" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>44</v>
       </c>
       <c r="B108">
-        <f>C108*1000+4</f>
+        <f t="shared" si="3"/>
         <v>843004</v>
       </c>
       <c r="C108">
@@ -4976,12 +5336,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="109" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>43</v>
       </c>
       <c r="B109">
-        <f>C109*1000+4</f>
+        <f t="shared" si="3"/>
         <v>844004</v>
       </c>
       <c r="C109">
@@ -4994,12 +5354,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="110" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>42</v>
       </c>
       <c r="B110">
-        <f>C110*1000+4</f>
+        <f t="shared" si="3"/>
         <v>851004</v>
       </c>
       <c r="C110">
@@ -5013,12 +5373,12 @@
         <v/>
       </c>
     </row>
-    <row r="111" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>41</v>
       </c>
       <c r="B111">
-        <f>C111*1000+4</f>
+        <f t="shared" si="3"/>
         <v>852004</v>
       </c>
       <c r="C111">
@@ -5032,12 +5392,12 @@
         <v/>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>40</v>
       </c>
       <c r="B112">
-        <f>C112*1000+4</f>
+        <f t="shared" si="3"/>
         <v>853004</v>
       </c>
       <c r="C112">
@@ -5051,12 +5411,12 @@
         <v/>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>39</v>
       </c>
       <c r="B113">
-        <f>C113*1000+4</f>
+        <f t="shared" si="3"/>
         <v>854004</v>
       </c>
       <c r="C113">
@@ -5070,12 +5430,12 @@
         <v/>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>38</v>
       </c>
       <c r="B114">
-        <f>C114*1000+4</f>
+        <f t="shared" si="3"/>
         <v>855004</v>
       </c>
       <c r="C114">
@@ -5089,12 +5449,12 @@
         <v/>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>37</v>
       </c>
       <c r="B115">
-        <f>C115*1000+4</f>
+        <f t="shared" si="3"/>
         <v>856004</v>
       </c>
       <c r="C115">
@@ -5108,12 +5468,12 @@
         <v/>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>36</v>
       </c>
       <c r="B116">
-        <f>C116*1000+4</f>
+        <f t="shared" si="3"/>
         <v>871004</v>
       </c>
       <c r="C116">
@@ -5127,12 +5487,12 @@
         <v/>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>35</v>
       </c>
       <c r="B117">
-        <f>C117*1000+4</f>
+        <f t="shared" si="3"/>
         <v>872004</v>
       </c>
       <c r="C117">
@@ -5146,12 +5506,12 @@
         <v/>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>34</v>
       </c>
       <c r="B118">
-        <f>C118*1000+4</f>
+        <f t="shared" si="3"/>
         <v>881004</v>
       </c>
       <c r="C118">
@@ -5165,12 +5525,12 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>33</v>
       </c>
       <c r="B119">
-        <f>C119*1000+4</f>
+        <f t="shared" si="3"/>
         <v>882004</v>
       </c>
       <c r="C119">
@@ -5184,12 +5544,12 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>32</v>
       </c>
       <c r="B120">
-        <f>C120*1000+4</f>
+        <f t="shared" si="3"/>
         <v>883004</v>
       </c>
       <c r="C120">
@@ -5203,12 +5563,12 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>31</v>
       </c>
       <c r="B121">
-        <f>C121*1000+4</f>
+        <f t="shared" si="3"/>
         <v>884004</v>
       </c>
       <c r="C121">
@@ -5222,12 +5582,12 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>30</v>
       </c>
       <c r="B122">
-        <f>C122*1000+4</f>
+        <f t="shared" si="3"/>
         <v>885004</v>
       </c>
       <c r="C122">
@@ -5241,12 +5601,12 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>29</v>
       </c>
       <c r="B123">
-        <f>C123*1000+4</f>
+        <f t="shared" si="3"/>
         <v>886004</v>
       </c>
       <c r="C123">
@@ -5260,12 +5620,12 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>28</v>
       </c>
       <c r="B124">
-        <f>C124*1000+4</f>
+        <f t="shared" si="3"/>
         <v>887004</v>
       </c>
       <c r="C124">
@@ -5279,12 +5639,12 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>27</v>
       </c>
       <c r="B125">
-        <f>C125*1000+4</f>
+        <f t="shared" si="3"/>
         <v>888004</v>
       </c>
       <c r="C125">
@@ -5298,12 +5658,12 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>26</v>
       </c>
       <c r="B126">
-        <f>C126*1000+4</f>
+        <f t="shared" si="3"/>
         <v>889004</v>
       </c>
       <c r="C126">
@@ -5317,12 +5677,12 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>25</v>
       </c>
       <c r="B127">
-        <f>C127*1000+4</f>
+        <f t="shared" si="3"/>
         <v>890004</v>
       </c>
       <c r="C127">
@@ -5336,12 +5696,12 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>24</v>
       </c>
       <c r="B128">
-        <f>C128*1000+4</f>
+        <f t="shared" si="3"/>
         <v>891004</v>
       </c>
       <c r="C128">
@@ -5355,12 +5715,12 @@
         <v/>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>23</v>
       </c>
       <c r="B129">
-        <f>C129*1000+4</f>
+        <f t="shared" si="3"/>
         <v>892004</v>
       </c>
       <c r="C129">
@@ -5374,12 +5734,12 @@
         <v/>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>22</v>
       </c>
       <c r="B130">
-        <f>C130*1000+4</f>
+        <f t="shared" ref="B130:B161" si="4">C130*1000+4</f>
         <v>921004</v>
       </c>
       <c r="C130">
@@ -5393,12 +5753,12 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>21</v>
       </c>
       <c r="B131">
-        <f>C131*1000+4</f>
+        <f t="shared" si="4"/>
         <v>922004</v>
       </c>
       <c r="C131">
@@ -5412,12 +5772,12 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>20</v>
       </c>
       <c r="B132">
-        <f>C132*1000+4</f>
+        <f t="shared" si="4"/>
         <v>923004</v>
       </c>
       <c r="C132">
@@ -5430,12 +5790,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>19</v>
       </c>
       <c r="B133">
-        <f>C133*1000+4</f>
+        <f t="shared" si="4"/>
         <v>924004</v>
       </c>
       <c r="C133">
@@ -5448,12 +5808,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>18</v>
       </c>
       <c r="B134">
-        <f>C134*1000+4</f>
+        <f t="shared" si="4"/>
         <v>925004</v>
       </c>
       <c r="C134">
@@ -5466,12 +5826,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>17</v>
       </c>
       <c r="B135">
-        <f>C135*1000+4</f>
+        <f t="shared" si="4"/>
         <v>926004</v>
       </c>
       <c r="C135">
@@ -5484,12 +5844,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>15</v>
       </c>
       <c r="B136">
-        <f>C136*1000+4</f>
+        <f t="shared" si="4"/>
         <v>981004</v>
       </c>
       <c r="C136">
@@ -5499,12 +5859,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>14</v>
       </c>
       <c r="B137">
-        <f>C137*1000+4</f>
+        <f t="shared" si="4"/>
         <v>982004</v>
       </c>
       <c r="C137">
@@ -5514,12 +5874,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>13</v>
       </c>
       <c r="B138">
-        <f>C138*1000+4</f>
+        <f t="shared" si="4"/>
         <v>879004</v>
       </c>
       <c r="C138">
@@ -5529,12 +5889,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>12</v>
       </c>
       <c r="B139">
-        <f>C139*1000+4</f>
+        <f t="shared" si="4"/>
         <v>880004</v>
       </c>
       <c r="C139">
@@ -5544,12 +5904,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>11</v>
       </c>
       <c r="B140">
-        <f>C140*1000+4</f>
+        <f t="shared" si="4"/>
         <v>135004</v>
       </c>
       <c r="C140">
@@ -5559,12 +5919,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>10</v>
       </c>
       <c r="B141">
-        <f>C141*1000+4</f>
+        <f t="shared" si="4"/>
         <v>136004</v>
       </c>
       <c r="C141">
@@ -5574,12 +5934,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>9</v>
       </c>
       <c r="B142">
-        <f>C142*1000+4</f>
+        <f t="shared" si="4"/>
         <v>245004</v>
       </c>
       <c r="C142">
@@ -5589,12 +5949,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>8</v>
       </c>
       <c r="B143">
-        <f>C143*1000+4</f>
+        <f t="shared" si="4"/>
         <v>246004</v>
       </c>
       <c r="C143">
@@ -5604,12 +5964,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>7</v>
       </c>
       <c r="B144">
-        <f>C144*1000+4</f>
+        <f t="shared" si="4"/>
         <v>407004</v>
       </c>
       <c r="C144">
@@ -5619,12 +5979,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>6</v>
       </c>
       <c r="B145">
-        <f>C145*1000+4</f>
+        <f t="shared" si="4"/>
         <v>408004</v>
       </c>
       <c r="C145">
@@ -5634,12 +5994,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>5</v>
       </c>
       <c r="B146">
-        <f>C146*1000+4</f>
+        <f t="shared" si="4"/>
         <v>137004</v>
       </c>
       <c r="C146">
@@ -5649,12 +6009,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>4</v>
       </c>
       <c r="B147">
-        <f>C147*1000+4</f>
+        <f t="shared" si="4"/>
         <v>138004</v>
       </c>
       <c r="C147">
@@ -5664,12 +6024,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>3</v>
       </c>
       <c r="B148">
-        <f>C148*1000+4</f>
+        <f t="shared" si="4"/>
         <v>289004</v>
       </c>
       <c r="C148">
@@ -5679,12 +6039,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>2</v>
       </c>
       <c r="B149">
-        <f>C149*1000+4</f>
+        <f t="shared" si="4"/>
         <v>290004</v>
       </c>
       <c r="C149">
@@ -5694,12 +6054,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>1</v>
       </c>
       <c r="B150">
-        <f>C150*1000+4</f>
+        <f t="shared" si="4"/>
         <v>927004</v>
       </c>
       <c r="C150">
@@ -5709,18 +6069,1992 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>0</v>
       </c>
       <c r="B151">
-        <f>C151*1000+4</f>
+        <f t="shared" si="4"/>
         <v>928004</v>
       </c>
       <c r="C151">
         <v>928</v>
       </c>
       <c r="D151" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>156</v>
+      </c>
+      <c r="B152">
+        <v>990408001</v>
+      </c>
+      <c r="C152">
+        <v>990408</v>
+      </c>
+      <c r="D152">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>157</v>
+      </c>
+      <c r="B153">
+        <v>990407001</v>
+      </c>
+      <c r="C153">
+        <v>990407</v>
+      </c>
+      <c r="D153">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>158</v>
+      </c>
+      <c r="B154">
+        <v>990243001</v>
+      </c>
+      <c r="C154">
+        <v>990243</v>
+      </c>
+      <c r="D154">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>159</v>
+      </c>
+      <c r="B155">
+        <v>990684001</v>
+      </c>
+      <c r="C155">
+        <v>990684</v>
+      </c>
+      <c r="D155">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>160</v>
+      </c>
+      <c r="B156">
+        <v>990245001</v>
+      </c>
+      <c r="C156">
+        <v>990245</v>
+      </c>
+      <c r="D156">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>161</v>
+      </c>
+      <c r="B157">
+        <v>990246001</v>
+      </c>
+      <c r="C157">
+        <v>990246</v>
+      </c>
+      <c r="D157">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>162</v>
+      </c>
+      <c r="B158">
+        <v>990683001</v>
+      </c>
+      <c r="C158">
+        <v>990683</v>
+      </c>
+      <c r="D158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>163</v>
+      </c>
+      <c r="B159">
+        <v>990402001</v>
+      </c>
+      <c r="C159">
+        <v>990402</v>
+      </c>
+      <c r="D159">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>164</v>
+      </c>
+      <c r="B160">
+        <v>990401001</v>
+      </c>
+      <c r="C160">
+        <v>990401</v>
+      </c>
+      <c r="D160">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>165</v>
+      </c>
+      <c r="B161">
+        <v>990242001</v>
+      </c>
+      <c r="C161">
+        <v>990242</v>
+      </c>
+      <c r="D161">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>166</v>
+      </c>
+      <c r="B162">
+        <v>990581001</v>
+      </c>
+      <c r="C162">
+        <v>990581</v>
+      </c>
+      <c r="D162">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>167</v>
+      </c>
+      <c r="B163">
+        <v>990981001</v>
+      </c>
+      <c r="C163">
+        <v>990981</v>
+      </c>
+      <c r="D163">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>168</v>
+      </c>
+      <c r="B164">
+        <v>990082001</v>
+      </c>
+      <c r="C164">
+        <v>990082</v>
+      </c>
+      <c r="D164">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>169</v>
+      </c>
+      <c r="B165">
+        <v>990079001</v>
+      </c>
+      <c r="C165">
+        <v>990079</v>
+      </c>
+      <c r="D165">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>170</v>
+      </c>
+      <c r="B166">
+        <v>990582001</v>
+      </c>
+      <c r="C166">
+        <v>990582</v>
+      </c>
+      <c r="D166">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>171</v>
+      </c>
+      <c r="B167">
+        <v>990240001</v>
+      </c>
+      <c r="C167">
+        <v>990240</v>
+      </c>
+      <c r="D167">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>172</v>
+      </c>
+      <c r="B168">
+        <v>990882001</v>
+      </c>
+      <c r="C168">
+        <v>990882</v>
+      </c>
+      <c r="D168">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>173</v>
+      </c>
+      <c r="B169">
+        <v>990120001</v>
+      </c>
+      <c r="C169">
+        <v>990120</v>
+      </c>
+      <c r="D169">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>174</v>
+      </c>
+      <c r="B170">
+        <v>990855001</v>
+      </c>
+      <c r="C170">
+        <v>990855</v>
+      </c>
+      <c r="D170">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>175</v>
+      </c>
+      <c r="B171">
+        <v>990856001</v>
+      </c>
+      <c r="C171">
+        <v>990856</v>
+      </c>
+      <c r="D171">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>176</v>
+      </c>
+      <c r="B172">
+        <v>990872001</v>
+      </c>
+      <c r="C172">
+        <v>990872</v>
+      </c>
+      <c r="D172">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>177</v>
+      </c>
+      <c r="B173">
+        <v>990285001</v>
+      </c>
+      <c r="C173">
+        <v>990285</v>
+      </c>
+      <c r="D173">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>178</v>
+      </c>
+      <c r="B174">
+        <v>990171001</v>
+      </c>
+      <c r="C174">
+        <v>990171</v>
+      </c>
+      <c r="D174">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>179</v>
+      </c>
+      <c r="B175">
+        <v>990172001</v>
+      </c>
+      <c r="C175">
+        <v>990172</v>
+      </c>
+      <c r="D175">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>180</v>
+      </c>
+      <c r="B176">
+        <v>990286001</v>
+      </c>
+      <c r="C176">
+        <v>990286</v>
+      </c>
+      <c r="D176">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>181</v>
+      </c>
+      <c r="B177">
+        <v>990892001</v>
+      </c>
+      <c r="C177">
+        <v>990892</v>
+      </c>
+      <c r="D177">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>182</v>
+      </c>
+      <c r="B178">
+        <v>990871001</v>
+      </c>
+      <c r="C178">
+        <v>990871</v>
+      </c>
+      <c r="D178">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>183</v>
+      </c>
+      <c r="B179">
+        <v>990119001</v>
+      </c>
+      <c r="C179">
+        <v>990119</v>
+      </c>
+      <c r="D179">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>184</v>
+      </c>
+      <c r="B180">
+        <v>990891001</v>
+      </c>
+      <c r="C180">
+        <v>990891</v>
+      </c>
+      <c r="D180">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>185</v>
+      </c>
+      <c r="B181">
+        <v>990692001</v>
+      </c>
+      <c r="C181">
+        <v>990692</v>
+      </c>
+      <c r="D181">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>186</v>
+      </c>
+      <c r="B182">
+        <v>990118001</v>
+      </c>
+      <c r="C182">
+        <v>990118</v>
+      </c>
+      <c r="D182">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>187</v>
+      </c>
+      <c r="B183">
+        <v>990116001</v>
+      </c>
+      <c r="C183">
+        <v>990116</v>
+      </c>
+      <c r="D183">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>188</v>
+      </c>
+      <c r="B184">
+        <v>990890001</v>
+      </c>
+      <c r="C184">
+        <v>990890</v>
+      </c>
+      <c r="D184">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>189</v>
+      </c>
+      <c r="B185">
+        <v>990231001</v>
+      </c>
+      <c r="C185">
+        <v>990231</v>
+      </c>
+      <c r="D185">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>190</v>
+      </c>
+      <c r="B186">
+        <v>990232001</v>
+      </c>
+      <c r="C186">
+        <v>990232</v>
+      </c>
+      <c r="D186">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>191</v>
+      </c>
+      <c r="B187">
+        <v>990234001</v>
+      </c>
+      <c r="C187">
+        <v>990234</v>
+      </c>
+      <c r="D187">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>192</v>
+      </c>
+      <c r="B188">
+        <v>990290001</v>
+      </c>
+      <c r="C188">
+        <v>990290</v>
+      </c>
+      <c r="D188">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>193</v>
+      </c>
+      <c r="B189">
+        <v>990289001</v>
+      </c>
+      <c r="C189">
+        <v>990289</v>
+      </c>
+      <c r="D189">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>194</v>
+      </c>
+      <c r="B190">
+        <v>990927001</v>
+      </c>
+      <c r="C190">
+        <v>990927</v>
+      </c>
+      <c r="D190">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>195</v>
+      </c>
+      <c r="B191">
+        <v>990928001</v>
+      </c>
+      <c r="C191">
+        <v>990928</v>
+      </c>
+      <c r="D191">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>196</v>
+      </c>
+      <c r="B192">
+        <v>990108001</v>
+      </c>
+      <c r="C192">
+        <v>990108</v>
+      </c>
+      <c r="D192">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>197</v>
+      </c>
+      <c r="B193">
+        <v>990924001</v>
+      </c>
+      <c r="C193">
+        <v>990924</v>
+      </c>
+      <c r="D193">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>198</v>
+      </c>
+      <c r="B194">
+        <v>990109001</v>
+      </c>
+      <c r="C194">
+        <v>990109</v>
+      </c>
+      <c r="D194">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>199</v>
+      </c>
+      <c r="B195">
+        <v>990382001</v>
+      </c>
+      <c r="C195">
+        <v>990382</v>
+      </c>
+      <c r="D195">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>200</v>
+      </c>
+      <c r="B196">
+        <v>990381001</v>
+      </c>
+      <c r="C196">
+        <v>990381</v>
+      </c>
+      <c r="D196">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>201</v>
+      </c>
+      <c r="B197">
+        <v>990287001</v>
+      </c>
+      <c r="C197">
+        <v>990287</v>
+      </c>
+      <c r="D197">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>202</v>
+      </c>
+      <c r="B198">
+        <v>990106001</v>
+      </c>
+      <c r="C198">
+        <v>990106</v>
+      </c>
+      <c r="D198">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>203</v>
+      </c>
+      <c r="B199">
+        <v>990281001</v>
+      </c>
+      <c r="C199">
+        <v>990281</v>
+      </c>
+      <c r="D199">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>204</v>
+      </c>
+      <c r="B200">
+        <v>990282001</v>
+      </c>
+      <c r="C200">
+        <v>990282</v>
+      </c>
+      <c r="D200">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>205</v>
+      </c>
+      <c r="B201">
+        <v>990138001</v>
+      </c>
+      <c r="C201">
+        <v>990138</v>
+      </c>
+      <c r="D201">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>206</v>
+      </c>
+      <c r="B202">
+        <v>990137001</v>
+      </c>
+      <c r="C202">
+        <v>990137</v>
+      </c>
+      <c r="D202">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>207</v>
+      </c>
+      <c r="B203">
+        <v>990135001</v>
+      </c>
+      <c r="C203">
+        <v>990135</v>
+      </c>
+      <c r="D203">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>208</v>
+      </c>
+      <c r="B204">
+        <v>990136001</v>
+      </c>
+      <c r="C204">
+        <v>990136</v>
+      </c>
+      <c r="D204">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>207</v>
+      </c>
+      <c r="B205">
+        <v>990135002</v>
+      </c>
+      <c r="C205">
+        <v>990135</v>
+      </c>
+      <c r="D205">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>208</v>
+      </c>
+      <c r="B206">
+        <v>990136002</v>
+      </c>
+      <c r="C206">
+        <v>990136</v>
+      </c>
+      <c r="D206">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>209</v>
+      </c>
+      <c r="B207">
+        <v>990092001</v>
+      </c>
+      <c r="C207">
+        <v>990092</v>
+      </c>
+      <c r="D207">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>210</v>
+      </c>
+      <c r="B208">
+        <v>990091001</v>
+      </c>
+      <c r="C208">
+        <v>990091</v>
+      </c>
+      <c r="D208">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>211</v>
+      </c>
+      <c r="B209">
+        <v>990244001</v>
+      </c>
+      <c r="C209">
+        <v>990244</v>
+      </c>
+      <c r="D209">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>212</v>
+      </c>
+      <c r="B210">
+        <v>990083001</v>
+      </c>
+      <c r="C210">
+        <v>990083</v>
+      </c>
+      <c r="D210">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>213</v>
+      </c>
+      <c r="B211">
+        <v>990084001</v>
+      </c>
+      <c r="C211">
+        <v>990084</v>
+      </c>
+      <c r="D211">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>214</v>
+      </c>
+      <c r="B212">
+        <v>990085001</v>
+      </c>
+      <c r="C212">
+        <v>990085</v>
+      </c>
+      <c r="D212">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>215</v>
+      </c>
+      <c r="B213">
+        <v>990086001</v>
+      </c>
+      <c r="C213">
+        <v>990086</v>
+      </c>
+      <c r="D213">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>216</v>
+      </c>
+      <c r="B214">
+        <v>990879001</v>
+      </c>
+      <c r="C214">
+        <v>990879</v>
+      </c>
+      <c r="D214">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>217</v>
+      </c>
+      <c r="B215">
+        <v>990880001</v>
+      </c>
+      <c r="C215">
+        <v>990880</v>
+      </c>
+      <c r="D215">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
+        <v>218</v>
+      </c>
+      <c r="B216">
+        <v>990081001</v>
+      </c>
+      <c r="C216">
+        <v>990081</v>
+      </c>
+      <c r="D216">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
+        <v>219</v>
+      </c>
+      <c r="B217">
+        <v>990884001</v>
+      </c>
+      <c r="C217">
+        <v>990884</v>
+      </c>
+      <c r="D217">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
+        <v>220</v>
+      </c>
+      <c r="B218">
+        <v>990883001</v>
+      </c>
+      <c r="C218">
+        <v>990883</v>
+      </c>
+      <c r="D218">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
+        <v>221</v>
+      </c>
+      <c r="B219">
+        <v>990241001</v>
+      </c>
+      <c r="C219">
+        <v>990241</v>
+      </c>
+      <c r="D219">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
+        <v>222</v>
+      </c>
+      <c r="B220">
+        <v>990583001</v>
+      </c>
+      <c r="C220">
+        <v>990583</v>
+      </c>
+      <c r="D220">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
+        <v>223</v>
+      </c>
+      <c r="B221">
+        <v>990982001</v>
+      </c>
+      <c r="C221">
+        <v>990982</v>
+      </c>
+      <c r="D221">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
+        <v>224</v>
+      </c>
+      <c r="B222">
+        <v>990585001</v>
+      </c>
+      <c r="C222">
+        <v>990585</v>
+      </c>
+      <c r="D222">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
+        <v>225</v>
+      </c>
+      <c r="B223">
+        <v>990586001</v>
+      </c>
+      <c r="C223">
+        <v>990586</v>
+      </c>
+      <c r="D223">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
+        <v>226</v>
+      </c>
+      <c r="B224">
+        <v>990588001</v>
+      </c>
+      <c r="C224">
+        <v>990588</v>
+      </c>
+      <c r="D224">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
+        <v>227</v>
+      </c>
+      <c r="B225">
+        <v>990587001</v>
+      </c>
+      <c r="C225">
+        <v>990587</v>
+      </c>
+      <c r="D225">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
+        <v>228</v>
+      </c>
+      <c r="B226">
+        <v>990589001</v>
+      </c>
+      <c r="C226">
+        <v>990589</v>
+      </c>
+      <c r="D226">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
+        <v>229</v>
+      </c>
+      <c r="B227">
+        <v>990584001</v>
+      </c>
+      <c r="C227">
+        <v>990584</v>
+      </c>
+      <c r="D227">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
+        <v>230</v>
+      </c>
+      <c r="B228">
+        <v>990590001</v>
+      </c>
+      <c r="C228">
+        <v>990590</v>
+      </c>
+      <c r="D228">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A229" t="s">
+        <v>231</v>
+      </c>
+      <c r="B229">
+        <v>990881001</v>
+      </c>
+      <c r="C229">
+        <v>990881</v>
+      </c>
+      <c r="D229">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
+        <v>232</v>
+      </c>
+      <c r="B230">
+        <v>990239001</v>
+      </c>
+      <c r="C230">
+        <v>990239</v>
+      </c>
+      <c r="D230">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
+        <v>233</v>
+      </c>
+      <c r="B231">
+        <v>990690001</v>
+      </c>
+      <c r="C231">
+        <v>990690</v>
+      </c>
+      <c r="D231">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>234</v>
+      </c>
+      <c r="B232">
+        <v>990885001</v>
+      </c>
+      <c r="C232">
+        <v>990885</v>
+      </c>
+      <c r="D232">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
+        <v>235</v>
+      </c>
+      <c r="B233">
+        <v>990888001</v>
+      </c>
+      <c r="C233">
+        <v>990888</v>
+      </c>
+      <c r="D233">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
+        <v>236</v>
+      </c>
+      <c r="B234">
+        <v>990886001</v>
+      </c>
+      <c r="C234">
+        <v>990886</v>
+      </c>
+      <c r="D234">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
+        <v>237</v>
+      </c>
+      <c r="B235">
+        <v>990689001</v>
+      </c>
+      <c r="C235">
+        <v>990689</v>
+      </c>
+      <c r="D235">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
+        <v>238</v>
+      </c>
+      <c r="B236">
+        <v>990123001</v>
+      </c>
+      <c r="C236">
+        <v>990123</v>
+      </c>
+      <c r="D236">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
+        <v>239</v>
+      </c>
+      <c r="B237">
+        <v>990124001</v>
+      </c>
+      <c r="C237">
+        <v>990124</v>
+      </c>
+      <c r="D237">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
+        <v>240</v>
+      </c>
+      <c r="B238">
+        <v>990887001</v>
+      </c>
+      <c r="C238">
+        <v>990887</v>
+      </c>
+      <c r="D238">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
+        <v>241</v>
+      </c>
+      <c r="B239">
+        <v>990121001</v>
+      </c>
+      <c r="C239">
+        <v>990121</v>
+      </c>
+      <c r="D239">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A240" t="s">
+        <v>242</v>
+      </c>
+      <c r="B240">
+        <v>990122001</v>
+      </c>
+      <c r="C240">
+        <v>990122</v>
+      </c>
+      <c r="D240">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A241" t="s">
+        <v>243</v>
+      </c>
+      <c r="B241">
+        <v>990854001</v>
+      </c>
+      <c r="C241">
+        <v>990854</v>
+      </c>
+      <c r="D241">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A242" t="s">
+        <v>244</v>
+      </c>
+      <c r="B242">
+        <v>990853001</v>
+      </c>
+      <c r="C242">
+        <v>990853</v>
+      </c>
+      <c r="D242">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A243" t="s">
+        <v>245</v>
+      </c>
+      <c r="B243">
+        <v>990691001</v>
+      </c>
+      <c r="C243">
+        <v>990691</v>
+      </c>
+      <c r="D243">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A244" t="s">
+        <v>246</v>
+      </c>
+      <c r="B244">
+        <v>990283001</v>
+      </c>
+      <c r="C244">
+        <v>990283</v>
+      </c>
+      <c r="D244">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A245" t="s">
+        <v>247</v>
+      </c>
+      <c r="B245">
+        <v>990284001</v>
+      </c>
+      <c r="C245">
+        <v>990284</v>
+      </c>
+      <c r="D245">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A246" t="s">
+        <v>248</v>
+      </c>
+      <c r="B246">
+        <v>990889001</v>
+      </c>
+      <c r="C246">
+        <v>990889</v>
+      </c>
+      <c r="D246">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A247" t="s">
+        <v>249</v>
+      </c>
+      <c r="B247">
+        <v>990233001</v>
+      </c>
+      <c r="C247">
+        <v>990233</v>
+      </c>
+      <c r="D247">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A248" t="s">
+        <v>250</v>
+      </c>
+      <c r="B248">
+        <v>990117001</v>
+      </c>
+      <c r="C248">
+        <v>990117</v>
+      </c>
+      <c r="D248">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A249" t="s">
+        <v>251</v>
+      </c>
+      <c r="B249">
+        <v>990115001</v>
+      </c>
+      <c r="C249">
+        <v>990115</v>
+      </c>
+      <c r="D249">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A250" t="s">
+        <v>252</v>
+      </c>
+      <c r="B250">
+        <v>990111001</v>
+      </c>
+      <c r="C250">
+        <v>990111</v>
+      </c>
+      <c r="D250">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A251" t="s">
+        <v>253</v>
+      </c>
+      <c r="B251">
+        <v>990112001</v>
+      </c>
+      <c r="C251">
+        <v>990112</v>
+      </c>
+      <c r="D251">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A252" t="s">
+        <v>254</v>
+      </c>
+      <c r="B252">
+        <v>990113001</v>
+      </c>
+      <c r="C252">
+        <v>990113</v>
+      </c>
+      <c r="D252">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A253" t="s">
+        <v>255</v>
+      </c>
+      <c r="B253">
+        <v>990105001</v>
+      </c>
+      <c r="C253">
+        <v>990105</v>
+      </c>
+      <c r="D253">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A254" t="s">
+        <v>256</v>
+      </c>
+      <c r="B254">
+        <v>990114001</v>
+      </c>
+      <c r="C254">
+        <v>990114</v>
+      </c>
+      <c r="D254">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A255" t="s">
+        <v>257</v>
+      </c>
+      <c r="B255">
+        <v>990107001</v>
+      </c>
+      <c r="C255">
+        <v>990107</v>
+      </c>
+      <c r="D255">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A256" t="s">
+        <v>258</v>
+      </c>
+      <c r="B256">
+        <v>990288001</v>
+      </c>
+      <c r="C256">
+        <v>990288</v>
+      </c>
+      <c r="D256">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A257" t="s">
+        <v>259</v>
+      </c>
+      <c r="B257">
+        <v>990110001</v>
+      </c>
+      <c r="C257">
+        <v>990110</v>
+      </c>
+      <c r="D257">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="258" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A258" t="s">
+        <v>260</v>
+      </c>
+      <c r="B258">
+        <v>990923001</v>
+      </c>
+      <c r="C258">
+        <v>990923</v>
+      </c>
+      <c r="D258">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A259" t="s">
+        <v>261</v>
+      </c>
+      <c r="B259">
+        <v>990104001</v>
+      </c>
+      <c r="C259">
+        <v>990104</v>
+      </c>
+      <c r="D259">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A260" t="s">
+        <v>262</v>
+      </c>
+      <c r="B260">
+        <v>990103001</v>
+      </c>
+      <c r="C260">
+        <v>990103</v>
+      </c>
+      <c r="D260">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A261" t="s">
+        <v>263</v>
+      </c>
+      <c r="B261">
+        <v>990101001</v>
+      </c>
+      <c r="C261">
+        <v>990101</v>
+      </c>
+      <c r="D261">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="262" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A262" t="s">
+        <v>264</v>
+      </c>
+      <c r="B262">
+        <v>990102001</v>
+      </c>
+      <c r="C262">
+        <v>990102</v>
+      </c>
+      <c r="D262">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="263" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A263" t="s">
+        <v>265</v>
+      </c>
+      <c r="B263">
+        <v>990078001</v>
+      </c>
+      <c r="C263">
+        <v>990078</v>
+      </c>
+      <c r="D263">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A264" t="s">
+        <v>266</v>
+      </c>
+      <c r="B264">
+        <v>990077001</v>
+      </c>
+      <c r="C264">
+        <v>990077</v>
+      </c>
+      <c r="D264">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A265" t="s">
+        <v>267</v>
+      </c>
+      <c r="B265">
+        <v>990076001</v>
+      </c>
+      <c r="C265">
+        <v>990076</v>
+      </c>
+      <c r="D265">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="266" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A266" t="s">
+        <v>268</v>
+      </c>
+      <c r="B266">
+        <v>990075001</v>
+      </c>
+      <c r="C266">
+        <v>990075</v>
+      </c>
+      <c r="D266">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="267" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A267" t="s">
+        <v>269</v>
+      </c>
+      <c r="B267">
+        <v>990131001</v>
+      </c>
+      <c r="C267">
+        <v>990131</v>
+      </c>
+      <c r="D267">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="268" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A268" t="s">
+        <v>270</v>
+      </c>
+      <c r="B268">
+        <v>990132001</v>
+      </c>
+      <c r="C268">
+        <v>990132</v>
+      </c>
+      <c r="D268">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="269" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A269" t="s">
+        <v>271</v>
+      </c>
+      <c r="B269">
+        <v>990089001</v>
+      </c>
+      <c r="C269">
+        <v>990089</v>
+      </c>
+      <c r="D269">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="270" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A270" t="s">
+        <v>272</v>
+      </c>
+      <c r="B270">
+        <v>990090001</v>
+      </c>
+      <c r="C270">
+        <v>990090</v>
+      </c>
+      <c r="D270">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="271" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A271" t="s">
+        <v>215</v>
+      </c>
+      <c r="B271">
+        <v>990086003</v>
+      </c>
+      <c r="C271">
+        <v>990086</v>
+      </c>
+      <c r="D271">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="272" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A272" t="s">
+        <v>214</v>
+      </c>
+      <c r="B272">
+        <v>990085003</v>
+      </c>
+      <c r="C272">
+        <v>990085</v>
+      </c>
+      <c r="D272">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="273" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A273" t="s">
+        <v>190</v>
+      </c>
+      <c r="B273">
+        <v>990232003</v>
+      </c>
+      <c r="C273">
+        <v>990232</v>
+      </c>
+      <c r="D273">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="274" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A274" t="s">
+        <v>189</v>
+      </c>
+      <c r="B274">
+        <v>990231003</v>
+      </c>
+      <c r="C274">
+        <v>990231</v>
+      </c>
+      <c r="D274">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="275" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A275" t="s">
+        <v>173</v>
+      </c>
+      <c r="B275">
+        <v>990120003</v>
+      </c>
+      <c r="C275">
+        <v>990120</v>
+      </c>
+      <c r="D275">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="276" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A276" t="s">
+        <v>183</v>
+      </c>
+      <c r="B276">
+        <v>990119003</v>
+      </c>
+      <c r="C276">
+        <v>990119</v>
+      </c>
+      <c r="D276">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="277" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A277" t="s">
+        <v>176</v>
+      </c>
+      <c r="B277">
+        <v>990872003</v>
+      </c>
+      <c r="C277">
+        <v>990872</v>
+      </c>
+      <c r="D277">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="278" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A278" t="s">
+        <v>233</v>
+      </c>
+      <c r="B278">
+        <v>990690003</v>
+      </c>
+      <c r="C278">
+        <v>990690</v>
+      </c>
+      <c r="D278">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="279" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A279" t="s">
+        <v>237</v>
+      </c>
+      <c r="B279">
+        <v>990689003</v>
+      </c>
+      <c r="C279">
+        <v>990689</v>
+      </c>
+      <c r="D279">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="280" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A280" t="s">
+        <v>210</v>
+      </c>
+      <c r="B280">
+        <v>990091003</v>
+      </c>
+      <c r="C280">
+        <v>990091</v>
+      </c>
+      <c r="D280">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="281" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A281" t="s">
+        <v>209</v>
+      </c>
+      <c r="B281">
+        <v>990092003</v>
+      </c>
+      <c r="C281">
+        <v>990092</v>
+      </c>
+      <c r="D281">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="282" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A282" t="s">
+        <v>182</v>
+      </c>
+      <c r="B282">
+        <v>990871003</v>
+      </c>
+      <c r="C282">
+        <v>990871</v>
+      </c>
+      <c r="D282">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="283" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A283" t="s">
+        <v>227</v>
+      </c>
+      <c r="B283">
+        <v>990587003</v>
+      </c>
+      <c r="C283">
+        <v>990587</v>
+      </c>
+      <c r="D283">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="284" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A284" t="s">
+        <v>226</v>
+      </c>
+      <c r="B284">
+        <v>990588003</v>
+      </c>
+      <c r="C284">
+        <v>990588</v>
+      </c>
+      <c r="D284">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="285" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A285" t="s">
+        <v>269</v>
+      </c>
+      <c r="B285">
+        <v>990131002</v>
+      </c>
+      <c r="C285">
+        <v>990131</v>
+      </c>
+      <c r="D285">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="286" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A286" t="s">
+        <v>188</v>
+      </c>
+      <c r="B286">
+        <v>990890003</v>
+      </c>
+      <c r="C286">
+        <v>990890</v>
+      </c>
+      <c r="D286">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="287" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A287" t="s">
+        <v>248</v>
+      </c>
+      <c r="B287">
+        <v>990889003</v>
+      </c>
+      <c r="C287">
+        <v>990889</v>
+      </c>
+      <c r="D287">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="288" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A288" t="s">
+        <v>213</v>
+      </c>
+      <c r="B288">
+        <v>990084003</v>
+      </c>
+      <c r="C288">
+        <v>990084</v>
+      </c>
+      <c r="D288">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="289" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A289" t="s">
+        <v>270</v>
+      </c>
+      <c r="B289">
+        <v>990132002</v>
+      </c>
+      <c r="C289">
+        <v>990132</v>
+      </c>
+      <c r="D289">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="290" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A290" t="s">
+        <v>273</v>
+      </c>
+      <c r="B290">
+        <v>990403002</v>
+      </c>
+      <c r="C290">
+        <v>990403</v>
+      </c>
+      <c r="D290">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="291" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A291" t="s">
+        <v>274</v>
+      </c>
+      <c r="B291">
+        <v>990087001</v>
+      </c>
+      <c r="C291">
+        <v>990087</v>
+      </c>
+      <c r="D291">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="292" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A292" t="s">
+        <v>275</v>
+      </c>
+      <c r="B292">
+        <v>990088001</v>
+      </c>
+      <c r="C292">
+        <v>990088</v>
+      </c>
+      <c r="D292">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add new all lane tolling tollclass
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/TOLLCLASS_Designations.xlsx
+++ b/utilities/NextGenFwys/TOLLCLASS_Designations.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natchison\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63B8B8F9-E0C6-4AF3-AC55-C0C5E6B1206D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{639178F9-A20B-40A7-91C5-70EAC8CC9C57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{0F0A9957-56E7-4C48-967B-2AB2A1965C2F}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{0F0A9957-56E7-4C48-967B-2AB2A1965C2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs_for_tollcalib" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="277">
   <si>
     <t>SR92 SM - I-280 Interchange to US101 Interchange - WB</t>
   </si>
@@ -866,6 +866,9 @@
   </si>
   <si>
     <t>SR-37 - WB</t>
+  </si>
+  <si>
+    <t>SR4 - I-680 (Grayson Creek) to Port Chicago  (Per Mile Tolling) - WB</t>
   </si>
 </sst>
 </file>
@@ -923,7 +926,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -932,7 +935,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1251,21 +1253,21 @@
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
-  <dimension ref="A1:D293"/>
+  <dimension ref="A1:D294"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A278" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D286" sqref="D286"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="67.1796875" customWidth="1"/>
-    <col min="3" max="3" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.1796875" customWidth="1"/>
+    <col min="1" max="1" width="67.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>153</v>
       </c>
@@ -1277,17 +1279,17 @@
       </c>
       <c r="D1" s="2"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>275</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2">
         <v>37</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>150</v>
       </c>
@@ -1298,7 +1300,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>149</v>
       </c>
@@ -1309,7 +1311,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>148</v>
       </c>
@@ -1320,7 +1322,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>147</v>
       </c>
@@ -1331,7 +1333,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>146</v>
       </c>
@@ -1342,7 +1344,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>145</v>
       </c>
@@ -1353,7 +1355,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>144</v>
       </c>
@@ -1364,7 +1366,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>143</v>
       </c>
@@ -1375,7 +1377,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>142</v>
       </c>
@@ -1386,7 +1388,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>141</v>
       </c>
@@ -1397,7 +1399,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>140</v>
       </c>
@@ -1408,7 +1410,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>139</v>
       </c>
@@ -1419,7 +1421,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>138</v>
       </c>
@@ -1430,7 +1432,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>137</v>
       </c>
@@ -1441,7 +1443,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>136</v>
       </c>
@@ -1452,7 +1454,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>135</v>
       </c>
@@ -1463,7 +1465,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>134</v>
       </c>
@@ -1474,7 +1476,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>133</v>
       </c>
@@ -1485,7 +1487,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>132</v>
       </c>
@@ -1496,7 +1498,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>131</v>
       </c>
@@ -1507,7 +1509,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>130</v>
       </c>
@@ -1518,7 +1520,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>129</v>
       </c>
@@ -1529,7 +1531,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>128</v>
       </c>
@@ -1540,7 +1542,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>127</v>
       </c>
@@ -1551,7 +1553,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>126</v>
       </c>
@@ -1562,7 +1564,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>125</v>
       </c>
@@ -1573,7 +1575,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>124</v>
       </c>
@@ -1584,7 +1586,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>123</v>
       </c>
@@ -1595,7 +1597,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>122</v>
       </c>
@@ -1606,7 +1608,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>121</v>
       </c>
@@ -1617,7 +1619,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>120</v>
       </c>
@@ -1628,7 +1630,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>119</v>
       </c>
@@ -1639,7 +1641,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>118</v>
       </c>
@@ -1650,7 +1652,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>117</v>
       </c>
@@ -1661,7 +1663,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>116</v>
       </c>
@@ -1672,7 +1674,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>115</v>
       </c>
@@ -1683,7 +1685,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>114</v>
       </c>
@@ -1694,7 +1696,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>113</v>
       </c>
@@ -1705,7 +1707,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>112</v>
       </c>
@@ -1716,7 +1718,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>111</v>
       </c>
@@ -1727,7 +1729,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>110</v>
       </c>
@@ -1738,7 +1740,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>109</v>
       </c>
@@ -1749,7 +1751,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>108</v>
       </c>
@@ -1760,7 +1762,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>107</v>
       </c>
@@ -1771,7 +1773,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>106</v>
       </c>
@@ -1782,7 +1784,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>105</v>
       </c>
@@ -1793,7 +1795,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>104</v>
       </c>
@@ -1804,7 +1806,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>103</v>
       </c>
@@ -1815,7 +1817,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>102</v>
       </c>
@@ -1826,7 +1828,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>101</v>
       </c>
@@ -1837,7 +1839,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>100</v>
       </c>
@@ -1848,7 +1850,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>99</v>
       </c>
@@ -1859,7 +1861,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>98</v>
       </c>
@@ -1870,7 +1872,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>97</v>
       </c>
@@ -1881,7 +1883,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>96</v>
       </c>
@@ -1892,7 +1894,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>95</v>
       </c>
@@ -1903,7 +1905,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>94</v>
       </c>
@@ -1914,7 +1916,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>93</v>
       </c>
@@ -1925,7 +1927,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>92</v>
       </c>
@@ -1936,7 +1938,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>91</v>
       </c>
@@ -1947,7 +1949,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>90</v>
       </c>
@@ -1958,7 +1960,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>89</v>
       </c>
@@ -1969,7 +1971,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>88</v>
       </c>
@@ -1980,7 +1982,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>87</v>
       </c>
@@ -1991,7 +1993,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>86</v>
       </c>
@@ -2002,7 +2004,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>85</v>
       </c>
@@ -2013,7 +2015,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>84</v>
       </c>
@@ -2024,7 +2026,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>83</v>
       </c>
@@ -2035,7 +2037,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>82</v>
       </c>
@@ -2046,7 +2048,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>81</v>
       </c>
@@ -2057,7 +2059,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>80</v>
       </c>
@@ -2068,7 +2070,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>79</v>
       </c>
@@ -2079,7 +2081,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>78</v>
       </c>
@@ -2087,7 +2089,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>77</v>
       </c>
@@ -2095,7 +2097,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>76</v>
       </c>
@@ -2103,7 +2105,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>75</v>
       </c>
@@ -2111,7 +2113,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>74</v>
       </c>
@@ -2122,7 +2124,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>73</v>
       </c>
@@ -2133,7 +2135,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>72</v>
       </c>
@@ -2144,7 +2146,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>71</v>
       </c>
@@ -2155,7 +2157,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>70</v>
       </c>
@@ -2166,7 +2168,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>69</v>
       </c>
@@ -2177,7 +2179,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>68</v>
       </c>
@@ -2188,7 +2190,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>67</v>
       </c>
@@ -2199,7 +2201,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>66</v>
       </c>
@@ -2210,7 +2212,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>65</v>
       </c>
@@ -2221,7 +2223,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>64</v>
       </c>
@@ -2232,7 +2234,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>63</v>
       </c>
@@ -2243,7 +2245,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>62</v>
       </c>
@@ -2254,7 +2256,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>61</v>
       </c>
@@ -2265,7 +2267,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>60</v>
       </c>
@@ -2276,7 +2278,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>59</v>
       </c>
@@ -2287,7 +2289,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>58</v>
       </c>
@@ -2298,7 +2300,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>57</v>
       </c>
@@ -2309,7 +2311,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>56</v>
       </c>
@@ -2320,7 +2322,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>55</v>
       </c>
@@ -2331,7 +2333,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="99" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>54</v>
       </c>
@@ -2342,7 +2344,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>53</v>
       </c>
@@ -2353,7 +2355,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="101" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>52</v>
       </c>
@@ -2364,7 +2366,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="102" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>51</v>
       </c>
@@ -2375,7 +2377,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>50</v>
       </c>
@@ -2386,7 +2388,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>49</v>
       </c>
@@ -2397,7 +2399,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>48</v>
       </c>
@@ -2408,7 +2410,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>47</v>
       </c>
@@ -2419,7 +2421,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>46</v>
       </c>
@@ -2430,7 +2432,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>45</v>
       </c>
@@ -2441,7 +2443,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>44</v>
       </c>
@@ -2452,7 +2454,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="110" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>43</v>
       </c>
@@ -2463,7 +2465,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="111" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>42</v>
       </c>
@@ -2474,7 +2476,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="112" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>41</v>
       </c>
@@ -2485,7 +2487,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>40</v>
       </c>
@@ -2496,7 +2498,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>39</v>
       </c>
@@ -2507,7 +2509,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>38</v>
       </c>
@@ -2518,7 +2520,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>37</v>
       </c>
@@ -2529,7 +2531,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>36</v>
       </c>
@@ -2540,7 +2542,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>35</v>
       </c>
@@ -2551,7 +2553,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>34</v>
       </c>
@@ -2562,7 +2564,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>33</v>
       </c>
@@ -2573,7 +2575,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>32</v>
       </c>
@@ -2584,7 +2586,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>31</v>
       </c>
@@ -2595,7 +2597,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>30</v>
       </c>
@@ -2606,7 +2608,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>29</v>
       </c>
@@ -2617,7 +2619,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>28</v>
       </c>
@@ -2628,7 +2630,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>27</v>
       </c>
@@ -2639,7 +2641,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>26</v>
       </c>
@@ -2650,7 +2652,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>25</v>
       </c>
@@ -2661,7 +2663,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>24</v>
       </c>
@@ -2672,7 +2674,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>23</v>
       </c>
@@ -2683,7 +2685,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>22</v>
       </c>
@@ -2694,7 +2696,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>21</v>
       </c>
@@ -2705,7 +2707,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>20</v>
       </c>
@@ -2716,7 +2718,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>19</v>
       </c>
@@ -2727,7 +2729,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>18</v>
       </c>
@@ -2738,7 +2740,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>17</v>
       </c>
@@ -2749,7 +2751,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>15</v>
       </c>
@@ -2757,7 +2759,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>14</v>
       </c>
@@ -2765,7 +2767,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>13</v>
       </c>
@@ -2773,7 +2775,7 @@
         <v>879</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>12</v>
       </c>
@@ -2781,7 +2783,7 @@
         <v>880</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>11</v>
       </c>
@@ -2789,7 +2791,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>10</v>
       </c>
@@ -2797,7 +2799,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>9</v>
       </c>
@@ -2805,7 +2807,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>8</v>
       </c>
@@ -2813,7 +2815,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>7</v>
       </c>
@@ -2821,7 +2823,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>6</v>
       </c>
@@ -2829,7 +2831,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>5</v>
       </c>
@@ -2837,7 +2839,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>4</v>
       </c>
@@ -2845,7 +2847,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>3</v>
       </c>
@@ -2853,7 +2855,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>2</v>
       </c>
@@ -2861,7 +2863,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>1</v>
       </c>
@@ -2869,7 +2871,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>0</v>
       </c>
@@ -2877,7 +2879,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>154</v>
       </c>
@@ -2885,7 +2887,7 @@
         <v>990408</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>155</v>
       </c>
@@ -2893,7 +2895,7 @@
         <v>990407</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>156</v>
       </c>
@@ -2901,7 +2903,7 @@
         <v>990243</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>157</v>
       </c>
@@ -2909,7 +2911,7 @@
         <v>990684</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>158</v>
       </c>
@@ -2917,7 +2919,7 @@
         <v>990245</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>159</v>
       </c>
@@ -2925,7 +2927,7 @@
         <v>990246</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>160</v>
       </c>
@@ -2933,7 +2935,7 @@
         <v>990683</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>161</v>
       </c>
@@ -2941,7 +2943,7 @@
         <v>990402</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>162</v>
       </c>
@@ -2949,7 +2951,7 @@
         <v>990401</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>163</v>
       </c>
@@ -2957,7 +2959,7 @@
         <v>990242</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>164</v>
       </c>
@@ -2965,7 +2967,7 @@
         <v>990581</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>165</v>
       </c>
@@ -2973,7 +2975,7 @@
         <v>990981</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>166</v>
       </c>
@@ -2981,7 +2983,7 @@
         <v>990082</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>167</v>
       </c>
@@ -2989,7 +2991,7 @@
         <v>990079</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>168</v>
       </c>
@@ -2997,7 +2999,7 @@
         <v>990582</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>169</v>
       </c>
@@ -3005,7 +3007,7 @@
         <v>990240</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>170</v>
       </c>
@@ -3013,7 +3015,7 @@
         <v>990882</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>171</v>
       </c>
@@ -3021,7 +3023,7 @@
         <v>990120</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>172</v>
       </c>
@@ -3029,7 +3031,7 @@
         <v>990855</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>173</v>
       </c>
@@ -3037,7 +3039,7 @@
         <v>990856</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>174</v>
       </c>
@@ -3045,7 +3047,7 @@
         <v>990872</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>175</v>
       </c>
@@ -3053,7 +3055,7 @@
         <v>990285</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>176</v>
       </c>
@@ -3061,7 +3063,7 @@
         <v>990171</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>177</v>
       </c>
@@ -3069,7 +3071,7 @@
         <v>990172</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>178</v>
       </c>
@@ -3077,7 +3079,7 @@
         <v>990286</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>179</v>
       </c>
@@ -3085,7 +3087,7 @@
         <v>990892</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>180</v>
       </c>
@@ -3093,7 +3095,7 @@
         <v>990871</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>181</v>
       </c>
@@ -3101,7 +3103,7 @@
         <v>990119</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>182</v>
       </c>
@@ -3109,7 +3111,7 @@
         <v>990891</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>183</v>
       </c>
@@ -3117,7 +3119,7 @@
         <v>990692</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>184</v>
       </c>
@@ -3125,7 +3127,7 @@
         <v>990118</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>185</v>
       </c>
@@ -3133,7 +3135,7 @@
         <v>990116</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>186</v>
       </c>
@@ -3141,7 +3143,7 @@
         <v>990890</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>187</v>
       </c>
@@ -3149,7 +3151,7 @@
         <v>990231</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>188</v>
       </c>
@@ -3157,7 +3159,7 @@
         <v>990232</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>189</v>
       </c>
@@ -3165,7 +3167,7 @@
         <v>990234</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>190</v>
       </c>
@@ -3173,7 +3175,7 @@
         <v>990290</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>191</v>
       </c>
@@ -3181,7 +3183,7 @@
         <v>990289</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>192</v>
       </c>
@@ -3189,7 +3191,7 @@
         <v>990927</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>193</v>
       </c>
@@ -3197,7 +3199,7 @@
         <v>990928</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>194</v>
       </c>
@@ -3205,7 +3207,7 @@
         <v>990108</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>195</v>
       </c>
@@ -3213,7 +3215,7 @@
         <v>990924</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>196</v>
       </c>
@@ -3221,7 +3223,7 @@
         <v>990109</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>197</v>
       </c>
@@ -3229,7 +3231,7 @@
         <v>990382</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>198</v>
       </c>
@@ -3237,7 +3239,7 @@
         <v>990381</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>199</v>
       </c>
@@ -3245,7 +3247,7 @@
         <v>990287</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>200</v>
       </c>
@@ -3253,7 +3255,7 @@
         <v>990106</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>201</v>
       </c>
@@ -3261,7 +3263,7 @@
         <v>990281</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>202</v>
       </c>
@@ -3269,7 +3271,7 @@
         <v>990282</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>203</v>
       </c>
@@ -3277,7 +3279,7 @@
         <v>990138</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>204</v>
       </c>
@@ -3285,7 +3287,7 @@
         <v>990137</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>205</v>
       </c>
@@ -3293,7 +3295,7 @@
         <v>990135</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>206</v>
       </c>
@@ -3301,7 +3303,7 @@
         <v>990136</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>205</v>
       </c>
@@ -3309,7 +3311,7 @@
         <v>990135</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>206</v>
       </c>
@@ -3317,7 +3319,7 @@
         <v>990136</v>
       </c>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>207</v>
       </c>
@@ -3325,7 +3327,7 @@
         <v>990092</v>
       </c>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>208</v>
       </c>
@@ -3333,7 +3335,7 @@
         <v>990091</v>
       </c>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>209</v>
       </c>
@@ -3341,7 +3343,7 @@
         <v>990244</v>
       </c>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>210</v>
       </c>
@@ -3349,7 +3351,7 @@
         <v>990083</v>
       </c>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>211</v>
       </c>
@@ -3357,7 +3359,7 @@
         <v>990084</v>
       </c>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>212</v>
       </c>
@@ -3365,7 +3367,7 @@
         <v>990085</v>
       </c>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>213</v>
       </c>
@@ -3373,7 +3375,7 @@
         <v>990086</v>
       </c>
     </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>214</v>
       </c>
@@ -3381,7 +3383,7 @@
         <v>990879</v>
       </c>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>215</v>
       </c>
@@ -3389,7 +3391,7 @@
         <v>990880</v>
       </c>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>216</v>
       </c>
@@ -3397,7 +3399,7 @@
         <v>990081</v>
       </c>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>217</v>
       </c>
@@ -3405,7 +3407,7 @@
         <v>990884</v>
       </c>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>218</v>
       </c>
@@ -3413,7 +3415,7 @@
         <v>990883</v>
       </c>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>219</v>
       </c>
@@ -3421,7 +3423,7 @@
         <v>990241</v>
       </c>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>220</v>
       </c>
@@ -3429,7 +3431,7 @@
         <v>990583</v>
       </c>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>221</v>
       </c>
@@ -3437,7 +3439,7 @@
         <v>990982</v>
       </c>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>222</v>
       </c>
@@ -3445,7 +3447,7 @@
         <v>990585</v>
       </c>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>223</v>
       </c>
@@ -3453,7 +3455,7 @@
         <v>990586</v>
       </c>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>224</v>
       </c>
@@ -3461,7 +3463,7 @@
         <v>990588</v>
       </c>
     </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>225</v>
       </c>
@@ -3469,7 +3471,7 @@
         <v>990587</v>
       </c>
     </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>226</v>
       </c>
@@ -3477,7 +3479,7 @@
         <v>990589</v>
       </c>
     </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>227</v>
       </c>
@@ -3485,7 +3487,7 @@
         <v>990584</v>
       </c>
     </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>228</v>
       </c>
@@ -3493,7 +3495,7 @@
         <v>990590</v>
       </c>
     </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>229</v>
       </c>
@@ -3501,7 +3503,7 @@
         <v>990881</v>
       </c>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>230</v>
       </c>
@@ -3509,7 +3511,7 @@
         <v>990239</v>
       </c>
     </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>231</v>
       </c>
@@ -3517,7 +3519,7 @@
         <v>990690</v>
       </c>
     </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>232</v>
       </c>
@@ -3525,7 +3527,7 @@
         <v>990885</v>
       </c>
     </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>233</v>
       </c>
@@ -3533,7 +3535,7 @@
         <v>990888</v>
       </c>
     </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>234</v>
       </c>
@@ -3541,7 +3543,7 @@
         <v>990886</v>
       </c>
     </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>235</v>
       </c>
@@ -3549,7 +3551,7 @@
         <v>990689</v>
       </c>
     </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>236</v>
       </c>
@@ -3557,7 +3559,7 @@
         <v>990123</v>
       </c>
     </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>237</v>
       </c>
@@ -3565,7 +3567,7 @@
         <v>990124</v>
       </c>
     </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>238</v>
       </c>
@@ -3573,7 +3575,7 @@
         <v>990887</v>
       </c>
     </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>239</v>
       </c>
@@ -3581,7 +3583,7 @@
         <v>990121</v>
       </c>
     </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>240</v>
       </c>
@@ -3589,7 +3591,7 @@
         <v>990122</v>
       </c>
     </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>241</v>
       </c>
@@ -3597,7 +3599,7 @@
         <v>990854</v>
       </c>
     </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>242</v>
       </c>
@@ -3605,7 +3607,7 @@
         <v>990853</v>
       </c>
     </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>243</v>
       </c>
@@ -3613,7 +3615,7 @@
         <v>990691</v>
       </c>
     </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>244</v>
       </c>
@@ -3621,7 +3623,7 @@
         <v>990283</v>
       </c>
     </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>245</v>
       </c>
@@ -3629,7 +3631,7 @@
         <v>990284</v>
       </c>
     </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>246</v>
       </c>
@@ -3637,7 +3639,7 @@
         <v>990889</v>
       </c>
     </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>247</v>
       </c>
@@ -3645,7 +3647,7 @@
         <v>990233</v>
       </c>
     </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>248</v>
       </c>
@@ -3653,7 +3655,7 @@
         <v>990117</v>
       </c>
     </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>249</v>
       </c>
@@ -3661,7 +3663,7 @@
         <v>990115</v>
       </c>
     </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>250</v>
       </c>
@@ -3669,7 +3671,7 @@
         <v>990111</v>
       </c>
     </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>251</v>
       </c>
@@ -3677,7 +3679,7 @@
         <v>990112</v>
       </c>
     </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>252</v>
       </c>
@@ -3685,7 +3687,7 @@
         <v>990113</v>
       </c>
     </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>253</v>
       </c>
@@ -3693,7 +3695,7 @@
         <v>990105</v>
       </c>
     </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>254</v>
       </c>
@@ -3701,7 +3703,7 @@
         <v>990114</v>
       </c>
     </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>255</v>
       </c>
@@ -3709,7 +3711,7 @@
         <v>990107</v>
       </c>
     </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>256</v>
       </c>
@@ -3717,7 +3719,7 @@
         <v>990288</v>
       </c>
     </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>257</v>
       </c>
@@ -3725,7 +3727,7 @@
         <v>990110</v>
       </c>
     </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>258</v>
       </c>
@@ -3733,7 +3735,7 @@
         <v>990923</v>
       </c>
     </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>259</v>
       </c>
@@ -3741,7 +3743,7 @@
         <v>990104</v>
       </c>
     </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>260</v>
       </c>
@@ -3749,7 +3751,7 @@
         <v>990103</v>
       </c>
     </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>261</v>
       </c>
@@ -3757,7 +3759,7 @@
         <v>990101</v>
       </c>
     </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>262</v>
       </c>
@@ -3765,7 +3767,7 @@
         <v>990102</v>
       </c>
     </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>263</v>
       </c>
@@ -3773,7 +3775,7 @@
         <v>990078</v>
       </c>
     </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>264</v>
       </c>
@@ -3781,7 +3783,7 @@
         <v>990077</v>
       </c>
     </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>265</v>
       </c>
@@ -3789,7 +3791,7 @@
         <v>990076</v>
       </c>
     </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>266</v>
       </c>
@@ -3797,7 +3799,7 @@
         <v>990075</v>
       </c>
     </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>267</v>
       </c>
@@ -3805,7 +3807,7 @@
         <v>990131</v>
       </c>
     </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>268</v>
       </c>
@@ -3813,7 +3815,7 @@
         <v>990132</v>
       </c>
     </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>269</v>
       </c>
@@ -3821,7 +3823,7 @@
         <v>990089</v>
       </c>
     </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>270</v>
       </c>
@@ -3829,7 +3831,7 @@
         <v>990090</v>
       </c>
     </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>213</v>
       </c>
@@ -3837,7 +3839,7 @@
         <v>990086</v>
       </c>
     </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>212</v>
       </c>
@@ -3845,7 +3847,7 @@
         <v>990085</v>
       </c>
     </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>188</v>
       </c>
@@ -3853,7 +3855,7 @@
         <v>990232</v>
       </c>
     </row>
-    <row r="275" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>187</v>
       </c>
@@ -3861,7 +3863,7 @@
         <v>990231</v>
       </c>
     </row>
-    <row r="276" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>171</v>
       </c>
@@ -3869,7 +3871,7 @@
         <v>990120</v>
       </c>
     </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>181</v>
       </c>
@@ -3877,7 +3879,7 @@
         <v>990119</v>
       </c>
     </row>
-    <row r="278" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>174</v>
       </c>
@@ -3885,7 +3887,7 @@
         <v>990872</v>
       </c>
     </row>
-    <row r="279" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>231</v>
       </c>
@@ -3893,7 +3895,7 @@
         <v>990690</v>
       </c>
     </row>
-    <row r="280" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>235</v>
       </c>
@@ -3901,7 +3903,7 @@
         <v>990689</v>
       </c>
     </row>
-    <row r="281" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>208</v>
       </c>
@@ -3909,7 +3911,7 @@
         <v>990091</v>
       </c>
     </row>
-    <row r="282" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>207</v>
       </c>
@@ -3917,7 +3919,7 @@
         <v>990092</v>
       </c>
     </row>
-    <row r="283" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>180</v>
       </c>
@@ -3925,7 +3927,7 @@
         <v>990871</v>
       </c>
     </row>
-    <row r="284" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>225</v>
       </c>
@@ -3933,7 +3935,7 @@
         <v>990587</v>
       </c>
     </row>
-    <row r="285" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>224</v>
       </c>
@@ -3941,7 +3943,7 @@
         <v>990588</v>
       </c>
     </row>
-    <row r="286" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>267</v>
       </c>
@@ -3949,7 +3951,7 @@
         <v>990131</v>
       </c>
     </row>
-    <row r="287" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>186</v>
       </c>
@@ -3957,7 +3959,7 @@
         <v>990890</v>
       </c>
     </row>
-    <row r="288" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>246</v>
       </c>
@@ -3965,7 +3967,7 @@
         <v>990889</v>
       </c>
     </row>
-    <row r="289" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>211</v>
       </c>
@@ -3973,7 +3975,7 @@
         <v>990084</v>
       </c>
     </row>
-    <row r="290" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>268</v>
       </c>
@@ -3981,7 +3983,7 @@
         <v>990132</v>
       </c>
     </row>
-    <row r="291" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>271</v>
       </c>
@@ -3989,19 +3991,27 @@
         <v>990403</v>
       </c>
     </row>
-    <row r="292" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
+        <v>276</v>
+      </c>
+      <c r="B292">
+        <v>990404</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A293" t="s">
         <v>272</v>
       </c>
-      <c r="B292">
+      <c r="B293">
         <v>990087</v>
       </c>
     </row>
-    <row r="293" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A293" t="s">
+    <row r="294" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A294" t="s">
         <v>273</v>
       </c>
-      <c r="B293">
+      <c r="B294">
         <v>990088</v>
       </c>
     </row>

</xml_diff>

<commit_message>
remove duplicates in the toll designation file
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/TOLLCLASS_Designations.xlsx
+++ b/utilities/NextGenFwys/TOLLCLASS_Designations.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natchison\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{639178F9-A20B-40A7-91C5-70EAC8CC9C57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8E70CA0-1A54-465F-8524-FF761A60A601}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{0F0A9957-56E7-4C48-967B-2AB2A1965C2F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{0F0A9957-56E7-4C48-967B-2AB2A1965C2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs_for_tollcalib" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Inputs_for_tollcalib!$A$1:$C$152</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Inputs_for_tollcalib!$A$1:$C$273</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="277">
   <si>
     <t>SR92 SM - I-280 Interchange to US101 Interchange - WB</t>
   </si>
@@ -926,13 +926,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -1253,43 +1250,40 @@
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
-  <dimension ref="A1:D294"/>
+  <dimension ref="A1:C273"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A278" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D286" sqref="D286"/>
+      <pane ySplit="1" topLeftCell="A221" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A236" sqref="A236"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="67.140625" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" customWidth="1"/>
+    <col min="1" max="1" width="67.1796875" customWidth="1"/>
+    <col min="3" max="3" width="15.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="D1" s="2"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>275</v>
       </c>
       <c r="B2">
         <v>37</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>150</v>
       </c>
@@ -1300,7 +1294,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>149</v>
       </c>
@@ -1311,7 +1305,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>148</v>
       </c>
@@ -1322,7 +1316,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>147</v>
       </c>
@@ -1333,7 +1327,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>146</v>
       </c>
@@ -1344,7 +1338,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>145</v>
       </c>
@@ -1355,7 +1349,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>144</v>
       </c>
@@ -1366,7 +1360,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>143</v>
       </c>
@@ -1377,7 +1371,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>142</v>
       </c>
@@ -1388,7 +1382,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>141</v>
       </c>
@@ -1399,7 +1393,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>140</v>
       </c>
@@ -1410,7 +1404,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>139</v>
       </c>
@@ -1421,7 +1415,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>138</v>
       </c>
@@ -1432,7 +1426,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>137</v>
       </c>
@@ -1443,7 +1437,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>136</v>
       </c>
@@ -1454,7 +1448,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>135</v>
       </c>
@@ -1465,7 +1459,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>134</v>
       </c>
@@ -1476,7 +1470,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>133</v>
       </c>
@@ -1487,7 +1481,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>132</v>
       </c>
@@ -1498,7 +1492,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>131</v>
       </c>
@@ -1509,7 +1503,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>130</v>
       </c>
@@ -1520,7 +1514,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>129</v>
       </c>
@@ -1531,7 +1525,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>128</v>
       </c>
@@ -1542,7 +1536,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>127</v>
       </c>
@@ -1553,7 +1547,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>126</v>
       </c>
@@ -1564,7 +1558,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>125</v>
       </c>
@@ -1575,7 +1569,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>124</v>
       </c>
@@ -1586,7 +1580,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>123</v>
       </c>
@@ -1597,7 +1591,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>122</v>
       </c>
@@ -1608,7 +1602,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>121</v>
       </c>
@@ -1619,7 +1613,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>120</v>
       </c>
@@ -1630,7 +1624,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>119</v>
       </c>
@@ -1641,7 +1635,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>118</v>
       </c>
@@ -1652,7 +1646,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>117</v>
       </c>
@@ -1663,7 +1657,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>116</v>
       </c>
@@ -1674,7 +1668,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>115</v>
       </c>
@@ -1685,7 +1679,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>114</v>
       </c>
@@ -1696,7 +1690,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>113</v>
       </c>
@@ -1707,7 +1701,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>112</v>
       </c>
@@ -1718,7 +1712,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>111</v>
       </c>
@@ -1729,7 +1723,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>110</v>
       </c>
@@ -1740,7 +1734,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>109</v>
       </c>
@@ -1751,7 +1745,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>108</v>
       </c>
@@ -1762,7 +1756,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>107</v>
       </c>
@@ -1773,7 +1767,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>106</v>
       </c>
@@ -1784,7 +1778,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>105</v>
       </c>
@@ -1795,7 +1789,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>104</v>
       </c>
@@ -1806,7 +1800,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>103</v>
       </c>
@@ -1817,7 +1811,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>102</v>
       </c>
@@ -1828,7 +1822,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>101</v>
       </c>
@@ -1839,7 +1833,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>100</v>
       </c>
@@ -1850,7 +1844,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>99</v>
       </c>
@@ -1861,7 +1855,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>98</v>
       </c>
@@ -1872,7 +1866,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>97</v>
       </c>
@@ -1883,7 +1877,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>96</v>
       </c>
@@ -1894,7 +1888,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>95</v>
       </c>
@@ -1905,7 +1899,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>94</v>
       </c>
@@ -1916,7 +1910,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>93</v>
       </c>
@@ -1927,7 +1921,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>92</v>
       </c>
@@ -1938,7 +1932,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>91</v>
       </c>
@@ -1949,7 +1943,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>90</v>
       </c>
@@ -1960,7 +1954,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>89</v>
       </c>
@@ -1971,7 +1965,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>88</v>
       </c>
@@ -1982,7 +1976,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>87</v>
       </c>
@@ -1993,7 +1987,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>86</v>
       </c>
@@ -2004,7 +1998,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>85</v>
       </c>
@@ -2015,7 +2009,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>84</v>
       </c>
@@ -2026,7 +2020,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>83</v>
       </c>
@@ -2037,7 +2031,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>82</v>
       </c>
@@ -2048,7 +2042,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>81</v>
       </c>
@@ -2059,7 +2053,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
         <v>80</v>
       </c>
@@ -2070,7 +2064,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
         <v>79</v>
       </c>
@@ -2081,7 +2075,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
         <v>78</v>
       </c>
@@ -2089,7 +2083,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
         <v>77</v>
       </c>
@@ -2097,7 +2091,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
         <v>76</v>
       </c>
@@ -2105,7 +2099,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
         <v>75</v>
       </c>
@@ -2113,7 +2107,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>74</v>
       </c>
@@ -2124,7 +2118,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>73</v>
       </c>
@@ -2135,7 +2129,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>72</v>
       </c>
@@ -2146,7 +2140,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>71</v>
       </c>
@@ -2157,7 +2151,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>70</v>
       </c>
@@ -2168,7 +2162,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>69</v>
       </c>
@@ -2179,7 +2173,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>68</v>
       </c>
@@ -2190,7 +2184,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>67</v>
       </c>
@@ -2201,7 +2195,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>66</v>
       </c>
@@ -2212,7 +2206,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>65</v>
       </c>
@@ -2223,7 +2217,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>64</v>
       </c>
@@ -2234,7 +2228,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>63</v>
       </c>
@@ -2245,7 +2239,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>62</v>
       </c>
@@ -2256,7 +2250,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>61</v>
       </c>
@@ -2267,7 +2261,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>60</v>
       </c>
@@ -2278,7 +2272,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>59</v>
       </c>
@@ -2289,7 +2283,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>58</v>
       </c>
@@ -2300,7 +2294,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>57</v>
       </c>
@@ -2311,7 +2305,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>56</v>
       </c>
@@ -2322,7 +2316,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>55</v>
       </c>
@@ -2333,7 +2327,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="99" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>54</v>
       </c>
@@ -2344,7 +2338,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>53</v>
       </c>
@@ -2355,7 +2349,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="101" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>52</v>
       </c>
@@ -2366,7 +2360,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="102" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>51</v>
       </c>
@@ -2377,7 +2371,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>50</v>
       </c>
@@ -2388,7 +2382,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>49</v>
       </c>
@@ -2399,7 +2393,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>48</v>
       </c>
@@ -2410,7 +2404,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>47</v>
       </c>
@@ -2421,7 +2415,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>46</v>
       </c>
@@ -2432,7 +2426,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>45</v>
       </c>
@@ -2443,7 +2437,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>44</v>
       </c>
@@ -2454,7 +2448,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="110" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>43</v>
       </c>
@@ -2465,7 +2459,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="111" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>42</v>
       </c>
@@ -2476,7 +2470,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="112" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>41</v>
       </c>
@@ -2487,7 +2481,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>40</v>
       </c>
@@ -2498,7 +2492,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>39</v>
       </c>
@@ -2509,7 +2503,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>38</v>
       </c>
@@ -2520,7 +2514,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>37</v>
       </c>
@@ -2531,7 +2525,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>36</v>
       </c>
@@ -2542,7 +2536,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>35</v>
       </c>
@@ -2553,7 +2547,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>34</v>
       </c>
@@ -2564,7 +2558,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>33</v>
       </c>
@@ -2575,7 +2569,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>32</v>
       </c>
@@ -2586,7 +2580,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>31</v>
       </c>
@@ -2597,7 +2591,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>30</v>
       </c>
@@ -2608,7 +2602,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>29</v>
       </c>
@@ -2619,7 +2613,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>28</v>
       </c>
@@ -2630,7 +2624,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>27</v>
       </c>
@@ -2641,7 +2635,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>26</v>
       </c>
@@ -2652,7 +2646,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>25</v>
       </c>
@@ -2663,7 +2657,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>24</v>
       </c>
@@ -2674,7 +2668,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>23</v>
       </c>
@@ -2685,7 +2679,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>22</v>
       </c>
@@ -2696,7 +2690,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>21</v>
       </c>
@@ -2707,7 +2701,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>20</v>
       </c>
@@ -2718,7 +2712,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>19</v>
       </c>
@@ -2729,7 +2723,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>18</v>
       </c>
@@ -2740,7 +2734,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>17</v>
       </c>
@@ -2751,7 +2745,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>15</v>
       </c>
@@ -2759,7 +2753,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>14</v>
       </c>
@@ -2767,7 +2761,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>13</v>
       </c>
@@ -2775,7 +2769,7 @@
         <v>879</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>12</v>
       </c>
@@ -2783,7 +2777,7 @@
         <v>880</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>11</v>
       </c>
@@ -2791,7 +2785,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>10</v>
       </c>
@@ -2799,7 +2793,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>9</v>
       </c>
@@ -2807,7 +2801,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>8</v>
       </c>
@@ -2815,7 +2809,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>7</v>
       </c>
@@ -2823,7 +2817,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>6</v>
       </c>
@@ -2831,7 +2825,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>5</v>
       </c>
@@ -2839,7 +2833,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>4</v>
       </c>
@@ -2847,7 +2841,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>3</v>
       </c>
@@ -2855,7 +2849,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>2</v>
       </c>
@@ -2863,7 +2857,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>1</v>
       </c>
@@ -2871,7 +2865,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>0</v>
       </c>
@@ -2879,7 +2873,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>154</v>
       </c>
@@ -2887,7 +2881,7 @@
         <v>990408</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>155</v>
       </c>
@@ -2895,7 +2889,7 @@
         <v>990407</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>156</v>
       </c>
@@ -2903,7 +2897,7 @@
         <v>990243</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>157</v>
       </c>
@@ -2911,7 +2905,7 @@
         <v>990684</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>158</v>
       </c>
@@ -2919,7 +2913,7 @@
         <v>990245</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>159</v>
       </c>
@@ -2927,7 +2921,7 @@
         <v>990246</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>160</v>
       </c>
@@ -2935,7 +2929,7 @@
         <v>990683</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>161</v>
       </c>
@@ -2943,7 +2937,7 @@
         <v>990402</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>162</v>
       </c>
@@ -2951,7 +2945,7 @@
         <v>990401</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>163</v>
       </c>
@@ -2959,7 +2953,7 @@
         <v>990242</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>164</v>
       </c>
@@ -2967,7 +2961,7 @@
         <v>990581</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>165</v>
       </c>
@@ -2975,7 +2969,7 @@
         <v>990981</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>166</v>
       </c>
@@ -2983,7 +2977,7 @@
         <v>990082</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>167</v>
       </c>
@@ -2991,7 +2985,7 @@
         <v>990079</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>168</v>
       </c>
@@ -2999,7 +2993,7 @@
         <v>990582</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>169</v>
       </c>
@@ -3007,7 +3001,7 @@
         <v>990240</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>170</v>
       </c>
@@ -3015,7 +3009,7 @@
         <v>990882</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>171</v>
       </c>
@@ -3023,7 +3017,7 @@
         <v>990120</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>172</v>
       </c>
@@ -3031,7 +3025,7 @@
         <v>990855</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>173</v>
       </c>
@@ -3039,7 +3033,7 @@
         <v>990856</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>174</v>
       </c>
@@ -3047,7 +3041,7 @@
         <v>990872</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>175</v>
       </c>
@@ -3055,7 +3049,7 @@
         <v>990285</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>176</v>
       </c>
@@ -3063,7 +3057,7 @@
         <v>990171</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>177</v>
       </c>
@@ -3071,7 +3065,7 @@
         <v>990172</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>178</v>
       </c>
@@ -3079,7 +3073,7 @@
         <v>990286</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>179</v>
       </c>
@@ -3087,7 +3081,7 @@
         <v>990892</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>180</v>
       </c>
@@ -3095,7 +3089,7 @@
         <v>990871</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>181</v>
       </c>
@@ -3103,7 +3097,7 @@
         <v>990119</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>182</v>
       </c>
@@ -3111,7 +3105,7 @@
         <v>990891</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>183</v>
       </c>
@@ -3119,7 +3113,7 @@
         <v>990692</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>184</v>
       </c>
@@ -3127,7 +3121,7 @@
         <v>990118</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>185</v>
       </c>
@@ -3135,7 +3129,7 @@
         <v>990116</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>186</v>
       </c>
@@ -3143,7 +3137,7 @@
         <v>990890</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>187</v>
       </c>
@@ -3151,7 +3145,7 @@
         <v>990231</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>188</v>
       </c>
@@ -3159,7 +3153,7 @@
         <v>990232</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>189</v>
       </c>
@@ -3167,7 +3161,7 @@
         <v>990234</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>190</v>
       </c>
@@ -3175,7 +3169,7 @@
         <v>990290</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>191</v>
       </c>
@@ -3183,7 +3177,7 @@
         <v>990289</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>192</v>
       </c>
@@ -3191,7 +3185,7 @@
         <v>990927</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>193</v>
       </c>
@@ -3199,7 +3193,7 @@
         <v>990928</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
         <v>194</v>
       </c>
@@ -3207,7 +3201,7 @@
         <v>990108</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>195</v>
       </c>
@@ -3215,7 +3209,7 @@
         <v>990924</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
         <v>196</v>
       </c>
@@ -3223,7 +3217,7 @@
         <v>990109</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>197</v>
       </c>
@@ -3231,7 +3225,7 @@
         <v>990382</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
         <v>198</v>
       </c>
@@ -3239,7 +3233,7 @@
         <v>990381</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
         <v>199</v>
       </c>
@@ -3247,7 +3241,7 @@
         <v>990287</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
         <v>200</v>
       </c>
@@ -3255,7 +3249,7 @@
         <v>990106</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
         <v>201</v>
       </c>
@@ -3263,7 +3257,7 @@
         <v>990281</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
         <v>202</v>
       </c>
@@ -3271,7 +3265,7 @@
         <v>990282</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
         <v>203</v>
       </c>
@@ -3279,7 +3273,7 @@
         <v>990138</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
         <v>204</v>
       </c>
@@ -3287,7 +3281,7 @@
         <v>990137</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
         <v>205</v>
       </c>
@@ -3295,7 +3289,7 @@
         <v>990135</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
         <v>206</v>
       </c>
@@ -3303,715 +3297,547 @@
         <v>990136</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B206">
-        <v>990135</v>
-      </c>
-    </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990092</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B207">
-        <v>990136</v>
-      </c>
-    </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990091</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B208">
-        <v>990092</v>
-      </c>
-    </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990244</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B209">
-        <v>990091</v>
-      </c>
-    </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990083</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B210">
-        <v>990244</v>
-      </c>
-    </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990084</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B211">
-        <v>990083</v>
-      </c>
-    </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990085</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="B212">
-        <v>990084</v>
-      </c>
-    </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990086</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B213">
-        <v>990085</v>
-      </c>
-    </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990879</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B214">
-        <v>990086</v>
-      </c>
-    </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990880</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B215">
-        <v>990879</v>
-      </c>
-    </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990081</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B216">
-        <v>990880</v>
-      </c>
-    </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990884</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B217">
-        <v>990081</v>
-      </c>
-    </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990883</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="B218">
-        <v>990884</v>
-      </c>
-    </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990241</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B219">
-        <v>990883</v>
-      </c>
-    </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990583</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B220">
-        <v>990241</v>
-      </c>
-    </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990982</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B221">
-        <v>990583</v>
-      </c>
-    </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990585</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="B222">
-        <v>990982</v>
-      </c>
-    </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990586</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B223">
-        <v>990585</v>
-      </c>
-    </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990588</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B224">
-        <v>990586</v>
-      </c>
-    </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990587</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B225">
-        <v>990588</v>
-      </c>
-    </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990589</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="B226">
-        <v>990587</v>
-      </c>
-    </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990584</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B227">
-        <v>990589</v>
-      </c>
-    </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990590</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B228">
-        <v>990584</v>
-      </c>
-    </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990881</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B229">
-        <v>990590</v>
-      </c>
-    </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990239</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B230">
-        <v>990881</v>
-      </c>
-    </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990690</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B231">
-        <v>990239</v>
-      </c>
-    </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990885</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B232">
-        <v>990690</v>
-      </c>
-    </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990888</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B233">
-        <v>990885</v>
-      </c>
-    </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990886</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="B234">
-        <v>990888</v>
-      </c>
-    </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990689</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B235">
-        <v>990886</v>
-      </c>
-    </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990123</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B236">
-        <v>990689</v>
-      </c>
-    </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990124</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B237">
-        <v>990123</v>
-      </c>
-    </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990887</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="B238">
-        <v>990124</v>
-      </c>
-    </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990121</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B239">
-        <v>990887</v>
-      </c>
-    </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990122</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="B240">
-        <v>990121</v>
-      </c>
-    </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990854</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B241">
-        <v>990122</v>
-      </c>
-    </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990853</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B242">
-        <v>990854</v>
-      </c>
-    </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990691</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B243">
-        <v>990853</v>
-      </c>
-    </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990283</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="B244">
-        <v>990691</v>
-      </c>
-    </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990284</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B245">
-        <v>990283</v>
-      </c>
-    </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990889</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="B246">
-        <v>990284</v>
-      </c>
-    </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990233</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B247">
-        <v>990889</v>
-      </c>
-    </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990117</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="B248">
-        <v>990233</v>
-      </c>
-    </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990115</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B249">
-        <v>990117</v>
-      </c>
-    </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990111</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A250" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="B250">
-        <v>990115</v>
-      </c>
-    </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990112</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="B251">
-        <v>990111</v>
-      </c>
-    </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990113</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A252" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="B252">
-        <v>990112</v>
-      </c>
-    </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990105</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A253" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B253">
-        <v>990113</v>
-      </c>
-    </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990114</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A254" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="B254">
-        <v>990105</v>
-      </c>
-    </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990107</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B255">
-        <v>990114</v>
-      </c>
-    </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990288</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A256" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="B256">
-        <v>990107</v>
-      </c>
-    </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990110</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A257" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B257">
-        <v>990288</v>
-      </c>
-    </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990923</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A258" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="B258">
-        <v>990110</v>
-      </c>
-    </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990104</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A259" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B259">
-        <v>990923</v>
-      </c>
-    </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990103</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A260" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="B260">
-        <v>990104</v>
-      </c>
-    </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990101</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A261" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="B261">
-        <v>990103</v>
-      </c>
-    </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990102</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A262" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="B262">
-        <v>990101</v>
-      </c>
-    </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990078</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A263" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="B263">
-        <v>990102</v>
-      </c>
-    </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990077</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A264" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="B264">
-        <v>990078</v>
-      </c>
-    </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990076</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A265" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="B265">
-        <v>990077</v>
-      </c>
-    </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990075</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A266" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="B266">
-        <v>990076</v>
-      </c>
-    </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990131</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A267" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="B267">
-        <v>990075</v>
-      </c>
-    </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990132</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A268" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="B268">
-        <v>990131</v>
-      </c>
-    </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990089</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A269" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="B269">
-        <v>990132</v>
-      </c>
-    </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990090</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A270" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B270">
-        <v>990089</v>
-      </c>
-    </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990403</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A271" t="s">
-        <v>270</v>
+        <v>276</v>
       </c>
       <c r="B271">
-        <v>990090</v>
-      </c>
-    </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990404</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A272" t="s">
-        <v>213</v>
+        <v>272</v>
       </c>
       <c r="B272">
-        <v>990086</v>
-      </c>
-    </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
+        <v>990087</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A273" t="s">
-        <v>212</v>
+        <v>273</v>
       </c>
       <c r="B273">
-        <v>990085</v>
-      </c>
-    </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A274" t="s">
-        <v>188</v>
-      </c>
-      <c r="B274">
-        <v>990232</v>
-      </c>
-    </row>
-    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A275" t="s">
-        <v>187</v>
-      </c>
-      <c r="B275">
-        <v>990231</v>
-      </c>
-    </row>
-    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A276" t="s">
-        <v>171</v>
-      </c>
-      <c r="B276">
-        <v>990120</v>
-      </c>
-    </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A277" t="s">
-        <v>181</v>
-      </c>
-      <c r="B277">
-        <v>990119</v>
-      </c>
-    </row>
-    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A278" t="s">
-        <v>174</v>
-      </c>
-      <c r="B278">
-        <v>990872</v>
-      </c>
-    </row>
-    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A279" t="s">
-        <v>231</v>
-      </c>
-      <c r="B279">
-        <v>990690</v>
-      </c>
-    </row>
-    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A280" t="s">
-        <v>235</v>
-      </c>
-      <c r="B280">
-        <v>990689</v>
-      </c>
-    </row>
-    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A281" t="s">
-        <v>208</v>
-      </c>
-      <c r="B281">
-        <v>990091</v>
-      </c>
-    </row>
-    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A282" t="s">
-        <v>207</v>
-      </c>
-      <c r="B282">
-        <v>990092</v>
-      </c>
-    </row>
-    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A283" t="s">
-        <v>180</v>
-      </c>
-      <c r="B283">
-        <v>990871</v>
-      </c>
-    </row>
-    <row r="284" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A284" t="s">
-        <v>225</v>
-      </c>
-      <c r="B284">
-        <v>990587</v>
-      </c>
-    </row>
-    <row r="285" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A285" t="s">
-        <v>224</v>
-      </c>
-      <c r="B285">
-        <v>990588</v>
-      </c>
-    </row>
-    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A286" t="s">
-        <v>267</v>
-      </c>
-      <c r="B286">
-        <v>990131</v>
-      </c>
-    </row>
-    <row r="287" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A287" t="s">
-        <v>186</v>
-      </c>
-      <c r="B287">
-        <v>990890</v>
-      </c>
-    </row>
-    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A288" t="s">
-        <v>246</v>
-      </c>
-      <c r="B288">
-        <v>990889</v>
-      </c>
-    </row>
-    <row r="289" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A289" t="s">
-        <v>211</v>
-      </c>
-      <c r="B289">
-        <v>990084</v>
-      </c>
-    </row>
-    <row r="290" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A290" t="s">
-        <v>268</v>
-      </c>
-      <c r="B290">
-        <v>990132</v>
-      </c>
-    </row>
-    <row r="291" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A291" t="s">
-        <v>271</v>
-      </c>
-      <c r="B291">
-        <v>990403</v>
-      </c>
-    </row>
-    <row r="292" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A292" t="s">
-        <v>276</v>
-      </c>
-      <c r="B292">
-        <v>990404</v>
-      </c>
-    </row>
-    <row r="293" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A293" t="s">
-        <v>272</v>
-      </c>
-      <c r="B293">
-        <v>990087</v>
-      </c>
-    </row>
-    <row r="294" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A294" t="s">
-        <v>273</v>
-      </c>
-      <c r="B294">
         <v>990088</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Assigned toll classes for major arterials
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/TOLLCLASS_Designations.xlsx
+++ b/utilities/NextGenFwys/TOLLCLASS_Designations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8E70CA0-1A54-465F-8524-FF761A60A601}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A90757D2-920A-4047-9563-366E9D3A8A0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{0F0A9957-56E7-4C48-967B-2AB2A1965C2F}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="296">
   <si>
     <t>SR92 SM - I-280 Interchange to US101 Interchange - WB</t>
   </si>
@@ -869,6 +869,63 @@
   </si>
   <si>
     <t>SR4 - I-680 (Grayson Creek) to Port Chicago  (Per Mile Tolling) - WB</t>
+  </si>
+  <si>
+    <t>[Santa Clara: paralleling US-101] Monterey Rd - NB</t>
+  </si>
+  <si>
+    <t>[Santa Clara: paralleling US-101] Monterey Rd - SB</t>
+  </si>
+  <si>
+    <t>[Alameda: paralleling I-880/I-580] International Blvd (to E 14th St to Mission Blvd) - NB</t>
+  </si>
+  <si>
+    <t>[Alameda: paralleling I-880/I-580] International Blvd (to E 14th St to Mission Blvd) - SB</t>
+  </si>
+  <si>
+    <t>[San Francisco: paralleling US-101] 3rd (to Bayshore Blvd to Airport Blvd) - NB</t>
+  </si>
+  <si>
+    <t>[San Francisco: paralleling US-101] 3rd (to Bayshore Blvd to Airport Blvd) - SB</t>
+  </si>
+  <si>
+    <t>[Alameda: paralleling I-80] San Pablo - NB</t>
+  </si>
+  <si>
+    <t>[Alameda: paralleling I-80] San Pablo - SB</t>
+  </si>
+  <si>
+    <t>[Santa Clara: paralleling I-280] Foothill Expy - NB</t>
+  </si>
+  <si>
+    <t>[Santa Clara: paralleling I-280] Foothill Expy - SB</t>
+  </si>
+  <si>
+    <t>[Contra Costa: paralleling SR-4] Leland Rd (to Delta Fair Blvd) - EB</t>
+  </si>
+  <si>
+    <t>[Contra Costa: paralleling SR-4] Leland Rd (to Delta Fair Blvd) -WB</t>
+  </si>
+  <si>
+    <t>[Solano: paralleling I-80] Texas St - EB</t>
+  </si>
+  <si>
+    <t>[Solano: paralleling I-80] Texas St - WB</t>
+  </si>
+  <si>
+    <t>[Santa Clara: paralleling 237/680] Tasman Dr (to N Capitol Ave to E Capitol Expy) - EB</t>
+  </si>
+  <si>
+    <t>[Sonoma: paralleling US-101] Mendocino Ave +  Santa Rosa Ave - NB</t>
+  </si>
+  <si>
+    <t>[Sonoma: paralleling US-101] Mendocino Ave +  Santa Rosa Ave - SB</t>
+  </si>
+  <si>
+    <t>[San Mateo: paralleling US-101/I-280] El Camino Real - NB</t>
+  </si>
+  <si>
+    <t>[San Mateo: paralleling US-101/I-280] El Camino Real - SB</t>
   </si>
 </sst>
 </file>
@@ -1250,16 +1307,16 @@
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
-  <dimension ref="A1:C273"/>
+  <dimension ref="A1:C293"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A221" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A236" sqref="A236"/>
+      <pane ySplit="1" topLeftCell="A229" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C279" sqref="C279"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="67.1796875" customWidth="1"/>
+    <col min="1" max="1" width="79.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3841,6 +3898,166 @@
         <v>990088</v>
       </c>
     </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A274" t="s">
+        <v>279</v>
+      </c>
+      <c r="B274">
+        <v>770580</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A275" t="s">
+        <v>280</v>
+      </c>
+      <c r="B275">
+        <v>770851</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A276" t="s">
+        <v>277</v>
+      </c>
+      <c r="B276">
+        <v>770101</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A277" t="s">
+        <v>278</v>
+      </c>
+      <c r="B277">
+        <v>770102</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A278" t="s">
+        <v>281</v>
+      </c>
+      <c r="B278">
+        <v>770103</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A279" t="s">
+        <v>282</v>
+      </c>
+      <c r="B279">
+        <v>770104</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A280" t="s">
+        <v>283</v>
+      </c>
+      <c r="B280">
+        <v>770080</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A281" t="s">
+        <v>284</v>
+      </c>
+      <c r="B281">
+        <v>770081</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A282" t="s">
+        <v>294</v>
+      </c>
+      <c r="B282">
+        <v>770105</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A283" t="s">
+        <v>295</v>
+      </c>
+      <c r="B283">
+        <v>770106</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A284" t="s">
+        <v>292</v>
+      </c>
+      <c r="B284">
+        <v>770107</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A285" t="s">
+        <v>293</v>
+      </c>
+      <c r="B285">
+        <v>770108</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A286" t="s">
+        <v>291</v>
+      </c>
+      <c r="B286">
+        <v>770237</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A287" t="s">
+        <v>291</v>
+      </c>
+      <c r="B287">
+        <v>770238</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A288" t="s">
+        <v>289</v>
+      </c>
+      <c r="B288">
+        <v>770082</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A289" t="s">
+        <v>290</v>
+      </c>
+      <c r="B289">
+        <v>770083</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A290" t="s">
+        <v>287</v>
+      </c>
+      <c r="B290">
+        <v>770004</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A291" t="s">
+        <v>288</v>
+      </c>
+      <c r="B291">
+        <v>770005</v>
+      </c>
+    </row>
+    <row r="292" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A292" t="s">
+        <v>285</v>
+      </c>
+      <c r="B292">
+        <v>770280</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A293" t="s">
+        <v>286</v>
+      </c>
+      <c r="B293">
+        <v>770281</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated typo for tollclass value
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/TOLLCLASS_Designations.xlsx
+++ b/utilities/NextGenFwys/TOLLCLASS_Designations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sisrael\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A90757D2-920A-4047-9563-366E9D3A8A0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A46D614-EFF9-4A11-8594-A87A68B702C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{0F0A9957-56E7-4C48-967B-2AB2A1965C2F}"/>
   </bookViews>
@@ -1310,8 +1310,8 @@
   <dimension ref="A1:C293"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A229" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C279" sqref="C279"/>
+      <pane ySplit="1" topLeftCell="A265" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A281" sqref="A281"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3911,7 +3911,7 @@
         <v>280</v>
       </c>
       <c r="B275">
-        <v>770851</v>
+        <v>770581</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Fixed a typo for Tasman Drive Arterial (both directions said EB)
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/TOLLCLASS_Designations.xlsx
+++ b/utilities/NextGenFwys/TOLLCLASS_Designations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sisrael\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A46D614-EFF9-4A11-8594-A87A68B702C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B1F8081-8FE5-41A8-B28B-067092000E93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{0F0A9957-56E7-4C48-967B-2AB2A1965C2F}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="297">
   <si>
     <t>SR92 SM - I-280 Interchange to US101 Interchange - WB</t>
   </si>
@@ -926,6 +926,9 @@
   </si>
   <si>
     <t>[San Mateo: paralleling US-101/I-280] El Camino Real - SB</t>
+  </si>
+  <si>
+    <t>[Santa Clara: paralleling 237/680] Tasman Dr (to N Capitol Ave to E Capitol Expy) - WB</t>
   </si>
 </sst>
 </file>
@@ -1311,7 +1314,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A265" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A281" sqref="A281"/>
+      <selection pane="bottomLeft" activeCell="A287" sqref="A287"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4004,7 +4007,7 @@
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A287" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="B287">
         <v>770238</v>

</xml_diff>

<commit_message>
Broke tollclasses up into 13 segments, by direction
Network project is here: NGF_BPALT13Segments
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/TOLLCLASS_Designations.xlsx
+++ b/utilities/NextGenFwys/TOLLCLASS_Designations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sisrael\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B1F8081-8FE5-41A8-B28B-067092000E93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0931EB2-42A2-4EC8-9E10-70068C55C665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{0F0A9957-56E7-4C48-967B-2AB2A1965C2F}"/>
+    <workbookView xWindow="33720" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0F0A9957-56E7-4C48-967B-2AB2A1965C2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs_for_tollcalib" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="323">
   <si>
     <t>SR92 SM - I-280 Interchange to US101 Interchange - WB</t>
   </si>
@@ -929,6 +929,84 @@
   </si>
   <si>
     <t>[Santa Clara: paralleling 237/680] Tasman Dr (to N Capitol Ave to E Capitol Expy) - WB</t>
+  </si>
+  <si>
+    <t>101_Marin_N - NGF_BPALT13Segments</t>
+  </si>
+  <si>
+    <t>101_Marin_S - NGF_BPALT13Segments</t>
+  </si>
+  <si>
+    <t>101_Peninsula_N - NGF_BPALT13Segments</t>
+  </si>
+  <si>
+    <t>101_Peninsula_S - NGF_BPALT13Segments</t>
+  </si>
+  <si>
+    <t>237_E - NGF_BPALT13Segments</t>
+  </si>
+  <si>
+    <t>237_W - NGF_BPALT13Segments</t>
+  </si>
+  <si>
+    <t>238_N - NGF_BPALT13Segments</t>
+  </si>
+  <si>
+    <t>238_S - NGF_BPALT13Segments</t>
+  </si>
+  <si>
+    <t>280_N - NGF_BPALT13Segments</t>
+  </si>
+  <si>
+    <t>280_S - NGF_BPALT13Segments</t>
+  </si>
+  <si>
+    <t>380_E - NGF_BPALT13Segments</t>
+  </si>
+  <si>
+    <t>380_W - NGF_BPALT13Segments</t>
+  </si>
+  <si>
+    <t>580_E - NGF_BPALT13Segments</t>
+  </si>
+  <si>
+    <t>580_W - NGF_BPALT13Segments</t>
+  </si>
+  <si>
+    <t>680_N - NGF_BPALT13Segments</t>
+  </si>
+  <si>
+    <t>680_S - NGF_BPALT13Segments</t>
+  </si>
+  <si>
+    <t>80_E - NGF_BPALT13Segments</t>
+  </si>
+  <si>
+    <t>80_W - NGF_BPALT13Segments</t>
+  </si>
+  <si>
+    <t>85_87_N - NGF_BPALT13Segments</t>
+  </si>
+  <si>
+    <t>85_87_S - NGF_BPALT13Segments</t>
+  </si>
+  <si>
+    <t>880_17_N - NGF_BPALT13Segments</t>
+  </si>
+  <si>
+    <t>880_17_S - NGF_BPALT13Segments</t>
+  </si>
+  <si>
+    <t>92_E - NGF_BPALT13Segments</t>
+  </si>
+  <si>
+    <t>92_W - NGF_BPALT13Segments</t>
+  </si>
+  <si>
+    <t>980_24_680_242_4_E - NGF_BPALT13Segments</t>
+  </si>
+  <si>
+    <t>980_24_680_242_4_W - NGF_BPALT13Segments</t>
   </si>
 </sst>
 </file>
@@ -1310,11 +1388,11 @@
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
-  <dimension ref="A1:C293"/>
+  <dimension ref="A1:C319"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A265" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A287" sqref="A287"/>
+      <pane ySplit="1" topLeftCell="A290" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A305" sqref="A305"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4061,6 +4139,214 @@
         <v>770281</v>
       </c>
     </row>
+    <row r="294" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A294" t="s">
+        <v>297</v>
+      </c>
+      <c r="B294">
+        <v>980001</v>
+      </c>
+    </row>
+    <row r="295" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A295" t="s">
+        <v>298</v>
+      </c>
+      <c r="B295">
+        <v>980002</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A296" t="s">
+        <v>299</v>
+      </c>
+      <c r="B296">
+        <v>980003</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A297" t="s">
+        <v>300</v>
+      </c>
+      <c r="B297">
+        <v>980004</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A298" t="s">
+        <v>301</v>
+      </c>
+      <c r="B298">
+        <v>980005</v>
+      </c>
+    </row>
+    <row r="299" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A299" t="s">
+        <v>302</v>
+      </c>
+      <c r="B299">
+        <v>980006</v>
+      </c>
+    </row>
+    <row r="300" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A300" t="s">
+        <v>303</v>
+      </c>
+      <c r="B300">
+        <v>980007</v>
+      </c>
+    </row>
+    <row r="301" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A301" t="s">
+        <v>304</v>
+      </c>
+      <c r="B301">
+        <v>980008</v>
+      </c>
+    </row>
+    <row r="302" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A302" t="s">
+        <v>305</v>
+      </c>
+      <c r="B302">
+        <v>980009</v>
+      </c>
+    </row>
+    <row r="303" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A303" t="s">
+        <v>306</v>
+      </c>
+      <c r="B303">
+        <v>980010</v>
+      </c>
+    </row>
+    <row r="304" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A304" t="s">
+        <v>307</v>
+      </c>
+      <c r="B304">
+        <v>980011</v>
+      </c>
+    </row>
+    <row r="305" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A305" t="s">
+        <v>308</v>
+      </c>
+      <c r="B305">
+        <v>980012</v>
+      </c>
+    </row>
+    <row r="306" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A306" t="s">
+        <v>309</v>
+      </c>
+      <c r="B306">
+        <v>980013</v>
+      </c>
+    </row>
+    <row r="307" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A307" t="s">
+        <v>310</v>
+      </c>
+      <c r="B307">
+        <v>980014</v>
+      </c>
+    </row>
+    <row r="308" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A308" t="s">
+        <v>311</v>
+      </c>
+      <c r="B308">
+        <v>980015</v>
+      </c>
+    </row>
+    <row r="309" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A309" t="s">
+        <v>312</v>
+      </c>
+      <c r="B309">
+        <v>980016</v>
+      </c>
+    </row>
+    <row r="310" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A310" t="s">
+        <v>313</v>
+      </c>
+      <c r="B310">
+        <v>980017</v>
+      </c>
+    </row>
+    <row r="311" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A311" t="s">
+        <v>314</v>
+      </c>
+      <c r="B311">
+        <v>980018</v>
+      </c>
+    </row>
+    <row r="312" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A312" t="s">
+        <v>315</v>
+      </c>
+      <c r="B312">
+        <v>980019</v>
+      </c>
+    </row>
+    <row r="313" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A313" t="s">
+        <v>316</v>
+      </c>
+      <c r="B313">
+        <v>980020</v>
+      </c>
+    </row>
+    <row r="314" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A314" t="s">
+        <v>317</v>
+      </c>
+      <c r="B314">
+        <v>980021</v>
+      </c>
+    </row>
+    <row r="315" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A315" t="s">
+        <v>318</v>
+      </c>
+      <c r="B315">
+        <v>980022</v>
+      </c>
+    </row>
+    <row r="316" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A316" t="s">
+        <v>319</v>
+      </c>
+      <c r="B316">
+        <v>980023</v>
+      </c>
+    </row>
+    <row r="317" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A317" t="s">
+        <v>320</v>
+      </c>
+      <c r="B317">
+        <v>980024</v>
+      </c>
+    </row>
+    <row r="318" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A318" t="s">
+        <v>321</v>
+      </c>
+      <c r="B318">
+        <v>980025</v>
+      </c>
+    </row>
+    <row r="319" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A319" t="s">
+        <v>322</v>
+      </c>
+      <c r="B319">
+        <v>980026</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated tollclass numbering convention
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/TOLLCLASS_Designations.xlsx
+++ b/utilities/NextGenFwys/TOLLCLASS_Designations.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sisrael\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0931EB2-42A2-4EC8-9E10-70068C55C665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B907B276-C8E2-4850-9C0C-9411FD8D61D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33720" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0F0A9957-56E7-4C48-967B-2AB2A1965C2F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" activeTab="1" xr2:uid="{0F0A9957-56E7-4C48-967B-2AB2A1965C2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs_for_tollcalib" sheetId="1" r:id="rId1"/>
+    <sheet name="Readme - numbering convention" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Inputs_for_tollcalib!$A$1:$C$273</definedName>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="330">
   <si>
     <t>SR92 SM - I-280 Interchange to US101 Interchange - WB</t>
   </si>
@@ -1007,13 +1008,34 @@
   </si>
   <si>
     <t>980_24_680_242_4_W - NGF_BPALT13Segments</t>
+  </si>
+  <si>
+    <t>tollclass &gt; 900000</t>
+  </si>
+  <si>
+    <t>tollclass = 99</t>
+  </si>
+  <si>
+    <t>all-lane tolling system in the blueprint</t>
+  </si>
+  <si>
+    <t>NGF arterial tolling</t>
+  </si>
+  <si>
+    <t>NGF highway tolling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">900000 &gt; tollclass &gt; 700000 </t>
+  </si>
+  <si>
+    <t>Tollclass numbering convention</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1042,6 +1064,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1064,12 +1094,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1390,9 +1421,9 @@
   </sheetPr>
   <dimension ref="A1:C319"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A290" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A305" sqref="A305"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4351,4 +4382,56 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DF77F54-B726-43F2-A3A6-3E118A23C251}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="27.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="3" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>324</v>
+      </c>
+      <c r="B3" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>328</v>
+      </c>
+      <c r="B4" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>323</v>
+      </c>
+      <c r="B5" t="s">
+        <v>327</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add MIX_TOLL to make it configurable in TollCalib_CheckSpeeds.R
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/TOLLCLASS_Designations.xlsx
+++ b/utilities/NextGenFwys/TOLLCLASS_Designations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\llin\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F8B33C2-1AF0-49C0-B1EF-50607EC94B01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9E26F03-D581-44EC-8024-515E51BAF117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2955" yWindow="1410" windowWidth="16905" windowHeight="16155" xr2:uid="{0F0A9957-56E7-4C48-967B-2AB2A1965C2F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{0F0A9957-56E7-4C48-967B-2AB2A1965C2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs_for_tollcalib" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="333">
   <si>
     <t>SR92 SM - I-280 Interchange to US101 Interchange - WB</t>
   </si>
@@ -1035,6 +1035,9 @@
   </si>
   <si>
     <t>MAX_TOLL</t>
+  </si>
+  <si>
+    <t>MIN_TOLL</t>
   </si>
 </sst>
 </file>
@@ -1425,20 +1428,21 @@
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
-  <dimension ref="A1:E319"/>
+  <dimension ref="A1:F319"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomLeft" activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="79.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>153</v>
       </c>
@@ -1454,8 +1458,11 @@
       <c r="E1" s="2" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="2" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>275</v>
       </c>
@@ -1469,8 +1476,11 @@
       <c r="E2">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>150</v>
       </c>
@@ -1486,8 +1496,11 @@
       <c r="E3">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>149</v>
       </c>
@@ -1503,8 +1516,11 @@
       <c r="E4">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>148</v>
       </c>
@@ -1520,8 +1536,11 @@
       <c r="E5">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>147</v>
       </c>
@@ -1537,8 +1556,11 @@
       <c r="E6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>146</v>
       </c>
@@ -1554,8 +1576,11 @@
       <c r="E7">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>145</v>
       </c>
@@ -1571,8 +1596,11 @@
       <c r="E8">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>144</v>
       </c>
@@ -1588,8 +1616,11 @@
       <c r="E9">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>143</v>
       </c>
@@ -1605,8 +1636,11 @@
       <c r="E10">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>142</v>
       </c>
@@ -1622,8 +1656,11 @@
       <c r="E11">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>141</v>
       </c>
@@ -1639,8 +1676,11 @@
       <c r="E12">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>140</v>
       </c>
@@ -1656,8 +1696,11 @@
       <c r="E13">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>139</v>
       </c>
@@ -1673,8 +1716,11 @@
       <c r="E14">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>138</v>
       </c>
@@ -1690,8 +1736,11 @@
       <c r="E15">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>137</v>
       </c>
@@ -1707,8 +1756,11 @@
       <c r="E16">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>136</v>
       </c>
@@ -1724,8 +1776,11 @@
       <c r="E17">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>135</v>
       </c>
@@ -1741,8 +1796,11 @@
       <c r="E18">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>134</v>
       </c>
@@ -1758,8 +1816,11 @@
       <c r="E19">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>133</v>
       </c>
@@ -1775,8 +1836,11 @@
       <c r="E20">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>132</v>
       </c>
@@ -1792,8 +1856,11 @@
       <c r="E21">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>131</v>
       </c>
@@ -1809,8 +1876,11 @@
       <c r="E22">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F22">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>130</v>
       </c>
@@ -1826,8 +1896,11 @@
       <c r="E23">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F23">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>129</v>
       </c>
@@ -1843,8 +1916,11 @@
       <c r="E24">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F24">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>128</v>
       </c>
@@ -1860,8 +1936,11 @@
       <c r="E25">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F25">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>127</v>
       </c>
@@ -1877,8 +1956,11 @@
       <c r="E26">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F26">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>126</v>
       </c>
@@ -1894,8 +1976,11 @@
       <c r="E27">
         <v>5</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F27">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>125</v>
       </c>
@@ -1911,8 +1996,11 @@
       <c r="E28">
         <v>5</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F28">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>124</v>
       </c>
@@ -1928,8 +2016,11 @@
       <c r="E29">
         <v>5</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F29">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>123</v>
       </c>
@@ -1945,8 +2036,11 @@
       <c r="E30">
         <v>5</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F30">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>122</v>
       </c>
@@ -1962,8 +2056,11 @@
       <c r="E31">
         <v>5</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F31">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>121</v>
       </c>
@@ -1979,8 +2076,11 @@
       <c r="E32">
         <v>5</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F32">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>120</v>
       </c>
@@ -1996,8 +2096,11 @@
       <c r="E33">
         <v>5</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F33">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>119</v>
       </c>
@@ -2013,8 +2116,11 @@
       <c r="E34">
         <v>5</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F34">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>118</v>
       </c>
@@ -2030,8 +2136,11 @@
       <c r="E35">
         <v>5</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F35">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>117</v>
       </c>
@@ -2047,8 +2156,11 @@
       <c r="E36">
         <v>5</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F36">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>116</v>
       </c>
@@ -2064,8 +2176,11 @@
       <c r="E37">
         <v>5</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F37">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>115</v>
       </c>
@@ -2081,8 +2196,11 @@
       <c r="E38">
         <v>5</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F38">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>114</v>
       </c>
@@ -2098,8 +2216,11 @@
       <c r="E39">
         <v>5</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F39">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>113</v>
       </c>
@@ -2115,8 +2236,11 @@
       <c r="E40">
         <v>5</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F40">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>112</v>
       </c>
@@ -2132,8 +2256,11 @@
       <c r="E41">
         <v>5</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F41">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>111</v>
       </c>
@@ -2149,8 +2276,11 @@
       <c r="E42">
         <v>5</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F42">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>110</v>
       </c>
@@ -2166,8 +2296,11 @@
       <c r="E43">
         <v>5</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F43">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>109</v>
       </c>
@@ -2183,8 +2316,11 @@
       <c r="E44">
         <v>5</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F44">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>108</v>
       </c>
@@ -2200,8 +2336,11 @@
       <c r="E45">
         <v>5</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F45">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>107</v>
       </c>
@@ -2217,8 +2356,11 @@
       <c r="E46">
         <v>5</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F46">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>106</v>
       </c>
@@ -2234,8 +2376,11 @@
       <c r="E47">
         <v>5</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F47">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>105</v>
       </c>
@@ -2251,8 +2396,11 @@
       <c r="E48">
         <v>5</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F48">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>104</v>
       </c>
@@ -2268,8 +2416,11 @@
       <c r="E49">
         <v>5</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F49">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>103</v>
       </c>
@@ -2285,8 +2436,11 @@
       <c r="E50">
         <v>5</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F50">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>102</v>
       </c>
@@ -2302,8 +2456,11 @@
       <c r="E51">
         <v>5</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F51">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>101</v>
       </c>
@@ -2319,8 +2476,11 @@
       <c r="E52">
         <v>5</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F52">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>100</v>
       </c>
@@ -2336,8 +2496,11 @@
       <c r="E53">
         <v>5</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F53">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>99</v>
       </c>
@@ -2353,8 +2516,11 @@
       <c r="E54">
         <v>5</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F54">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>98</v>
       </c>
@@ -2370,8 +2536,11 @@
       <c r="E55">
         <v>5</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F55">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>97</v>
       </c>
@@ -2387,8 +2556,11 @@
       <c r="E56">
         <v>5</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F56">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>96</v>
       </c>
@@ -2404,8 +2576,11 @@
       <c r="E57">
         <v>5</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F57">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>95</v>
       </c>
@@ -2421,8 +2596,11 @@
       <c r="E58">
         <v>5</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F58">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>94</v>
       </c>
@@ -2438,8 +2616,11 @@
       <c r="E59">
         <v>5</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F59">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>93</v>
       </c>
@@ -2455,8 +2636,11 @@
       <c r="E60">
         <v>5</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F60">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>92</v>
       </c>
@@ -2472,8 +2656,11 @@
       <c r="E61">
         <v>5</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F61">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>91</v>
       </c>
@@ -2489,8 +2676,11 @@
       <c r="E62">
         <v>5</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F62">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>90</v>
       </c>
@@ -2506,8 +2696,11 @@
       <c r="E63">
         <v>5</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F63">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>89</v>
       </c>
@@ -2523,8 +2716,11 @@
       <c r="E64">
         <v>5</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F64">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>88</v>
       </c>
@@ -2540,8 +2736,11 @@
       <c r="E65">
         <v>5</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F65">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>87</v>
       </c>
@@ -2557,8 +2756,11 @@
       <c r="E66">
         <v>5</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F66">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>86</v>
       </c>
@@ -2574,8 +2776,11 @@
       <c r="E67">
         <v>5</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F67">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>85</v>
       </c>
@@ -2591,8 +2796,11 @@
       <c r="E68">
         <v>5</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F68">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>84</v>
       </c>
@@ -2608,8 +2816,11 @@
       <c r="E69">
         <v>5</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F69">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>83</v>
       </c>
@@ -2625,8 +2836,11 @@
       <c r="E70">
         <v>5</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F70">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>82</v>
       </c>
@@ -2642,8 +2856,11 @@
       <c r="E71">
         <v>5</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F71">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>81</v>
       </c>
@@ -2659,8 +2876,11 @@
       <c r="E72">
         <v>5</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F72">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>80</v>
       </c>
@@ -2676,8 +2896,11 @@
       <c r="E73">
         <v>5</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F73">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>79</v>
       </c>
@@ -2693,8 +2916,11 @@
       <c r="E74">
         <v>5</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F74">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>78</v>
       </c>
@@ -2707,8 +2933,11 @@
       <c r="E75">
         <v>5</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F75">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>77</v>
       </c>
@@ -2721,8 +2950,11 @@
       <c r="E76">
         <v>5</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F76">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>76</v>
       </c>
@@ -2735,8 +2967,11 @@
       <c r="E77">
         <v>5</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F77">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>75</v>
       </c>
@@ -2749,8 +2984,11 @@
       <c r="E78">
         <v>5</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F78">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>74</v>
       </c>
@@ -2766,8 +3004,11 @@
       <c r="E79">
         <v>5</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F79">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>73</v>
       </c>
@@ -2783,8 +3024,11 @@
       <c r="E80">
         <v>5</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F80">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>72</v>
       </c>
@@ -2800,8 +3044,11 @@
       <c r="E81">
         <v>5</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F81">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>71</v>
       </c>
@@ -2817,8 +3064,11 @@
       <c r="E82">
         <v>5</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F82">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>70</v>
       </c>
@@ -2834,8 +3084,11 @@
       <c r="E83">
         <v>5</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F83">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>69</v>
       </c>
@@ -2851,8 +3104,11 @@
       <c r="E84">
         <v>5</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F84">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>68</v>
       </c>
@@ -2868,8 +3124,11 @@
       <c r="E85">
         <v>5</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F85">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>67</v>
       </c>
@@ -2885,8 +3144,11 @@
       <c r="E86">
         <v>5</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F86">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>66</v>
       </c>
@@ -2902,8 +3164,11 @@
       <c r="E87">
         <v>5</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F87">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>65</v>
       </c>
@@ -2919,8 +3184,11 @@
       <c r="E88">
         <v>5</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F88">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>64</v>
       </c>
@@ -2936,8 +3204,11 @@
       <c r="E89">
         <v>5</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F89">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>63</v>
       </c>
@@ -2953,8 +3224,11 @@
       <c r="E90">
         <v>5</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F90">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>62</v>
       </c>
@@ -2970,8 +3244,11 @@
       <c r="E91">
         <v>5</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F91">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>61</v>
       </c>
@@ -2987,8 +3264,11 @@
       <c r="E92">
         <v>5</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F92">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>60</v>
       </c>
@@ -3004,8 +3284,11 @@
       <c r="E93">
         <v>5</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F93">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>59</v>
       </c>
@@ -3021,8 +3304,11 @@
       <c r="E94">
         <v>5</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F94">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>58</v>
       </c>
@@ -3038,8 +3324,11 @@
       <c r="E95">
         <v>5</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F95">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>57</v>
       </c>
@@ -3055,8 +3344,11 @@
       <c r="E96">
         <v>5</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F96">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>56</v>
       </c>
@@ -3072,8 +3364,11 @@
       <c r="E97">
         <v>5</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F97">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>55</v>
       </c>
@@ -3089,8 +3384,11 @@
       <c r="E98">
         <v>5</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F98">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>54</v>
       </c>
@@ -3106,8 +3404,11 @@
       <c r="E99">
         <v>5</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F99">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>53</v>
       </c>
@@ -3123,8 +3424,11 @@
       <c r="E100">
         <v>5</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F100">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>52</v>
       </c>
@@ -3140,8 +3444,11 @@
       <c r="E101">
         <v>5</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F101">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>51</v>
       </c>
@@ -3157,8 +3464,11 @@
       <c r="E102">
         <v>5</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F102">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>50</v>
       </c>
@@ -3174,8 +3484,11 @@
       <c r="E103">
         <v>5</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F103">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>49</v>
       </c>
@@ -3191,8 +3504,11 @@
       <c r="E104">
         <v>5</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F104">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>48</v>
       </c>
@@ -3208,8 +3524,11 @@
       <c r="E105">
         <v>5</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F105">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>47</v>
       </c>
@@ -3225,8 +3544,11 @@
       <c r="E106">
         <v>5</v>
       </c>
-    </row>
-    <row r="107" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F106">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>46</v>
       </c>
@@ -3242,8 +3564,11 @@
       <c r="E107">
         <v>5</v>
       </c>
-    </row>
-    <row r="108" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F107">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>45</v>
       </c>
@@ -3259,8 +3584,11 @@
       <c r="E108">
         <v>5</v>
       </c>
-    </row>
-    <row r="109" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F108">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>44</v>
       </c>
@@ -3276,8 +3604,11 @@
       <c r="E109">
         <v>5</v>
       </c>
-    </row>
-    <row r="110" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F109">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>43</v>
       </c>
@@ -3293,8 +3624,11 @@
       <c r="E110">
         <v>5</v>
       </c>
-    </row>
-    <row r="111" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F110">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>42</v>
       </c>
@@ -3310,8 +3644,11 @@
       <c r="E111">
         <v>5</v>
       </c>
-    </row>
-    <row r="112" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F111">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>41</v>
       </c>
@@ -3327,8 +3664,11 @@
       <c r="E112">
         <v>5</v>
       </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F112">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>40</v>
       </c>
@@ -3344,8 +3684,11 @@
       <c r="E113">
         <v>5</v>
       </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F113">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>39</v>
       </c>
@@ -3361,8 +3704,11 @@
       <c r="E114">
         <v>5</v>
       </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F114">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>38</v>
       </c>
@@ -3378,8 +3724,11 @@
       <c r="E115">
         <v>5</v>
       </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F115">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>37</v>
       </c>
@@ -3395,8 +3744,11 @@
       <c r="E116">
         <v>5</v>
       </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F116">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>36</v>
       </c>
@@ -3412,8 +3764,11 @@
       <c r="E117">
         <v>5</v>
       </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F117">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>35</v>
       </c>
@@ -3429,8 +3784,11 @@
       <c r="E118">
         <v>5</v>
       </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F118">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>34</v>
       </c>
@@ -3446,8 +3804,11 @@
       <c r="E119">
         <v>5</v>
       </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F119">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>33</v>
       </c>
@@ -3463,8 +3824,11 @@
       <c r="E120">
         <v>5</v>
       </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F120">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>32</v>
       </c>
@@ -3480,8 +3844,11 @@
       <c r="E121">
         <v>5</v>
       </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F121">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>31</v>
       </c>
@@ -3497,8 +3864,11 @@
       <c r="E122">
         <v>5</v>
       </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F122">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>30</v>
       </c>
@@ -3514,8 +3884,11 @@
       <c r="E123">
         <v>5</v>
       </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F123">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>29</v>
       </c>
@@ -3531,8 +3904,11 @@
       <c r="E124">
         <v>5</v>
       </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F124">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>28</v>
       </c>
@@ -3548,8 +3924,11 @@
       <c r="E125">
         <v>5</v>
       </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F125">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>27</v>
       </c>
@@ -3565,8 +3944,11 @@
       <c r="E126">
         <v>5</v>
       </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F126">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>26</v>
       </c>
@@ -3582,8 +3964,11 @@
       <c r="E127">
         <v>5</v>
       </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F127">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>25</v>
       </c>
@@ -3599,8 +3984,11 @@
       <c r="E128">
         <v>5</v>
       </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F128">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>24</v>
       </c>
@@ -3616,8 +4004,11 @@
       <c r="E129">
         <v>5</v>
       </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F129">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>23</v>
       </c>
@@ -3633,8 +4024,11 @@
       <c r="E130">
         <v>5</v>
       </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F130">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>22</v>
       </c>
@@ -3650,8 +4044,11 @@
       <c r="E131">
         <v>5</v>
       </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F131">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>21</v>
       </c>
@@ -3667,8 +4064,11 @@
       <c r="E132">
         <v>5</v>
       </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F132">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>20</v>
       </c>
@@ -3684,8 +4084,11 @@
       <c r="E133">
         <v>5</v>
       </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F133">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>19</v>
       </c>
@@ -3701,8 +4104,11 @@
       <c r="E134">
         <v>5</v>
       </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F134">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>18</v>
       </c>
@@ -3718,8 +4124,11 @@
       <c r="E135">
         <v>5</v>
       </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F135">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>17</v>
       </c>
@@ -3735,8 +4144,11 @@
       <c r="E136">
         <v>5</v>
       </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F136">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>15</v>
       </c>
@@ -3749,8 +4161,11 @@
       <c r="E137">
         <v>5</v>
       </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F137">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>14</v>
       </c>
@@ -3763,8 +4178,11 @@
       <c r="E138">
         <v>5</v>
       </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F138">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>13</v>
       </c>
@@ -3777,8 +4195,11 @@
       <c r="E139">
         <v>5</v>
       </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F139">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>12</v>
       </c>
@@ -3791,8 +4212,11 @@
       <c r="E140">
         <v>5</v>
       </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F140">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>11</v>
       </c>
@@ -3805,8 +4229,11 @@
       <c r="E141">
         <v>5</v>
       </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F141">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>10</v>
       </c>
@@ -3819,8 +4246,11 @@
       <c r="E142">
         <v>5</v>
       </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F142">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>9</v>
       </c>
@@ -3833,8 +4263,11 @@
       <c r="E143">
         <v>5</v>
       </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F143">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>8</v>
       </c>
@@ -3847,8 +4280,11 @@
       <c r="E144">
         <v>5</v>
       </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F144">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>7</v>
       </c>
@@ -3861,8 +4297,11 @@
       <c r="E145">
         <v>5</v>
       </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F145">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>6</v>
       </c>
@@ -3875,8 +4314,11 @@
       <c r="E146">
         <v>5</v>
       </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F146">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>5</v>
       </c>
@@ -3889,8 +4331,11 @@
       <c r="E147">
         <v>5</v>
       </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F147">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>4</v>
       </c>
@@ -3903,8 +4348,11 @@
       <c r="E148">
         <v>5</v>
       </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F148">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>3</v>
       </c>
@@ -3917,8 +4365,11 @@
       <c r="E149">
         <v>5</v>
       </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F149">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>2</v>
       </c>
@@ -3931,8 +4382,11 @@
       <c r="E150">
         <v>5</v>
       </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F150">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>1</v>
       </c>
@@ -3945,8 +4399,11 @@
       <c r="E151">
         <v>5</v>
       </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F151">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>0</v>
       </c>
@@ -3959,8 +4416,11 @@
       <c r="E152">
         <v>5</v>
       </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F152">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>154</v>
       </c>
@@ -3973,8 +4433,11 @@
       <c r="E153">
         <v>5</v>
       </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F153">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>155</v>
       </c>
@@ -3987,8 +4450,11 @@
       <c r="E154">
         <v>5</v>
       </c>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F154">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>156</v>
       </c>
@@ -4001,8 +4467,11 @@
       <c r="E155">
         <v>5</v>
       </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F155">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>157</v>
       </c>
@@ -4015,8 +4484,11 @@
       <c r="E156">
         <v>5</v>
       </c>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F156">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>158</v>
       </c>
@@ -4029,8 +4501,11 @@
       <c r="E157">
         <v>5</v>
       </c>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F157">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>159</v>
       </c>
@@ -4043,8 +4518,11 @@
       <c r="E158">
         <v>5</v>
       </c>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F158">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>160</v>
       </c>
@@ -4057,8 +4535,11 @@
       <c r="E159">
         <v>5</v>
       </c>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F159">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>161</v>
       </c>
@@ -4071,8 +4552,11 @@
       <c r="E160">
         <v>5</v>
       </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F160">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>162</v>
       </c>
@@ -4085,8 +4569,11 @@
       <c r="E161">
         <v>5</v>
       </c>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F161">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>163</v>
       </c>
@@ -4099,8 +4586,11 @@
       <c r="E162">
         <v>5</v>
       </c>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F162">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>164</v>
       </c>
@@ -4113,8 +4603,11 @@
       <c r="E163">
         <v>5</v>
       </c>
-    </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F163">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>165</v>
       </c>
@@ -4127,8 +4620,11 @@
       <c r="E164">
         <v>5</v>
       </c>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F164">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>166</v>
       </c>
@@ -4141,8 +4637,11 @@
       <c r="E165">
         <v>5</v>
       </c>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F165">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>167</v>
       </c>
@@ -4155,8 +4654,11 @@
       <c r="E166">
         <v>5</v>
       </c>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F166">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>168</v>
       </c>
@@ -4169,8 +4671,11 @@
       <c r="E167">
         <v>5</v>
       </c>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F167">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>169</v>
       </c>
@@ -4183,8 +4688,11 @@
       <c r="E168">
         <v>5</v>
       </c>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F168">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>170</v>
       </c>
@@ -4197,8 +4705,11 @@
       <c r="E169">
         <v>5</v>
       </c>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F169">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>171</v>
       </c>
@@ -4211,8 +4722,11 @@
       <c r="E170">
         <v>5</v>
       </c>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F170">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>172</v>
       </c>
@@ -4225,8 +4739,11 @@
       <c r="E171">
         <v>5</v>
       </c>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F171">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>173</v>
       </c>
@@ -4239,8 +4756,11 @@
       <c r="E172">
         <v>5</v>
       </c>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F172">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>174</v>
       </c>
@@ -4253,8 +4773,11 @@
       <c r="E173">
         <v>5</v>
       </c>
-    </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F173">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>175</v>
       </c>
@@ -4267,8 +4790,11 @@
       <c r="E174">
         <v>5</v>
       </c>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F174">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>176</v>
       </c>
@@ -4281,8 +4807,11 @@
       <c r="E175">
         <v>5</v>
       </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F175">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>177</v>
       </c>
@@ -4295,8 +4824,11 @@
       <c r="E176">
         <v>5</v>
       </c>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F176">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>178</v>
       </c>
@@ -4309,8 +4841,11 @@
       <c r="E177">
         <v>5</v>
       </c>
-    </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F177">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>179</v>
       </c>
@@ -4323,8 +4858,11 @@
       <c r="E178">
         <v>5</v>
       </c>
-    </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F178">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>180</v>
       </c>
@@ -4337,8 +4875,11 @@
       <c r="E179">
         <v>5</v>
       </c>
-    </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F179">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>181</v>
       </c>
@@ -4351,8 +4892,11 @@
       <c r="E180">
         <v>5</v>
       </c>
-    </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F180">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>182</v>
       </c>
@@ -4365,8 +4909,11 @@
       <c r="E181">
         <v>5</v>
       </c>
-    </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F181">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>183</v>
       </c>
@@ -4379,8 +4926,11 @@
       <c r="E182">
         <v>5</v>
       </c>
-    </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F182">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>184</v>
       </c>
@@ -4393,8 +4943,11 @@
       <c r="E183">
         <v>5</v>
       </c>
-    </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F183">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>185</v>
       </c>
@@ -4407,8 +4960,11 @@
       <c r="E184">
         <v>5</v>
       </c>
-    </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F184">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>186</v>
       </c>
@@ -4421,8 +4977,11 @@
       <c r="E185">
         <v>5</v>
       </c>
-    </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F185">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>187</v>
       </c>
@@ -4435,8 +4994,11 @@
       <c r="E186">
         <v>5</v>
       </c>
-    </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F186">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>188</v>
       </c>
@@ -4449,8 +5011,11 @@
       <c r="E187">
         <v>5</v>
       </c>
-    </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F187">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>189</v>
       </c>
@@ -4463,8 +5028,11 @@
       <c r="E188">
         <v>5</v>
       </c>
-    </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F188">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>190</v>
       </c>
@@ -4477,8 +5045,11 @@
       <c r="E189">
         <v>5</v>
       </c>
-    </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F189">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>191</v>
       </c>
@@ -4491,8 +5062,11 @@
       <c r="E190">
         <v>5</v>
       </c>
-    </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F190">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>192</v>
       </c>
@@ -4505,8 +5079,11 @@
       <c r="E191">
         <v>5</v>
       </c>
-    </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F191">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>193</v>
       </c>
@@ -4519,8 +5096,11 @@
       <c r="E192">
         <v>5</v>
       </c>
-    </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F192">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>194</v>
       </c>
@@ -4533,8 +5113,11 @@
       <c r="E193">
         <v>5</v>
       </c>
-    </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F193">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>195</v>
       </c>
@@ -4547,8 +5130,11 @@
       <c r="E194">
         <v>5</v>
       </c>
-    </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F194">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>196</v>
       </c>
@@ -4561,8 +5147,11 @@
       <c r="E195">
         <v>5</v>
       </c>
-    </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F195">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>197</v>
       </c>
@@ -4575,8 +5164,11 @@
       <c r="E196">
         <v>5</v>
       </c>
-    </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F196">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>198</v>
       </c>
@@ -4589,8 +5181,11 @@
       <c r="E197">
         <v>5</v>
       </c>
-    </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F197">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>199</v>
       </c>
@@ -4603,8 +5198,11 @@
       <c r="E198">
         <v>5</v>
       </c>
-    </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F198">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>200</v>
       </c>
@@ -4617,8 +5215,11 @@
       <c r="E199">
         <v>5</v>
       </c>
-    </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F199">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>201</v>
       </c>
@@ -4631,8 +5232,11 @@
       <c r="E200">
         <v>5</v>
       </c>
-    </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F200">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>202</v>
       </c>
@@ -4645,8 +5249,11 @@
       <c r="E201">
         <v>5</v>
       </c>
-    </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F201">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>203</v>
       </c>
@@ -4659,8 +5266,11 @@
       <c r="E202">
         <v>5</v>
       </c>
-    </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F202">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>204</v>
       </c>
@@ -4673,8 +5283,11 @@
       <c r="E203">
         <v>5</v>
       </c>
-    </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F203">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>205</v>
       </c>
@@ -4687,8 +5300,11 @@
       <c r="E204">
         <v>5</v>
       </c>
-    </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F204">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>206</v>
       </c>
@@ -4701,8 +5317,11 @@
       <c r="E205">
         <v>5</v>
       </c>
-    </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F205">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>207</v>
       </c>
@@ -4715,8 +5334,11 @@
       <c r="E206">
         <v>5</v>
       </c>
-    </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F206">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>208</v>
       </c>
@@ -4729,8 +5351,11 @@
       <c r="E207">
         <v>5</v>
       </c>
-    </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F207">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>209</v>
       </c>
@@ -4743,8 +5368,11 @@
       <c r="E208">
         <v>5</v>
       </c>
-    </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F208">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>210</v>
       </c>
@@ -4757,8 +5385,11 @@
       <c r="E209">
         <v>5</v>
       </c>
-    </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F209">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>211</v>
       </c>
@@ -4771,8 +5402,11 @@
       <c r="E210">
         <v>5</v>
       </c>
-    </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F210">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>212</v>
       </c>
@@ -4785,8 +5419,11 @@
       <c r="E211">
         <v>5</v>
       </c>
-    </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F211">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>213</v>
       </c>
@@ -4799,8 +5436,11 @@
       <c r="E212">
         <v>5</v>
       </c>
-    </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F212">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>214</v>
       </c>
@@ -4813,8 +5453,11 @@
       <c r="E213">
         <v>5</v>
       </c>
-    </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F213">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>215</v>
       </c>
@@ -4827,8 +5470,11 @@
       <c r="E214">
         <v>5</v>
       </c>
-    </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F214">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>216</v>
       </c>
@@ -4841,8 +5487,11 @@
       <c r="E215">
         <v>5</v>
       </c>
-    </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F215">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>217</v>
       </c>
@@ -4855,8 +5504,11 @@
       <c r="E216">
         <v>5</v>
       </c>
-    </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F216">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>218</v>
       </c>
@@ -4869,8 +5521,11 @@
       <c r="E217">
         <v>5</v>
       </c>
-    </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F217">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>219</v>
       </c>
@@ -4883,8 +5538,11 @@
       <c r="E218">
         <v>5</v>
       </c>
-    </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F218">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>220</v>
       </c>
@@ -4897,8 +5555,11 @@
       <c r="E219">
         <v>5</v>
       </c>
-    </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F219">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>221</v>
       </c>
@@ -4911,8 +5572,11 @@
       <c r="E220">
         <v>5</v>
       </c>
-    </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F220">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>222</v>
       </c>
@@ -4925,8 +5589,11 @@
       <c r="E221">
         <v>5</v>
       </c>
-    </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F221">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>223</v>
       </c>
@@ -4939,8 +5606,11 @@
       <c r="E222">
         <v>5</v>
       </c>
-    </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F222">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>224</v>
       </c>
@@ -4953,8 +5623,11 @@
       <c r="E223">
         <v>5</v>
       </c>
-    </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F223">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>225</v>
       </c>
@@ -4967,8 +5640,11 @@
       <c r="E224">
         <v>5</v>
       </c>
-    </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F224">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>226</v>
       </c>
@@ -4981,8 +5657,11 @@
       <c r="E225">
         <v>5</v>
       </c>
-    </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F225">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>227</v>
       </c>
@@ -4995,8 +5674,11 @@
       <c r="E226">
         <v>5</v>
       </c>
-    </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F226">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>228</v>
       </c>
@@ -5009,8 +5691,11 @@
       <c r="E227">
         <v>5</v>
       </c>
-    </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F227">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>229</v>
       </c>
@@ -5023,8 +5708,11 @@
       <c r="E228">
         <v>5</v>
       </c>
-    </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F228">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>230</v>
       </c>
@@ -5037,8 +5725,11 @@
       <c r="E229">
         <v>5</v>
       </c>
-    </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F229">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>231</v>
       </c>
@@ -5051,8 +5742,11 @@
       <c r="E230">
         <v>5</v>
       </c>
-    </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F230">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>232</v>
       </c>
@@ -5065,8 +5759,11 @@
       <c r="E231">
         <v>5</v>
       </c>
-    </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F231">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>233</v>
       </c>
@@ -5079,8 +5776,11 @@
       <c r="E232">
         <v>5</v>
       </c>
-    </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F232">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>234</v>
       </c>
@@ -5093,8 +5793,11 @@
       <c r="E233">
         <v>5</v>
       </c>
-    </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F233">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>235</v>
       </c>
@@ -5107,8 +5810,11 @@
       <c r="E234">
         <v>5</v>
       </c>
-    </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F234">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>236</v>
       </c>
@@ -5121,8 +5827,11 @@
       <c r="E235">
         <v>5</v>
       </c>
-    </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F235">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>237</v>
       </c>
@@ -5135,8 +5844,11 @@
       <c r="E236">
         <v>5</v>
       </c>
-    </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F236">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>238</v>
       </c>
@@ -5149,8 +5861,11 @@
       <c r="E237">
         <v>5</v>
       </c>
-    </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F237">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>239</v>
       </c>
@@ -5163,8 +5878,11 @@
       <c r="E238">
         <v>5</v>
       </c>
-    </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F238">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>240</v>
       </c>
@@ -5177,8 +5895,11 @@
       <c r="E239">
         <v>5</v>
       </c>
-    </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F239">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>241</v>
       </c>
@@ -5191,8 +5912,11 @@
       <c r="E240">
         <v>5</v>
       </c>
-    </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F240">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>242</v>
       </c>
@@ -5205,8 +5929,11 @@
       <c r="E241">
         <v>5</v>
       </c>
-    </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F241">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>243</v>
       </c>
@@ -5219,8 +5946,11 @@
       <c r="E242">
         <v>5</v>
       </c>
-    </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F242">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>244</v>
       </c>
@@ -5233,8 +5963,11 @@
       <c r="E243">
         <v>5</v>
       </c>
-    </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F243">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>245</v>
       </c>
@@ -5247,8 +5980,11 @@
       <c r="E244">
         <v>5</v>
       </c>
-    </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F244">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>246</v>
       </c>
@@ -5261,8 +5997,11 @@
       <c r="E245">
         <v>5</v>
       </c>
-    </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F245">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>247</v>
       </c>
@@ -5275,8 +6014,11 @@
       <c r="E246">
         <v>5</v>
       </c>
-    </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F246">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>248</v>
       </c>
@@ -5289,8 +6031,11 @@
       <c r="E247">
         <v>5</v>
       </c>
-    </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F247">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="248" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>249</v>
       </c>
@@ -5303,8 +6048,11 @@
       <c r="E248">
         <v>5</v>
       </c>
-    </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F248">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>250</v>
       </c>
@@ -5317,8 +6065,11 @@
       <c r="E249">
         <v>5</v>
       </c>
-    </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F249">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>251</v>
       </c>
@@ -5331,8 +6082,11 @@
       <c r="E250">
         <v>5</v>
       </c>
-    </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F250">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>252</v>
       </c>
@@ -5345,8 +6099,11 @@
       <c r="E251">
         <v>5</v>
       </c>
-    </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F251">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>253</v>
       </c>
@@ -5359,8 +6116,11 @@
       <c r="E252">
         <v>5</v>
       </c>
-    </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F252">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="253" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>254</v>
       </c>
@@ -5373,8 +6133,11 @@
       <c r="E253">
         <v>5</v>
       </c>
-    </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F253">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="254" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>255</v>
       </c>
@@ -5387,8 +6150,11 @@
       <c r="E254">
         <v>5</v>
       </c>
-    </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F254">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>256</v>
       </c>
@@ -5401,8 +6167,11 @@
       <c r="E255">
         <v>5</v>
       </c>
-    </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F255">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="256" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>257</v>
       </c>
@@ -5415,8 +6184,11 @@
       <c r="E256">
         <v>5</v>
       </c>
-    </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F256">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="257" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>258</v>
       </c>
@@ -5429,8 +6201,11 @@
       <c r="E257">
         <v>5</v>
       </c>
-    </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F257">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="258" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>259</v>
       </c>
@@ -5443,8 +6218,11 @@
       <c r="E258">
         <v>5</v>
       </c>
-    </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F258">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="259" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>260</v>
       </c>
@@ -5457,8 +6235,11 @@
       <c r="E259">
         <v>5</v>
       </c>
-    </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F259">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="260" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>261</v>
       </c>
@@ -5471,8 +6252,11 @@
       <c r="E260">
         <v>5</v>
       </c>
-    </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F260">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="261" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>262</v>
       </c>
@@ -5485,8 +6269,11 @@
       <c r="E261">
         <v>5</v>
       </c>
-    </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F261">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="262" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>263</v>
       </c>
@@ -5499,8 +6286,11 @@
       <c r="E262">
         <v>5</v>
       </c>
-    </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F262">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="263" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>264</v>
       </c>
@@ -5513,8 +6303,11 @@
       <c r="E263">
         <v>5</v>
       </c>
-    </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F263">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="264" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>265</v>
       </c>
@@ -5527,8 +6320,11 @@
       <c r="E264">
         <v>5</v>
       </c>
-    </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F264">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>266</v>
       </c>
@@ -5541,8 +6337,11 @@
       <c r="E265">
         <v>5</v>
       </c>
-    </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F265">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>267</v>
       </c>
@@ -5555,8 +6354,11 @@
       <c r="E266">
         <v>5</v>
       </c>
-    </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F266">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>268</v>
       </c>
@@ -5569,8 +6371,11 @@
       <c r="E267">
         <v>5</v>
       </c>
-    </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F267">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="268" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>269</v>
       </c>
@@ -5583,8 +6388,11 @@
       <c r="E268">
         <v>5</v>
       </c>
-    </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F268">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="269" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>270</v>
       </c>
@@ -5597,8 +6405,11 @@
       <c r="E269">
         <v>5</v>
       </c>
-    </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F269">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="270" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>271</v>
       </c>
@@ -5611,8 +6422,11 @@
       <c r="E270">
         <v>5</v>
       </c>
-    </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F270">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="271" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>276</v>
       </c>
@@ -5625,8 +6439,11 @@
       <c r="E271">
         <v>5</v>
       </c>
-    </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F271">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="272" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>272</v>
       </c>
@@ -5639,8 +6456,11 @@
       <c r="E272">
         <v>5</v>
       </c>
-    </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F272">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>273</v>
       </c>
@@ -5653,8 +6473,11 @@
       <c r="E273">
         <v>5</v>
       </c>
-    </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F273">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="274" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>279</v>
       </c>
@@ -5667,8 +6490,11 @@
       <c r="E274">
         <v>5</v>
       </c>
-    </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F274">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="275" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>280</v>
       </c>
@@ -5681,8 +6507,11 @@
       <c r="E275">
         <v>5</v>
       </c>
-    </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F275">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="276" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>277</v>
       </c>
@@ -5695,8 +6524,11 @@
       <c r="E276">
         <v>5</v>
       </c>
-    </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F276">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="277" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>278</v>
       </c>
@@ -5709,8 +6541,11 @@
       <c r="E277">
         <v>5</v>
       </c>
-    </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F277">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="278" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>281</v>
       </c>
@@ -5723,8 +6558,11 @@
       <c r="E278">
         <v>5</v>
       </c>
-    </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F278">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="279" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>282</v>
       </c>
@@ -5737,8 +6575,11 @@
       <c r="E279">
         <v>5</v>
       </c>
-    </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F279">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="280" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>283</v>
       </c>
@@ -5751,8 +6592,11 @@
       <c r="E280">
         <v>5</v>
       </c>
-    </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F280">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="281" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>284</v>
       </c>
@@ -5765,8 +6609,11 @@
       <c r="E281">
         <v>5</v>
       </c>
-    </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F281">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="282" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>294</v>
       </c>
@@ -5779,8 +6626,11 @@
       <c r="E282">
         <v>5</v>
       </c>
-    </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F282">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="283" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>295</v>
       </c>
@@ -5793,8 +6643,11 @@
       <c r="E283">
         <v>5</v>
       </c>
-    </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F283">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="284" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>292</v>
       </c>
@@ -5807,8 +6660,11 @@
       <c r="E284">
         <v>5</v>
       </c>
-    </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F284">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="285" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>293</v>
       </c>
@@ -5821,8 +6677,11 @@
       <c r="E285">
         <v>5</v>
       </c>
-    </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F285">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="286" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>291</v>
       </c>
@@ -5835,8 +6694,11 @@
       <c r="E286">
         <v>5</v>
       </c>
-    </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F286">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="287" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>296</v>
       </c>
@@ -5849,8 +6711,11 @@
       <c r="E287">
         <v>5</v>
       </c>
-    </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F287">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="288" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>289</v>
       </c>
@@ -5863,8 +6728,11 @@
       <c r="E288">
         <v>5</v>
       </c>
-    </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F288">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="289" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>290</v>
       </c>
@@ -5877,8 +6745,11 @@
       <c r="E289">
         <v>5</v>
       </c>
-    </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F289">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="290" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>287</v>
       </c>
@@ -5891,8 +6762,11 @@
       <c r="E290">
         <v>5</v>
       </c>
-    </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F290">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="291" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>288</v>
       </c>
@@ -5905,8 +6779,11 @@
       <c r="E291">
         <v>5</v>
       </c>
-    </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F291">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="292" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>285</v>
       </c>
@@ -5919,8 +6796,11 @@
       <c r="E292">
         <v>5</v>
       </c>
-    </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F292">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="293" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>286</v>
       </c>
@@ -5933,8 +6813,11 @@
       <c r="E293">
         <v>5</v>
       </c>
-    </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F293">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="294" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>297</v>
       </c>
@@ -5947,8 +6830,11 @@
       <c r="E294">
         <v>5</v>
       </c>
-    </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F294">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="295" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>298</v>
       </c>
@@ -5961,8 +6847,11 @@
       <c r="E295">
         <v>5</v>
       </c>
-    </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F295">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="296" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>299</v>
       </c>
@@ -5975,8 +6864,11 @@
       <c r="E296">
         <v>5</v>
       </c>
-    </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F296">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="297" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>300</v>
       </c>
@@ -5989,8 +6881,11 @@
       <c r="E297">
         <v>5</v>
       </c>
-    </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F297">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="298" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>301</v>
       </c>
@@ -6003,8 +6898,11 @@
       <c r="E298">
         <v>5</v>
       </c>
-    </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F298">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="299" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>302</v>
       </c>
@@ -6017,8 +6915,11 @@
       <c r="E299">
         <v>5</v>
       </c>
-    </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F299">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="300" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>303</v>
       </c>
@@ -6031,8 +6932,11 @@
       <c r="E300">
         <v>5</v>
       </c>
-    </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F300">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="301" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>304</v>
       </c>
@@ -6045,8 +6949,11 @@
       <c r="E301">
         <v>5</v>
       </c>
-    </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F301">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="302" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>305</v>
       </c>
@@ -6059,8 +6966,11 @@
       <c r="E302">
         <v>5</v>
       </c>
-    </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F302">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="303" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>306</v>
       </c>
@@ -6073,8 +6983,11 @@
       <c r="E303">
         <v>5</v>
       </c>
-    </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F303">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="304" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>307</v>
       </c>
@@ -6087,8 +7000,11 @@
       <c r="E304">
         <v>5</v>
       </c>
-    </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F304">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="305" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>308</v>
       </c>
@@ -6101,8 +7017,11 @@
       <c r="E305">
         <v>5</v>
       </c>
-    </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F305">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="306" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>309</v>
       </c>
@@ -6115,8 +7034,11 @@
       <c r="E306">
         <v>5</v>
       </c>
-    </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F306">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="307" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>310</v>
       </c>
@@ -6129,8 +7051,11 @@
       <c r="E307">
         <v>5</v>
       </c>
-    </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F307">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="308" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>311</v>
       </c>
@@ -6143,8 +7068,11 @@
       <c r="E308">
         <v>5</v>
       </c>
-    </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F308">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="309" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>312</v>
       </c>
@@ -6157,8 +7085,11 @@
       <c r="E309">
         <v>5</v>
       </c>
-    </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F309">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="310" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>313</v>
       </c>
@@ -6171,8 +7102,11 @@
       <c r="E310">
         <v>5</v>
       </c>
-    </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F310">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="311" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>314</v>
       </c>
@@ -6185,8 +7119,11 @@
       <c r="E311">
         <v>5</v>
       </c>
-    </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F311">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="312" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>315</v>
       </c>
@@ -6199,8 +7136,11 @@
       <c r="E312">
         <v>5</v>
       </c>
-    </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F312">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="313" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>316</v>
       </c>
@@ -6213,8 +7153,11 @@
       <c r="E313">
         <v>5</v>
       </c>
-    </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F313">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="314" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>317</v>
       </c>
@@ -6227,8 +7170,11 @@
       <c r="E314">
         <v>5</v>
       </c>
-    </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F314">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="315" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>318</v>
       </c>
@@ -6241,8 +7187,11 @@
       <c r="E315">
         <v>5</v>
       </c>
-    </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F315">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="316" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>319</v>
       </c>
@@ -6255,8 +7204,11 @@
       <c r="E316">
         <v>5</v>
       </c>
-    </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F316">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="317" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>320</v>
       </c>
@@ -6269,8 +7221,11 @@
       <c r="E317">
         <v>5</v>
       </c>
-    </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F317">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="318" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>321</v>
       </c>
@@ -6283,8 +7238,11 @@
       <c r="E318">
         <v>5</v>
       </c>
-    </row>
-    <row r="319" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F318">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="319" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>322</v>
       </c>
@@ -6296,6 +7254,9 @@
       </c>
       <c r="E319">
         <v>5</v>
+      </c>
+      <c r="F319">
+        <v>0.03</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change the TARGET_SPEED to THRESHOLD_SPEED
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/TOLLCLASS_Designations.xlsx
+++ b/utilities/NextGenFwys/TOLLCLASS_Designations.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\llin\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\llin\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9E26F03-D581-44EC-8024-515E51BAF117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09E8EBCA-DA9D-4312-9C25-153321D43338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{0F0A9957-56E7-4C48-967B-2AB2A1965C2F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{0F0A9957-56E7-4C48-967B-2AB2A1965C2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs_for_tollcalib" sheetId="1" r:id="rId1"/>
@@ -1031,13 +1031,13 @@
     <t>Tollclass numbering convention</t>
   </si>
   <si>
-    <t>TARGET_SPEED</t>
-  </si>
-  <si>
     <t>MAX_TOLL</t>
   </si>
   <si>
     <t>MIN_TOLL</t>
+  </si>
+  <si>
+    <t>THRESHOLD_SPEED</t>
   </si>
 </sst>
 </file>
@@ -1432,7 +1432,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H20" sqref="H20"/>
+      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1453,13 +1453,13 @@
         <v>151</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>331</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Register toll class 12 as the San Jose cordon in toll class designation file
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/TOLLCLASS_Designations.xlsx
+++ b/utilities/NextGenFwys/TOLLCLASS_Designations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\llin\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09E8EBCA-DA9D-4312-9C25-153321D43338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2E4AE11-E584-4324-B216-BE511EB7E4E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{0F0A9957-56E7-4C48-967B-2AB2A1965C2F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{0F0A9957-56E7-4C48-967B-2AB2A1965C2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs_for_tollcalib" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="334">
   <si>
     <t>SR92 SM - I-280 Interchange to US101 Interchange - WB</t>
   </si>
@@ -1038,6 +1038,9 @@
   </si>
   <si>
     <t>THRESHOLD_SPEED</t>
+  </si>
+  <si>
+    <t>NGF_SC_Cordon</t>
   </si>
 </sst>
 </file>
@@ -1428,11 +1431,11 @@
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
-  <dimension ref="A1:F319"/>
+  <dimension ref="A1:F320"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
+      <pane ySplit="1" topLeftCell="A289" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H312" sqref="H312"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7256,6 +7259,23 @@
         <v>5</v>
       </c>
       <c r="F319">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="320" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A320" t="s">
+        <v>333</v>
+      </c>
+      <c r="B320">
+        <v>12</v>
+      </c>
+      <c r="D320">
+        <v>45</v>
+      </c>
+      <c r="E320">
+        <v>5</v>
+      </c>
+      <c r="F320">
         <v>0.03</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Oakland and SF TOLLCLASS values
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/TOLLCLASS_Designations.xlsx
+++ b/utilities/NextGenFwys/TOLLCLASS_Designations.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\llin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sisrael\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2E4AE11-E584-4324-B216-BE511EB7E4E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC8F0F3E-8C56-4CBC-9BF8-C567681763A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{0F0A9957-56E7-4C48-967B-2AB2A1965C2F}"/>
+    <workbookView xWindow="33720" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{0F0A9957-56E7-4C48-967B-2AB2A1965C2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs_for_tollcalib" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="336">
   <si>
     <t>SR92 SM - I-280 Interchange to US101 Interchange - WB</t>
   </si>
@@ -1041,6 +1041,12 @@
   </si>
   <si>
     <t>NGF_SC_Cordon</t>
+  </si>
+  <si>
+    <t>MAJ_SF_Congestion_Pricing</t>
+  </si>
+  <si>
+    <t>NGF_AL_Cordon</t>
   </si>
 </sst>
 </file>
@@ -1431,21 +1437,21 @@
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
-  <dimension ref="A1:F320"/>
+  <dimension ref="A1:F322"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A289" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H312" sqref="H312"/>
+      <pane ySplit="1" topLeftCell="A304" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A322" sqref="A322"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="79.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="79.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7265625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>153</v>
       </c>
@@ -1465,7 +1471,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>275</v>
       </c>
@@ -1483,7 +1489,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>150</v>
       </c>
@@ -1503,7 +1509,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>149</v>
       </c>
@@ -1523,7 +1529,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>148</v>
       </c>
@@ -1543,7 +1549,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>147</v>
       </c>
@@ -1563,7 +1569,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>146</v>
       </c>
@@ -1583,7 +1589,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>145</v>
       </c>
@@ -1603,7 +1609,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>144</v>
       </c>
@@ -1623,7 +1629,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>143</v>
       </c>
@@ -1643,7 +1649,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>142</v>
       </c>
@@ -1663,7 +1669,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>141</v>
       </c>
@@ -1683,7 +1689,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>140</v>
       </c>
@@ -1703,7 +1709,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>139</v>
       </c>
@@ -1723,7 +1729,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>138</v>
       </c>
@@ -1743,7 +1749,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>137</v>
       </c>
@@ -1763,7 +1769,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>136</v>
       </c>
@@ -1783,7 +1789,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>135</v>
       </c>
@@ -1803,7 +1809,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>134</v>
       </c>
@@ -1823,7 +1829,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>133</v>
       </c>
@@ -1843,7 +1849,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>132</v>
       </c>
@@ -1863,7 +1869,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>131</v>
       </c>
@@ -1883,7 +1889,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>130</v>
       </c>
@@ -1903,7 +1909,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>129</v>
       </c>
@@ -1923,7 +1929,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>128</v>
       </c>
@@ -1943,7 +1949,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>127</v>
       </c>
@@ -1963,7 +1969,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>126</v>
       </c>
@@ -1983,7 +1989,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>125</v>
       </c>
@@ -2003,7 +2009,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>124</v>
       </c>
@@ -2023,7 +2029,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>123</v>
       </c>
@@ -2043,7 +2049,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>122</v>
       </c>
@@ -2063,7 +2069,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>121</v>
       </c>
@@ -2083,7 +2089,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>120</v>
       </c>
@@ -2103,7 +2109,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>119</v>
       </c>
@@ -2123,7 +2129,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>118</v>
       </c>
@@ -2143,7 +2149,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>117</v>
       </c>
@@ -2163,7 +2169,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>116</v>
       </c>
@@ -2183,7 +2189,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>115</v>
       </c>
@@ -2203,7 +2209,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>114</v>
       </c>
@@ -2223,7 +2229,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>113</v>
       </c>
@@ -2243,7 +2249,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>112</v>
       </c>
@@ -2263,7 +2269,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>111</v>
       </c>
@@ -2283,7 +2289,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>110</v>
       </c>
@@ -2303,7 +2309,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>109</v>
       </c>
@@ -2323,7 +2329,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>108</v>
       </c>
@@ -2343,7 +2349,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>107</v>
       </c>
@@ -2363,7 +2369,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>106</v>
       </c>
@@ -2383,7 +2389,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>105</v>
       </c>
@@ -2403,7 +2409,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>104</v>
       </c>
@@ -2423,7 +2429,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>103</v>
       </c>
@@ -2443,7 +2449,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>102</v>
       </c>
@@ -2463,7 +2469,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>101</v>
       </c>
@@ -2483,7 +2489,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>100</v>
       </c>
@@ -2503,7 +2509,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>99</v>
       </c>
@@ -2523,7 +2529,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>98</v>
       </c>
@@ -2543,7 +2549,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>97</v>
       </c>
@@ -2563,7 +2569,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>96</v>
       </c>
@@ -2583,7 +2589,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>95</v>
       </c>
@@ -2603,7 +2609,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>94</v>
       </c>
@@ -2623,7 +2629,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>93</v>
       </c>
@@ -2643,7 +2649,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>92</v>
       </c>
@@ -2663,7 +2669,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>91</v>
       </c>
@@ -2683,7 +2689,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>90</v>
       </c>
@@ -2703,7 +2709,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>89</v>
       </c>
@@ -2723,7 +2729,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>88</v>
       </c>
@@ -2743,7 +2749,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>87</v>
       </c>
@@ -2763,7 +2769,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>86</v>
       </c>
@@ -2783,7 +2789,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>85</v>
       </c>
@@ -2803,7 +2809,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>84</v>
       </c>
@@ -2823,7 +2829,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>83</v>
       </c>
@@ -2843,7 +2849,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>82</v>
       </c>
@@ -2863,7 +2869,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>81</v>
       </c>
@@ -2883,7 +2889,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
         <v>80</v>
       </c>
@@ -2903,7 +2909,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
         <v>79</v>
       </c>
@@ -2923,7 +2929,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
         <v>78</v>
       </c>
@@ -2940,7 +2946,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
         <v>77</v>
       </c>
@@ -2957,7 +2963,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
         <v>76</v>
       </c>
@@ -2974,7 +2980,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
         <v>75</v>
       </c>
@@ -2991,7 +2997,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>74</v>
       </c>
@@ -3011,7 +3017,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>73</v>
       </c>
@@ -3031,7 +3037,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>72</v>
       </c>
@@ -3051,7 +3057,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>71</v>
       </c>
@@ -3071,7 +3077,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>70</v>
       </c>
@@ -3091,7 +3097,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>69</v>
       </c>
@@ -3111,7 +3117,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>68</v>
       </c>
@@ -3131,7 +3137,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>67</v>
       </c>
@@ -3151,7 +3157,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>66</v>
       </c>
@@ -3171,7 +3177,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>65</v>
       </c>
@@ -3191,7 +3197,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>64</v>
       </c>
@@ -3211,7 +3217,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>63</v>
       </c>
@@ -3231,7 +3237,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>62</v>
       </c>
@@ -3251,7 +3257,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>61</v>
       </c>
@@ -3271,7 +3277,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>60</v>
       </c>
@@ -3291,7 +3297,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>59</v>
       </c>
@@ -3311,7 +3317,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="95" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>58</v>
       </c>
@@ -3331,7 +3337,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>57</v>
       </c>
@@ -3351,7 +3357,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>56</v>
       </c>
@@ -3371,7 +3377,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="98" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>55</v>
       </c>
@@ -3391,7 +3397,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="99" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>54</v>
       </c>
@@ -3411,7 +3417,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="100" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>53</v>
       </c>
@@ -3431,7 +3437,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="101" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>52</v>
       </c>
@@ -3451,7 +3457,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="102" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>51</v>
       </c>
@@ -3471,7 +3477,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="103" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>50</v>
       </c>
@@ -3491,7 +3497,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="104" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>49</v>
       </c>
@@ -3511,7 +3517,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>48</v>
       </c>
@@ -3531,7 +3537,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>47</v>
       </c>
@@ -3551,7 +3557,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="107" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>46</v>
       </c>
@@ -3571,7 +3577,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="108" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>45</v>
       </c>
@@ -3591,7 +3597,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="109" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>44</v>
       </c>
@@ -3611,7 +3617,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="110" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>43</v>
       </c>
@@ -3631,7 +3637,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="111" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>42</v>
       </c>
@@ -3651,7 +3657,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="112" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>41</v>
       </c>
@@ -3671,7 +3677,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>40</v>
       </c>
@@ -3691,7 +3697,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>39</v>
       </c>
@@ -3711,7 +3717,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>38</v>
       </c>
@@ -3731,7 +3737,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>37</v>
       </c>
@@ -3751,7 +3757,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>36</v>
       </c>
@@ -3771,7 +3777,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>35</v>
       </c>
@@ -3791,7 +3797,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>34</v>
       </c>
@@ -3811,7 +3817,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>33</v>
       </c>
@@ -3831,7 +3837,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>32</v>
       </c>
@@ -3851,7 +3857,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>31</v>
       </c>
@@ -3871,7 +3877,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>30</v>
       </c>
@@ -3891,7 +3897,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>29</v>
       </c>
@@ -3911,7 +3917,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>28</v>
       </c>
@@ -3931,7 +3937,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>27</v>
       </c>
@@ -3951,7 +3957,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>26</v>
       </c>
@@ -3971,7 +3977,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>25</v>
       </c>
@@ -3991,7 +3997,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>24</v>
       </c>
@@ -4011,7 +4017,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>23</v>
       </c>
@@ -4031,7 +4037,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>22</v>
       </c>
@@ -4051,7 +4057,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>21</v>
       </c>
@@ -4071,7 +4077,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>20</v>
       </c>
@@ -4091,7 +4097,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>19</v>
       </c>
@@ -4111,7 +4117,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>18</v>
       </c>
@@ -4131,7 +4137,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>17</v>
       </c>
@@ -4151,7 +4157,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>15</v>
       </c>
@@ -4168,7 +4174,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>14</v>
       </c>
@@ -4185,7 +4191,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>13</v>
       </c>
@@ -4202,7 +4208,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>12</v>
       </c>
@@ -4219,7 +4225,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>11</v>
       </c>
@@ -4236,7 +4242,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>10</v>
       </c>
@@ -4253,7 +4259,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>9</v>
       </c>
@@ -4270,7 +4276,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>8</v>
       </c>
@@ -4287,7 +4293,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>7</v>
       </c>
@@ -4304,7 +4310,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>6</v>
       </c>
@@ -4321,7 +4327,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>5</v>
       </c>
@@ -4338,7 +4344,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>4</v>
       </c>
@@ -4355,7 +4361,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>3</v>
       </c>
@@ -4372,7 +4378,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>2</v>
       </c>
@@ -4389,7 +4395,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>1</v>
       </c>
@@ -4406,7 +4412,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>0</v>
       </c>
@@ -4423,7 +4429,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>154</v>
       </c>
@@ -4440,7 +4446,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>155</v>
       </c>
@@ -4457,7 +4463,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>156</v>
       </c>
@@ -4474,7 +4480,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>157</v>
       </c>
@@ -4491,7 +4497,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>158</v>
       </c>
@@ -4508,7 +4514,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>159</v>
       </c>
@@ -4525,7 +4531,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>160</v>
       </c>
@@ -4542,7 +4548,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>161</v>
       </c>
@@ -4559,7 +4565,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>162</v>
       </c>
@@ -4576,7 +4582,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>163</v>
       </c>
@@ -4593,7 +4599,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>164</v>
       </c>
@@ -4610,7 +4616,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>165</v>
       </c>
@@ -4627,7 +4633,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>166</v>
       </c>
@@ -4644,7 +4650,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>167</v>
       </c>
@@ -4661,7 +4667,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>168</v>
       </c>
@@ -4678,7 +4684,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>169</v>
       </c>
@@ -4695,7 +4701,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>170</v>
       </c>
@@ -4712,7 +4718,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>171</v>
       </c>
@@ -4729,7 +4735,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>172</v>
       </c>
@@ -4746,7 +4752,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>173</v>
       </c>
@@ -4763,7 +4769,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>174</v>
       </c>
@@ -4780,7 +4786,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>175</v>
       </c>
@@ -4797,7 +4803,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>176</v>
       </c>
@@ -4814,7 +4820,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>177</v>
       </c>
@@ -4831,7 +4837,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>178</v>
       </c>
@@ -4848,7 +4854,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>179</v>
       </c>
@@ -4865,7 +4871,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>180</v>
       </c>
@@ -4882,7 +4888,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>181</v>
       </c>
@@ -4899,7 +4905,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>182</v>
       </c>
@@ -4916,7 +4922,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>183</v>
       </c>
@@ -4933,7 +4939,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>184</v>
       </c>
@@ -4950,7 +4956,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>185</v>
       </c>
@@ -4967,7 +4973,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>186</v>
       </c>
@@ -4984,7 +4990,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>187</v>
       </c>
@@ -5001,7 +5007,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>188</v>
       </c>
@@ -5018,7 +5024,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>189</v>
       </c>
@@ -5035,7 +5041,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>190</v>
       </c>
@@ -5052,7 +5058,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>191</v>
       </c>
@@ -5069,7 +5075,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>192</v>
       </c>
@@ -5086,7 +5092,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>193</v>
       </c>
@@ -5103,7 +5109,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
         <v>194</v>
       </c>
@@ -5120,7 +5126,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>195</v>
       </c>
@@ -5137,7 +5143,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
         <v>196</v>
       </c>
@@ -5154,7 +5160,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>197</v>
       </c>
@@ -5171,7 +5177,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
         <v>198</v>
       </c>
@@ -5188,7 +5194,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
         <v>199</v>
       </c>
@@ -5205,7 +5211,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
         <v>200</v>
       </c>
@@ -5222,7 +5228,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
         <v>201</v>
       </c>
@@ -5239,7 +5245,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
         <v>202</v>
       </c>
@@ -5256,7 +5262,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
         <v>203</v>
       </c>
@@ -5273,7 +5279,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
         <v>204</v>
       </c>
@@ -5290,7 +5296,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
         <v>205</v>
       </c>
@@ -5307,7 +5313,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
         <v>206</v>
       </c>
@@ -5324,7 +5330,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
         <v>207</v>
       </c>
@@ -5341,7 +5347,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
         <v>208</v>
       </c>
@@ -5358,7 +5364,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
         <v>209</v>
       </c>
@@ -5375,7 +5381,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
         <v>210</v>
       </c>
@@ -5392,7 +5398,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
         <v>211</v>
       </c>
@@ -5409,7 +5415,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
         <v>212</v>
       </c>
@@ -5426,7 +5432,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
         <v>213</v>
       </c>
@@ -5443,7 +5449,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
         <v>214</v>
       </c>
@@ -5460,7 +5466,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
         <v>215</v>
       </c>
@@ -5477,7 +5483,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
         <v>216</v>
       </c>
@@ -5494,7 +5500,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
         <v>217</v>
       </c>
@@ -5511,7 +5517,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
         <v>218</v>
       </c>
@@ -5528,7 +5534,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
         <v>219</v>
       </c>
@@ -5545,7 +5551,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
         <v>220</v>
       </c>
@@ -5562,7 +5568,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
         <v>221</v>
       </c>
@@ -5579,7 +5585,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
         <v>222</v>
       </c>
@@ -5596,7 +5602,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
         <v>223</v>
       </c>
@@ -5613,7 +5619,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
         <v>224</v>
       </c>
@@ -5630,7 +5636,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
         <v>225</v>
       </c>
@@ -5647,7 +5653,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
         <v>226</v>
       </c>
@@ -5664,7 +5670,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
         <v>227</v>
       </c>
@@ -5681,7 +5687,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
         <v>228</v>
       </c>
@@ -5698,7 +5704,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
         <v>229</v>
       </c>
@@ -5715,7 +5721,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
         <v>230</v>
       </c>
@@ -5732,7 +5738,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
         <v>231</v>
       </c>
@@ -5749,7 +5755,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
         <v>232</v>
       </c>
@@ -5766,7 +5772,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
         <v>233</v>
       </c>
@@ -5783,7 +5789,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
         <v>234</v>
       </c>
@@ -5800,7 +5806,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
         <v>235</v>
       </c>
@@ -5817,7 +5823,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
         <v>236</v>
       </c>
@@ -5834,7 +5840,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
         <v>237</v>
       </c>
@@ -5851,7 +5857,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
         <v>238</v>
       </c>
@@ -5868,7 +5874,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
         <v>239</v>
       </c>
@@ -5885,7 +5891,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
         <v>240</v>
       </c>
@@ -5902,7 +5908,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
         <v>241</v>
       </c>
@@ -5919,7 +5925,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
         <v>242</v>
       </c>
@@ -5936,7 +5942,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
         <v>243</v>
       </c>
@@ -5953,7 +5959,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
         <v>244</v>
       </c>
@@ -5970,7 +5976,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
         <v>245</v>
       </c>
@@ -5987,7 +5993,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
         <v>246</v>
       </c>
@@ -6004,7 +6010,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
         <v>247</v>
       </c>
@@ -6021,7 +6027,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
         <v>248</v>
       </c>
@@ -6038,7 +6044,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="248" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
         <v>249</v>
       </c>
@@ -6055,7 +6061,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
         <v>250</v>
       </c>
@@ -6072,7 +6078,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A250" t="s">
         <v>251</v>
       </c>
@@ -6089,7 +6095,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
         <v>252</v>
       </c>
@@ -6106,7 +6112,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A252" t="s">
         <v>253</v>
       </c>
@@ -6123,7 +6129,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="253" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A253" t="s">
         <v>254</v>
       </c>
@@ -6140,7 +6146,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="254" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A254" t="s">
         <v>255</v>
       </c>
@@ -6157,7 +6163,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
         <v>256</v>
       </c>
@@ -6174,7 +6180,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="256" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A256" t="s">
         <v>257</v>
       </c>
@@ -6191,7 +6197,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="257" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A257" t="s">
         <v>258</v>
       </c>
@@ -6208,7 +6214,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="258" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A258" t="s">
         <v>259</v>
       </c>
@@ -6225,7 +6231,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="259" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A259" t="s">
         <v>260</v>
       </c>
@@ -6242,7 +6248,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="260" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A260" t="s">
         <v>261</v>
       </c>
@@ -6259,7 +6265,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="261" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A261" t="s">
         <v>262</v>
       </c>
@@ -6276,7 +6282,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="262" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A262" t="s">
         <v>263</v>
       </c>
@@ -6293,7 +6299,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="263" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A263" t="s">
         <v>264</v>
       </c>
@@ -6310,7 +6316,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="264" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A264" t="s">
         <v>265</v>
       </c>
@@ -6327,7 +6333,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A265" t="s">
         <v>266</v>
       </c>
@@ -6344,7 +6350,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A266" t="s">
         <v>267</v>
       </c>
@@ -6361,7 +6367,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A267" t="s">
         <v>268</v>
       </c>
@@ -6378,7 +6384,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="268" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A268" t="s">
         <v>269</v>
       </c>
@@ -6395,7 +6401,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="269" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A269" t="s">
         <v>270</v>
       </c>
@@ -6412,7 +6418,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="270" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A270" t="s">
         <v>271</v>
       </c>
@@ -6429,7 +6435,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="271" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A271" t="s">
         <v>276</v>
       </c>
@@ -6446,7 +6452,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="272" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A272" t="s">
         <v>272</v>
       </c>
@@ -6463,7 +6469,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A273" t="s">
         <v>273</v>
       </c>
@@ -6480,7 +6486,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="274" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A274" t="s">
         <v>279</v>
       </c>
@@ -6497,7 +6503,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="275" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A275" t="s">
         <v>280</v>
       </c>
@@ -6514,7 +6520,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="276" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A276" t="s">
         <v>277</v>
       </c>
@@ -6531,7 +6537,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="277" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A277" t="s">
         <v>278</v>
       </c>
@@ -6548,7 +6554,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="278" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A278" t="s">
         <v>281</v>
       </c>
@@ -6565,7 +6571,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="279" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A279" t="s">
         <v>282</v>
       </c>
@@ -6582,7 +6588,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="280" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A280" t="s">
         <v>283</v>
       </c>
@@ -6599,7 +6605,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="281" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A281" t="s">
         <v>284</v>
       </c>
@@ -6616,7 +6622,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="282" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A282" t="s">
         <v>294</v>
       </c>
@@ -6633,7 +6639,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="283" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A283" t="s">
         <v>295</v>
       </c>
@@ -6650,7 +6656,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="284" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A284" t="s">
         <v>292</v>
       </c>
@@ -6667,7 +6673,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="285" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A285" t="s">
         <v>293</v>
       </c>
@@ -6684,7 +6690,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="286" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A286" t="s">
         <v>291</v>
       </c>
@@ -6701,7 +6707,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="287" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A287" t="s">
         <v>296</v>
       </c>
@@ -6718,7 +6724,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="288" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A288" t="s">
         <v>289</v>
       </c>
@@ -6735,7 +6741,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="289" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A289" t="s">
         <v>290</v>
       </c>
@@ -6752,7 +6758,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="290" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A290" t="s">
         <v>287</v>
       </c>
@@ -6769,7 +6775,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="291" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A291" t="s">
         <v>288</v>
       </c>
@@ -6786,7 +6792,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="292" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A292" t="s">
         <v>285</v>
       </c>
@@ -6803,7 +6809,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="293" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A293" t="s">
         <v>286</v>
       </c>
@@ -6820,7 +6826,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="294" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A294" t="s">
         <v>297</v>
       </c>
@@ -6837,7 +6843,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="295" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A295" t="s">
         <v>298</v>
       </c>
@@ -6854,7 +6860,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="296" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A296" t="s">
         <v>299</v>
       </c>
@@ -6871,7 +6877,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="297" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A297" t="s">
         <v>300</v>
       </c>
@@ -6888,7 +6894,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="298" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A298" t="s">
         <v>301</v>
       </c>
@@ -6905,7 +6911,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="299" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A299" t="s">
         <v>302</v>
       </c>
@@ -6922,7 +6928,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="300" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A300" t="s">
         <v>303</v>
       </c>
@@ -6939,7 +6945,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="301" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A301" t="s">
         <v>304</v>
       </c>
@@ -6956,7 +6962,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="302" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A302" t="s">
         <v>305</v>
       </c>
@@ -6973,7 +6979,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="303" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A303" t="s">
         <v>306</v>
       </c>
@@ -6990,7 +6996,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="304" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A304" t="s">
         <v>307</v>
       </c>
@@ -7007,7 +7013,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="305" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A305" t="s">
         <v>308</v>
       </c>
@@ -7024,7 +7030,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="306" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A306" t="s">
         <v>309</v>
       </c>
@@ -7041,7 +7047,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="307" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A307" t="s">
         <v>310</v>
       </c>
@@ -7058,7 +7064,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="308" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A308" t="s">
         <v>311</v>
       </c>
@@ -7075,7 +7081,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="309" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A309" t="s">
         <v>312</v>
       </c>
@@ -7092,7 +7098,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="310" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A310" t="s">
         <v>313</v>
       </c>
@@ -7109,7 +7115,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="311" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A311" t="s">
         <v>314</v>
       </c>
@@ -7126,7 +7132,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="312" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A312" t="s">
         <v>315</v>
       </c>
@@ -7143,7 +7149,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="313" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A313" t="s">
         <v>316</v>
       </c>
@@ -7160,7 +7166,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="314" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A314" t="s">
         <v>317</v>
       </c>
@@ -7177,7 +7183,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="315" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A315" t="s">
         <v>318</v>
       </c>
@@ -7194,7 +7200,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="316" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A316" t="s">
         <v>319</v>
       </c>
@@ -7211,7 +7217,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="317" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A317" t="s">
         <v>320</v>
       </c>
@@ -7228,7 +7234,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="318" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A318" t="s">
         <v>321</v>
       </c>
@@ -7245,7 +7251,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="319" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A319" t="s">
         <v>322</v>
       </c>
@@ -7262,20 +7268,54 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="320" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A320" t="s">
+        <v>334</v>
+      </c>
+      <c r="B320">
+        <v>10</v>
+      </c>
+      <c r="D320">
+        <v>45</v>
+      </c>
+      <c r="E320">
+        <v>5</v>
+      </c>
+      <c r="F320">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="321" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A321" t="s">
+        <v>335</v>
+      </c>
+      <c r="B321">
+        <v>11</v>
+      </c>
+      <c r="D321">
+        <v>45</v>
+      </c>
+      <c r="E321">
+        <v>5</v>
+      </c>
+      <c r="F321">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="322" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A322" t="s">
         <v>333</v>
       </c>
-      <c r="B320">
+      <c r="B322">
         <v>12</v>
       </c>
-      <c r="D320">
-        <v>45</v>
-      </c>
-      <c r="E320">
-        <v>5</v>
-      </c>
-      <c r="F320">
+      <c r="D322">
+        <v>45</v>
+      </c>
+      <c r="E322">
+        <v>5</v>
+      </c>
+      <c r="F322">
         <v>0.03</v>
       </c>
     </row>
@@ -7296,18 +7336,18 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>324</v>
       </c>
@@ -7315,7 +7355,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>328</v>
       </c>
@@ -7323,7 +7363,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>323</v>
       </c>

</xml_diff>

<commit_message>
set MIN_TOLL to 0.1 cents for all-lane tolling
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/TOLLCLASS_Designations.xlsx
+++ b/utilities/NextGenFwys/TOLLCLASS_Designations.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\NextGenFwys\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64CC3770-CA0B-4922-8568-B326E07A3DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAEBB626-00A5-430E-9AB1-93EA16D58C32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="252" yWindow="2004" windowWidth="22956" windowHeight="14088" xr2:uid="{0F0A9957-56E7-4C48-967B-2AB2A1965C2F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{0F0A9957-56E7-4C48-967B-2AB2A1965C2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs_for_tollcalib" sheetId="1" r:id="rId1"/>
     <sheet name="Readme - numbering convention" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Inputs_for_tollcalib!$B$1:$G$322</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Inputs_for_tollcalib!$B$1:$G$331</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1579,7 +1579,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1592,22 +1592,22 @@
   </sheetPr>
   <dimension ref="A1:I331"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A309" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B336" sqref="B336"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" customWidth="1"/>
-    <col min="2" max="2" width="79.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.36328125" customWidth="1"/>
+    <col min="2" max="2" width="79.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.81640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.109375" customWidth="1"/>
-    <col min="9" max="9" width="15.77734375" customWidth="1"/>
+    <col min="8" max="8" width="21.08984375" customWidth="1"/>
+    <col min="9" max="9" width="15.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>336</v>
       </c>
@@ -1636,7 +1636,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>386</v>
       </c>
@@ -1663,7 +1663,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>150</v>
       </c>
@@ -1689,7 +1689,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>149</v>
       </c>
@@ -1715,7 +1715,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>148</v>
       </c>
@@ -1741,7 +1741,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>147</v>
       </c>
@@ -1767,7 +1767,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>146</v>
       </c>
@@ -1793,7 +1793,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>145</v>
       </c>
@@ -1819,7 +1819,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>144</v>
       </c>
@@ -1845,7 +1845,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>143</v>
       </c>
@@ -1871,7 +1871,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>142</v>
       </c>
@@ -1897,7 +1897,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>141</v>
       </c>
@@ -1923,7 +1923,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>140</v>
       </c>
@@ -1949,7 +1949,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>139</v>
       </c>
@@ -1975,7 +1975,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>138</v>
       </c>
@@ -2001,7 +2001,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>137</v>
       </c>
@@ -2027,7 +2027,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>136</v>
       </c>
@@ -2053,7 +2053,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>135</v>
       </c>
@@ -2079,7 +2079,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>134</v>
       </c>
@@ -2105,7 +2105,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>133</v>
       </c>
@@ -2131,7 +2131,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>132</v>
       </c>
@@ -2157,7 +2157,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>131</v>
       </c>
@@ -2183,7 +2183,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="23" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>130</v>
       </c>
@@ -2209,7 +2209,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="24" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>129</v>
       </c>
@@ -2235,7 +2235,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="25" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>128</v>
       </c>
@@ -2261,7 +2261,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="26" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>127</v>
       </c>
@@ -2287,7 +2287,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="27" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>126</v>
       </c>
@@ -2313,7 +2313,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="28" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
         <v>125</v>
       </c>
@@ -2339,7 +2339,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="29" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
         <v>124</v>
       </c>
@@ -2365,7 +2365,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="30" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
         <v>123</v>
       </c>
@@ -2391,7 +2391,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="31" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>122</v>
       </c>
@@ -2417,7 +2417,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="32" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
         <v>121</v>
       </c>
@@ -2443,7 +2443,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="33" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
         <v>120</v>
       </c>
@@ -2469,7 +2469,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="34" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
         <v>119</v>
       </c>
@@ -2495,7 +2495,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="35" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
         <v>118</v>
       </c>
@@ -2521,7 +2521,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="36" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
         <v>117</v>
       </c>
@@ -2547,7 +2547,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="37" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B37" t="s">
         <v>116</v>
       </c>
@@ -2573,7 +2573,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="38" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
         <v>115</v>
       </c>
@@ -2599,7 +2599,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="39" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B39" t="s">
         <v>114</v>
       </c>
@@ -2625,7 +2625,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="40" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B40" t="s">
         <v>113</v>
       </c>
@@ -2651,7 +2651,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="41" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B41" t="s">
         <v>112</v>
       </c>
@@ -2677,7 +2677,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="42" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B42" t="s">
         <v>111</v>
       </c>
@@ -2703,7 +2703,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="43" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B43" t="s">
         <v>110</v>
       </c>
@@ -2729,7 +2729,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="44" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B44" t="s">
         <v>109</v>
       </c>
@@ -2755,7 +2755,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B45" t="s">
         <v>108</v>
       </c>
@@ -2781,7 +2781,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B46" t="s">
         <v>107</v>
       </c>
@@ -2807,7 +2807,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="47" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B47" t="s">
         <v>106</v>
       </c>
@@ -2833,7 +2833,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="48" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B48" t="s">
         <v>105</v>
       </c>
@@ -2859,7 +2859,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="49" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B49" t="s">
         <v>104</v>
       </c>
@@ -2885,7 +2885,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="50" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B50" t="s">
         <v>103</v>
       </c>
@@ -2911,7 +2911,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B51" t="s">
         <v>102</v>
       </c>
@@ -2937,7 +2937,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="52" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B52" t="s">
         <v>101</v>
       </c>
@@ -2963,7 +2963,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B53" t="s">
         <v>100</v>
       </c>
@@ -2989,7 +2989,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B54" t="s">
         <v>99</v>
       </c>
@@ -3015,7 +3015,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="55" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B55" t="s">
         <v>98</v>
       </c>
@@ -3041,7 +3041,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="56" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B56" t="s">
         <v>97</v>
       </c>
@@ -3067,7 +3067,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B57" t="s">
         <v>96</v>
       </c>
@@ -3093,7 +3093,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B58" t="s">
         <v>95</v>
       </c>
@@ -3119,7 +3119,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="59" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B59" t="s">
         <v>94</v>
       </c>
@@ -3145,7 +3145,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="60" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B60" t="s">
         <v>93</v>
       </c>
@@ -3171,7 +3171,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="61" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B61" t="s">
         <v>92</v>
       </c>
@@ -3197,7 +3197,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="62" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B62" t="s">
         <v>91</v>
       </c>
@@ -3223,7 +3223,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="63" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B63" t="s">
         <v>90</v>
       </c>
@@ -3249,7 +3249,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="64" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B64" t="s">
         <v>89</v>
       </c>
@@ -3275,7 +3275,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="65" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B65" t="s">
         <v>88</v>
       </c>
@@ -3301,7 +3301,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="66" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B66" t="s">
         <v>87</v>
       </c>
@@ -3327,7 +3327,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="67" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B67" t="s">
         <v>86</v>
       </c>
@@ -3353,7 +3353,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="68" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B68" t="s">
         <v>85</v>
       </c>
@@ -3379,7 +3379,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="69" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B69" t="s">
         <v>84</v>
       </c>
@@ -3405,7 +3405,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="70" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B70" t="s">
         <v>83</v>
       </c>
@@ -3431,7 +3431,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="71" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B71" t="s">
         <v>82</v>
       </c>
@@ -3457,7 +3457,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="72" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B72" t="s">
         <v>81</v>
       </c>
@@ -3483,7 +3483,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="73" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B73" s="1" t="s">
         <v>80</v>
       </c>
@@ -3509,7 +3509,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="74" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B74" s="1" t="s">
         <v>79</v>
       </c>
@@ -3535,7 +3535,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="75" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B75" s="1" t="s">
         <v>78</v>
       </c>
@@ -3558,7 +3558,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="76" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B76" s="1" t="s">
         <v>77</v>
       </c>
@@ -3581,7 +3581,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="77" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B77" s="1" t="s">
         <v>76</v>
       </c>
@@ -3604,7 +3604,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="78" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B78" s="1" t="s">
         <v>75</v>
       </c>
@@ -3627,7 +3627,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="79" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B79" t="s">
         <v>74</v>
       </c>
@@ -3653,7 +3653,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="80" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B80" t="s">
         <v>73</v>
       </c>
@@ -3679,7 +3679,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B81" t="s">
         <v>72</v>
       </c>
@@ -3705,7 +3705,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B82" t="s">
         <v>71</v>
       </c>
@@ -3731,7 +3731,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B83" t="s">
         <v>70</v>
       </c>
@@ -3757,7 +3757,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B84" t="s">
         <v>69</v>
       </c>
@@ -3783,7 +3783,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B85" t="s">
         <v>68</v>
       </c>
@@ -3809,7 +3809,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B86" t="s">
         <v>67</v>
       </c>
@@ -3835,7 +3835,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="87" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B87" t="s">
         <v>66</v>
       </c>
@@ -3861,7 +3861,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B88" t="s">
         <v>65</v>
       </c>
@@ -3887,7 +3887,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="89" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B89" t="s">
         <v>64</v>
       </c>
@@ -3913,7 +3913,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="90" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B90" t="s">
         <v>63</v>
       </c>
@@ -3939,7 +3939,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B91" t="s">
         <v>62</v>
       </c>
@@ -3965,7 +3965,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B92" t="s">
         <v>61</v>
       </c>
@@ -3991,7 +3991,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B93" t="s">
         <v>60</v>
       </c>
@@ -4017,7 +4017,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B94" t="s">
         <v>59</v>
       </c>
@@ -4043,7 +4043,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="95" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>386</v>
       </c>
@@ -4072,7 +4072,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="96" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>386</v>
       </c>
@@ -4101,7 +4101,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="97" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>386</v>
       </c>
@@ -4130,7 +4130,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="98" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>386</v>
       </c>
@@ -4159,7 +4159,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>386</v>
       </c>
@@ -4188,7 +4188,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="100" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>386</v>
       </c>
@@ -4217,7 +4217,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="101" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>386</v>
       </c>
@@ -4246,7 +4246,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="102" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>386</v>
       </c>
@@ -4275,7 +4275,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="103" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>386</v>
       </c>
@@ -4304,7 +4304,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="104" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>386</v>
       </c>
@@ -4333,7 +4333,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B105" t="s">
         <v>48</v>
       </c>
@@ -4359,7 +4359,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B106" t="s">
         <v>47</v>
       </c>
@@ -4385,7 +4385,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="107" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B107" t="s">
         <v>46</v>
       </c>
@@ -4411,7 +4411,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="108" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B108" t="s">
         <v>45</v>
       </c>
@@ -4437,7 +4437,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="109" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B109" t="s">
         <v>44</v>
       </c>
@@ -4463,7 +4463,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="110" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B110" t="s">
         <v>43</v>
       </c>
@@ -4489,7 +4489,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="111" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>386</v>
       </c>
@@ -4518,7 +4518,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="112" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>386</v>
       </c>
@@ -4547,7 +4547,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>386</v>
       </c>
@@ -4576,7 +4576,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>386</v>
       </c>
@@ -4605,7 +4605,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>386</v>
       </c>
@@ -4634,7 +4634,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>386</v>
       </c>
@@ -4663,7 +4663,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B117" t="s">
         <v>36</v>
       </c>
@@ -4689,7 +4689,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B118" t="s">
         <v>35</v>
       </c>
@@ -4715,7 +4715,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B119" t="s">
         <v>34</v>
       </c>
@@ -4741,7 +4741,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B120" t="s">
         <v>33</v>
       </c>
@@ -4767,7 +4767,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B121" t="s">
         <v>32</v>
       </c>
@@ -4793,7 +4793,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B122" t="s">
         <v>31</v>
       </c>
@@ -4819,7 +4819,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B123" t="s">
         <v>30</v>
       </c>
@@ -4845,7 +4845,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B124" t="s">
         <v>29</v>
       </c>
@@ -4871,7 +4871,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B125" t="s">
         <v>28</v>
       </c>
@@ -4897,7 +4897,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B126" t="s">
         <v>27</v>
       </c>
@@ -4923,7 +4923,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B127" t="s">
         <v>26</v>
       </c>
@@ -4949,7 +4949,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B128" t="s">
         <v>25</v>
       </c>
@@ -4975,7 +4975,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="129" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B129" t="s">
         <v>24</v>
       </c>
@@ -5001,7 +5001,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="130" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B130" t="s">
         <v>23</v>
       </c>
@@ -5027,7 +5027,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="131" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B131" t="s">
         <v>22</v>
       </c>
@@ -5053,7 +5053,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="132" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B132" t="s">
         <v>21</v>
       </c>
@@ -5079,7 +5079,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="133" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B133" t="s">
         <v>20</v>
       </c>
@@ -5105,7 +5105,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="134" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B134" t="s">
         <v>19</v>
       </c>
@@ -5131,7 +5131,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="135" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B135" t="s">
         <v>18</v>
       </c>
@@ -5157,7 +5157,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="136" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B136" t="s">
         <v>17</v>
       </c>
@@ -5183,7 +5183,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="137" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B137" t="s">
         <v>15</v>
       </c>
@@ -5206,7 +5206,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="138" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B138" t="s">
         <v>14</v>
       </c>
@@ -5229,7 +5229,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="139" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B139" t="s">
         <v>13</v>
       </c>
@@ -5252,7 +5252,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="140" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B140" t="s">
         <v>12</v>
       </c>
@@ -5275,7 +5275,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="141" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B141" t="s">
         <v>11</v>
       </c>
@@ -5298,7 +5298,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="142" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="142" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B142" t="s">
         <v>10</v>
       </c>
@@ -5321,7 +5321,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="143" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="143" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B143" t="s">
         <v>9</v>
       </c>
@@ -5344,7 +5344,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="144" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="144" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B144" t="s">
         <v>8</v>
       </c>
@@ -5367,7 +5367,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B145" t="s">
         <v>7</v>
       </c>
@@ -5390,7 +5390,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B146" t="s">
         <v>6</v>
       </c>
@@ -5413,7 +5413,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B147" t="s">
         <v>5</v>
       </c>
@@ -5436,7 +5436,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B148" t="s">
         <v>4</v>
       </c>
@@ -5459,7 +5459,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B149" t="s">
         <v>3</v>
       </c>
@@ -5482,7 +5482,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B150" t="s">
         <v>2</v>
       </c>
@@ -5505,7 +5505,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B151" t="s">
         <v>1</v>
       </c>
@@ -5528,7 +5528,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B152" t="s">
         <v>0</v>
       </c>
@@ -5551,7 +5551,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>386</v>
       </c>
@@ -5568,7 +5568,7 @@
         <v>5</v>
       </c>
       <c r="G153">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H153" t="s">
         <v>340</v>
@@ -5577,7 +5577,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>386</v>
       </c>
@@ -5594,7 +5594,7 @@
         <v>5</v>
       </c>
       <c r="G154">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H154" t="s">
         <v>340</v>
@@ -5603,7 +5603,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>386</v>
       </c>
@@ -5620,7 +5620,7 @@
         <v>5</v>
       </c>
       <c r="G155">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H155" t="s">
         <v>341</v>
@@ -5629,7 +5629,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>386</v>
       </c>
@@ -5646,7 +5646,7 @@
         <v>5</v>
       </c>
       <c r="G156">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H156" t="s">
         <v>341</v>
@@ -5655,7 +5655,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>386</v>
       </c>
@@ -5672,7 +5672,7 @@
         <v>5</v>
       </c>
       <c r="G157">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H157" t="s">
         <v>341</v>
@@ -5681,7 +5681,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>386</v>
       </c>
@@ -5698,7 +5698,7 @@
         <v>5</v>
       </c>
       <c r="G158">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H158" t="s">
         <v>341</v>
@@ -5707,7 +5707,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>386</v>
       </c>
@@ -5724,7 +5724,7 @@
         <v>5</v>
       </c>
       <c r="G159">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H159" t="s">
         <v>341</v>
@@ -5733,7 +5733,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>386</v>
       </c>
@@ -5750,7 +5750,7 @@
         <v>5</v>
       </c>
       <c r="G160">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H160" t="s">
         <v>340</v>
@@ -5759,7 +5759,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>386</v>
       </c>
@@ -5776,7 +5776,7 @@
         <v>5</v>
       </c>
       <c r="G161">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H161" t="s">
         <v>340</v>
@@ -5785,7 +5785,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>386</v>
       </c>
@@ -5802,7 +5802,7 @@
         <v>5</v>
       </c>
       <c r="G162">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H162" t="s">
         <v>342</v>
@@ -5811,7 +5811,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>386</v>
       </c>
@@ -5828,7 +5828,7 @@
         <v>5</v>
       </c>
       <c r="G163">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H163" t="s">
         <v>342</v>
@@ -5837,7 +5837,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>386</v>
       </c>
@@ -5854,7 +5854,7 @@
         <v>5</v>
       </c>
       <c r="G164">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H164" t="s">
         <v>342</v>
@@ -5863,7 +5863,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>386</v>
       </c>
@@ -5880,7 +5880,7 @@
         <v>5</v>
       </c>
       <c r="G165">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H165" t="s">
         <v>342</v>
@@ -5889,7 +5889,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>386</v>
       </c>
@@ -5906,7 +5906,7 @@
         <v>5</v>
       </c>
       <c r="G166">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H166" t="s">
         <v>342</v>
@@ -5915,7 +5915,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>386</v>
       </c>
@@ -5932,7 +5932,7 @@
         <v>5</v>
       </c>
       <c r="G167">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H167" t="s">
         <v>342</v>
@@ -5941,7 +5941,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>386</v>
       </c>
@@ -5958,7 +5958,7 @@
         <v>5</v>
       </c>
       <c r="G168">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H168" t="s">
         <v>341</v>
@@ -5967,7 +5967,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>386</v>
       </c>
@@ -5984,7 +5984,7 @@
         <v>5</v>
       </c>
       <c r="G169">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H169" t="s">
         <v>341</v>
@@ -5993,7 +5993,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>386</v>
       </c>
@@ -6010,7 +6010,7 @@
         <v>5</v>
       </c>
       <c r="G170">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H170" t="s">
         <v>343</v>
@@ -6019,7 +6019,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>386</v>
       </c>
@@ -6036,7 +6036,7 @@
         <v>5</v>
       </c>
       <c r="G171">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H171" t="s">
         <v>343</v>
@@ -6045,7 +6045,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>386</v>
       </c>
@@ -6062,7 +6062,7 @@
         <v>5</v>
       </c>
       <c r="G172">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H172" t="s">
         <v>343</v>
@@ -6071,7 +6071,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>386</v>
       </c>
@@ -6088,7 +6088,7 @@
         <v>5</v>
       </c>
       <c r="G173">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H173" t="s">
         <v>343</v>
@@ -6097,7 +6097,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>386</v>
       </c>
@@ -6114,7 +6114,7 @@
         <v>5</v>
       </c>
       <c r="G174">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H174" t="s">
         <v>343</v>
@@ -6123,7 +6123,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>386</v>
       </c>
@@ -6140,7 +6140,7 @@
         <v>5</v>
       </c>
       <c r="G175">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H175" t="s">
         <v>343</v>
@@ -6149,7 +6149,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>386</v>
       </c>
@@ -6166,7 +6166,7 @@
         <v>5</v>
       </c>
       <c r="G176">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H176" t="s">
         <v>343</v>
@@ -6175,7 +6175,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>386</v>
       </c>
@@ -6192,7 +6192,7 @@
         <v>5</v>
       </c>
       <c r="G177">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H177" t="s">
         <v>343</v>
@@ -6201,7 +6201,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>386</v>
       </c>
@@ -6218,7 +6218,7 @@
         <v>5</v>
       </c>
       <c r="G178">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H178" t="s">
         <v>343</v>
@@ -6227,7 +6227,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>386</v>
       </c>
@@ -6244,7 +6244,7 @@
         <v>5</v>
       </c>
       <c r="G179">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H179" t="s">
         <v>343</v>
@@ -6253,7 +6253,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>386</v>
       </c>
@@ -6270,7 +6270,7 @@
         <v>5</v>
       </c>
       <c r="G180">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H180" t="s">
         <v>343</v>
@@ -6279,7 +6279,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>386</v>
       </c>
@@ -6296,7 +6296,7 @@
         <v>5</v>
       </c>
       <c r="G181">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H181" t="s">
         <v>343</v>
@@ -6305,7 +6305,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>386</v>
       </c>
@@ -6322,7 +6322,7 @@
         <v>5</v>
       </c>
       <c r="G182">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H182" t="s">
         <v>343</v>
@@ -6331,7 +6331,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>386</v>
       </c>
@@ -6348,7 +6348,7 @@
         <v>5</v>
       </c>
       <c r="G183">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H183" t="s">
         <v>343</v>
@@ -6357,7 +6357,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>386</v>
       </c>
@@ -6374,7 +6374,7 @@
         <v>5</v>
       </c>
       <c r="G184">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H184" t="s">
         <v>343</v>
@@ -6383,7 +6383,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>386</v>
       </c>
@@ -6400,7 +6400,7 @@
         <v>5</v>
       </c>
       <c r="G185">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H185" t="s">
         <v>343</v>
@@ -6409,7 +6409,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>386</v>
       </c>
@@ -6426,7 +6426,7 @@
         <v>5</v>
       </c>
       <c r="G186">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H186" t="s">
         <v>343</v>
@@ -6435,7 +6435,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>386</v>
       </c>
@@ -6452,7 +6452,7 @@
         <v>5</v>
       </c>
       <c r="G187">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H187" t="s">
         <v>343</v>
@@ -6461,7 +6461,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>386</v>
       </c>
@@ -6478,7 +6478,7 @@
         <v>5</v>
       </c>
       <c r="G188">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H188" t="s">
         <v>343</v>
@@ -6487,7 +6487,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>386</v>
       </c>
@@ -6504,7 +6504,7 @@
         <v>5</v>
       </c>
       <c r="G189">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H189" t="s">
         <v>344</v>
@@ -6513,7 +6513,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>386</v>
       </c>
@@ -6530,7 +6530,7 @@
         <v>5</v>
       </c>
       <c r="G190">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H190" t="s">
         <v>344</v>
@@ -6539,7 +6539,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>386</v>
       </c>
@@ -6556,7 +6556,7 @@
         <v>5</v>
       </c>
       <c r="G191">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H191" t="s">
         <v>344</v>
@@ -6565,7 +6565,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>386</v>
       </c>
@@ -6582,7 +6582,7 @@
         <v>5</v>
       </c>
       <c r="G192">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H192" t="s">
         <v>344</v>
@@ -6591,7 +6591,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
         <v>386</v>
       </c>
@@ -6608,7 +6608,7 @@
         <v>5</v>
       </c>
       <c r="G193">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H193" t="s">
         <v>344</v>
@@ -6617,7 +6617,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>386</v>
       </c>
@@ -6634,7 +6634,7 @@
         <v>5</v>
       </c>
       <c r="G194">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H194" t="s">
         <v>344</v>
@@ -6643,7 +6643,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
         <v>386</v>
       </c>
@@ -6660,7 +6660,7 @@
         <v>5</v>
       </c>
       <c r="G195">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H195" t="s">
         <v>344</v>
@@ -6669,7 +6669,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>386</v>
       </c>
@@ -6686,7 +6686,7 @@
         <v>5</v>
       </c>
       <c r="G196">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H196" t="s">
         <v>345</v>
@@ -6695,7 +6695,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
         <v>386</v>
       </c>
@@ -6712,7 +6712,7 @@
         <v>5</v>
       </c>
       <c r="G197">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H197" t="s">
         <v>345</v>
@@ -6721,7 +6721,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
         <v>386</v>
       </c>
@@ -6738,7 +6738,7 @@
         <v>5</v>
       </c>
       <c r="G198">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H198" t="s">
         <v>345</v>
@@ -6747,7 +6747,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
         <v>386</v>
       </c>
@@ -6764,7 +6764,7 @@
         <v>5</v>
       </c>
       <c r="G199">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H199" t="s">
         <v>345</v>
@@ -6773,7 +6773,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
         <v>386</v>
       </c>
@@ -6790,7 +6790,7 @@
         <v>5</v>
       </c>
       <c r="G200">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H200" t="s">
         <v>346</v>
@@ -6799,7 +6799,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
         <v>386</v>
       </c>
@@ -6816,7 +6816,7 @@
         <v>5</v>
       </c>
       <c r="G201">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H201" t="s">
         <v>346</v>
@@ -6825,7 +6825,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
         <v>386</v>
       </c>
@@ -6842,7 +6842,7 @@
         <v>5</v>
       </c>
       <c r="G202">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H202" t="s">
         <v>346</v>
@@ -6851,7 +6851,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
         <v>386</v>
       </c>
@@ -6868,7 +6868,7 @@
         <v>5</v>
       </c>
       <c r="G203">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H203" t="s">
         <v>346</v>
@@ -6877,7 +6877,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
         <v>386</v>
       </c>
@@ -6894,7 +6894,7 @@
         <v>5</v>
       </c>
       <c r="G204">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H204" t="s">
         <v>340</v>
@@ -6903,7 +6903,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
         <v>386</v>
       </c>
@@ -6920,7 +6920,7 @@
         <v>5</v>
       </c>
       <c r="G205">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H205" t="s">
         <v>340</v>
@@ -6929,7 +6929,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
         <v>386</v>
       </c>
@@ -6946,7 +6946,7 @@
         <v>5</v>
       </c>
       <c r="G206">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H206" t="s">
         <v>340</v>
@@ -6955,7 +6955,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
         <v>386</v>
       </c>
@@ -6972,7 +6972,7 @@
         <v>5</v>
       </c>
       <c r="G207">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H207" t="s">
         <v>340</v>
@@ -6981,7 +6981,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
         <v>386</v>
       </c>
@@ -6998,7 +6998,7 @@
         <v>5</v>
       </c>
       <c r="G208">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H208" t="s">
         <v>341</v>
@@ -7007,7 +7007,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="209" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
         <v>386</v>
       </c>
@@ -7024,7 +7024,7 @@
         <v>5</v>
       </c>
       <c r="G209">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H209" t="s">
         <v>341</v>
@@ -7033,7 +7033,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="210" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
         <v>386</v>
       </c>
@@ -7050,7 +7050,7 @@
         <v>5</v>
       </c>
       <c r="G210">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H210" t="s">
         <v>341</v>
@@ -7059,7 +7059,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
         <v>386</v>
       </c>
@@ -7076,7 +7076,7 @@
         <v>5</v>
       </c>
       <c r="G211">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H211" t="s">
         <v>341</v>
@@ -7085,7 +7085,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="212" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
         <v>386</v>
       </c>
@@ -7102,7 +7102,7 @@
         <v>5</v>
       </c>
       <c r="G212">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H212" t="s">
         <v>341</v>
@@ -7111,7 +7111,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="213" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
         <v>386</v>
       </c>
@@ -7128,7 +7128,7 @@
         <v>5</v>
       </c>
       <c r="G213">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H213" t="s">
         <v>342</v>
@@ -7137,7 +7137,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="214" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
         <v>386</v>
       </c>
@@ -7154,7 +7154,7 @@
         <v>5</v>
       </c>
       <c r="G214">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H214" t="s">
         <v>342</v>
@@ -7163,7 +7163,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="215" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
         <v>386</v>
       </c>
@@ -7180,7 +7180,7 @@
         <v>5</v>
       </c>
       <c r="G215">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H215" t="s">
         <v>342</v>
@@ -7189,7 +7189,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="216" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
         <v>386</v>
       </c>
@@ -7206,7 +7206,7 @@
         <v>5</v>
       </c>
       <c r="G216">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H216" t="s">
         <v>341</v>
@@ -7215,7 +7215,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="217" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
         <v>386</v>
       </c>
@@ -7232,7 +7232,7 @@
         <v>5</v>
       </c>
       <c r="G217">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H217" t="s">
         <v>341</v>
@@ -7241,7 +7241,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="218" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
         <v>386</v>
       </c>
@@ -7258,7 +7258,7 @@
         <v>5</v>
       </c>
       <c r="G218">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H218" t="s">
         <v>342</v>
@@ -7267,7 +7267,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="219" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
         <v>386</v>
       </c>
@@ -7284,7 +7284,7 @@
         <v>5</v>
       </c>
       <c r="G219">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H219" t="s">
         <v>342</v>
@@ -7293,7 +7293,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="220" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
         <v>386</v>
       </c>
@@ -7310,7 +7310,7 @@
         <v>5</v>
       </c>
       <c r="G220">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H220" t="s">
         <v>342</v>
@@ -7319,7 +7319,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="221" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
         <v>386</v>
       </c>
@@ -7336,7 +7336,7 @@
         <v>5</v>
       </c>
       <c r="G221">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H221" t="s">
         <v>341</v>
@@ -7345,7 +7345,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="222" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
         <v>386</v>
       </c>
@@ -7362,7 +7362,7 @@
         <v>5</v>
       </c>
       <c r="G222">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H222" t="s">
         <v>341</v>
@@ -7371,7 +7371,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="223" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
         <v>386</v>
       </c>
@@ -7388,7 +7388,7 @@
         <v>5</v>
       </c>
       <c r="G223">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H223" t="s">
         <v>340</v>
@@ -7397,7 +7397,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="224" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
         <v>386</v>
       </c>
@@ -7414,7 +7414,7 @@
         <v>5</v>
       </c>
       <c r="G224">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H224" t="s">
         <v>340</v>
@@ -7423,7 +7423,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="225" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
         <v>386</v>
       </c>
@@ -7440,7 +7440,7 @@
         <v>5</v>
       </c>
       <c r="G225">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H225" t="s">
         <v>340</v>
@@ -7449,7 +7449,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="226" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
         <v>386</v>
       </c>
@@ -7466,7 +7466,7 @@
         <v>5</v>
       </c>
       <c r="G226">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H226" t="s">
         <v>342</v>
@@ -7475,7 +7475,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="227" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
         <v>386</v>
       </c>
@@ -7492,7 +7492,7 @@
         <v>5</v>
       </c>
       <c r="G227">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H227" t="s">
         <v>340</v>
@@ -7501,7 +7501,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="228" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
         <v>386</v>
       </c>
@@ -7518,7 +7518,7 @@
         <v>5</v>
       </c>
       <c r="G228">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H228" t="s">
         <v>341</v>
@@ -7527,7 +7527,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="229" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
         <v>386</v>
       </c>
@@ -7544,7 +7544,7 @@
         <v>5</v>
       </c>
       <c r="G229">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H229" t="s">
         <v>341</v>
@@ -7553,7 +7553,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="230" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
         <v>386</v>
       </c>
@@ -7570,7 +7570,7 @@
         <v>5</v>
       </c>
       <c r="G230">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H230" t="s">
         <v>341</v>
@@ -7579,7 +7579,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="231" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
         <v>386</v>
       </c>
@@ -7596,7 +7596,7 @@
         <v>5</v>
       </c>
       <c r="G231">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H231" t="s">
         <v>341</v>
@@ -7605,7 +7605,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="232" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
         <v>386</v>
       </c>
@@ -7622,7 +7622,7 @@
         <v>5</v>
       </c>
       <c r="G232">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H232" t="s">
         <v>343</v>
@@ -7631,7 +7631,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="233" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
         <v>386</v>
       </c>
@@ -7648,7 +7648,7 @@
         <v>5</v>
       </c>
       <c r="G233">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H233" t="s">
         <v>341</v>
@@ -7657,7 +7657,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="234" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
         <v>386</v>
       </c>
@@ -7674,7 +7674,7 @@
         <v>5</v>
       </c>
       <c r="G234">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H234" t="s">
         <v>341</v>
@@ -7683,7 +7683,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="235" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
         <v>386</v>
       </c>
@@ -7700,7 +7700,7 @@
         <v>5</v>
       </c>
       <c r="G235">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H235" t="s">
         <v>340</v>
@@ -7709,7 +7709,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="236" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
         <v>386</v>
       </c>
@@ -7726,7 +7726,7 @@
         <v>5</v>
       </c>
       <c r="G236">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H236" t="s">
         <v>340</v>
@@ -7735,7 +7735,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="237" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
         <v>386</v>
       </c>
@@ -7752,7 +7752,7 @@
         <v>5</v>
       </c>
       <c r="G237">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H237" t="s">
         <v>343</v>
@@ -7761,7 +7761,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="238" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
         <v>386</v>
       </c>
@@ -7778,7 +7778,7 @@
         <v>5</v>
       </c>
       <c r="G238">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H238" t="s">
         <v>340</v>
@@ -7787,7 +7787,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="239" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
         <v>386</v>
       </c>
@@ -7804,7 +7804,7 @@
         <v>5</v>
       </c>
       <c r="G239">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H239" t="s">
         <v>340</v>
@@ -7813,7 +7813,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="240" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
         <v>386</v>
       </c>
@@ -7830,7 +7830,7 @@
         <v>5</v>
       </c>
       <c r="G240">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H240" t="s">
         <v>343</v>
@@ -7839,7 +7839,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="241" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
         <v>386</v>
       </c>
@@ -7856,7 +7856,7 @@
         <v>5</v>
       </c>
       <c r="G241">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H241" t="s">
         <v>343</v>
@@ -7865,7 +7865,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="242" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
         <v>386</v>
       </c>
@@ -7882,7 +7882,7 @@
         <v>5</v>
       </c>
       <c r="G242">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H242" t="s">
         <v>343</v>
@@ -7891,7 +7891,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="243" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
         <v>386</v>
       </c>
@@ -7908,7 +7908,7 @@
         <v>5</v>
       </c>
       <c r="G243">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H243" t="s">
         <v>343</v>
@@ -7917,7 +7917,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="244" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
         <v>386</v>
       </c>
@@ -7934,7 +7934,7 @@
         <v>5</v>
       </c>
       <c r="G244">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H244" t="s">
         <v>343</v>
@@ -7943,7 +7943,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="245" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
         <v>386</v>
       </c>
@@ -7960,7 +7960,7 @@
         <v>5</v>
       </c>
       <c r="G245">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H245" t="s">
         <v>343</v>
@@ -7969,7 +7969,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="246" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
         <v>386</v>
       </c>
@@ -7986,7 +7986,7 @@
         <v>5</v>
       </c>
       <c r="G246">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H246" t="s">
         <v>343</v>
@@ -7995,7 +7995,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="247" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
         <v>386</v>
       </c>
@@ -8012,7 +8012,7 @@
         <v>5</v>
       </c>
       <c r="G247">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H247" t="s">
         <v>343</v>
@@ -8021,7 +8021,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="248" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
         <v>386</v>
       </c>
@@ -8038,7 +8038,7 @@
         <v>5</v>
       </c>
       <c r="G248">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H248" t="s">
         <v>343</v>
@@ -8047,7 +8047,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="249" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
         <v>386</v>
       </c>
@@ -8064,7 +8064,7 @@
         <v>5</v>
       </c>
       <c r="G249">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H249" t="s">
         <v>344</v>
@@ -8073,7 +8073,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="250" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A250" t="s">
         <v>386</v>
       </c>
@@ -8090,7 +8090,7 @@
         <v>5</v>
       </c>
       <c r="G250">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H250" t="s">
         <v>344</v>
@@ -8099,7 +8099,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="251" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
         <v>386</v>
       </c>
@@ -8116,7 +8116,7 @@
         <v>5</v>
       </c>
       <c r="G251">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H251" t="s">
         <v>344</v>
@@ -8125,7 +8125,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="252" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A252" t="s">
         <v>386</v>
       </c>
@@ -8142,7 +8142,7 @@
         <v>5</v>
       </c>
       <c r="G252">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H252" t="s">
         <v>345</v>
@@ -8151,7 +8151,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="253" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A253" t="s">
         <v>386</v>
       </c>
@@ -8168,7 +8168,7 @@
         <v>5</v>
       </c>
       <c r="G253">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H253" t="s">
         <v>344</v>
@@ -8177,7 +8177,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="254" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A254" t="s">
         <v>386</v>
       </c>
@@ -8194,7 +8194,7 @@
         <v>5</v>
       </c>
       <c r="G254">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H254" t="s">
         <v>344</v>
@@ -8203,7 +8203,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="255" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
         <v>386</v>
       </c>
@@ -8220,7 +8220,7 @@
         <v>5</v>
       </c>
       <c r="G255">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H255" t="s">
         <v>345</v>
@@ -8229,7 +8229,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="256" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A256" t="s">
         <v>386</v>
       </c>
@@ -8246,7 +8246,7 @@
         <v>5</v>
       </c>
       <c r="G256">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H256" t="s">
         <v>344</v>
@@ -8255,7 +8255,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="257" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A257" t="s">
         <v>386</v>
       </c>
@@ -8272,7 +8272,7 @@
         <v>5</v>
       </c>
       <c r="G257">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H257" t="s">
         <v>344</v>
@@ -8281,7 +8281,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="258" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A258" t="s">
         <v>386</v>
       </c>
@@ -8298,7 +8298,7 @@
         <v>5</v>
       </c>
       <c r="G258">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H258" t="s">
         <v>345</v>
@@ -8307,7 +8307,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="259" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A259" t="s">
         <v>386</v>
       </c>
@@ -8324,7 +8324,7 @@
         <v>5</v>
       </c>
       <c r="G259">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H259" t="s">
         <v>345</v>
@@ -8333,7 +8333,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="260" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A260" t="s">
         <v>386</v>
       </c>
@@ -8350,7 +8350,7 @@
         <v>5</v>
       </c>
       <c r="G260">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H260" t="s">
         <v>346</v>
@@ -8359,7 +8359,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="261" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A261" t="s">
         <v>386</v>
       </c>
@@ -8376,7 +8376,7 @@
         <v>5</v>
       </c>
       <c r="G261">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H261" t="s">
         <v>346</v>
@@ -8385,7 +8385,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="262" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A262" t="s">
         <v>386</v>
       </c>
@@ -8402,7 +8402,7 @@
         <v>5</v>
       </c>
       <c r="G262">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H262" t="s">
         <v>346</v>
@@ -8411,7 +8411,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="263" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A263" t="s">
         <v>386</v>
       </c>
@@ -8428,7 +8428,7 @@
         <v>5</v>
       </c>
       <c r="G263">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H263" t="s">
         <v>346</v>
@@ -8437,7 +8437,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="264" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A264" t="s">
         <v>386</v>
       </c>
@@ -8454,7 +8454,7 @@
         <v>5</v>
       </c>
       <c r="G264">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H264" t="s">
         <v>346</v>
@@ -8463,7 +8463,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="265" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A265" t="s">
         <v>386</v>
       </c>
@@ -8480,7 +8480,7 @@
         <v>5</v>
       </c>
       <c r="G265">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H265" t="s">
         <v>346</v>
@@ -8489,7 +8489,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="266" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A266" t="s">
         <v>386</v>
       </c>
@@ -8506,7 +8506,7 @@
         <v>5</v>
       </c>
       <c r="G266">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H266" t="s">
         <v>340</v>
@@ -8515,7 +8515,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="267" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A267" t="s">
         <v>386</v>
       </c>
@@ -8532,7 +8532,7 @@
         <v>5</v>
       </c>
       <c r="G267">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H267" t="s">
         <v>340</v>
@@ -8541,7 +8541,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="268" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A268" t="s">
         <v>386</v>
       </c>
@@ -8558,7 +8558,7 @@
         <v>5</v>
       </c>
       <c r="G268">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H268" t="s">
         <v>340</v>
@@ -8567,7 +8567,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="269" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A269" t="s">
         <v>386</v>
       </c>
@@ -8584,7 +8584,7 @@
         <v>5</v>
       </c>
       <c r="G269">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H269" t="s">
         <v>340</v>
@@ -8593,7 +8593,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="270" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A270" t="s">
         <v>386</v>
       </c>
@@ -8610,7 +8610,7 @@
         <v>5</v>
       </c>
       <c r="G270">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H270" t="s">
         <v>340</v>
@@ -8619,7 +8619,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="271" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A271" t="s">
         <v>386</v>
       </c>
@@ -8636,7 +8636,7 @@
         <v>5</v>
       </c>
       <c r="G271">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H271" t="s">
         <v>340</v>
@@ -8645,7 +8645,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="272" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A272" t="s">
         <v>386</v>
       </c>
@@ -8662,7 +8662,7 @@
         <v>5</v>
       </c>
       <c r="G272">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H272" t="s">
         <v>340</v>
@@ -8671,7 +8671,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="273" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A273" t="s">
         <v>386</v>
       </c>
@@ -8688,7 +8688,7 @@
         <v>5</v>
       </c>
       <c r="G273">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H273" t="s">
         <v>340</v>
@@ -8697,7 +8697,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="274" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B274" t="s">
         <v>279</v>
       </c>
@@ -8711,7 +8711,7 @@
         <v>5</v>
       </c>
       <c r="G274">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H274" t="e">
         <v>#N/A</v>
@@ -8720,7 +8720,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="275" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B275" t="s">
         <v>280</v>
       </c>
@@ -8734,7 +8734,7 @@
         <v>5</v>
       </c>
       <c r="G275">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H275" t="e">
         <v>#N/A</v>
@@ -8743,7 +8743,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="276" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B276" t="s">
         <v>277</v>
       </c>
@@ -8757,7 +8757,7 @@
         <v>5</v>
       </c>
       <c r="G276">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H276" t="e">
         <v>#N/A</v>
@@ -8766,7 +8766,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="277" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B277" t="s">
         <v>278</v>
       </c>
@@ -8780,7 +8780,7 @@
         <v>5</v>
       </c>
       <c r="G277">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H277" t="e">
         <v>#N/A</v>
@@ -8789,7 +8789,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="278" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B278" t="s">
         <v>281</v>
       </c>
@@ -8803,7 +8803,7 @@
         <v>5</v>
       </c>
       <c r="G278">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H278" t="e">
         <v>#N/A</v>
@@ -8812,7 +8812,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="279" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B279" t="s">
         <v>282</v>
       </c>
@@ -8826,7 +8826,7 @@
         <v>5</v>
       </c>
       <c r="G279">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H279" t="e">
         <v>#N/A</v>
@@ -8835,7 +8835,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="280" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B280" t="s">
         <v>283</v>
       </c>
@@ -8849,7 +8849,7 @@
         <v>5</v>
       </c>
       <c r="G280">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H280" t="e">
         <v>#N/A</v>
@@ -8858,7 +8858,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="281" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B281" t="s">
         <v>284</v>
       </c>
@@ -8872,7 +8872,7 @@
         <v>5</v>
       </c>
       <c r="G281">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H281" t="e">
         <v>#N/A</v>
@@ -8881,7 +8881,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="282" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B282" t="s">
         <v>294</v>
       </c>
@@ -8895,7 +8895,7 @@
         <v>5</v>
       </c>
       <c r="G282">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H282" t="e">
         <v>#N/A</v>
@@ -8904,7 +8904,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="283" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B283" t="s">
         <v>295</v>
       </c>
@@ -8918,7 +8918,7 @@
         <v>5</v>
       </c>
       <c r="G283">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H283" t="e">
         <v>#N/A</v>
@@ -8927,7 +8927,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="284" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B284" t="s">
         <v>292</v>
       </c>
@@ -8941,7 +8941,7 @@
         <v>5</v>
       </c>
       <c r="G284">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H284" t="e">
         <v>#N/A</v>
@@ -8950,7 +8950,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="285" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B285" t="s">
         <v>293</v>
       </c>
@@ -8964,7 +8964,7 @@
         <v>5</v>
       </c>
       <c r="G285">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H285" t="e">
         <v>#N/A</v>
@@ -8973,7 +8973,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="286" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B286" t="s">
         <v>291</v>
       </c>
@@ -8987,7 +8987,7 @@
         <v>5</v>
       </c>
       <c r="G286">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H286" t="e">
         <v>#N/A</v>
@@ -8996,7 +8996,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="287" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B287" t="s">
         <v>296</v>
       </c>
@@ -9010,7 +9010,7 @@
         <v>5</v>
       </c>
       <c r="G287">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H287" t="e">
         <v>#N/A</v>
@@ -9019,7 +9019,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="288" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B288" t="s">
         <v>289</v>
       </c>
@@ -9033,7 +9033,7 @@
         <v>5</v>
       </c>
       <c r="G288">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H288" t="e">
         <v>#N/A</v>
@@ -9042,7 +9042,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="289" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="289" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B289" t="s">
         <v>290</v>
       </c>
@@ -9056,7 +9056,7 @@
         <v>5</v>
       </c>
       <c r="G289">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H289" t="e">
         <v>#N/A</v>
@@ -9065,7 +9065,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="290" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="290" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B290" t="s">
         <v>287</v>
       </c>
@@ -9079,7 +9079,7 @@
         <v>5</v>
       </c>
       <c r="G290">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H290" t="e">
         <v>#N/A</v>
@@ -9088,7 +9088,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="291" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="291" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B291" t="s">
         <v>288</v>
       </c>
@@ -9102,7 +9102,7 @@
         <v>5</v>
       </c>
       <c r="G291">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H291" t="e">
         <v>#N/A</v>
@@ -9111,7 +9111,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="292" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="292" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B292" t="s">
         <v>285</v>
       </c>
@@ -9125,7 +9125,7 @@
         <v>5</v>
       </c>
       <c r="G292">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H292" t="e">
         <v>#N/A</v>
@@ -9134,7 +9134,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="293" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="293" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B293" t="s">
         <v>286</v>
       </c>
@@ -9148,7 +9148,7 @@
         <v>5</v>
       </c>
       <c r="G293">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H293" t="e">
         <v>#N/A</v>
@@ -9157,7 +9157,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="294" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="294" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B294" t="s">
         <v>297</v>
       </c>
@@ -9171,7 +9171,7 @@
         <v>5</v>
       </c>
       <c r="G294">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H294" t="e">
         <v>#N/A</v>
@@ -9180,7 +9180,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="295" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="295" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B295" t="s">
         <v>298</v>
       </c>
@@ -9194,7 +9194,7 @@
         <v>5</v>
       </c>
       <c r="G295">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H295" t="e">
         <v>#N/A</v>
@@ -9203,7 +9203,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="296" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="296" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B296" t="s">
         <v>299</v>
       </c>
@@ -9217,7 +9217,7 @@
         <v>5</v>
       </c>
       <c r="G296">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H296" t="e">
         <v>#N/A</v>
@@ -9226,7 +9226,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="297" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="297" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B297" t="s">
         <v>300</v>
       </c>
@@ -9240,7 +9240,7 @@
         <v>5</v>
       </c>
       <c r="G297">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H297" t="e">
         <v>#N/A</v>
@@ -9249,7 +9249,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="298" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="298" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B298" t="s">
         <v>301</v>
       </c>
@@ -9263,7 +9263,7 @@
         <v>5</v>
       </c>
       <c r="G298">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H298" t="e">
         <v>#N/A</v>
@@ -9272,7 +9272,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="299" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="299" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B299" t="s">
         <v>302</v>
       </c>
@@ -9286,7 +9286,7 @@
         <v>5</v>
       </c>
       <c r="G299">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H299" t="e">
         <v>#N/A</v>
@@ -9295,7 +9295,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="300" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="300" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B300" t="s">
         <v>303</v>
       </c>
@@ -9309,7 +9309,7 @@
         <v>5</v>
       </c>
       <c r="G300">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H300" t="e">
         <v>#N/A</v>
@@ -9318,7 +9318,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="301" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="301" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B301" t="s">
         <v>304</v>
       </c>
@@ -9332,7 +9332,7 @@
         <v>5</v>
       </c>
       <c r="G301">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H301" t="e">
         <v>#N/A</v>
@@ -9341,7 +9341,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="302" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="302" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B302" t="s">
         <v>305</v>
       </c>
@@ -9355,7 +9355,7 @@
         <v>5</v>
       </c>
       <c r="G302">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H302" t="e">
         <v>#N/A</v>
@@ -9364,7 +9364,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="303" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="303" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B303" t="s">
         <v>306</v>
       </c>
@@ -9378,7 +9378,7 @@
         <v>5</v>
       </c>
       <c r="G303">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H303" t="e">
         <v>#N/A</v>
@@ -9387,7 +9387,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="304" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="304" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B304" t="s">
         <v>307</v>
       </c>
@@ -9401,7 +9401,7 @@
         <v>5</v>
       </c>
       <c r="G304">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H304" t="e">
         <v>#N/A</v>
@@ -9410,7 +9410,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="305" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B305" t="s">
         <v>308</v>
       </c>
@@ -9424,7 +9424,7 @@
         <v>5</v>
       </c>
       <c r="G305">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H305" t="e">
         <v>#N/A</v>
@@ -9433,7 +9433,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="306" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B306" t="s">
         <v>309</v>
       </c>
@@ -9447,7 +9447,7 @@
         <v>5</v>
       </c>
       <c r="G306">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H306" t="e">
         <v>#N/A</v>
@@ -9456,7 +9456,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="307" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B307" t="s">
         <v>310</v>
       </c>
@@ -9470,7 +9470,7 @@
         <v>5</v>
       </c>
       <c r="G307">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H307" t="e">
         <v>#N/A</v>
@@ -9479,7 +9479,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="308" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B308" t="s">
         <v>311</v>
       </c>
@@ -9493,7 +9493,7 @@
         <v>5</v>
       </c>
       <c r="G308">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H308" t="e">
         <v>#N/A</v>
@@ -9502,7 +9502,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="309" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B309" t="s">
         <v>312</v>
       </c>
@@ -9516,7 +9516,7 @@
         <v>5</v>
       </c>
       <c r="G309">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H309" t="e">
         <v>#N/A</v>
@@ -9525,7 +9525,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="310" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B310" t="s">
         <v>313</v>
       </c>
@@ -9539,7 +9539,7 @@
         <v>5</v>
       </c>
       <c r="G310">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H310" t="e">
         <v>#N/A</v>
@@ -9548,7 +9548,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="311" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B311" t="s">
         <v>314</v>
       </c>
@@ -9562,7 +9562,7 @@
         <v>5</v>
       </c>
       <c r="G311">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H311" t="e">
         <v>#N/A</v>
@@ -9571,7 +9571,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="312" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B312" t="s">
         <v>315</v>
       </c>
@@ -9585,7 +9585,7 @@
         <v>5</v>
       </c>
       <c r="G312">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H312" t="e">
         <v>#N/A</v>
@@ -9594,7 +9594,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="313" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B313" t="s">
         <v>316</v>
       </c>
@@ -9608,7 +9608,7 @@
         <v>5</v>
       </c>
       <c r="G313">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H313" t="e">
         <v>#N/A</v>
@@ -9617,7 +9617,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="314" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B314" t="s">
         <v>317</v>
       </c>
@@ -9631,7 +9631,7 @@
         <v>5</v>
       </c>
       <c r="G314">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H314" t="e">
         <v>#N/A</v>
@@ -9640,7 +9640,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="315" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B315" t="s">
         <v>318</v>
       </c>
@@ -9654,7 +9654,7 @@
         <v>5</v>
       </c>
       <c r="G315">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H315" t="e">
         <v>#N/A</v>
@@ -9663,7 +9663,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="316" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B316" t="s">
         <v>319</v>
       </c>
@@ -9677,7 +9677,7 @@
         <v>5</v>
       </c>
       <c r="G316">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H316" t="e">
         <v>#N/A</v>
@@ -9686,7 +9686,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="317" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B317" t="s">
         <v>320</v>
       </c>
@@ -9700,7 +9700,7 @@
         <v>5</v>
       </c>
       <c r="G317">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H317" t="e">
         <v>#N/A</v>
@@ -9709,7 +9709,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="318" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B318" t="s">
         <v>321</v>
       </c>
@@ -9723,7 +9723,7 @@
         <v>5</v>
       </c>
       <c r="G318">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H318" t="e">
         <v>#N/A</v>
@@ -9732,7 +9732,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="319" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B319" t="s">
         <v>322</v>
       </c>
@@ -9746,7 +9746,7 @@
         <v>5</v>
       </c>
       <c r="G319">
-        <v>0.03</v>
+        <v>1E-3</v>
       </c>
       <c r="H319" t="e">
         <v>#N/A</v>
@@ -9755,7 +9755,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="320" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A320" t="s">
         <v>385</v>
       </c>
@@ -9781,7 +9781,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="321" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B321" t="s">
         <v>335</v>
       </c>
@@ -9804,7 +9804,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="322" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B322" t="s">
         <v>333</v>
       </c>
@@ -9827,7 +9827,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="323" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A323" t="s">
         <v>384</v>
       </c>
@@ -9844,7 +9844,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="324" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A324" t="s">
         <v>384</v>
       </c>
@@ -9861,7 +9861,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="325" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A325" t="s">
         <v>384</v>
       </c>
@@ -9878,7 +9878,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="326" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A326" t="s">
         <v>384</v>
       </c>
@@ -9895,7 +9895,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="327" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A327" t="s">
         <v>384</v>
       </c>
@@ -9912,7 +9912,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="328" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A328" t="s">
         <v>384</v>
       </c>
@@ -9929,7 +9929,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="329" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A329" t="s">
         <v>384</v>
       </c>
@@ -9946,7 +9946,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="330" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A330" t="s">
         <v>384</v>
       </c>
@@ -9963,7 +9963,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="331" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A331" t="s">
         <v>385</v>
       </c>
@@ -9981,7 +9981,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:G322" xr:uid="{11CF1E80-DA68-4CB3-BCA6-87A36AC41371}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -9998,18 +9997,18 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>324</v>
       </c>
@@ -10017,7 +10016,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>328</v>
       </c>
@@ -10025,7 +10024,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>323</v>
       </c>

</xml_diff>

<commit_message>
removed duplicative tollclass values
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/TOLLCLASS_Designations.xlsx
+++ b/utilities/NextGenFwys/TOLLCLASS_Designations.xlsx
@@ -8,17 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4933EA6D-93C3-4E56-B2F0-9CF2787B1048}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBDFD8C1-111C-4818-8C77-890ACD69F603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{0F0A9957-56E7-4C48-967B-2AB2A1965C2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs_for_tollcalib" sheetId="1" r:id="rId1"/>
-    <sheet name="TollclassGrouping(fromAnup)" sheetId="3" r:id="rId2"/>
-    <sheet name="Readme - numbering convention" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
+    <sheet name="TollclassGrouping(fromAnup)" sheetId="3" r:id="rId3"/>
+    <sheet name="Readme - numbering convention" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Inputs_for_tollcalib!$A$1:$I$457</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$I$1:$L$122</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2041" uniqueCount="591">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2347" uniqueCount="593">
   <si>
     <t>SR92 SM - I-280 Interchange to US101 Interchange - WB</t>
   </si>
@@ -1813,6 +1815,12 @@
   </si>
   <si>
     <t>na</t>
+  </si>
+  <si>
+    <t>arterial toll class</t>
+  </si>
+  <si>
+    <t>right4</t>
   </si>
 </sst>
 </file>
@@ -2225,11 +2233,11 @@
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
-  <dimension ref="A1:I429"/>
+  <dimension ref="A1:I443"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <pane ySplit="1" topLeftCell="A411" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H443" sqref="H443:I443"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11679,13 +11687,13 @@
         <v>590</v>
       </c>
       <c r="C362">
-        <v>770121</v>
+        <v>770117</v>
       </c>
       <c r="H362" t="s">
-        <v>399</v>
+        <v>427</v>
       </c>
       <c r="I362" t="s">
-        <v>402</v>
+        <v>427</v>
       </c>
     </row>
     <row r="363" spans="1:9" x14ac:dyDescent="0.35">
@@ -11696,13 +11704,13 @@
         <v>590</v>
       </c>
       <c r="C363">
-        <v>770122</v>
+        <v>770118</v>
       </c>
       <c r="H363" t="s">
-        <v>405</v>
+        <v>428</v>
       </c>
       <c r="I363" t="s">
-        <v>408</v>
+        <v>428</v>
       </c>
     </row>
     <row r="364" spans="1:9" x14ac:dyDescent="0.35">
@@ -11713,13 +11721,13 @@
         <v>590</v>
       </c>
       <c r="C364">
-        <v>770123</v>
+        <v>770119</v>
       </c>
       <c r="H364" t="s">
-        <v>399</v>
+        <v>430</v>
       </c>
       <c r="I364" t="s">
-        <v>402</v>
+        <v>432</v>
       </c>
     </row>
     <row r="365" spans="1:9" x14ac:dyDescent="0.35">
@@ -11730,13 +11738,13 @@
         <v>590</v>
       </c>
       <c r="C365">
-        <v>770124</v>
+        <v>770120</v>
       </c>
       <c r="H365" t="s">
-        <v>405</v>
+        <v>435</v>
       </c>
       <c r="I365" t="s">
-        <v>408</v>
+        <v>436</v>
       </c>
     </row>
     <row r="366" spans="1:9" x14ac:dyDescent="0.35">
@@ -11747,13 +11755,13 @@
         <v>590</v>
       </c>
       <c r="C366">
-        <v>770135</v>
+        <v>770121</v>
       </c>
       <c r="H366" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="I366" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
     </row>
     <row r="367" spans="1:9" x14ac:dyDescent="0.35">
@@ -11764,13 +11772,13 @@
         <v>590</v>
       </c>
       <c r="C367">
-        <v>770136</v>
+        <v>770122</v>
       </c>
       <c r="H367" t="s">
-        <v>399</v>
+        <v>405</v>
       </c>
       <c r="I367" t="s">
-        <v>401</v>
+        <v>408</v>
       </c>
     </row>
     <row r="368" spans="1:9" x14ac:dyDescent="0.35">
@@ -11781,13 +11789,13 @@
         <v>590</v>
       </c>
       <c r="C368">
-        <v>770231</v>
+        <v>770123</v>
       </c>
       <c r="H368" t="s">
-        <v>428</v>
+        <v>399</v>
       </c>
       <c r="I368" t="s">
-        <v>428</v>
+        <v>402</v>
       </c>
     </row>
     <row r="369" spans="1:9" x14ac:dyDescent="0.35">
@@ -11798,13 +11806,13 @@
         <v>590</v>
       </c>
       <c r="C369">
-        <v>770232</v>
+        <v>770124</v>
       </c>
       <c r="H369" t="s">
-        <v>427</v>
+        <v>405</v>
       </c>
       <c r="I369" t="s">
-        <v>427</v>
+        <v>408</v>
       </c>
     </row>
     <row r="370" spans="1:9" x14ac:dyDescent="0.35">
@@ -11815,13 +11823,13 @@
         <v>590</v>
       </c>
       <c r="C370">
-        <v>770233</v>
+        <v>770135</v>
       </c>
       <c r="H370" t="s">
-        <v>428</v>
+        <v>405</v>
       </c>
       <c r="I370" t="s">
-        <v>428</v>
+        <v>407</v>
       </c>
     </row>
     <row r="371" spans="1:9" x14ac:dyDescent="0.35">
@@ -11832,13 +11840,13 @@
         <v>590</v>
       </c>
       <c r="C371">
-        <v>770234</v>
+        <v>770136</v>
       </c>
       <c r="H371" t="s">
-        <v>427</v>
+        <v>399</v>
       </c>
       <c r="I371" t="s">
-        <v>427</v>
+        <v>401</v>
       </c>
     </row>
     <row r="372" spans="1:9" x14ac:dyDescent="0.35">
@@ -11849,13 +11857,13 @@
         <v>590</v>
       </c>
       <c r="C372">
-        <v>770239</v>
+        <v>770171</v>
       </c>
       <c r="H372" t="s">
-        <v>388</v>
+        <v>430</v>
       </c>
       <c r="I372" t="s">
-        <v>394</v>
+        <v>434</v>
       </c>
     </row>
     <row r="373" spans="1:9" x14ac:dyDescent="0.35">
@@ -11866,13 +11874,13 @@
         <v>590</v>
       </c>
       <c r="C373">
-        <v>770240</v>
+        <v>770172</v>
       </c>
       <c r="H373" t="s">
-        <v>395</v>
+        <v>435</v>
       </c>
       <c r="I373" t="s">
-        <v>398</v>
+        <v>437</v>
       </c>
     </row>
     <row r="374" spans="1:9" x14ac:dyDescent="0.35">
@@ -11883,13 +11891,13 @@
         <v>590</v>
       </c>
       <c r="C374">
-        <v>770241</v>
+        <v>770231</v>
       </c>
       <c r="H374" t="s">
-        <v>384</v>
+        <v>428</v>
       </c>
       <c r="I374" t="s">
-        <v>385</v>
+        <v>428</v>
       </c>
     </row>
     <row r="375" spans="1:9" x14ac:dyDescent="0.35">
@@ -11900,13 +11908,13 @@
         <v>590</v>
       </c>
       <c r="C375">
-        <v>770242</v>
+        <v>770232</v>
       </c>
       <c r="H375" t="s">
-        <v>379</v>
+        <v>427</v>
       </c>
       <c r="I375" t="s">
-        <v>381</v>
+        <v>427</v>
       </c>
     </row>
     <row r="376" spans="1:9" x14ac:dyDescent="0.35">
@@ -11917,13 +11925,13 @@
         <v>590</v>
       </c>
       <c r="C376">
-        <v>770243</v>
+        <v>770233</v>
       </c>
       <c r="H376" t="s">
-        <v>388</v>
+        <v>428</v>
       </c>
       <c r="I376" t="s">
-        <v>390</v>
+        <v>428</v>
       </c>
     </row>
     <row r="377" spans="1:9" x14ac:dyDescent="0.35">
@@ -11934,13 +11942,13 @@
         <v>590</v>
       </c>
       <c r="C377">
-        <v>770244</v>
+        <v>770234</v>
       </c>
       <c r="H377" t="s">
-        <v>395</v>
+        <v>427</v>
       </c>
       <c r="I377" t="s">
-        <v>396</v>
+        <v>427</v>
       </c>
     </row>
     <row r="378" spans="1:9" x14ac:dyDescent="0.35">
@@ -11951,13 +11959,13 @@
         <v>590</v>
       </c>
       <c r="C378">
-        <v>770245</v>
+        <v>770239</v>
       </c>
       <c r="H378" t="s">
         <v>388</v>
       </c>
       <c r="I378" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
     </row>
     <row r="379" spans="1:9" x14ac:dyDescent="0.35">
@@ -11968,13 +11976,13 @@
         <v>590</v>
       </c>
       <c r="C379">
-        <v>770246</v>
+        <v>770240</v>
       </c>
       <c r="H379" t="s">
         <v>395</v>
       </c>
       <c r="I379" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
     </row>
     <row r="380" spans="1:9" x14ac:dyDescent="0.35">
@@ -11985,13 +11993,13 @@
         <v>590</v>
       </c>
       <c r="C380">
-        <v>770281</v>
+        <v>770241</v>
       </c>
       <c r="H380" t="s">
-        <v>417</v>
+        <v>384</v>
       </c>
       <c r="I380" t="s">
-        <v>417</v>
+        <v>385</v>
       </c>
     </row>
     <row r="381" spans="1:9" x14ac:dyDescent="0.35">
@@ -12002,13 +12010,13 @@
         <v>590</v>
       </c>
       <c r="C381">
-        <v>770282</v>
+        <v>770242</v>
       </c>
       <c r="H381" t="s">
-        <v>418</v>
+        <v>379</v>
       </c>
       <c r="I381" t="s">
-        <v>418</v>
+        <v>381</v>
       </c>
     </row>
     <row r="382" spans="1:9" x14ac:dyDescent="0.35">
@@ -12019,13 +12027,13 @@
         <v>590</v>
       </c>
       <c r="C382">
-        <v>770283</v>
+        <v>770243</v>
       </c>
       <c r="H382" t="s">
-        <v>430</v>
+        <v>388</v>
       </c>
       <c r="I382" t="s">
-        <v>434</v>
+        <v>390</v>
       </c>
     </row>
     <row r="383" spans="1:9" x14ac:dyDescent="0.35">
@@ -12036,13 +12044,13 @@
         <v>590</v>
       </c>
       <c r="C383">
-        <v>770284</v>
+        <v>770244</v>
       </c>
       <c r="H383" t="s">
-        <v>435</v>
+        <v>395</v>
       </c>
       <c r="I383" t="s">
-        <v>437</v>
+        <v>396</v>
       </c>
     </row>
     <row r="384" spans="1:9" x14ac:dyDescent="0.35">
@@ -12053,13 +12061,13 @@
         <v>590</v>
       </c>
       <c r="C384">
-        <v>770287</v>
+        <v>770245</v>
       </c>
       <c r="H384" t="s">
-        <v>420</v>
+        <v>388</v>
       </c>
       <c r="I384" t="s">
-        <v>421</v>
+        <v>390</v>
       </c>
     </row>
     <row r="385" spans="1:9" x14ac:dyDescent="0.35">
@@ -12070,13 +12078,13 @@
         <v>590</v>
       </c>
       <c r="C385">
-        <v>770288</v>
+        <v>770246</v>
       </c>
       <c r="H385" t="s">
-        <v>423</v>
+        <v>395</v>
       </c>
       <c r="I385" t="s">
-        <v>424</v>
+        <v>396</v>
       </c>
     </row>
     <row r="386" spans="1:9" x14ac:dyDescent="0.35">
@@ -12087,13 +12095,13 @@
         <v>590</v>
       </c>
       <c r="C386">
-        <v>770289</v>
+        <v>770281</v>
       </c>
       <c r="H386" t="s">
-        <v>411</v>
+        <v>417</v>
       </c>
       <c r="I386" t="s">
-        <v>413</v>
+        <v>417</v>
       </c>
     </row>
     <row r="387" spans="1:9" x14ac:dyDescent="0.35">
@@ -12104,13 +12112,13 @@
         <v>590</v>
       </c>
       <c r="C387">
-        <v>770290</v>
+        <v>770282</v>
       </c>
       <c r="H387" t="s">
-        <v>414</v>
+        <v>418</v>
       </c>
       <c r="I387" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
     </row>
     <row r="388" spans="1:9" x14ac:dyDescent="0.35">
@@ -12121,13 +12129,13 @@
         <v>590</v>
       </c>
       <c r="C388">
-        <v>770381</v>
+        <v>770283</v>
       </c>
       <c r="H388" t="s">
-        <v>420</v>
+        <v>430</v>
       </c>
       <c r="I388" t="s">
-        <v>421</v>
+        <v>434</v>
       </c>
     </row>
     <row r="389" spans="1:9" x14ac:dyDescent="0.35">
@@ -12138,13 +12146,13 @@
         <v>590</v>
       </c>
       <c r="C389">
-        <v>770382</v>
+        <v>770284</v>
       </c>
       <c r="H389" t="s">
-        <v>423</v>
+        <v>435</v>
       </c>
       <c r="I389" t="s">
-        <v>424</v>
+        <v>437</v>
       </c>
     </row>
     <row r="390" spans="1:9" x14ac:dyDescent="0.35">
@@ -12155,13 +12163,13 @@
         <v>590</v>
       </c>
       <c r="C390">
-        <v>770401</v>
+        <v>770285</v>
       </c>
       <c r="H390" t="s">
-        <v>405</v>
+        <v>430</v>
       </c>
       <c r="I390" t="s">
-        <v>410</v>
+        <v>434</v>
       </c>
     </row>
     <row r="391" spans="1:9" x14ac:dyDescent="0.35">
@@ -12172,13 +12180,13 @@
         <v>590</v>
       </c>
       <c r="C391">
-        <v>770402</v>
+        <v>770286</v>
       </c>
       <c r="H391" t="s">
-        <v>399</v>
+        <v>435</v>
       </c>
       <c r="I391" t="s">
-        <v>404</v>
+        <v>437</v>
       </c>
     </row>
     <row r="392" spans="1:9" x14ac:dyDescent="0.35">
@@ -12189,13 +12197,13 @@
         <v>590</v>
       </c>
       <c r="C392">
-        <v>770403</v>
+        <v>770287</v>
       </c>
       <c r="H392" t="s">
-        <v>405</v>
+        <v>420</v>
       </c>
       <c r="I392" t="s">
-        <v>410</v>
+        <v>421</v>
       </c>
     </row>
     <row r="393" spans="1:9" x14ac:dyDescent="0.35">
@@ -12206,13 +12214,13 @@
         <v>590</v>
       </c>
       <c r="C393">
-        <v>770404</v>
+        <v>770288</v>
       </c>
       <c r="H393" t="s">
-        <v>399</v>
+        <v>423</v>
       </c>
       <c r="I393" t="s">
-        <v>404</v>
+        <v>424</v>
       </c>
     </row>
     <row r="394" spans="1:9" x14ac:dyDescent="0.35">
@@ -12223,13 +12231,13 @@
         <v>590</v>
       </c>
       <c r="C394">
-        <v>770407</v>
+        <v>770289</v>
       </c>
       <c r="H394" t="s">
-        <v>405</v>
+        <v>411</v>
       </c>
       <c r="I394" t="s">
-        <v>410</v>
+        <v>413</v>
       </c>
     </row>
     <row r="395" spans="1:9" x14ac:dyDescent="0.35">
@@ -12240,13 +12248,13 @@
         <v>590</v>
       </c>
       <c r="C395">
-        <v>770408</v>
+        <v>770290</v>
       </c>
       <c r="H395" t="s">
-        <v>399</v>
+        <v>414</v>
       </c>
       <c r="I395" t="s">
-        <v>404</v>
+        <v>416</v>
       </c>
     </row>
     <row r="396" spans="1:9" x14ac:dyDescent="0.35">
@@ -12257,13 +12265,13 @@
         <v>590</v>
       </c>
       <c r="C396">
-        <v>770581</v>
+        <v>770381</v>
       </c>
       <c r="H396" t="s">
-        <v>384</v>
+        <v>420</v>
       </c>
       <c r="I396" t="s">
-        <v>386</v>
+        <v>421</v>
       </c>
     </row>
     <row r="397" spans="1:9" x14ac:dyDescent="0.35">
@@ -12274,13 +12282,13 @@
         <v>590</v>
       </c>
       <c r="C397">
-        <v>770582</v>
+        <v>770382</v>
       </c>
       <c r="H397" t="s">
-        <v>379</v>
+        <v>423</v>
       </c>
       <c r="I397" t="s">
-        <v>383</v>
+        <v>424</v>
       </c>
     </row>
     <row r="398" spans="1:9" x14ac:dyDescent="0.35">
@@ -12291,13 +12299,13 @@
         <v>590</v>
       </c>
       <c r="C398">
-        <v>770583</v>
+        <v>770401</v>
       </c>
       <c r="H398" t="s">
-        <v>384</v>
+        <v>405</v>
       </c>
       <c r="I398" t="s">
-        <v>385</v>
+        <v>410</v>
       </c>
     </row>
     <row r="399" spans="1:9" x14ac:dyDescent="0.35">
@@ -12308,13 +12316,13 @@
         <v>590</v>
       </c>
       <c r="C399">
-        <v>770584</v>
+        <v>770402</v>
       </c>
       <c r="H399" t="s">
-        <v>379</v>
+        <v>399</v>
       </c>
       <c r="I399" t="s">
-        <v>381</v>
+        <v>404</v>
       </c>
     </row>
     <row r="400" spans="1:9" x14ac:dyDescent="0.35">
@@ -12325,13 +12333,13 @@
         <v>590</v>
       </c>
       <c r="C400">
-        <v>770585</v>
+        <v>770403</v>
       </c>
       <c r="H400" t="s">
-        <v>388</v>
+        <v>405</v>
       </c>
       <c r="I400" t="s">
-        <v>394</v>
+        <v>410</v>
       </c>
     </row>
     <row r="401" spans="1:9" x14ac:dyDescent="0.35">
@@ -12342,13 +12350,13 @@
         <v>590</v>
       </c>
       <c r="C401">
-        <v>770586</v>
+        <v>770404</v>
       </c>
       <c r="H401" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="I401" t="s">
-        <v>398</v>
+        <v>404</v>
       </c>
     </row>
     <row r="402" spans="1:9" x14ac:dyDescent="0.35">
@@ -12359,13 +12367,13 @@
         <v>590</v>
       </c>
       <c r="C402">
-        <v>770587</v>
+        <v>770407</v>
       </c>
       <c r="H402" t="s">
         <v>405</v>
       </c>
       <c r="I402" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="403" spans="1:9" x14ac:dyDescent="0.35">
@@ -12376,13 +12384,13 @@
         <v>590</v>
       </c>
       <c r="C403">
-        <v>770588</v>
+        <v>770408</v>
       </c>
       <c r="H403" t="s">
         <v>399</v>
       </c>
       <c r="I403" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
     </row>
     <row r="404" spans="1:9" x14ac:dyDescent="0.35">
@@ -12393,13 +12401,13 @@
         <v>590</v>
       </c>
       <c r="C404">
-        <v>770589</v>
+        <v>770581</v>
       </c>
       <c r="H404" t="s">
-        <v>405</v>
+        <v>384</v>
       </c>
       <c r="I404" t="s">
-        <v>409</v>
+        <v>386</v>
       </c>
     </row>
     <row r="405" spans="1:9" x14ac:dyDescent="0.35">
@@ -12410,13 +12418,13 @@
         <v>590</v>
       </c>
       <c r="C405">
-        <v>770590</v>
+        <v>770582</v>
       </c>
       <c r="H405" t="s">
-        <v>399</v>
+        <v>379</v>
       </c>
       <c r="I405" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
     </row>
     <row r="406" spans="1:9" x14ac:dyDescent="0.35">
@@ -12427,13 +12435,13 @@
         <v>590</v>
       </c>
       <c r="C406">
-        <v>770683</v>
+        <v>770583</v>
       </c>
       <c r="H406" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="I406" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
     </row>
     <row r="407" spans="1:9" x14ac:dyDescent="0.35">
@@ -12444,13 +12452,13 @@
         <v>590</v>
       </c>
       <c r="C407">
-        <v>770684</v>
+        <v>770584</v>
       </c>
       <c r="H407" t="s">
-        <v>395</v>
+        <v>379</v>
       </c>
       <c r="I407" t="s">
-        <v>396</v>
+        <v>381</v>
       </c>
     </row>
     <row r="408" spans="1:9" x14ac:dyDescent="0.35">
@@ -12461,7 +12469,7 @@
         <v>590</v>
       </c>
       <c r="C408">
-        <v>770689</v>
+        <v>770585</v>
       </c>
       <c r="H408" t="s">
         <v>388</v>
@@ -12478,7 +12486,7 @@
         <v>590</v>
       </c>
       <c r="C409">
-        <v>770690</v>
+        <v>770586</v>
       </c>
       <c r="H409" t="s">
         <v>395</v>
@@ -12495,13 +12503,13 @@
         <v>590</v>
       </c>
       <c r="C410">
-        <v>770853</v>
+        <v>770587</v>
       </c>
       <c r="H410" t="s">
-        <v>435</v>
+        <v>405</v>
       </c>
       <c r="I410" t="s">
-        <v>436</v>
+        <v>409</v>
       </c>
     </row>
     <row r="411" spans="1:9" x14ac:dyDescent="0.35">
@@ -12512,13 +12520,13 @@
         <v>590</v>
       </c>
       <c r="C411">
-        <v>770854</v>
+        <v>770588</v>
       </c>
       <c r="H411" t="s">
-        <v>435</v>
+        <v>399</v>
       </c>
       <c r="I411" t="s">
-        <v>436</v>
+        <v>403</v>
       </c>
     </row>
     <row r="412" spans="1:9" x14ac:dyDescent="0.35">
@@ -12529,13 +12537,13 @@
         <v>590</v>
       </c>
       <c r="C412">
-        <v>770855</v>
+        <v>770589</v>
       </c>
       <c r="H412" t="s">
-        <v>435</v>
+        <v>405</v>
       </c>
       <c r="I412" t="s">
-        <v>436</v>
+        <v>409</v>
       </c>
     </row>
     <row r="413" spans="1:9" x14ac:dyDescent="0.35">
@@ -12546,13 +12554,13 @@
         <v>590</v>
       </c>
       <c r="C413">
-        <v>770856</v>
+        <v>770590</v>
       </c>
       <c r="H413" t="s">
-        <v>430</v>
+        <v>399</v>
       </c>
       <c r="I413" t="s">
-        <v>432</v>
+        <v>403</v>
       </c>
     </row>
     <row r="414" spans="1:9" x14ac:dyDescent="0.35">
@@ -12563,13 +12571,13 @@
         <v>590</v>
       </c>
       <c r="C414">
-        <v>770871</v>
+        <v>770683</v>
       </c>
       <c r="H414" t="s">
-        <v>430</v>
+        <v>388</v>
       </c>
       <c r="I414" t="s">
-        <v>432</v>
+        <v>390</v>
       </c>
     </row>
     <row r="415" spans="1:9" x14ac:dyDescent="0.35">
@@ -12580,13 +12588,13 @@
         <v>590</v>
       </c>
       <c r="C415">
-        <v>770872</v>
+        <v>770684</v>
       </c>
       <c r="H415" t="s">
-        <v>435</v>
+        <v>395</v>
       </c>
       <c r="I415" t="s">
-        <v>436</v>
+        <v>396</v>
       </c>
     </row>
     <row r="416" spans="1:9" x14ac:dyDescent="0.35">
@@ -12597,13 +12605,13 @@
         <v>590</v>
       </c>
       <c r="C416">
-        <v>770879</v>
+        <v>770689</v>
       </c>
       <c r="H416" t="s">
-        <v>379</v>
+        <v>388</v>
       </c>
       <c r="I416" t="s">
-        <v>383</v>
+        <v>394</v>
       </c>
     </row>
     <row r="417" spans="1:9" x14ac:dyDescent="0.35">
@@ -12614,13 +12622,13 @@
         <v>590</v>
       </c>
       <c r="C417">
-        <v>770880</v>
+        <v>770690</v>
       </c>
       <c r="H417" t="s">
-        <v>384</v>
+        <v>395</v>
       </c>
       <c r="I417" t="s">
-        <v>386</v>
+        <v>398</v>
       </c>
     </row>
     <row r="418" spans="1:9" x14ac:dyDescent="0.35">
@@ -12631,13 +12639,13 @@
         <v>590</v>
       </c>
       <c r="C418">
-        <v>770881</v>
+        <v>770691</v>
       </c>
       <c r="H418" t="s">
-        <v>388</v>
+        <v>435</v>
       </c>
       <c r="I418" t="s">
-        <v>394</v>
+        <v>437</v>
       </c>
     </row>
     <row r="419" spans="1:9" x14ac:dyDescent="0.35">
@@ -12648,13 +12656,13 @@
         <v>590</v>
       </c>
       <c r="C419">
-        <v>770882</v>
+        <v>770692</v>
       </c>
       <c r="H419" t="s">
-        <v>395</v>
+        <v>430</v>
       </c>
       <c r="I419" t="s">
-        <v>398</v>
+        <v>434</v>
       </c>
     </row>
     <row r="420" spans="1:9" x14ac:dyDescent="0.35">
@@ -12665,13 +12673,13 @@
         <v>590</v>
       </c>
       <c r="C420">
-        <v>770883</v>
+        <v>770853</v>
       </c>
       <c r="H420" t="s">
-        <v>388</v>
+        <v>435</v>
       </c>
       <c r="I420" t="s">
-        <v>394</v>
+        <v>436</v>
       </c>
     </row>
     <row r="421" spans="1:9" x14ac:dyDescent="0.35">
@@ -12682,13 +12690,13 @@
         <v>590</v>
       </c>
       <c r="C421">
-        <v>770884</v>
+        <v>770854</v>
       </c>
       <c r="H421" t="s">
-        <v>395</v>
+        <v>435</v>
       </c>
       <c r="I421" t="s">
-        <v>398</v>
+        <v>436</v>
       </c>
     </row>
     <row r="422" spans="1:9" x14ac:dyDescent="0.35">
@@ -12699,13 +12707,13 @@
         <v>590</v>
       </c>
       <c r="C422">
-        <v>770885</v>
+        <v>770855</v>
       </c>
       <c r="H422" t="s">
-        <v>388</v>
+        <v>435</v>
       </c>
       <c r="I422" t="s">
-        <v>394</v>
+        <v>436</v>
       </c>
     </row>
     <row r="423" spans="1:9" x14ac:dyDescent="0.35">
@@ -12716,13 +12724,13 @@
         <v>590</v>
       </c>
       <c r="C423">
-        <v>770886</v>
+        <v>770856</v>
       </c>
       <c r="H423" t="s">
-        <v>395</v>
+        <v>430</v>
       </c>
       <c r="I423" t="s">
-        <v>398</v>
+        <v>432</v>
       </c>
     </row>
     <row r="424" spans="1:9" x14ac:dyDescent="0.35">
@@ -12733,13 +12741,13 @@
         <v>590</v>
       </c>
       <c r="C424">
-        <v>770887</v>
+        <v>770871</v>
       </c>
       <c r="H424" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="I424" t="s">
-        <v>428</v>
+        <v>432</v>
       </c>
     </row>
     <row r="425" spans="1:9" x14ac:dyDescent="0.35">
@@ -12750,13 +12758,13 @@
         <v>590</v>
       </c>
       <c r="C425">
-        <v>770888</v>
+        <v>770872</v>
       </c>
       <c r="H425" t="s">
-        <v>427</v>
+        <v>435</v>
       </c>
       <c r="I425" t="s">
-        <v>427</v>
+        <v>436</v>
       </c>
     </row>
     <row r="426" spans="1:9" x14ac:dyDescent="0.35">
@@ -12767,13 +12775,13 @@
         <v>590</v>
       </c>
       <c r="C426">
-        <v>770923</v>
+        <v>770879</v>
       </c>
       <c r="H426" t="s">
-        <v>411</v>
+        <v>379</v>
       </c>
       <c r="I426" t="s">
-        <v>413</v>
+        <v>383</v>
       </c>
     </row>
     <row r="427" spans="1:9" x14ac:dyDescent="0.35">
@@ -12784,13 +12792,13 @@
         <v>590</v>
       </c>
       <c r="C427">
-        <v>770924</v>
+        <v>770880</v>
       </c>
       <c r="H427" t="s">
-        <v>414</v>
+        <v>384</v>
       </c>
       <c r="I427" t="s">
-        <v>416</v>
+        <v>386</v>
       </c>
     </row>
     <row r="428" spans="1:9" x14ac:dyDescent="0.35">
@@ -12801,13 +12809,13 @@
         <v>590</v>
       </c>
       <c r="C428">
-        <v>770981</v>
+        <v>770881</v>
       </c>
       <c r="H428" t="s">
-        <v>384</v>
+        <v>388</v>
       </c>
       <c r="I428" t="s">
-        <v>385</v>
+        <v>394</v>
       </c>
     </row>
     <row r="429" spans="1:9" x14ac:dyDescent="0.35">
@@ -12818,12 +12826,250 @@
         <v>590</v>
       </c>
       <c r="C429">
+        <v>770882</v>
+      </c>
+      <c r="H429" t="s">
+        <v>395</v>
+      </c>
+      <c r="I429" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="430" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A430" t="s">
+        <v>374</v>
+      </c>
+      <c r="B430" t="s">
+        <v>590</v>
+      </c>
+      <c r="C430">
+        <v>770883</v>
+      </c>
+      <c r="H430" t="s">
+        <v>388</v>
+      </c>
+      <c r="I430" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="431" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A431" t="s">
+        <v>374</v>
+      </c>
+      <c r="B431" t="s">
+        <v>590</v>
+      </c>
+      <c r="C431">
+        <v>770884</v>
+      </c>
+      <c r="H431" t="s">
+        <v>395</v>
+      </c>
+      <c r="I431" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="432" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A432" t="s">
+        <v>374</v>
+      </c>
+      <c r="B432" t="s">
+        <v>590</v>
+      </c>
+      <c r="C432">
+        <v>770885</v>
+      </c>
+      <c r="H432" t="s">
+        <v>388</v>
+      </c>
+      <c r="I432" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="433" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A433" t="s">
+        <v>374</v>
+      </c>
+      <c r="B433" t="s">
+        <v>590</v>
+      </c>
+      <c r="C433">
+        <v>770886</v>
+      </c>
+      <c r="H433" t="s">
+        <v>395</v>
+      </c>
+      <c r="I433" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="434" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A434" t="s">
+        <v>374</v>
+      </c>
+      <c r="B434" t="s">
+        <v>590</v>
+      </c>
+      <c r="C434">
+        <v>770887</v>
+      </c>
+      <c r="H434" t="s">
+        <v>428</v>
+      </c>
+      <c r="I434" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="435" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A435" t="s">
+        <v>374</v>
+      </c>
+      <c r="B435" t="s">
+        <v>590</v>
+      </c>
+      <c r="C435">
+        <v>770888</v>
+      </c>
+      <c r="H435" t="s">
+        <v>427</v>
+      </c>
+      <c r="I435" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="436" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A436" t="s">
+        <v>374</v>
+      </c>
+      <c r="B436" t="s">
+        <v>590</v>
+      </c>
+      <c r="C436">
+        <v>770889</v>
+      </c>
+      <c r="H436" t="s">
+        <v>428</v>
+      </c>
+      <c r="I436" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="437" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A437" t="s">
+        <v>374</v>
+      </c>
+      <c r="B437" t="s">
+        <v>590</v>
+      </c>
+      <c r="C437">
+        <v>770890</v>
+      </c>
+      <c r="H437" t="s">
+        <v>427</v>
+      </c>
+      <c r="I437" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="438" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A438" t="s">
+        <v>374</v>
+      </c>
+      <c r="B438" t="s">
+        <v>590</v>
+      </c>
+      <c r="C438">
+        <v>770891</v>
+      </c>
+      <c r="H438" t="s">
+        <v>430</v>
+      </c>
+      <c r="I438" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="439" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A439" t="s">
+        <v>374</v>
+      </c>
+      <c r="B439" t="s">
+        <v>590</v>
+      </c>
+      <c r="C439">
+        <v>770892</v>
+      </c>
+      <c r="H439" t="s">
+        <v>435</v>
+      </c>
+      <c r="I439" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="440" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A440" t="s">
+        <v>374</v>
+      </c>
+      <c r="B440" t="s">
+        <v>590</v>
+      </c>
+      <c r="C440">
+        <v>770923</v>
+      </c>
+      <c r="H440" t="s">
+        <v>411</v>
+      </c>
+      <c r="I440" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="441" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A441" t="s">
+        <v>374</v>
+      </c>
+      <c r="B441" t="s">
+        <v>590</v>
+      </c>
+      <c r="C441">
+        <v>770924</v>
+      </c>
+      <c r="H441" t="s">
+        <v>414</v>
+      </c>
+      <c r="I441" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="442" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A442" t="s">
+        <v>374</v>
+      </c>
+      <c r="B442" t="s">
+        <v>590</v>
+      </c>
+      <c r="C442">
+        <v>770981</v>
+      </c>
+      <c r="H442" t="s">
+        <v>384</v>
+      </c>
+      <c r="I442" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="443" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A443" t="s">
+        <v>374</v>
+      </c>
+      <c r="B443" t="s">
+        <v>590</v>
+      </c>
+      <c r="C443">
         <v>770982</v>
       </c>
-      <c r="H429" t="s">
+      <c r="H443" t="s">
         <v>379</v>
       </c>
-      <c r="I429" t="s">
+      <c r="I443" t="s">
         <v>381</v>
       </c>
     </row>
@@ -12835,6 +13081,3541 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6E8173F-978E-4C06-BD6A-29F17B918A7B}">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:L122"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K69" sqref="K69:L69"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.26953125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.08984375" customWidth="1"/>
+    <col min="12" max="12" width="15.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>591</v>
+      </c>
+      <c r="B1" t="s">
+        <v>592</v>
+      </c>
+      <c r="C1" t="s">
+        <v>337</v>
+      </c>
+      <c r="D1" t="s">
+        <v>338</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>592</v>
+      </c>
+      <c r="K1" t="s">
+        <v>337</v>
+      </c>
+      <c r="L1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>770075</v>
+      </c>
+      <c r="B2">
+        <f>RIGHT(A2,4)*1</f>
+        <v>75</v>
+      </c>
+      <c r="C2" t="str">
+        <f>VLOOKUP(B2,J:L,2,FALSE)</f>
+        <v>SF_AM</v>
+      </c>
+      <c r="D2" t="str">
+        <f>VLOOKUP(B2,J:L,3,FALSE)</f>
+        <v>SF_AM</v>
+      </c>
+      <c r="I2">
+        <v>990408</v>
+      </c>
+      <c r="J2">
+        <f>RIGHT(I2,4)*1</f>
+        <v>408</v>
+      </c>
+      <c r="K2" t="s">
+        <v>399</v>
+      </c>
+      <c r="L2" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>770076</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B66" si="0">RIGHT(A3,4)*1</f>
+        <v>76</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C66" si="1">VLOOKUP(B3,J:L,2,FALSE)</f>
+        <v>SF_PM</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D66" si="2">VLOOKUP(B3,J:L,3,FALSE)</f>
+        <v>SF_PM</v>
+      </c>
+      <c r="I3">
+        <v>990407</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J66" si="3">RIGHT(I3,4)*1</f>
+        <v>407</v>
+      </c>
+      <c r="K3" t="s">
+        <v>405</v>
+      </c>
+      <c r="L3" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>770077</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>77</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="1"/>
+        <v>SF_PM</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="2"/>
+        <v>SF_PM</v>
+      </c>
+      <c r="I4">
+        <v>990243</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="3"/>
+        <v>243</v>
+      </c>
+      <c r="K4" t="s">
+        <v>388</v>
+      </c>
+      <c r="L4" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>770078</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>78</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="1"/>
+        <v>SF_AM</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="2"/>
+        <v>SF_AM</v>
+      </c>
+      <c r="I5">
+        <v>990684</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="3"/>
+        <v>684</v>
+      </c>
+      <c r="K5" t="s">
+        <v>395</v>
+      </c>
+      <c r="L5" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>770081</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>81</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="1"/>
+        <v>EastBay_Inner_PM</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="2"/>
+        <v>EastBayInner_BBApproach_PM</v>
+      </c>
+      <c r="I6">
+        <v>990245</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="3"/>
+        <v>245</v>
+      </c>
+      <c r="K6" t="s">
+        <v>388</v>
+      </c>
+      <c r="L6" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>770082</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>82</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="1"/>
+        <v>EastBay_Inner_AM</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="2"/>
+        <v>EastBayInner_BBApproach_AM</v>
+      </c>
+      <c r="I7">
+        <v>990246</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="3"/>
+        <v>246</v>
+      </c>
+      <c r="K7" t="s">
+        <v>395</v>
+      </c>
+      <c r="L7" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>770083</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>83</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="1"/>
+        <v>EastBay_Outer_PM</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="2"/>
+        <v>EastBayOuter_80_PM</v>
+      </c>
+      <c r="I8">
+        <v>990683</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="3"/>
+        <v>683</v>
+      </c>
+      <c r="K8" t="s">
+        <v>388</v>
+      </c>
+      <c r="L8" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>770084</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>84</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="1"/>
+        <v>EastBayOuter_AM</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="2"/>
+        <v>EastBayOuter_80_AM</v>
+      </c>
+      <c r="I9">
+        <v>990402</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="3"/>
+        <v>402</v>
+      </c>
+      <c r="K9" t="s">
+        <v>399</v>
+      </c>
+      <c r="L9" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>770085</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>85</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="1"/>
+        <v>EastBay_Outer_PM</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="2"/>
+        <v>EastBayOuter_80_PM</v>
+      </c>
+      <c r="I10">
+        <v>990401</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="3"/>
+        <v>401</v>
+      </c>
+      <c r="K10" t="s">
+        <v>405</v>
+      </c>
+      <c r="L10" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>770086</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>86</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="1"/>
+        <v>EastBayOuter_AM</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="2"/>
+        <v>EastBayOuter_80_AM</v>
+      </c>
+      <c r="I11">
+        <v>990242</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="3"/>
+        <v>242</v>
+      </c>
+      <c r="K11" t="s">
+        <v>379</v>
+      </c>
+      <c r="L11" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>770087</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>87</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="1"/>
+        <v>Periphery_PM</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="2"/>
+        <v>Periphery_80Solano_PM</v>
+      </c>
+      <c r="I12">
+        <v>990581</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="3"/>
+        <v>581</v>
+      </c>
+      <c r="K12" t="s">
+        <v>384</v>
+      </c>
+      <c r="L12" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>770088</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>88</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="1"/>
+        <v>Periphery_AM</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="2"/>
+        <v>Periphery_80Solano_AM</v>
+      </c>
+      <c r="I13">
+        <v>990981</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="3"/>
+        <v>981</v>
+      </c>
+      <c r="K13" t="s">
+        <v>384</v>
+      </c>
+      <c r="L13" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>770091</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>91</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="1"/>
+        <v>Periphery_PM</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="2"/>
+        <v>Periphery_80Solano_PM</v>
+      </c>
+      <c r="I14">
+        <v>990082</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="3"/>
+        <v>82</v>
+      </c>
+      <c r="K14" t="s">
+        <v>379</v>
+      </c>
+      <c r="L14" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>770092</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>92</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="1"/>
+        <v>Periphery_AM</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="2"/>
+        <v>Periphery_80Solano_AM</v>
+      </c>
+      <c r="I15">
+        <v>990079</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="3"/>
+        <v>79</v>
+      </c>
+      <c r="K15" t="s">
+        <v>384</v>
+      </c>
+      <c r="L15" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>770101</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>101</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="1"/>
+        <v>SF_AM</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="2"/>
+        <v>SF_AM</v>
+      </c>
+      <c r="I16">
+        <v>990582</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="3"/>
+        <v>582</v>
+      </c>
+      <c r="K16" t="s">
+        <v>379</v>
+      </c>
+      <c r="L16" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>770102</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>102</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="1"/>
+        <v>SF_PM</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="2"/>
+        <v>SF_PM</v>
+      </c>
+      <c r="I17">
+        <v>990240</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="3"/>
+        <v>240</v>
+      </c>
+      <c r="K17" t="s">
+        <v>395</v>
+      </c>
+      <c r="L17" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>770103</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>103</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="1"/>
+        <v>SFOSanMateo_AM</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="2"/>
+        <v>SFOSanMateo_101_AM</v>
+      </c>
+      <c r="I18">
+        <v>990882</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="3"/>
+        <v>882</v>
+      </c>
+      <c r="K18" t="s">
+        <v>395</v>
+      </c>
+      <c r="L18" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>770104</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>104</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="1"/>
+        <v>SFOSanMateo_PM</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="2"/>
+        <v>SFOSanMateo_101_PM</v>
+      </c>
+      <c r="I19">
+        <v>990120</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="3"/>
+        <v>120</v>
+      </c>
+      <c r="K19" t="s">
+        <v>435</v>
+      </c>
+      <c r="L19" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>770105</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>105</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="1"/>
+        <v>SFOSanMateo_AM</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="2"/>
+        <v>SFOSanMateo_101_AM</v>
+      </c>
+      <c r="I20">
+        <v>990855</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="3"/>
+        <v>855</v>
+      </c>
+      <c r="K20" t="s">
+        <v>435</v>
+      </c>
+      <c r="L20" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>770106</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>106</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="1"/>
+        <v>SFOSanMateo_PM</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="2"/>
+        <v>SFOSanMateo_101_PM</v>
+      </c>
+      <c r="I21">
+        <v>990856</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="3"/>
+        <v>856</v>
+      </c>
+      <c r="K21" t="s">
+        <v>430</v>
+      </c>
+      <c r="L21" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>770107</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>107</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="1"/>
+        <v>SanMateo_PM</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="2"/>
+        <v>SanMateo_101_PM</v>
+      </c>
+      <c r="I22">
+        <v>990872</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="3"/>
+        <v>872</v>
+      </c>
+      <c r="K22" t="s">
+        <v>435</v>
+      </c>
+      <c r="L22" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>770108</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>108</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="1"/>
+        <v>SanMateo_AM</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="2"/>
+        <v>SanMateo_101_AM</v>
+      </c>
+      <c r="I23">
+        <v>990285</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="3"/>
+        <v>285</v>
+      </c>
+      <c r="K23" t="s">
+        <v>430</v>
+      </c>
+      <c r="L23" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>770109</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="0"/>
+        <v>109</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="1"/>
+        <v>SanMateo_PM</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="2"/>
+        <v>SanMateo_101_PM</v>
+      </c>
+      <c r="I24">
+        <v>990171</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="3"/>
+        <v>171</v>
+      </c>
+      <c r="K24" t="s">
+        <v>430</v>
+      </c>
+      <c r="L24" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>770110</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="0"/>
+        <v>110</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="1"/>
+        <v>SanMateo_AM</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="2"/>
+        <v>SanMateo_101_AM</v>
+      </c>
+      <c r="I25">
+        <v>990172</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="3"/>
+        <v>172</v>
+      </c>
+      <c r="K25" t="s">
+        <v>435</v>
+      </c>
+      <c r="L25" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>770111</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="0"/>
+        <v>111</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="1"/>
+        <v>SanMateo_PM</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="2"/>
+        <v>SanMateo_101_PM</v>
+      </c>
+      <c r="I26">
+        <v>990286</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="3"/>
+        <v>286</v>
+      </c>
+      <c r="K26" t="s">
+        <v>435</v>
+      </c>
+      <c r="L26" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>770112</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="0"/>
+        <v>112</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" si="1"/>
+        <v>SanMateo_AM</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="2"/>
+        <v>SanMateo_101_AM</v>
+      </c>
+      <c r="I27">
+        <v>990892</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="3"/>
+        <v>892</v>
+      </c>
+      <c r="K27" t="s">
+        <v>435</v>
+      </c>
+      <c r="L27" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>770113</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="0"/>
+        <v>113</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" si="1"/>
+        <v>SanMateo_PM</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="2"/>
+        <v>SanMateo_101_PM</v>
+      </c>
+      <c r="I28">
+        <v>990871</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="3"/>
+        <v>871</v>
+      </c>
+      <c r="K28" t="s">
+        <v>430</v>
+      </c>
+      <c r="L28" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>770114</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="0"/>
+        <v>114</v>
+      </c>
+      <c r="C29" t="str">
+        <f t="shared" si="1"/>
+        <v>SanMateo_AM</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="2"/>
+        <v>SanMateo_101_AM</v>
+      </c>
+      <c r="I29">
+        <v>990119</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="3"/>
+        <v>119</v>
+      </c>
+      <c r="K29" t="s">
+        <v>430</v>
+      </c>
+      <c r="L29" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>770115</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="0"/>
+        <v>115</v>
+      </c>
+      <c r="C30" t="str">
+        <f t="shared" si="1"/>
+        <v>SouthBay_Inner_AM</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="2"/>
+        <v>SouthBay_Inner_AM</v>
+      </c>
+      <c r="I30">
+        <v>990891</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="3"/>
+        <v>891</v>
+      </c>
+      <c r="K30" t="s">
+        <v>430</v>
+      </c>
+      <c r="L30" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>770116</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="0"/>
+        <v>116</v>
+      </c>
+      <c r="C31" t="str">
+        <f t="shared" si="1"/>
+        <v>SouthBay_Inner_PM</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="2"/>
+        <v>SouthBay_Inner_PM</v>
+      </c>
+      <c r="I31">
+        <v>990692</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="3"/>
+        <v>692</v>
+      </c>
+      <c r="K31" t="s">
+        <v>430</v>
+      </c>
+      <c r="L31" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>770117</v>
+      </c>
+      <c r="B32">
+        <f t="shared" si="0"/>
+        <v>117</v>
+      </c>
+      <c r="C32" t="str">
+        <f t="shared" si="1"/>
+        <v>SouthBay_Inner_AM</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="2"/>
+        <v>SouthBay_Inner_AM</v>
+      </c>
+      <c r="I32">
+        <v>990118</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="3"/>
+        <v>118</v>
+      </c>
+      <c r="K32" t="s">
+        <v>428</v>
+      </c>
+      <c r="L32" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>770118</v>
+      </c>
+      <c r="B33">
+        <f t="shared" si="0"/>
+        <v>118</v>
+      </c>
+      <c r="C33" t="str">
+        <f t="shared" si="1"/>
+        <v>SouthBay_Inner_PM</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="2"/>
+        <v>SouthBay_Inner_PM</v>
+      </c>
+      <c r="I33">
+        <v>990116</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="3"/>
+        <v>116</v>
+      </c>
+      <c r="K33" t="s">
+        <v>428</v>
+      </c>
+      <c r="L33" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>770119</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="0"/>
+        <v>119</v>
+      </c>
+      <c r="C34" t="str">
+        <f t="shared" si="1"/>
+        <v>SouthBay_Outer_AM</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="2"/>
+        <v>SouthBay_Outer10187_AM</v>
+      </c>
+      <c r="I34">
+        <v>990890</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="3"/>
+        <v>890</v>
+      </c>
+      <c r="K34" t="s">
+        <v>427</v>
+      </c>
+      <c r="L34" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>770120</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="0"/>
+        <v>120</v>
+      </c>
+      <c r="C35" t="str">
+        <f t="shared" si="1"/>
+        <v>SouthBay_Outer_PM</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="2"/>
+        <v>SouthBay_Outer10187_PM</v>
+      </c>
+      <c r="I35">
+        <v>990231</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="3"/>
+        <v>231</v>
+      </c>
+      <c r="K35" t="s">
+        <v>428</v>
+      </c>
+      <c r="L35" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>770121</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="0"/>
+        <v>121</v>
+      </c>
+      <c r="C36" t="str">
+        <f t="shared" si="1"/>
+        <v>Periphery_AM</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" si="2"/>
+        <v>Periphery_101SouthBay_AM</v>
+      </c>
+      <c r="I36">
+        <v>990232</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="3"/>
+        <v>232</v>
+      </c>
+      <c r="K36" t="s">
+        <v>427</v>
+      </c>
+      <c r="L36" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>770122</v>
+      </c>
+      <c r="B37">
+        <f t="shared" si="0"/>
+        <v>122</v>
+      </c>
+      <c r="C37" t="str">
+        <f t="shared" si="1"/>
+        <v>Periphery_PM</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" si="2"/>
+        <v>Periphery_101SouthBay_PM</v>
+      </c>
+      <c r="I37">
+        <v>990234</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="3"/>
+        <v>234</v>
+      </c>
+      <c r="K37" t="s">
+        <v>427</v>
+      </c>
+      <c r="L37" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>770123</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="0"/>
+        <v>123</v>
+      </c>
+      <c r="C38" t="str">
+        <f t="shared" si="1"/>
+        <v>Periphery_AM</v>
+      </c>
+      <c r="D38" t="str">
+        <f t="shared" si="2"/>
+        <v>Periphery_101SouthBay_AM</v>
+      </c>
+      <c r="I38">
+        <v>990290</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="3"/>
+        <v>290</v>
+      </c>
+      <c r="K38" t="s">
+        <v>414</v>
+      </c>
+      <c r="L38" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>770124</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="0"/>
+        <v>124</v>
+      </c>
+      <c r="C39" t="str">
+        <f t="shared" si="1"/>
+        <v>Periphery_PM</v>
+      </c>
+      <c r="D39" t="str">
+        <f t="shared" si="2"/>
+        <v>Periphery_101SouthBay_PM</v>
+      </c>
+      <c r="I39">
+        <v>990289</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="3"/>
+        <v>289</v>
+      </c>
+      <c r="K39" t="s">
+        <v>411</v>
+      </c>
+      <c r="L39" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>770135</v>
+      </c>
+      <c r="B40">
+        <f t="shared" si="0"/>
+        <v>135</v>
+      </c>
+      <c r="C40" t="str">
+        <f t="shared" si="1"/>
+        <v>Periphery_PM</v>
+      </c>
+      <c r="D40" t="str">
+        <f t="shared" si="2"/>
+        <v>Periphery_101NorthBay_PM</v>
+      </c>
+      <c r="I40">
+        <v>990927</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="3"/>
+        <v>927</v>
+      </c>
+      <c r="K40" t="s">
+        <v>411</v>
+      </c>
+      <c r="L40" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>770136</v>
+      </c>
+      <c r="B41">
+        <f t="shared" si="0"/>
+        <v>136</v>
+      </c>
+      <c r="C41" t="str">
+        <f t="shared" si="1"/>
+        <v>Periphery_AM</v>
+      </c>
+      <c r="D41" t="str">
+        <f t="shared" si="2"/>
+        <v>Periphery_101NorthBay_AM</v>
+      </c>
+      <c r="I41">
+        <v>990928</v>
+      </c>
+      <c r="J41">
+        <f t="shared" si="3"/>
+        <v>928</v>
+      </c>
+      <c r="K41" t="s">
+        <v>414</v>
+      </c>
+      <c r="L41" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>770171</v>
+      </c>
+      <c r="B42">
+        <f t="shared" si="0"/>
+        <v>171</v>
+      </c>
+      <c r="C42" t="str">
+        <f t="shared" si="1"/>
+        <v>SouthBay_Outer_AM</v>
+      </c>
+      <c r="D42" t="str">
+        <f t="shared" si="2"/>
+        <v>SouthBay_Outer280680_AM</v>
+      </c>
+      <c r="I42">
+        <v>990108</v>
+      </c>
+      <c r="J42">
+        <f t="shared" si="3"/>
+        <v>108</v>
+      </c>
+      <c r="K42" t="s">
+        <v>411</v>
+      </c>
+      <c r="L42" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>770172</v>
+      </c>
+      <c r="B43">
+        <f t="shared" si="0"/>
+        <v>172</v>
+      </c>
+      <c r="C43" t="str">
+        <f t="shared" si="1"/>
+        <v>SouthBay_Outer_PM</v>
+      </c>
+      <c r="D43" t="str">
+        <f t="shared" si="2"/>
+        <v>SouthBay_Outer280680_PM</v>
+      </c>
+      <c r="I43">
+        <v>990924</v>
+      </c>
+      <c r="J43">
+        <f t="shared" si="3"/>
+        <v>924</v>
+      </c>
+      <c r="K43" t="s">
+        <v>414</v>
+      </c>
+      <c r="L43" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>770231</v>
+      </c>
+      <c r="B44">
+        <f t="shared" si="0"/>
+        <v>231</v>
+      </c>
+      <c r="C44" t="str">
+        <f t="shared" si="1"/>
+        <v>SouthBay_Inner_PM</v>
+      </c>
+      <c r="D44" t="str">
+        <f t="shared" si="2"/>
+        <v>SouthBay_Inner_PM</v>
+      </c>
+      <c r="I44">
+        <v>990109</v>
+      </c>
+      <c r="J44">
+        <f t="shared" si="3"/>
+        <v>109</v>
+      </c>
+      <c r="K44" t="s">
+        <v>414</v>
+      </c>
+      <c r="L44" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>770232</v>
+      </c>
+      <c r="B45">
+        <f t="shared" si="0"/>
+        <v>232</v>
+      </c>
+      <c r="C45" t="str">
+        <f t="shared" si="1"/>
+        <v>SouthBay_Inner_AM</v>
+      </c>
+      <c r="D45" t="str">
+        <f t="shared" si="2"/>
+        <v>SouthBay_Inner_AM</v>
+      </c>
+      <c r="I45">
+        <v>990382</v>
+      </c>
+      <c r="J45">
+        <f t="shared" si="3"/>
+        <v>382</v>
+      </c>
+      <c r="K45" t="s">
+        <v>423</v>
+      </c>
+      <c r="L45" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <v>770233</v>
+      </c>
+      <c r="B46">
+        <f t="shared" si="0"/>
+        <v>233</v>
+      </c>
+      <c r="C46" t="str">
+        <f t="shared" si="1"/>
+        <v>SouthBay_Inner_PM</v>
+      </c>
+      <c r="D46" t="str">
+        <f t="shared" si="2"/>
+        <v>SouthBay_Inner_PM</v>
+      </c>
+      <c r="I46">
+        <v>990381</v>
+      </c>
+      <c r="J46">
+        <f t="shared" si="3"/>
+        <v>381</v>
+      </c>
+      <c r="K46" t="s">
+        <v>420</v>
+      </c>
+      <c r="L46" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A47">
+        <v>770234</v>
+      </c>
+      <c r="B47">
+        <f t="shared" si="0"/>
+        <v>234</v>
+      </c>
+      <c r="C47" t="str">
+        <f t="shared" si="1"/>
+        <v>SouthBay_Inner_AM</v>
+      </c>
+      <c r="D47" t="str">
+        <f t="shared" si="2"/>
+        <v>SouthBay_Inner_AM</v>
+      </c>
+      <c r="I47">
+        <v>990287</v>
+      </c>
+      <c r="J47">
+        <f t="shared" si="3"/>
+        <v>287</v>
+      </c>
+      <c r="K47" t="s">
+        <v>420</v>
+      </c>
+      <c r="L47" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <v>770239</v>
+      </c>
+      <c r="B48">
+        <f t="shared" si="0"/>
+        <v>239</v>
+      </c>
+      <c r="C48" t="str">
+        <f t="shared" si="1"/>
+        <v>EastBay_Outer_PM</v>
+      </c>
+      <c r="D48" t="str">
+        <f t="shared" si="2"/>
+        <v>EastBayOuter_580880_PM</v>
+      </c>
+      <c r="I48">
+        <v>990106</v>
+      </c>
+      <c r="J48">
+        <f t="shared" si="3"/>
+        <v>106</v>
+      </c>
+      <c r="K48" t="s">
+        <v>423</v>
+      </c>
+      <c r="L48" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A49">
+        <v>770240</v>
+      </c>
+      <c r="B49">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+      <c r="C49" t="str">
+        <f t="shared" si="1"/>
+        <v>EastBayOuter_AM</v>
+      </c>
+      <c r="D49" t="str">
+        <f t="shared" si="2"/>
+        <v>EastBayOuter_580880_AM</v>
+      </c>
+      <c r="I49">
+        <v>990281</v>
+      </c>
+      <c r="J49">
+        <f t="shared" si="3"/>
+        <v>281</v>
+      </c>
+      <c r="K49" t="s">
+        <v>417</v>
+      </c>
+      <c r="L49" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A50">
+        <v>770241</v>
+      </c>
+      <c r="B50">
+        <f t="shared" si="0"/>
+        <v>241</v>
+      </c>
+      <c r="C50" t="str">
+        <f t="shared" si="1"/>
+        <v>EastBay_Inner_PM</v>
+      </c>
+      <c r="D50" t="str">
+        <f t="shared" si="2"/>
+        <v>EastBayInner_58098024_PM</v>
+      </c>
+      <c r="I50">
+        <v>990282</v>
+      </c>
+      <c r="J50">
+        <f t="shared" si="3"/>
+        <v>282</v>
+      </c>
+      <c r="K50" t="s">
+        <v>418</v>
+      </c>
+      <c r="L50" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A51">
+        <v>770242</v>
+      </c>
+      <c r="B51">
+        <f t="shared" si="0"/>
+        <v>242</v>
+      </c>
+      <c r="C51" t="str">
+        <f t="shared" si="1"/>
+        <v>EastBay_Inner_AM</v>
+      </c>
+      <c r="D51" t="str">
+        <f t="shared" si="2"/>
+        <v>EastBayInner_58098024_AM</v>
+      </c>
+      <c r="I51">
+        <v>990138</v>
+      </c>
+      <c r="J51">
+        <f t="shared" si="3"/>
+        <v>138</v>
+      </c>
+      <c r="K51" t="s">
+        <v>418</v>
+      </c>
+      <c r="L51" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A52">
+        <v>770243</v>
+      </c>
+      <c r="B52">
+        <f t="shared" si="0"/>
+        <v>243</v>
+      </c>
+      <c r="C52" t="str">
+        <f t="shared" si="1"/>
+        <v>EastBay_Outer_PM</v>
+      </c>
+      <c r="D52" t="str">
+        <f t="shared" si="2"/>
+        <v>EastBayOuter_24_PM</v>
+      </c>
+      <c r="I52">
+        <v>990137</v>
+      </c>
+      <c r="J52">
+        <f t="shared" si="3"/>
+        <v>137</v>
+      </c>
+      <c r="K52" t="s">
+        <v>418</v>
+      </c>
+      <c r="L52" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A53">
+        <v>770244</v>
+      </c>
+      <c r="B53">
+        <f t="shared" si="0"/>
+        <v>244</v>
+      </c>
+      <c r="C53" t="str">
+        <f t="shared" si="1"/>
+        <v>EastBayOuter_AM</v>
+      </c>
+      <c r="D53" t="str">
+        <f t="shared" si="2"/>
+        <v>EastBayOuter_24_AM</v>
+      </c>
+      <c r="I53">
+        <v>990135</v>
+      </c>
+      <c r="J53">
+        <f t="shared" si="3"/>
+        <v>135</v>
+      </c>
+      <c r="K53" t="s">
+        <v>405</v>
+      </c>
+      <c r="L53" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A54">
+        <v>770245</v>
+      </c>
+      <c r="B54">
+        <f t="shared" si="0"/>
+        <v>245</v>
+      </c>
+      <c r="C54" t="str">
+        <f t="shared" si="1"/>
+        <v>EastBay_Outer_PM</v>
+      </c>
+      <c r="D54" t="str">
+        <f t="shared" si="2"/>
+        <v>EastBayOuter_24_PM</v>
+      </c>
+      <c r="I54">
+        <v>990136</v>
+      </c>
+      <c r="J54">
+        <f t="shared" si="3"/>
+        <v>136</v>
+      </c>
+      <c r="K54" t="s">
+        <v>399</v>
+      </c>
+      <c r="L54" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A55">
+        <v>770246</v>
+      </c>
+      <c r="B55">
+        <f t="shared" si="0"/>
+        <v>246</v>
+      </c>
+      <c r="C55" t="str">
+        <f t="shared" si="1"/>
+        <v>EastBayOuter_AM</v>
+      </c>
+      <c r="D55" t="str">
+        <f t="shared" si="2"/>
+        <v>EastBayOuter_24_AM</v>
+      </c>
+      <c r="I55">
+        <v>990092</v>
+      </c>
+      <c r="J55">
+        <f t="shared" si="3"/>
+        <v>92</v>
+      </c>
+      <c r="K55" t="s">
+        <v>399</v>
+      </c>
+      <c r="L55" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A56">
+        <v>770281</v>
+      </c>
+      <c r="B56">
+        <f t="shared" si="0"/>
+        <v>281</v>
+      </c>
+      <c r="C56" t="str">
+        <f t="shared" si="1"/>
+        <v>SF_AM</v>
+      </c>
+      <c r="D56" t="str">
+        <f t="shared" si="2"/>
+        <v>SF_AM</v>
+      </c>
+      <c r="I56">
+        <v>990091</v>
+      </c>
+      <c r="J56">
+        <f t="shared" si="3"/>
+        <v>91</v>
+      </c>
+      <c r="K56" t="s">
+        <v>405</v>
+      </c>
+      <c r="L56" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A57">
+        <v>770282</v>
+      </c>
+      <c r="B57">
+        <f t="shared" si="0"/>
+        <v>282</v>
+      </c>
+      <c r="C57" t="str">
+        <f t="shared" si="1"/>
+        <v>SF_PM</v>
+      </c>
+      <c r="D57" t="str">
+        <f t="shared" si="2"/>
+        <v>SF_PM</v>
+      </c>
+      <c r="I57">
+        <v>990244</v>
+      </c>
+      <c r="J57">
+        <f t="shared" si="3"/>
+        <v>244</v>
+      </c>
+      <c r="K57" t="s">
+        <v>395</v>
+      </c>
+      <c r="L57" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A58">
+        <v>770283</v>
+      </c>
+      <c r="B58">
+        <f t="shared" si="0"/>
+        <v>283</v>
+      </c>
+      <c r="C58" t="str">
+        <f t="shared" si="1"/>
+        <v>SouthBay_Outer_AM</v>
+      </c>
+      <c r="D58" t="str">
+        <f t="shared" si="2"/>
+        <v>SouthBay_Outer280680_AM</v>
+      </c>
+      <c r="I58">
+        <v>990083</v>
+      </c>
+      <c r="J58">
+        <f t="shared" si="3"/>
+        <v>83</v>
+      </c>
+      <c r="K58" t="s">
+        <v>388</v>
+      </c>
+      <c r="L58" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A59">
+        <v>770284</v>
+      </c>
+      <c r="B59">
+        <f t="shared" si="0"/>
+        <v>284</v>
+      </c>
+      <c r="C59" t="str">
+        <f t="shared" si="1"/>
+        <v>SouthBay_Outer_PM</v>
+      </c>
+      <c r="D59" t="str">
+        <f t="shared" si="2"/>
+        <v>SouthBay_Outer280680_PM</v>
+      </c>
+      <c r="I59">
+        <v>990084</v>
+      </c>
+      <c r="J59">
+        <f t="shared" si="3"/>
+        <v>84</v>
+      </c>
+      <c r="K59" t="s">
+        <v>395</v>
+      </c>
+      <c r="L59" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A60">
+        <v>770285</v>
+      </c>
+      <c r="B60">
+        <f t="shared" si="0"/>
+        <v>285</v>
+      </c>
+      <c r="C60" t="str">
+        <f t="shared" si="1"/>
+        <v>SouthBay_Outer_AM</v>
+      </c>
+      <c r="D60" t="str">
+        <f t="shared" si="2"/>
+        <v>SouthBay_Outer280680_AM</v>
+      </c>
+      <c r="I60">
+        <v>990085</v>
+      </c>
+      <c r="J60">
+        <f t="shared" si="3"/>
+        <v>85</v>
+      </c>
+      <c r="K60" t="s">
+        <v>388</v>
+      </c>
+      <c r="L60" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A61">
+        <v>770286</v>
+      </c>
+      <c r="B61">
+        <f t="shared" si="0"/>
+        <v>286</v>
+      </c>
+      <c r="C61" t="str">
+        <f t="shared" si="1"/>
+        <v>SouthBay_Outer_PM</v>
+      </c>
+      <c r="D61" t="str">
+        <f t="shared" si="2"/>
+        <v>SouthBay_Outer280680_PM</v>
+      </c>
+      <c r="I61">
+        <v>990086</v>
+      </c>
+      <c r="J61">
+        <f t="shared" si="3"/>
+        <v>86</v>
+      </c>
+      <c r="K61" t="s">
+        <v>395</v>
+      </c>
+      <c r="L61" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A62">
+        <v>770287</v>
+      </c>
+      <c r="B62">
+        <f t="shared" si="0"/>
+        <v>287</v>
+      </c>
+      <c r="C62" t="str">
+        <f t="shared" si="1"/>
+        <v>SFOSanMateo_AM</v>
+      </c>
+      <c r="D62" t="str">
+        <f t="shared" si="2"/>
+        <v>SFOSanMateo280380_AM</v>
+      </c>
+      <c r="I62">
+        <v>990879</v>
+      </c>
+      <c r="J62">
+        <f t="shared" si="3"/>
+        <v>879</v>
+      </c>
+      <c r="K62" t="s">
+        <v>379</v>
+      </c>
+      <c r="L62" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A63">
+        <v>770288</v>
+      </c>
+      <c r="B63">
+        <f t="shared" si="0"/>
+        <v>288</v>
+      </c>
+      <c r="C63" t="str">
+        <f t="shared" si="1"/>
+        <v>SFOSanMateo_PM</v>
+      </c>
+      <c r="D63" t="str">
+        <f t="shared" si="2"/>
+        <v>SFOSanMateo280380_PM</v>
+      </c>
+      <c r="I63">
+        <v>990880</v>
+      </c>
+      <c r="J63">
+        <f t="shared" si="3"/>
+        <v>880</v>
+      </c>
+      <c r="K63" t="s">
+        <v>384</v>
+      </c>
+      <c r="L63" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A64">
+        <v>770289</v>
+      </c>
+      <c r="B64">
+        <f t="shared" si="0"/>
+        <v>289</v>
+      </c>
+      <c r="C64" t="str">
+        <f t="shared" si="1"/>
+        <v>SanMateo_AM</v>
+      </c>
+      <c r="D64" t="str">
+        <f t="shared" si="2"/>
+        <v>SanMateo_28092_AM</v>
+      </c>
+      <c r="I64">
+        <v>990081</v>
+      </c>
+      <c r="J64">
+        <f t="shared" si="3"/>
+        <v>81</v>
+      </c>
+      <c r="K64" t="s">
+        <v>384</v>
+      </c>
+      <c r="L64" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A65">
+        <v>770290</v>
+      </c>
+      <c r="B65">
+        <f t="shared" si="0"/>
+        <v>290</v>
+      </c>
+      <c r="C65" t="str">
+        <f t="shared" si="1"/>
+        <v>SanMateo_PM</v>
+      </c>
+      <c r="D65" t="str">
+        <f t="shared" si="2"/>
+        <v>SanMateo_28092_PM</v>
+      </c>
+      <c r="I65">
+        <v>990884</v>
+      </c>
+      <c r="J65">
+        <f t="shared" si="3"/>
+        <v>884</v>
+      </c>
+      <c r="K65" t="s">
+        <v>395</v>
+      </c>
+      <c r="L65" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A66">
+        <v>770381</v>
+      </c>
+      <c r="B66">
+        <f t="shared" si="0"/>
+        <v>381</v>
+      </c>
+      <c r="C66" t="str">
+        <f t="shared" si="1"/>
+        <v>SFOSanMateo_AM</v>
+      </c>
+      <c r="D66" t="str">
+        <f t="shared" si="2"/>
+        <v>SFOSanMateo280380_AM</v>
+      </c>
+      <c r="I66">
+        <v>990883</v>
+      </c>
+      <c r="J66">
+        <f t="shared" si="3"/>
+        <v>883</v>
+      </c>
+      <c r="K66" t="s">
+        <v>388</v>
+      </c>
+      <c r="L66" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A67">
+        <v>770382</v>
+      </c>
+      <c r="B67">
+        <f t="shared" ref="B67:B112" si="4">RIGHT(A67,4)*1</f>
+        <v>382</v>
+      </c>
+      <c r="C67" t="str">
+        <f t="shared" ref="C67:C112" si="5">VLOOKUP(B67,J:L,2,FALSE)</f>
+        <v>SFOSanMateo_PM</v>
+      </c>
+      <c r="D67" t="str">
+        <f t="shared" ref="D67:D112" si="6">VLOOKUP(B67,J:L,3,FALSE)</f>
+        <v>SFOSanMateo280380_PM</v>
+      </c>
+      <c r="I67">
+        <v>990241</v>
+      </c>
+      <c r="J67">
+        <f t="shared" ref="J67:J122" si="7">RIGHT(I67,4)*1</f>
+        <v>241</v>
+      </c>
+      <c r="K67" t="s">
+        <v>384</v>
+      </c>
+      <c r="L67" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A68">
+        <v>770401</v>
+      </c>
+      <c r="B68">
+        <f t="shared" si="4"/>
+        <v>401</v>
+      </c>
+      <c r="C68" t="str">
+        <f t="shared" si="5"/>
+        <v>Periphery_PM</v>
+      </c>
+      <c r="D68" t="str">
+        <f t="shared" si="6"/>
+        <v>Periphery_SR4_PM</v>
+      </c>
+      <c r="I68">
+        <v>990583</v>
+      </c>
+      <c r="J68">
+        <f t="shared" si="7"/>
+        <v>583</v>
+      </c>
+      <c r="K68" t="s">
+        <v>384</v>
+      </c>
+      <c r="L68" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A69">
+        <v>770402</v>
+      </c>
+      <c r="B69">
+        <f t="shared" si="4"/>
+        <v>402</v>
+      </c>
+      <c r="C69" t="str">
+        <f t="shared" si="5"/>
+        <v>Periphery_AM</v>
+      </c>
+      <c r="D69" t="str">
+        <f t="shared" si="6"/>
+        <v>Periphery_SR4_AM</v>
+      </c>
+      <c r="I69">
+        <v>990982</v>
+      </c>
+      <c r="J69">
+        <f t="shared" si="7"/>
+        <v>982</v>
+      </c>
+      <c r="K69" t="s">
+        <v>379</v>
+      </c>
+      <c r="L69" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A70">
+        <v>770403</v>
+      </c>
+      <c r="B70">
+        <f t="shared" si="4"/>
+        <v>403</v>
+      </c>
+      <c r="C70" t="str">
+        <f t="shared" si="5"/>
+        <v>Periphery_PM</v>
+      </c>
+      <c r="D70" t="str">
+        <f t="shared" si="6"/>
+        <v>Periphery_SR4_PM</v>
+      </c>
+      <c r="I70">
+        <v>990585</v>
+      </c>
+      <c r="J70">
+        <f t="shared" si="7"/>
+        <v>585</v>
+      </c>
+      <c r="K70" t="s">
+        <v>388</v>
+      </c>
+      <c r="L70" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A71">
+        <v>770404</v>
+      </c>
+      <c r="B71">
+        <f t="shared" si="4"/>
+        <v>404</v>
+      </c>
+      <c r="C71" t="str">
+        <f t="shared" si="5"/>
+        <v>Periphery_AM</v>
+      </c>
+      <c r="D71" t="str">
+        <f t="shared" si="6"/>
+        <v>Periphery_SR4_AM</v>
+      </c>
+      <c r="I71">
+        <v>990586</v>
+      </c>
+      <c r="J71">
+        <f t="shared" si="7"/>
+        <v>586</v>
+      </c>
+      <c r="K71" t="s">
+        <v>395</v>
+      </c>
+      <c r="L71" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A72">
+        <v>770407</v>
+      </c>
+      <c r="B72">
+        <f t="shared" si="4"/>
+        <v>407</v>
+      </c>
+      <c r="C72" t="str">
+        <f t="shared" si="5"/>
+        <v>Periphery_PM</v>
+      </c>
+      <c r="D72" t="str">
+        <f t="shared" si="6"/>
+        <v>Periphery_SR4_PM</v>
+      </c>
+      <c r="I72">
+        <v>990588</v>
+      </c>
+      <c r="J72">
+        <f t="shared" si="7"/>
+        <v>588</v>
+      </c>
+      <c r="K72" t="s">
+        <v>399</v>
+      </c>
+      <c r="L72" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A73">
+        <v>770408</v>
+      </c>
+      <c r="B73">
+        <f t="shared" si="4"/>
+        <v>408</v>
+      </c>
+      <c r="C73" t="str">
+        <f t="shared" si="5"/>
+        <v>Periphery_AM</v>
+      </c>
+      <c r="D73" t="str">
+        <f t="shared" si="6"/>
+        <v>Periphery_SR4_AM</v>
+      </c>
+      <c r="I73">
+        <v>990587</v>
+      </c>
+      <c r="J73">
+        <f t="shared" si="7"/>
+        <v>587</v>
+      </c>
+      <c r="K73" t="s">
+        <v>405</v>
+      </c>
+      <c r="L73" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A74">
+        <v>770581</v>
+      </c>
+      <c r="B74">
+        <f t="shared" si="4"/>
+        <v>581</v>
+      </c>
+      <c r="C74" t="str">
+        <f t="shared" si="5"/>
+        <v>EastBay_Inner_PM</v>
+      </c>
+      <c r="D74" t="str">
+        <f t="shared" si="6"/>
+        <v>EastBayInner_BBApproach_PM</v>
+      </c>
+      <c r="I74">
+        <v>990589</v>
+      </c>
+      <c r="J74">
+        <f t="shared" si="7"/>
+        <v>589</v>
+      </c>
+      <c r="K74" t="s">
+        <v>405</v>
+      </c>
+      <c r="L74" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A75">
+        <v>770582</v>
+      </c>
+      <c r="B75">
+        <f t="shared" si="4"/>
+        <v>582</v>
+      </c>
+      <c r="C75" t="str">
+        <f t="shared" si="5"/>
+        <v>EastBay_Inner_AM</v>
+      </c>
+      <c r="D75" t="str">
+        <f t="shared" si="6"/>
+        <v>EastBayInner_BBApproach_AM</v>
+      </c>
+      <c r="I75">
+        <v>990584</v>
+      </c>
+      <c r="J75">
+        <f t="shared" si="7"/>
+        <v>584</v>
+      </c>
+      <c r="K75" t="s">
+        <v>379</v>
+      </c>
+      <c r="L75" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A76">
+        <v>770583</v>
+      </c>
+      <c r="B76">
+        <f t="shared" si="4"/>
+        <v>583</v>
+      </c>
+      <c r="C76" t="str">
+        <f t="shared" si="5"/>
+        <v>EastBay_Inner_PM</v>
+      </c>
+      <c r="D76" t="str">
+        <f t="shared" si="6"/>
+        <v>EastBayInner_58098024_PM</v>
+      </c>
+      <c r="I76">
+        <v>990590</v>
+      </c>
+      <c r="J76">
+        <f t="shared" si="7"/>
+        <v>590</v>
+      </c>
+      <c r="K76" t="s">
+        <v>399</v>
+      </c>
+      <c r="L76" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A77">
+        <v>770584</v>
+      </c>
+      <c r="B77">
+        <f t="shared" si="4"/>
+        <v>584</v>
+      </c>
+      <c r="C77" t="str">
+        <f t="shared" si="5"/>
+        <v>EastBay_Inner_AM</v>
+      </c>
+      <c r="D77" t="str">
+        <f t="shared" si="6"/>
+        <v>EastBayInner_58098024_AM</v>
+      </c>
+      <c r="I77">
+        <v>990881</v>
+      </c>
+      <c r="J77">
+        <f t="shared" si="7"/>
+        <v>881</v>
+      </c>
+      <c r="K77" t="s">
+        <v>388</v>
+      </c>
+      <c r="L77" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A78">
+        <v>770585</v>
+      </c>
+      <c r="B78">
+        <f t="shared" si="4"/>
+        <v>585</v>
+      </c>
+      <c r="C78" t="str">
+        <f t="shared" si="5"/>
+        <v>EastBay_Outer_PM</v>
+      </c>
+      <c r="D78" t="str">
+        <f t="shared" si="6"/>
+        <v>EastBayOuter_580880_PM</v>
+      </c>
+      <c r="I78">
+        <v>990239</v>
+      </c>
+      <c r="J78">
+        <f t="shared" si="7"/>
+        <v>239</v>
+      </c>
+      <c r="K78" t="s">
+        <v>388</v>
+      </c>
+      <c r="L78" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A79">
+        <v>770586</v>
+      </c>
+      <c r="B79">
+        <f t="shared" si="4"/>
+        <v>586</v>
+      </c>
+      <c r="C79" t="str">
+        <f t="shared" si="5"/>
+        <v>EastBayOuter_AM</v>
+      </c>
+      <c r="D79" t="str">
+        <f t="shared" si="6"/>
+        <v>EastBayOuter_580880_AM</v>
+      </c>
+      <c r="I79">
+        <v>990690</v>
+      </c>
+      <c r="J79">
+        <f t="shared" si="7"/>
+        <v>690</v>
+      </c>
+      <c r="K79" t="s">
+        <v>395</v>
+      </c>
+      <c r="L79" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A80">
+        <v>770587</v>
+      </c>
+      <c r="B80">
+        <f t="shared" si="4"/>
+        <v>587</v>
+      </c>
+      <c r="C80" t="str">
+        <f t="shared" si="5"/>
+        <v>Periphery_PM</v>
+      </c>
+      <c r="D80" t="str">
+        <f t="shared" si="6"/>
+        <v>Periphery_580_PM</v>
+      </c>
+      <c r="I80">
+        <v>990885</v>
+      </c>
+      <c r="J80">
+        <f t="shared" si="7"/>
+        <v>885</v>
+      </c>
+      <c r="K80" t="s">
+        <v>388</v>
+      </c>
+      <c r="L80" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A81">
+        <v>770588</v>
+      </c>
+      <c r="B81">
+        <f t="shared" si="4"/>
+        <v>588</v>
+      </c>
+      <c r="C81" t="str">
+        <f t="shared" si="5"/>
+        <v>Periphery_AM</v>
+      </c>
+      <c r="D81" t="str">
+        <f t="shared" si="6"/>
+        <v>Periphery_580_AM</v>
+      </c>
+      <c r="I81">
+        <v>990888</v>
+      </c>
+      <c r="J81">
+        <f t="shared" si="7"/>
+        <v>888</v>
+      </c>
+      <c r="K81" t="s">
+        <v>427</v>
+      </c>
+      <c r="L81" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A82">
+        <v>770589</v>
+      </c>
+      <c r="B82">
+        <f t="shared" si="4"/>
+        <v>589</v>
+      </c>
+      <c r="C82" t="str">
+        <f t="shared" si="5"/>
+        <v>Periphery_PM</v>
+      </c>
+      <c r="D82" t="str">
+        <f t="shared" si="6"/>
+        <v>Periphery_580_PM</v>
+      </c>
+      <c r="I82">
+        <v>990886</v>
+      </c>
+      <c r="J82">
+        <f t="shared" si="7"/>
+        <v>886</v>
+      </c>
+      <c r="K82" t="s">
+        <v>395</v>
+      </c>
+      <c r="L82" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A83">
+        <v>770590</v>
+      </c>
+      <c r="B83">
+        <f t="shared" si="4"/>
+        <v>590</v>
+      </c>
+      <c r="C83" t="str">
+        <f t="shared" si="5"/>
+        <v>Periphery_AM</v>
+      </c>
+      <c r="D83" t="str">
+        <f t="shared" si="6"/>
+        <v>Periphery_580_AM</v>
+      </c>
+      <c r="I83">
+        <v>990689</v>
+      </c>
+      <c r="J83">
+        <f t="shared" si="7"/>
+        <v>689</v>
+      </c>
+      <c r="K83" t="s">
+        <v>388</v>
+      </c>
+      <c r="L83" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A84">
+        <v>770683</v>
+      </c>
+      <c r="B84">
+        <f t="shared" si="4"/>
+        <v>683</v>
+      </c>
+      <c r="C84" t="str">
+        <f t="shared" si="5"/>
+        <v>EastBay_Outer_PM</v>
+      </c>
+      <c r="D84" t="str">
+        <f t="shared" si="6"/>
+        <v>EastBayOuter_24_PM</v>
+      </c>
+      <c r="I84">
+        <v>990123</v>
+      </c>
+      <c r="J84">
+        <f t="shared" si="7"/>
+        <v>123</v>
+      </c>
+      <c r="K84" t="s">
+        <v>399</v>
+      </c>
+      <c r="L84" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A85">
+        <v>770684</v>
+      </c>
+      <c r="B85">
+        <f t="shared" si="4"/>
+        <v>684</v>
+      </c>
+      <c r="C85" t="str">
+        <f t="shared" si="5"/>
+        <v>EastBayOuter_AM</v>
+      </c>
+      <c r="D85" t="str">
+        <f t="shared" si="6"/>
+        <v>EastBayOuter_24_AM</v>
+      </c>
+      <c r="I85">
+        <v>990124</v>
+      </c>
+      <c r="J85">
+        <f t="shared" si="7"/>
+        <v>124</v>
+      </c>
+      <c r="K85" t="s">
+        <v>405</v>
+      </c>
+      <c r="L85" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A86">
+        <v>770689</v>
+      </c>
+      <c r="B86">
+        <f t="shared" si="4"/>
+        <v>689</v>
+      </c>
+      <c r="C86" t="str">
+        <f t="shared" si="5"/>
+        <v>EastBay_Outer_PM</v>
+      </c>
+      <c r="D86" t="str">
+        <f t="shared" si="6"/>
+        <v>EastBayOuter_580880_PM</v>
+      </c>
+      <c r="I86">
+        <v>990887</v>
+      </c>
+      <c r="J86">
+        <f t="shared" si="7"/>
+        <v>887</v>
+      </c>
+      <c r="K86" t="s">
+        <v>428</v>
+      </c>
+      <c r="L86" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A87">
+        <v>770690</v>
+      </c>
+      <c r="B87">
+        <f t="shared" si="4"/>
+        <v>690</v>
+      </c>
+      <c r="C87" t="str">
+        <f t="shared" si="5"/>
+        <v>EastBayOuter_AM</v>
+      </c>
+      <c r="D87" t="str">
+        <f t="shared" si="6"/>
+        <v>EastBayOuter_580880_AM</v>
+      </c>
+      <c r="I87">
+        <v>990121</v>
+      </c>
+      <c r="J87">
+        <f t="shared" si="7"/>
+        <v>121</v>
+      </c>
+      <c r="K87" t="s">
+        <v>399</v>
+      </c>
+      <c r="L87" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A88">
+        <v>770691</v>
+      </c>
+      <c r="B88">
+        <f t="shared" si="4"/>
+        <v>691</v>
+      </c>
+      <c r="C88" t="str">
+        <f t="shared" si="5"/>
+        <v>SouthBay_Outer_PM</v>
+      </c>
+      <c r="D88" t="str">
+        <f t="shared" si="6"/>
+        <v>SouthBay_Outer280680_PM</v>
+      </c>
+      <c r="I88">
+        <v>990122</v>
+      </c>
+      <c r="J88">
+        <f t="shared" si="7"/>
+        <v>122</v>
+      </c>
+      <c r="K88" t="s">
+        <v>405</v>
+      </c>
+      <c r="L88" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A89">
+        <v>770692</v>
+      </c>
+      <c r="B89">
+        <f t="shared" si="4"/>
+        <v>692</v>
+      </c>
+      <c r="C89" t="str">
+        <f t="shared" si="5"/>
+        <v>SouthBay_Outer_AM</v>
+      </c>
+      <c r="D89" t="str">
+        <f t="shared" si="6"/>
+        <v>SouthBay_Outer280680_AM</v>
+      </c>
+      <c r="I89">
+        <v>990854</v>
+      </c>
+      <c r="J89">
+        <f t="shared" si="7"/>
+        <v>854</v>
+      </c>
+      <c r="K89" t="s">
+        <v>435</v>
+      </c>
+      <c r="L89" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A90">
+        <v>770853</v>
+      </c>
+      <c r="B90">
+        <f t="shared" si="4"/>
+        <v>853</v>
+      </c>
+      <c r="C90" t="str">
+        <f t="shared" si="5"/>
+        <v>SouthBay_Outer_PM</v>
+      </c>
+      <c r="D90" t="str">
+        <f t="shared" si="6"/>
+        <v>SouthBay_Outer10187_PM</v>
+      </c>
+      <c r="I90">
+        <v>990853</v>
+      </c>
+      <c r="J90">
+        <f t="shared" si="7"/>
+        <v>853</v>
+      </c>
+      <c r="K90" t="s">
+        <v>435</v>
+      </c>
+      <c r="L90" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A91">
+        <v>770854</v>
+      </c>
+      <c r="B91">
+        <f t="shared" si="4"/>
+        <v>854</v>
+      </c>
+      <c r="C91" t="str">
+        <f t="shared" si="5"/>
+        <v>SouthBay_Outer_PM</v>
+      </c>
+      <c r="D91" t="str">
+        <f t="shared" si="6"/>
+        <v>SouthBay_Outer10187_PM</v>
+      </c>
+      <c r="I91">
+        <v>990691</v>
+      </c>
+      <c r="J91">
+        <f t="shared" si="7"/>
+        <v>691</v>
+      </c>
+      <c r="K91" t="s">
+        <v>435</v>
+      </c>
+      <c r="L91" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A92">
+        <v>770855</v>
+      </c>
+      <c r="B92">
+        <f t="shared" si="4"/>
+        <v>855</v>
+      </c>
+      <c r="C92" t="str">
+        <f t="shared" si="5"/>
+        <v>SouthBay_Outer_PM</v>
+      </c>
+      <c r="D92" t="str">
+        <f t="shared" si="6"/>
+        <v>SouthBay_Outer10187_PM</v>
+      </c>
+      <c r="I92">
+        <v>990283</v>
+      </c>
+      <c r="J92">
+        <f t="shared" si="7"/>
+        <v>283</v>
+      </c>
+      <c r="K92" t="s">
+        <v>430</v>
+      </c>
+      <c r="L92" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A93">
+        <v>770856</v>
+      </c>
+      <c r="B93">
+        <f t="shared" si="4"/>
+        <v>856</v>
+      </c>
+      <c r="C93" t="str">
+        <f t="shared" si="5"/>
+        <v>SouthBay_Outer_AM</v>
+      </c>
+      <c r="D93" t="str">
+        <f t="shared" si="6"/>
+        <v>SouthBay_Outer10187_AM</v>
+      </c>
+      <c r="I93">
+        <v>990284</v>
+      </c>
+      <c r="J93">
+        <f t="shared" si="7"/>
+        <v>284</v>
+      </c>
+      <c r="K93" t="s">
+        <v>435</v>
+      </c>
+      <c r="L93" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A94">
+        <v>770871</v>
+      </c>
+      <c r="B94">
+        <f t="shared" si="4"/>
+        <v>871</v>
+      </c>
+      <c r="C94" t="str">
+        <f t="shared" si="5"/>
+        <v>SouthBay_Outer_AM</v>
+      </c>
+      <c r="D94" t="str">
+        <f t="shared" si="6"/>
+        <v>SouthBay_Outer10187_AM</v>
+      </c>
+      <c r="I94">
+        <v>990889</v>
+      </c>
+      <c r="J94">
+        <f t="shared" si="7"/>
+        <v>889</v>
+      </c>
+      <c r="K94" t="s">
+        <v>428</v>
+      </c>
+      <c r="L94" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A95">
+        <v>770872</v>
+      </c>
+      <c r="B95">
+        <f t="shared" si="4"/>
+        <v>872</v>
+      </c>
+      <c r="C95" t="str">
+        <f t="shared" si="5"/>
+        <v>SouthBay_Outer_PM</v>
+      </c>
+      <c r="D95" t="str">
+        <f t="shared" si="6"/>
+        <v>SouthBay_Outer10187_PM</v>
+      </c>
+      <c r="I95">
+        <v>990233</v>
+      </c>
+      <c r="J95">
+        <f t="shared" si="7"/>
+        <v>233</v>
+      </c>
+      <c r="K95" t="s">
+        <v>428</v>
+      </c>
+      <c r="L95" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A96">
+        <v>770879</v>
+      </c>
+      <c r="B96">
+        <f t="shared" si="4"/>
+        <v>879</v>
+      </c>
+      <c r="C96" t="str">
+        <f t="shared" si="5"/>
+        <v>EastBay_Inner_AM</v>
+      </c>
+      <c r="D96" t="str">
+        <f t="shared" si="6"/>
+        <v>EastBayInner_BBApproach_AM</v>
+      </c>
+      <c r="I96">
+        <v>990117</v>
+      </c>
+      <c r="J96">
+        <f t="shared" si="7"/>
+        <v>117</v>
+      </c>
+      <c r="K96" t="s">
+        <v>427</v>
+      </c>
+      <c r="L96" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A97">
+        <v>770880</v>
+      </c>
+      <c r="B97">
+        <f t="shared" si="4"/>
+        <v>880</v>
+      </c>
+      <c r="C97" t="str">
+        <f t="shared" si="5"/>
+        <v>EastBay_Inner_PM</v>
+      </c>
+      <c r="D97" t="str">
+        <f t="shared" si="6"/>
+        <v>EastBayInner_BBApproach_PM</v>
+      </c>
+      <c r="I97">
+        <v>990115</v>
+      </c>
+      <c r="J97">
+        <f t="shared" si="7"/>
+        <v>115</v>
+      </c>
+      <c r="K97" t="s">
+        <v>427</v>
+      </c>
+      <c r="L97" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A98">
+        <v>770881</v>
+      </c>
+      <c r="B98">
+        <f t="shared" si="4"/>
+        <v>881</v>
+      </c>
+      <c r="C98" t="str">
+        <f t="shared" si="5"/>
+        <v>EastBay_Outer_PM</v>
+      </c>
+      <c r="D98" t="str">
+        <f t="shared" si="6"/>
+        <v>EastBayOuter_580880_PM</v>
+      </c>
+      <c r="I98">
+        <v>990111</v>
+      </c>
+      <c r="J98">
+        <f t="shared" si="7"/>
+        <v>111</v>
+      </c>
+      <c r="K98" t="s">
+        <v>414</v>
+      </c>
+      <c r="L98" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A99">
+        <v>770882</v>
+      </c>
+      <c r="B99">
+        <f t="shared" si="4"/>
+        <v>882</v>
+      </c>
+      <c r="C99" t="str">
+        <f t="shared" si="5"/>
+        <v>EastBayOuter_AM</v>
+      </c>
+      <c r="D99" t="str">
+        <f t="shared" si="6"/>
+        <v>EastBayOuter_580880_AM</v>
+      </c>
+      <c r="I99">
+        <v>990112</v>
+      </c>
+      <c r="J99">
+        <f t="shared" si="7"/>
+        <v>112</v>
+      </c>
+      <c r="K99" t="s">
+        <v>411</v>
+      </c>
+      <c r="L99" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A100">
+        <v>770883</v>
+      </c>
+      <c r="B100">
+        <f t="shared" si="4"/>
+        <v>883</v>
+      </c>
+      <c r="C100" t="str">
+        <f t="shared" si="5"/>
+        <v>EastBay_Outer_PM</v>
+      </c>
+      <c r="D100" t="str">
+        <f t="shared" si="6"/>
+        <v>EastBayOuter_580880_PM</v>
+      </c>
+      <c r="I100">
+        <v>990113</v>
+      </c>
+      <c r="J100">
+        <f t="shared" si="7"/>
+        <v>113</v>
+      </c>
+      <c r="K100" t="s">
+        <v>414</v>
+      </c>
+      <c r="L100" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A101">
+        <v>770884</v>
+      </c>
+      <c r="B101">
+        <f t="shared" si="4"/>
+        <v>884</v>
+      </c>
+      <c r="C101" t="str">
+        <f t="shared" si="5"/>
+        <v>EastBayOuter_AM</v>
+      </c>
+      <c r="D101" t="str">
+        <f t="shared" si="6"/>
+        <v>EastBayOuter_580880_AM</v>
+      </c>
+      <c r="I101">
+        <v>990105</v>
+      </c>
+      <c r="J101">
+        <f t="shared" si="7"/>
+        <v>105</v>
+      </c>
+      <c r="K101" t="s">
+        <v>420</v>
+      </c>
+      <c r="L101" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A102">
+        <v>770885</v>
+      </c>
+      <c r="B102">
+        <f t="shared" si="4"/>
+        <v>885</v>
+      </c>
+      <c r="C102" t="str">
+        <f t="shared" si="5"/>
+        <v>EastBay_Outer_PM</v>
+      </c>
+      <c r="D102" t="str">
+        <f t="shared" si="6"/>
+        <v>EastBayOuter_580880_PM</v>
+      </c>
+      <c r="I102">
+        <v>990114</v>
+      </c>
+      <c r="J102">
+        <f t="shared" si="7"/>
+        <v>114</v>
+      </c>
+      <c r="K102" t="s">
+        <v>411</v>
+      </c>
+      <c r="L102" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A103">
+        <v>770886</v>
+      </c>
+      <c r="B103">
+        <f t="shared" si="4"/>
+        <v>886</v>
+      </c>
+      <c r="C103" t="str">
+        <f t="shared" si="5"/>
+        <v>EastBayOuter_AM</v>
+      </c>
+      <c r="D103" t="str">
+        <f t="shared" si="6"/>
+        <v>EastBayOuter_580880_AM</v>
+      </c>
+      <c r="I103">
+        <v>990107</v>
+      </c>
+      <c r="J103">
+        <f t="shared" si="7"/>
+        <v>107</v>
+      </c>
+      <c r="K103" t="s">
+        <v>414</v>
+      </c>
+      <c r="L103" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A104">
+        <v>770887</v>
+      </c>
+      <c r="B104">
+        <f t="shared" si="4"/>
+        <v>887</v>
+      </c>
+      <c r="C104" t="str">
+        <f t="shared" si="5"/>
+        <v>SouthBay_Inner_PM</v>
+      </c>
+      <c r="D104" t="str">
+        <f t="shared" si="6"/>
+        <v>SouthBay_Inner_PM</v>
+      </c>
+      <c r="I104">
+        <v>990288</v>
+      </c>
+      <c r="J104">
+        <f t="shared" si="7"/>
+        <v>288</v>
+      </c>
+      <c r="K104" t="s">
+        <v>423</v>
+      </c>
+      <c r="L104" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A105">
+        <v>770888</v>
+      </c>
+      <c r="B105">
+        <f t="shared" si="4"/>
+        <v>888</v>
+      </c>
+      <c r="C105" t="str">
+        <f t="shared" si="5"/>
+        <v>SouthBay_Inner_AM</v>
+      </c>
+      <c r="D105" t="str">
+        <f t="shared" si="6"/>
+        <v>SouthBay_Inner_AM</v>
+      </c>
+      <c r="I105">
+        <v>990110</v>
+      </c>
+      <c r="J105">
+        <f t="shared" si="7"/>
+        <v>110</v>
+      </c>
+      <c r="K105" t="s">
+        <v>411</v>
+      </c>
+      <c r="L105" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A106">
+        <v>770889</v>
+      </c>
+      <c r="B106">
+        <f t="shared" si="4"/>
+        <v>889</v>
+      </c>
+      <c r="C106" t="str">
+        <f t="shared" si="5"/>
+        <v>SouthBay_Inner_PM</v>
+      </c>
+      <c r="D106" t="str">
+        <f t="shared" si="6"/>
+        <v>SouthBay_Inner_PM</v>
+      </c>
+      <c r="I106">
+        <v>990923</v>
+      </c>
+      <c r="J106">
+        <f t="shared" si="7"/>
+        <v>923</v>
+      </c>
+      <c r="K106" t="s">
+        <v>411</v>
+      </c>
+      <c r="L106" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A107">
+        <v>770890</v>
+      </c>
+      <c r="B107">
+        <f t="shared" si="4"/>
+        <v>890</v>
+      </c>
+      <c r="C107" t="str">
+        <f t="shared" si="5"/>
+        <v>SouthBay_Inner_AM</v>
+      </c>
+      <c r="D107" t="str">
+        <f t="shared" si="6"/>
+        <v>SouthBay_Inner_AM</v>
+      </c>
+      <c r="I107">
+        <v>990104</v>
+      </c>
+      <c r="J107">
+        <f t="shared" si="7"/>
+        <v>104</v>
+      </c>
+      <c r="K107" t="s">
+        <v>423</v>
+      </c>
+      <c r="L107" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A108">
+        <v>770891</v>
+      </c>
+      <c r="B108">
+        <f t="shared" si="4"/>
+        <v>891</v>
+      </c>
+      <c r="C108" t="str">
+        <f t="shared" si="5"/>
+        <v>SouthBay_Outer_AM</v>
+      </c>
+      <c r="D108" t="str">
+        <f t="shared" si="6"/>
+        <v>SouthBay_Outer10187_AM</v>
+      </c>
+      <c r="I108">
+        <v>990103</v>
+      </c>
+      <c r="J108">
+        <f t="shared" si="7"/>
+        <v>103</v>
+      </c>
+      <c r="K108" t="s">
+        <v>420</v>
+      </c>
+      <c r="L108" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A109">
+        <v>770892</v>
+      </c>
+      <c r="B109">
+        <f t="shared" si="4"/>
+        <v>892</v>
+      </c>
+      <c r="C109" t="str">
+        <f t="shared" si="5"/>
+        <v>SouthBay_Outer_PM</v>
+      </c>
+      <c r="D109" t="str">
+        <f t="shared" si="6"/>
+        <v>SouthBay_Outer10187_PM</v>
+      </c>
+      <c r="I109">
+        <v>990101</v>
+      </c>
+      <c r="J109">
+        <f t="shared" si="7"/>
+        <v>101</v>
+      </c>
+      <c r="K109" t="s">
+        <v>417</v>
+      </c>
+      <c r="L109" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A110">
+        <v>770923</v>
+      </c>
+      <c r="B110">
+        <f t="shared" si="4"/>
+        <v>923</v>
+      </c>
+      <c r="C110" t="str">
+        <f t="shared" si="5"/>
+        <v>SanMateo_AM</v>
+      </c>
+      <c r="D110" t="str">
+        <f t="shared" si="6"/>
+        <v>SanMateo_28092_AM</v>
+      </c>
+      <c r="I110">
+        <v>990102</v>
+      </c>
+      <c r="J110">
+        <f t="shared" si="7"/>
+        <v>102</v>
+      </c>
+      <c r="K110" t="s">
+        <v>418</v>
+      </c>
+      <c r="L110" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A111">
+        <v>770924</v>
+      </c>
+      <c r="B111">
+        <f t="shared" si="4"/>
+        <v>924</v>
+      </c>
+      <c r="C111" t="str">
+        <f t="shared" si="5"/>
+        <v>SanMateo_PM</v>
+      </c>
+      <c r="D111" t="str">
+        <f t="shared" si="6"/>
+        <v>SanMateo_28092_PM</v>
+      </c>
+      <c r="I111">
+        <v>990078</v>
+      </c>
+      <c r="J111">
+        <f t="shared" si="7"/>
+        <v>78</v>
+      </c>
+      <c r="K111" t="s">
+        <v>417</v>
+      </c>
+      <c r="L111" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A112">
+        <v>770981</v>
+      </c>
+      <c r="B112">
+        <f t="shared" si="4"/>
+        <v>981</v>
+      </c>
+      <c r="C112" t="str">
+        <f t="shared" si="5"/>
+        <v>EastBay_Inner_PM</v>
+      </c>
+      <c r="D112" t="str">
+        <f t="shared" si="6"/>
+        <v>EastBayInner_58098024_PM</v>
+      </c>
+      <c r="I112">
+        <v>990077</v>
+      </c>
+      <c r="J112">
+        <f t="shared" si="7"/>
+        <v>77</v>
+      </c>
+      <c r="K112" t="s">
+        <v>418</v>
+      </c>
+      <c r="L112" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="113" spans="9:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="I113">
+        <v>990076</v>
+      </c>
+      <c r="J113">
+        <f t="shared" si="7"/>
+        <v>76</v>
+      </c>
+      <c r="K113" t="s">
+        <v>418</v>
+      </c>
+      <c r="L113" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="114" spans="9:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="I114">
+        <v>990075</v>
+      </c>
+      <c r="J114">
+        <f t="shared" si="7"/>
+        <v>75</v>
+      </c>
+      <c r="K114" t="s">
+        <v>417</v>
+      </c>
+      <c r="L114" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="115" spans="9:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="I115">
+        <v>990131</v>
+      </c>
+      <c r="J115">
+        <f t="shared" si="7"/>
+        <v>131</v>
+      </c>
+      <c r="K115" t="s">
+        <v>405</v>
+      </c>
+      <c r="L115" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="116" spans="9:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="I116">
+        <v>990132</v>
+      </c>
+      <c r="J116">
+        <f t="shared" si="7"/>
+        <v>132</v>
+      </c>
+      <c r="K116" t="s">
+        <v>399</v>
+      </c>
+      <c r="L116" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="117" spans="9:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="I117">
+        <v>990089</v>
+      </c>
+      <c r="J117">
+        <f t="shared" si="7"/>
+        <v>89</v>
+      </c>
+      <c r="K117" t="s">
+        <v>405</v>
+      </c>
+      <c r="L117" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="118" spans="9:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="I118">
+        <v>990090</v>
+      </c>
+      <c r="J118">
+        <f t="shared" si="7"/>
+        <v>90</v>
+      </c>
+      <c r="K118" t="s">
+        <v>399</v>
+      </c>
+      <c r="L118" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="119" spans="9:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="I119">
+        <v>990403</v>
+      </c>
+      <c r="J119">
+        <f t="shared" si="7"/>
+        <v>403</v>
+      </c>
+      <c r="K119" t="s">
+        <v>405</v>
+      </c>
+      <c r="L119" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="120" spans="9:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="I120">
+        <v>990404</v>
+      </c>
+      <c r="J120">
+        <f t="shared" si="7"/>
+        <v>404</v>
+      </c>
+      <c r="K120" t="s">
+        <v>399</v>
+      </c>
+      <c r="L120" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="121" spans="9:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="I121">
+        <v>990087</v>
+      </c>
+      <c r="J121">
+        <f t="shared" si="7"/>
+        <v>87</v>
+      </c>
+      <c r="K121" t="s">
+        <v>405</v>
+      </c>
+      <c r="L121" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="122" spans="9:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="I122">
+        <v>990088</v>
+      </c>
+      <c r="J122">
+        <f t="shared" si="7"/>
+        <v>88</v>
+      </c>
+      <c r="K122" t="s">
+        <v>399</v>
+      </c>
+      <c r="L122" t="s">
+        <v>400</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="I1:L122" xr:uid="{D6E8173F-978E-4C06-BD6A-29F17B918A7B}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="990982"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F2F96A3-2267-4825-A37F-38ADB47D606F}">
   <dimension ref="A1:F141"/>
   <sheetViews>
@@ -15384,7 +19165,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DF77F54-B726-43F2-A3A6-3E118A23C251}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>

</xml_diff>

<commit_message>
tidy up the project field
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/TOLLCLASS_Designations.xlsx
+++ b/utilities/NextGenFwys/TOLLCLASS_Designations.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\NextGenFwys\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBDFD8C1-111C-4818-8C77-890ACD69F603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABAF7453-E439-4006-8127-1085DE30FE48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{0F0A9957-56E7-4C48-967B-2AB2A1965C2F}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2347" uniqueCount="593">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2347" uniqueCount="444">
   <si>
     <t>SR92 SM - I-280 Interchange to US101 Interchange - WB</t>
   </si>
@@ -1356,453 +1356,6 @@
   </si>
   <si>
     <t>SouthBay_Outer280680_PM</t>
-  </si>
-  <si>
-    <t>RTP2022</t>
-  </si>
-  <si>
-    <t>RTP2023</t>
-  </si>
-  <si>
-    <t>RTP2024</t>
-  </si>
-  <si>
-    <t>RTP2025</t>
-  </si>
-  <si>
-    <t>RTP2026</t>
-  </si>
-  <si>
-    <t>RTP2027</t>
-  </si>
-  <si>
-    <t>RTP2028</t>
-  </si>
-  <si>
-    <t>RTP2029</t>
-  </si>
-  <si>
-    <t>RTP2030</t>
-  </si>
-  <si>
-    <t>RTP2031</t>
-  </si>
-  <si>
-    <t>RTP2032</t>
-  </si>
-  <si>
-    <t>RTP2033</t>
-  </si>
-  <si>
-    <t>RTP2034</t>
-  </si>
-  <si>
-    <t>RTP2035</t>
-  </si>
-  <si>
-    <t>RTP2036</t>
-  </si>
-  <si>
-    <t>RTP2037</t>
-  </si>
-  <si>
-    <t>RTP2038</t>
-  </si>
-  <si>
-    <t>RTP2039</t>
-  </si>
-  <si>
-    <t>RTP2040</t>
-  </si>
-  <si>
-    <t>RTP2041</t>
-  </si>
-  <si>
-    <t>RTP2042</t>
-  </si>
-  <si>
-    <t>RTP2043</t>
-  </si>
-  <si>
-    <t>RTP2044</t>
-  </si>
-  <si>
-    <t>RTP2045</t>
-  </si>
-  <si>
-    <t>RTP2046</t>
-  </si>
-  <si>
-    <t>RTP2047</t>
-  </si>
-  <si>
-    <t>RTP2048</t>
-  </si>
-  <si>
-    <t>RTP2049</t>
-  </si>
-  <si>
-    <t>RTP2050</t>
-  </si>
-  <si>
-    <t>RTP2051</t>
-  </si>
-  <si>
-    <t>RTP2052</t>
-  </si>
-  <si>
-    <t>RTP2053</t>
-  </si>
-  <si>
-    <t>RTP2054</t>
-  </si>
-  <si>
-    <t>RTP2055</t>
-  </si>
-  <si>
-    <t>RTP2056</t>
-  </si>
-  <si>
-    <t>RTP2057</t>
-  </si>
-  <si>
-    <t>RTP2058</t>
-  </si>
-  <si>
-    <t>RTP2059</t>
-  </si>
-  <si>
-    <t>RTP2060</t>
-  </si>
-  <si>
-    <t>RTP2061</t>
-  </si>
-  <si>
-    <t>RTP2062</t>
-  </si>
-  <si>
-    <t>RTP2063</t>
-  </si>
-  <si>
-    <t>RTP2064</t>
-  </si>
-  <si>
-    <t>RTP2065</t>
-  </si>
-  <si>
-    <t>RTP2066</t>
-  </si>
-  <si>
-    <t>RTP2067</t>
-  </si>
-  <si>
-    <t>RTP2068</t>
-  </si>
-  <si>
-    <t>RTP2069</t>
-  </si>
-  <si>
-    <t>RTP2070</t>
-  </si>
-  <si>
-    <t>RTP2071</t>
-  </si>
-  <si>
-    <t>RTP2072</t>
-  </si>
-  <si>
-    <t>RTP2073</t>
-  </si>
-  <si>
-    <t>RTP2074</t>
-  </si>
-  <si>
-    <t>RTP2075</t>
-  </si>
-  <si>
-    <t>RTP2076</t>
-  </si>
-  <si>
-    <t>RTP2077</t>
-  </si>
-  <si>
-    <t>RTP2078</t>
-  </si>
-  <si>
-    <t>RTP2079</t>
-  </si>
-  <si>
-    <t>RTP2080</t>
-  </si>
-  <si>
-    <t>RTP2081</t>
-  </si>
-  <si>
-    <t>RTP2082</t>
-  </si>
-  <si>
-    <t>RTP2083</t>
-  </si>
-  <si>
-    <t>RTP2084</t>
-  </si>
-  <si>
-    <t>RTP2085</t>
-  </si>
-  <si>
-    <t>RTP2086</t>
-  </si>
-  <si>
-    <t>RTP2087</t>
-  </si>
-  <si>
-    <t>RTP2088</t>
-  </si>
-  <si>
-    <t>RTP2089</t>
-  </si>
-  <si>
-    <t>RTP2090</t>
-  </si>
-  <si>
-    <t>RTP2091</t>
-  </si>
-  <si>
-    <t>RTP2092</t>
-  </si>
-  <si>
-    <t>RTP2093</t>
-  </si>
-  <si>
-    <t>RTP2094</t>
-  </si>
-  <si>
-    <t>RTP2095</t>
-  </si>
-  <si>
-    <t>RTP2096</t>
-  </si>
-  <si>
-    <t>RTP2097</t>
-  </si>
-  <si>
-    <t>RTP2098</t>
-  </si>
-  <si>
-    <t>RTP2099</t>
-  </si>
-  <si>
-    <t>RTP2100</t>
-  </si>
-  <si>
-    <t>RTP2101</t>
-  </si>
-  <si>
-    <t>RTP2102</t>
-  </si>
-  <si>
-    <t>RTP2103</t>
-  </si>
-  <si>
-    <t>RTP2104</t>
-  </si>
-  <si>
-    <t>RTP2105</t>
-  </si>
-  <si>
-    <t>RTP2106</t>
-  </si>
-  <si>
-    <t>RTP2107</t>
-  </si>
-  <si>
-    <t>RTP2108</t>
-  </si>
-  <si>
-    <t>RTP2109</t>
-  </si>
-  <si>
-    <t>RTP2110</t>
-  </si>
-  <si>
-    <t>RTP2111</t>
-  </si>
-  <si>
-    <t>RTP2112</t>
-  </si>
-  <si>
-    <t>RTP2113</t>
-  </si>
-  <si>
-    <t>RTP2114</t>
-  </si>
-  <si>
-    <t>RTP2115</t>
-  </si>
-  <si>
-    <t>RTP2116</t>
-  </si>
-  <si>
-    <t>RTP2117</t>
-  </si>
-  <si>
-    <t>RTP2118</t>
-  </si>
-  <si>
-    <t>RTP2119</t>
-  </si>
-  <si>
-    <t>RTP2120</t>
-  </si>
-  <si>
-    <t>RTP2121</t>
-  </si>
-  <si>
-    <t>RTP2122</t>
-  </si>
-  <si>
-    <t>RTP2123</t>
-  </si>
-  <si>
-    <t>RTP2124</t>
-  </si>
-  <si>
-    <t>RTP2125</t>
-  </si>
-  <si>
-    <t>RTP2126</t>
-  </si>
-  <si>
-    <t>RTP2127</t>
-  </si>
-  <si>
-    <t>RTP2128</t>
-  </si>
-  <si>
-    <t>RTP2129</t>
-  </si>
-  <si>
-    <t>RTP2130</t>
-  </si>
-  <si>
-    <t>RTP2131</t>
-  </si>
-  <si>
-    <t>RTP2132</t>
-  </si>
-  <si>
-    <t>RTP2133</t>
-  </si>
-  <si>
-    <t>RTP2134</t>
-  </si>
-  <si>
-    <t>RTP2135</t>
-  </si>
-  <si>
-    <t>RTP2136</t>
-  </si>
-  <si>
-    <t>RTP2137</t>
-  </si>
-  <si>
-    <t>RTP2138</t>
-  </si>
-  <si>
-    <t>RTP2139</t>
-  </si>
-  <si>
-    <t>RTP2140</t>
-  </si>
-  <si>
-    <t>RTP2141</t>
-  </si>
-  <si>
-    <t>RTP2142</t>
-  </si>
-  <si>
-    <t>RTP2143</t>
-  </si>
-  <si>
-    <t>RTP2144</t>
-  </si>
-  <si>
-    <t>RTP2145</t>
-  </si>
-  <si>
-    <t>RTP2146</t>
-  </si>
-  <si>
-    <t>RTP2147</t>
-  </si>
-  <si>
-    <t>RTP2148</t>
-  </si>
-  <si>
-    <t>RTP2149</t>
-  </si>
-  <si>
-    <t>RTP2150</t>
-  </si>
-  <si>
-    <t>RTP2151</t>
-  </si>
-  <si>
-    <t>RTP2152</t>
-  </si>
-  <si>
-    <t>RTP2153</t>
-  </si>
-  <si>
-    <t>RTP2154</t>
-  </si>
-  <si>
-    <t>RTP2155</t>
-  </si>
-  <si>
-    <t>RTP2156</t>
-  </si>
-  <si>
-    <t>RTP2157</t>
-  </si>
-  <si>
-    <t>RTP2158</t>
-  </si>
-  <si>
-    <t>RTP2159</t>
-  </si>
-  <si>
-    <t>RTP2160</t>
-  </si>
-  <si>
-    <t>RTP2161</t>
-  </si>
-  <si>
-    <t>RTP2162</t>
-  </si>
-  <si>
-    <t>RTP2163</t>
-  </si>
-  <si>
-    <t>RTP2164</t>
-  </si>
-  <si>
-    <t>RTP2165</t>
-  </si>
-  <si>
-    <t>RTP2166</t>
-  </si>
-  <si>
-    <t>RTP2167</t>
-  </si>
-  <si>
-    <t>RTP2168</t>
-  </si>
-  <si>
-    <t>RTP2169</t>
-  </si>
-  <si>
-    <t>RTP2170</t>
   </si>
   <si>
     <t>Cordon toll</t>
@@ -2236,8 +1789,8 @@
   <dimension ref="A1:I443"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A411" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H443" sqref="H443:I443"/>
+      <pane ySplit="1" topLeftCell="A154" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B162" sqref="B162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2426,7 +1979,7 @@
         <v>9</v>
       </c>
       <c r="H10" t="s">
-        <v>587</v>
+        <v>438</v>
       </c>
       <c r="I10" t="s">
         <v>363</v>
@@ -2452,7 +2005,7 @@
         <v>0.03</v>
       </c>
       <c r="H11" t="s">
-        <v>587</v>
+        <v>438</v>
       </c>
       <c r="I11" t="s">
         <v>353</v>
@@ -2478,10 +2031,10 @@
         <v>0.03</v>
       </c>
       <c r="H12" t="s">
-        <v>587</v>
+        <v>438</v>
       </c>
       <c r="I12" t="s">
-        <v>588</v>
+        <v>439</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
@@ -2504,10 +2057,10 @@
         <v>0.03</v>
       </c>
       <c r="H13" t="s">
-        <v>587</v>
+        <v>438</v>
       </c>
       <c r="I13" t="s">
-        <v>589</v>
+        <v>440</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
@@ -2568,7 +2121,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>438</v>
+        <v>373</v>
       </c>
       <c r="B16" t="s">
         <v>149</v>
@@ -2597,7 +2150,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>439</v>
+        <v>373</v>
       </c>
       <c r="B17" t="s">
         <v>148</v>
@@ -2626,7 +2179,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>440</v>
+        <v>373</v>
       </c>
       <c r="B18" t="s">
         <v>147</v>
@@ -2655,7 +2208,7 @@
     </row>
     <row r="19" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>441</v>
+        <v>373</v>
       </c>
       <c r="B19" t="s">
         <v>146</v>
@@ -2684,7 +2237,7 @@
     </row>
     <row r="20" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>442</v>
+        <v>373</v>
       </c>
       <c r="B20" t="s">
         <v>145</v>
@@ -2713,7 +2266,7 @@
     </row>
     <row r="21" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>443</v>
+        <v>373</v>
       </c>
       <c r="B21" t="s">
         <v>144</v>
@@ -2742,7 +2295,7 @@
     </row>
     <row r="22" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>444</v>
+        <v>373</v>
       </c>
       <c r="B22" t="s">
         <v>143</v>
@@ -2771,7 +2324,7 @@
     </row>
     <row r="23" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>445</v>
+        <v>373</v>
       </c>
       <c r="B23" t="s">
         <v>142</v>
@@ -2800,7 +2353,7 @@
     </row>
     <row r="24" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>446</v>
+        <v>373</v>
       </c>
       <c r="B24" t="s">
         <v>141</v>
@@ -2829,7 +2382,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>447</v>
+        <v>373</v>
       </c>
       <c r="B25" t="s">
         <v>140</v>
@@ -2858,7 +2411,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>448</v>
+        <v>373</v>
       </c>
       <c r="B26" t="s">
         <v>139</v>
@@ -2887,7 +2440,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>449</v>
+        <v>373</v>
       </c>
       <c r="B27" t="s">
         <v>138</v>
@@ -2916,7 +2469,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>450</v>
+        <v>373</v>
       </c>
       <c r="B28" t="s">
         <v>137</v>
@@ -2945,7 +2498,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>451</v>
+        <v>373</v>
       </c>
       <c r="B29" t="s">
         <v>136</v>
@@ -2974,7 +2527,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>452</v>
+        <v>373</v>
       </c>
       <c r="B30" t="s">
         <v>135</v>
@@ -3003,7 +2556,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>453</v>
+        <v>373</v>
       </c>
       <c r="B31" t="s">
         <v>134</v>
@@ -3032,7 +2585,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>454</v>
+        <v>373</v>
       </c>
       <c r="B32" t="s">
         <v>133</v>
@@ -3061,7 +2614,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>455</v>
+        <v>373</v>
       </c>
       <c r="B33" t="s">
         <v>132</v>
@@ -3090,7 +2643,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>456</v>
+        <v>373</v>
       </c>
       <c r="B34" t="s">
         <v>131</v>
@@ -3119,7 +2672,7 @@
     </row>
     <row r="35" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>457</v>
+        <v>373</v>
       </c>
       <c r="B35" t="s">
         <v>130</v>
@@ -3148,7 +2701,7 @@
     </row>
     <row r="36" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>458</v>
+        <v>373</v>
       </c>
       <c r="B36" t="s">
         <v>129</v>
@@ -3177,7 +2730,7 @@
     </row>
     <row r="37" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>459</v>
+        <v>373</v>
       </c>
       <c r="B37" t="s">
         <v>128</v>
@@ -3206,7 +2759,7 @@
     </row>
     <row r="38" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>460</v>
+        <v>373</v>
       </c>
       <c r="B38" t="s">
         <v>127</v>
@@ -3235,7 +2788,7 @@
     </row>
     <row r="39" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>461</v>
+        <v>373</v>
       </c>
       <c r="B39" t="s">
         <v>126</v>
@@ -3264,7 +2817,7 @@
     </row>
     <row r="40" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>462</v>
+        <v>373</v>
       </c>
       <c r="B40" t="s">
         <v>125</v>
@@ -3293,7 +2846,7 @@
     </row>
     <row r="41" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>463</v>
+        <v>373</v>
       </c>
       <c r="B41" t="s">
         <v>124</v>
@@ -3322,7 +2875,7 @@
     </row>
     <row r="42" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>464</v>
+        <v>373</v>
       </c>
       <c r="B42" t="s">
         <v>123</v>
@@ -3351,7 +2904,7 @@
     </row>
     <row r="43" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>465</v>
+        <v>373</v>
       </c>
       <c r="B43" t="s">
         <v>122</v>
@@ -3380,7 +2933,7 @@
     </row>
     <row r="44" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>466</v>
+        <v>373</v>
       </c>
       <c r="B44" t="s">
         <v>121</v>
@@ -3409,7 +2962,7 @@
     </row>
     <row r="45" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>467</v>
+        <v>373</v>
       </c>
       <c r="B45" t="s">
         <v>120</v>
@@ -3438,7 +2991,7 @@
     </row>
     <row r="46" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>468</v>
+        <v>373</v>
       </c>
       <c r="B46" t="s">
         <v>119</v>
@@ -3467,7 +3020,7 @@
     </row>
     <row r="47" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>469</v>
+        <v>373</v>
       </c>
       <c r="B47" t="s">
         <v>118</v>
@@ -3496,7 +3049,7 @@
     </row>
     <row r="48" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>470</v>
+        <v>373</v>
       </c>
       <c r="B48" t="s">
         <v>117</v>
@@ -3525,7 +3078,7 @@
     </row>
     <row r="49" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>471</v>
+        <v>373</v>
       </c>
       <c r="B49" t="s">
         <v>116</v>
@@ -3554,7 +3107,7 @@
     </row>
     <row r="50" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>472</v>
+        <v>373</v>
       </c>
       <c r="B50" t="s">
         <v>115</v>
@@ -3583,7 +3136,7 @@
     </row>
     <row r="51" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>473</v>
+        <v>373</v>
       </c>
       <c r="B51" t="s">
         <v>114</v>
@@ -3612,7 +3165,7 @@
     </row>
     <row r="52" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>474</v>
+        <v>373</v>
       </c>
       <c r="B52" t="s">
         <v>113</v>
@@ -3641,7 +3194,7 @@
     </row>
     <row r="53" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>475</v>
+        <v>373</v>
       </c>
       <c r="B53" t="s">
         <v>112</v>
@@ -3670,7 +3223,7 @@
     </row>
     <row r="54" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>476</v>
+        <v>373</v>
       </c>
       <c r="B54" t="s">
         <v>111</v>
@@ -3699,7 +3252,7 @@
     </row>
     <row r="55" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>477</v>
+        <v>373</v>
       </c>
       <c r="B55" t="s">
         <v>110</v>
@@ -3728,7 +3281,7 @@
     </row>
     <row r="56" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>478</v>
+        <v>373</v>
       </c>
       <c r="B56" t="s">
         <v>109</v>
@@ -3757,7 +3310,7 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>479</v>
+        <v>373</v>
       </c>
       <c r="B57" t="s">
         <v>108</v>
@@ -3786,7 +3339,7 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>480</v>
+        <v>373</v>
       </c>
       <c r="B58" t="s">
         <v>107</v>
@@ -3815,7 +3368,7 @@
     </row>
     <row r="59" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>481</v>
+        <v>373</v>
       </c>
       <c r="B59" t="s">
         <v>106</v>
@@ -3844,7 +3397,7 @@
     </row>
     <row r="60" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>482</v>
+        <v>373</v>
       </c>
       <c r="B60" t="s">
         <v>105</v>
@@ -3873,7 +3426,7 @@
     </row>
     <row r="61" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>483</v>
+        <v>373</v>
       </c>
       <c r="B61" t="s">
         <v>104</v>
@@ -3902,7 +3455,7 @@
     </row>
     <row r="62" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>484</v>
+        <v>373</v>
       </c>
       <c r="B62" t="s">
         <v>103</v>
@@ -3931,7 +3484,7 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>485</v>
+        <v>373</v>
       </c>
       <c r="B63" t="s">
         <v>102</v>
@@ -3960,7 +3513,7 @@
     </row>
     <row r="64" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>486</v>
+        <v>373</v>
       </c>
       <c r="B64" t="s">
         <v>101</v>
@@ -3989,7 +3542,7 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>487</v>
+        <v>373</v>
       </c>
       <c r="B65" t="s">
         <v>100</v>
@@ -4018,7 +3571,7 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>488</v>
+        <v>373</v>
       </c>
       <c r="B66" t="s">
         <v>99</v>
@@ -4047,7 +3600,7 @@
     </row>
     <row r="67" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>489</v>
+        <v>373</v>
       </c>
       <c r="B67" t="s">
         <v>98</v>
@@ -4076,7 +3629,7 @@
     </row>
     <row r="68" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>490</v>
+        <v>373</v>
       </c>
       <c r="B68" t="s">
         <v>97</v>
@@ -4105,7 +3658,7 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>491</v>
+        <v>373</v>
       </c>
       <c r="B69" t="s">
         <v>96</v>
@@ -4134,7 +3687,7 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>492</v>
+        <v>373</v>
       </c>
       <c r="B70" t="s">
         <v>95</v>
@@ -4163,7 +3716,7 @@
     </row>
     <row r="71" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>493</v>
+        <v>373</v>
       </c>
       <c r="B71" t="s">
         <v>94</v>
@@ -4192,7 +3745,7 @@
     </row>
     <row r="72" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>494</v>
+        <v>373</v>
       </c>
       <c r="B72" t="s">
         <v>93</v>
@@ -4221,7 +3774,7 @@
     </row>
     <row r="73" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>495</v>
+        <v>373</v>
       </c>
       <c r="B73" t="s">
         <v>92</v>
@@ -4250,7 +3803,7 @@
     </row>
     <row r="74" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>496</v>
+        <v>373</v>
       </c>
       <c r="B74" t="s">
         <v>91</v>
@@ -4279,7 +3832,7 @@
     </row>
     <row r="75" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>497</v>
+        <v>373</v>
       </c>
       <c r="B75" t="s">
         <v>90</v>
@@ -4308,7 +3861,7 @@
     </row>
     <row r="76" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>498</v>
+        <v>373</v>
       </c>
       <c r="B76" t="s">
         <v>89</v>
@@ -4337,7 +3890,7 @@
     </row>
     <row r="77" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>499</v>
+        <v>373</v>
       </c>
       <c r="B77" t="s">
         <v>88</v>
@@ -4366,7 +3919,7 @@
     </row>
     <row r="78" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>500</v>
+        <v>373</v>
       </c>
       <c r="B78" t="s">
         <v>87</v>
@@ -4395,7 +3948,7 @@
     </row>
     <row r="79" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>501</v>
+        <v>373</v>
       </c>
       <c r="B79" t="s">
         <v>86</v>
@@ -4424,7 +3977,7 @@
     </row>
     <row r="80" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>502</v>
+        <v>373</v>
       </c>
       <c r="B80" t="s">
         <v>85</v>
@@ -4453,7 +4006,7 @@
     </row>
     <row r="81" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>503</v>
+        <v>373</v>
       </c>
       <c r="B81" t="s">
         <v>84</v>
@@ -4482,7 +4035,7 @@
     </row>
     <row r="82" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>504</v>
+        <v>373</v>
       </c>
       <c r="B82" t="s">
         <v>83</v>
@@ -4511,7 +4064,7 @@
     </row>
     <row r="83" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>505</v>
+        <v>373</v>
       </c>
       <c r="B83" t="s">
         <v>82</v>
@@ -4540,7 +4093,7 @@
     </row>
     <row r="84" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>506</v>
+        <v>373</v>
       </c>
       <c r="B84" t="s">
         <v>81</v>
@@ -4569,7 +4122,7 @@
     </row>
     <row r="85" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>507</v>
+        <v>373</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>80</v>
@@ -4598,7 +4151,7 @@
     </row>
     <row r="86" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>508</v>
+        <v>373</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>79</v>
@@ -4627,7 +4180,7 @@
     </row>
     <row r="87" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>509</v>
+        <v>373</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>78</v>
@@ -4653,7 +4206,7 @@
     </row>
     <row r="88" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>510</v>
+        <v>373</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>77</v>
@@ -4679,7 +4232,7 @@
     </row>
     <row r="89" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>511</v>
+        <v>373</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>76</v>
@@ -4705,7 +4258,7 @@
     </row>
     <row r="90" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>512</v>
+        <v>373</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>75</v>
@@ -4731,7 +4284,7 @@
     </row>
     <row r="91" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>513</v>
+        <v>373</v>
       </c>
       <c r="B91" t="s">
         <v>74</v>
@@ -4760,7 +4313,7 @@
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>514</v>
+        <v>373</v>
       </c>
       <c r="B92" t="s">
         <v>73</v>
@@ -4789,7 +4342,7 @@
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>515</v>
+        <v>373</v>
       </c>
       <c r="B93" t="s">
         <v>72</v>
@@ -4818,7 +4371,7 @@
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>516</v>
+        <v>373</v>
       </c>
       <c r="B94" t="s">
         <v>71</v>
@@ -4847,7 +4400,7 @@
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>517</v>
+        <v>373</v>
       </c>
       <c r="B95" t="s">
         <v>70</v>
@@ -4876,7 +4429,7 @@
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>518</v>
+        <v>373</v>
       </c>
       <c r="B96" t="s">
         <v>69</v>
@@ -4905,7 +4458,7 @@
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>519</v>
+        <v>373</v>
       </c>
       <c r="B97" t="s">
         <v>68</v>
@@ -4934,7 +4487,7 @@
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>520</v>
+        <v>373</v>
       </c>
       <c r="B98" t="s">
         <v>67</v>
@@ -4963,7 +4516,7 @@
     </row>
     <row r="99" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>521</v>
+        <v>373</v>
       </c>
       <c r="B99" t="s">
         <v>66</v>
@@ -4992,7 +4545,7 @@
     </row>
     <row r="100" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>522</v>
+        <v>373</v>
       </c>
       <c r="B100" t="s">
         <v>65</v>
@@ -5021,7 +4574,7 @@
     </row>
     <row r="101" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>523</v>
+        <v>373</v>
       </c>
       <c r="B101" t="s">
         <v>64</v>
@@ -5050,7 +4603,7 @@
     </row>
     <row r="102" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>524</v>
+        <v>373</v>
       </c>
       <c r="B102" t="s">
         <v>63</v>
@@ -5079,7 +4632,7 @@
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>525</v>
+        <v>373</v>
       </c>
       <c r="B103" t="s">
         <v>62</v>
@@ -5108,7 +4661,7 @@
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>526</v>
+        <v>373</v>
       </c>
       <c r="B104" t="s">
         <v>61</v>
@@ -5137,7 +4690,7 @@
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>527</v>
+        <v>373</v>
       </c>
       <c r="B105" t="s">
         <v>60</v>
@@ -5166,7 +4719,7 @@
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>528</v>
+        <v>373</v>
       </c>
       <c r="B106" t="s">
         <v>59</v>
@@ -5195,7 +4748,7 @@
     </row>
     <row r="107" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>529</v>
+        <v>373</v>
       </c>
       <c r="B107" t="s">
         <v>58</v>
@@ -5224,7 +4777,7 @@
     </row>
     <row r="108" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>530</v>
+        <v>373</v>
       </c>
       <c r="B108" t="s">
         <v>57</v>
@@ -5253,7 +4806,7 @@
     </row>
     <row r="109" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>531</v>
+        <v>373</v>
       </c>
       <c r="B109" t="s">
         <v>56</v>
@@ -5282,7 +4835,7 @@
     </row>
     <row r="110" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>532</v>
+        <v>373</v>
       </c>
       <c r="B110" t="s">
         <v>55</v>
@@ -5311,7 +4864,7 @@
     </row>
     <row r="111" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>533</v>
+        <v>373</v>
       </c>
       <c r="B111" t="s">
         <v>54</v>
@@ -5340,7 +4893,7 @@
     </row>
     <row r="112" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>534</v>
+        <v>373</v>
       </c>
       <c r="B112" t="s">
         <v>53</v>
@@ -5369,7 +4922,7 @@
     </row>
     <row r="113" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>535</v>
+        <v>373</v>
       </c>
       <c r="B113" t="s">
         <v>52</v>
@@ -5398,7 +4951,7 @@
     </row>
     <row r="114" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>536</v>
+        <v>373</v>
       </c>
       <c r="B114" t="s">
         <v>51</v>
@@ -5427,7 +4980,7 @@
     </row>
     <row r="115" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>537</v>
+        <v>373</v>
       </c>
       <c r="B115" t="s">
         <v>50</v>
@@ -5456,7 +5009,7 @@
     </row>
     <row r="116" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>538</v>
+        <v>373</v>
       </c>
       <c r="B116" t="s">
         <v>49</v>
@@ -5485,7 +5038,7 @@
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>539</v>
+        <v>373</v>
       </c>
       <c r="B117" t="s">
         <v>48</v>
@@ -5514,7 +5067,7 @@
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>540</v>
+        <v>373</v>
       </c>
       <c r="B118" t="s">
         <v>47</v>
@@ -5543,7 +5096,7 @@
     </row>
     <row r="119" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>541</v>
+        <v>373</v>
       </c>
       <c r="B119" t="s">
         <v>46</v>
@@ -5572,7 +5125,7 @@
     </row>
     <row r="120" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>542</v>
+        <v>373</v>
       </c>
       <c r="B120" t="s">
         <v>45</v>
@@ -5601,7 +5154,7 @@
     </row>
     <row r="121" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>543</v>
+        <v>373</v>
       </c>
       <c r="B121" t="s">
         <v>44</v>
@@ -5630,7 +5183,7 @@
     </row>
     <row r="122" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>544</v>
+        <v>373</v>
       </c>
       <c r="B122" t="s">
         <v>43</v>
@@ -5659,7 +5212,7 @@
     </row>
     <row r="123" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>545</v>
+        <v>373</v>
       </c>
       <c r="B123" t="s">
         <v>42</v>
@@ -5688,7 +5241,7 @@
     </row>
     <row r="124" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>546</v>
+        <v>373</v>
       </c>
       <c r="B124" t="s">
         <v>41</v>
@@ -5717,7 +5270,7 @@
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>547</v>
+        <v>373</v>
       </c>
       <c r="B125" t="s">
         <v>40</v>
@@ -5746,7 +5299,7 @@
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>548</v>
+        <v>373</v>
       </c>
       <c r="B126" t="s">
         <v>39</v>
@@ -5775,7 +5328,7 @@
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>549</v>
+        <v>373</v>
       </c>
       <c r="B127" t="s">
         <v>38</v>
@@ -5804,7 +5357,7 @@
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>550</v>
+        <v>373</v>
       </c>
       <c r="B128" t="s">
         <v>37</v>
@@ -5833,7 +5386,7 @@
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>551</v>
+        <v>373</v>
       </c>
       <c r="B129" t="s">
         <v>36</v>
@@ -5862,7 +5415,7 @@
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>552</v>
+        <v>373</v>
       </c>
       <c r="B130" t="s">
         <v>35</v>
@@ -5891,7 +5444,7 @@
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>553</v>
+        <v>373</v>
       </c>
       <c r="B131" t="s">
         <v>34</v>
@@ -5920,7 +5473,7 @@
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>554</v>
+        <v>373</v>
       </c>
       <c r="B132" t="s">
         <v>33</v>
@@ -5949,7 +5502,7 @@
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>555</v>
+        <v>373</v>
       </c>
       <c r="B133" t="s">
         <v>32</v>
@@ -5978,7 +5531,7 @@
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>556</v>
+        <v>373</v>
       </c>
       <c r="B134" t="s">
         <v>31</v>
@@ -6007,7 +5560,7 @@
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>557</v>
+        <v>373</v>
       </c>
       <c r="B135" t="s">
         <v>30</v>
@@ -6036,7 +5589,7 @@
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>558</v>
+        <v>373</v>
       </c>
       <c r="B136" t="s">
         <v>29</v>
@@ -6065,7 +5618,7 @@
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>559</v>
+        <v>373</v>
       </c>
       <c r="B137" t="s">
         <v>28</v>
@@ -6094,7 +5647,7 @@
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>560</v>
+        <v>373</v>
       </c>
       <c r="B138" t="s">
         <v>27</v>
@@ -6123,7 +5676,7 @@
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>561</v>
+        <v>373</v>
       </c>
       <c r="B139" t="s">
         <v>26</v>
@@ -6152,7 +5705,7 @@
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>562</v>
+        <v>373</v>
       </c>
       <c r="B140" t="s">
         <v>25</v>
@@ -6181,7 +5734,7 @@
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>563</v>
+        <v>373</v>
       </c>
       <c r="B141" t="s">
         <v>24</v>
@@ -6210,7 +5763,7 @@
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>564</v>
+        <v>373</v>
       </c>
       <c r="B142" t="s">
         <v>23</v>
@@ -6239,7 +5792,7 @@
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>565</v>
+        <v>373</v>
       </c>
       <c r="B143" t="s">
         <v>22</v>
@@ -6268,7 +5821,7 @@
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>566</v>
+        <v>373</v>
       </c>
       <c r="B144" t="s">
         <v>21</v>
@@ -6297,7 +5850,7 @@
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>567</v>
+        <v>373</v>
       </c>
       <c r="B145" t="s">
         <v>20</v>
@@ -6326,7 +5879,7 @@
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>568</v>
+        <v>373</v>
       </c>
       <c r="B146" t="s">
         <v>19</v>
@@ -6355,7 +5908,7 @@
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>569</v>
+        <v>373</v>
       </c>
       <c r="B147" t="s">
         <v>18</v>
@@ -6384,7 +5937,7 @@
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>570</v>
+        <v>373</v>
       </c>
       <c r="B148" t="s">
         <v>17</v>
@@ -6413,7 +5966,7 @@
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>571</v>
+        <v>373</v>
       </c>
       <c r="B149" t="s">
         <v>15</v>
@@ -6439,7 +5992,7 @@
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>572</v>
+        <v>373</v>
       </c>
       <c r="B150" t="s">
         <v>14</v>
@@ -6465,7 +6018,7 @@
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>573</v>
+        <v>373</v>
       </c>
       <c r="B151" t="s">
         <v>13</v>
@@ -6491,7 +6044,7 @@
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>574</v>
+        <v>373</v>
       </c>
       <c r="B152" t="s">
         <v>12</v>
@@ -6517,7 +6070,7 @@
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>575</v>
+        <v>373</v>
       </c>
       <c r="B153" t="s">
         <v>11</v>
@@ -6543,7 +6096,7 @@
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>576</v>
+        <v>373</v>
       </c>
       <c r="B154" t="s">
         <v>10</v>
@@ -6569,7 +6122,7 @@
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>577</v>
+        <v>373</v>
       </c>
       <c r="B155" t="s">
         <v>9</v>
@@ -6595,7 +6148,7 @@
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>578</v>
+        <v>373</v>
       </c>
       <c r="B156" t="s">
         <v>8</v>
@@ -6621,7 +6174,7 @@
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>579</v>
+        <v>373</v>
       </c>
       <c r="B157" t="s">
         <v>7</v>
@@ -6647,7 +6200,7 @@
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>580</v>
+        <v>373</v>
       </c>
       <c r="B158" t="s">
         <v>6</v>
@@ -6673,7 +6226,7 @@
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>581</v>
+        <v>373</v>
       </c>
       <c r="B159" t="s">
         <v>5</v>
@@ -6699,7 +6252,7 @@
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>582</v>
+        <v>373</v>
       </c>
       <c r="B160" t="s">
         <v>4</v>
@@ -6725,7 +6278,7 @@
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>583</v>
+        <v>373</v>
       </c>
       <c r="B161" t="s">
         <v>3</v>
@@ -6751,7 +6304,7 @@
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>584</v>
+        <v>373</v>
       </c>
       <c r="B162" t="s">
         <v>2</v>
@@ -6777,7 +6330,7 @@
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>585</v>
+        <v>373</v>
       </c>
       <c r="B163" t="s">
         <v>1</v>
@@ -6803,7 +6356,7 @@
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>586</v>
+        <v>373</v>
       </c>
       <c r="B164" t="s">
         <v>0</v>
@@ -11174,7 +10727,7 @@
         <v>374</v>
       </c>
       <c r="B332" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C332">
         <v>770075</v>
@@ -11191,7 +10744,7 @@
         <v>374</v>
       </c>
       <c r="B333" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C333">
         <v>770076</v>
@@ -11208,7 +10761,7 @@
         <v>374</v>
       </c>
       <c r="B334" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C334">
         <v>770077</v>
@@ -11225,7 +10778,7 @@
         <v>374</v>
       </c>
       <c r="B335" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C335">
         <v>770078</v>
@@ -11242,7 +10795,7 @@
         <v>374</v>
       </c>
       <c r="B336" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C336">
         <v>770081</v>
@@ -11259,7 +10812,7 @@
         <v>374</v>
       </c>
       <c r="B337" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C337">
         <v>770082</v>
@@ -11276,7 +10829,7 @@
         <v>374</v>
       </c>
       <c r="B338" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C338">
         <v>770083</v>
@@ -11293,7 +10846,7 @@
         <v>374</v>
       </c>
       <c r="B339" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C339">
         <v>770084</v>
@@ -11310,7 +10863,7 @@
         <v>374</v>
       </c>
       <c r="B340" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C340">
         <v>770085</v>
@@ -11327,7 +10880,7 @@
         <v>374</v>
       </c>
       <c r="B341" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C341">
         <v>770086</v>
@@ -11344,7 +10897,7 @@
         <v>374</v>
       </c>
       <c r="B342" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C342">
         <v>770087</v>
@@ -11361,7 +10914,7 @@
         <v>374</v>
       </c>
       <c r="B343" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C343">
         <v>770088</v>
@@ -11378,7 +10931,7 @@
         <v>374</v>
       </c>
       <c r="B344" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C344">
         <v>770091</v>
@@ -11395,7 +10948,7 @@
         <v>374</v>
       </c>
       <c r="B345" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C345">
         <v>770092</v>
@@ -11412,7 +10965,7 @@
         <v>374</v>
       </c>
       <c r="B346" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C346">
         <v>770101</v>
@@ -11429,7 +10982,7 @@
         <v>374</v>
       </c>
       <c r="B347" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C347">
         <v>770102</v>
@@ -11446,7 +10999,7 @@
         <v>374</v>
       </c>
       <c r="B348" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C348">
         <v>770103</v>
@@ -11463,7 +11016,7 @@
         <v>374</v>
       </c>
       <c r="B349" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C349">
         <v>770104</v>
@@ -11480,7 +11033,7 @@
         <v>374</v>
       </c>
       <c r="B350" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C350">
         <v>770105</v>
@@ -11497,7 +11050,7 @@
         <v>374</v>
       </c>
       <c r="B351" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C351">
         <v>770106</v>
@@ -11514,7 +11067,7 @@
         <v>374</v>
       </c>
       <c r="B352" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C352">
         <v>770107</v>
@@ -11531,7 +11084,7 @@
         <v>374</v>
       </c>
       <c r="B353" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C353">
         <v>770108</v>
@@ -11548,7 +11101,7 @@
         <v>374</v>
       </c>
       <c r="B354" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C354">
         <v>770109</v>
@@ -11565,7 +11118,7 @@
         <v>374</v>
       </c>
       <c r="B355" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C355">
         <v>770110</v>
@@ -11582,7 +11135,7 @@
         <v>374</v>
       </c>
       <c r="B356" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C356">
         <v>770111</v>
@@ -11599,7 +11152,7 @@
         <v>374</v>
       </c>
       <c r="B357" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C357">
         <v>770112</v>
@@ -11616,7 +11169,7 @@
         <v>374</v>
       </c>
       <c r="B358" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C358">
         <v>770113</v>
@@ -11633,7 +11186,7 @@
         <v>374</v>
       </c>
       <c r="B359" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C359">
         <v>770114</v>
@@ -11650,7 +11203,7 @@
         <v>374</v>
       </c>
       <c r="B360" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C360">
         <v>770115</v>
@@ -11667,7 +11220,7 @@
         <v>374</v>
       </c>
       <c r="B361" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C361">
         <v>770116</v>
@@ -11684,7 +11237,7 @@
         <v>374</v>
       </c>
       <c r="B362" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C362">
         <v>770117</v>
@@ -11701,7 +11254,7 @@
         <v>374</v>
       </c>
       <c r="B363" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C363">
         <v>770118</v>
@@ -11718,7 +11271,7 @@
         <v>374</v>
       </c>
       <c r="B364" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C364">
         <v>770119</v>
@@ -11735,7 +11288,7 @@
         <v>374</v>
       </c>
       <c r="B365" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C365">
         <v>770120</v>
@@ -11752,7 +11305,7 @@
         <v>374</v>
       </c>
       <c r="B366" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C366">
         <v>770121</v>
@@ -11769,7 +11322,7 @@
         <v>374</v>
       </c>
       <c r="B367" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C367">
         <v>770122</v>
@@ -11786,7 +11339,7 @@
         <v>374</v>
       </c>
       <c r="B368" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C368">
         <v>770123</v>
@@ -11803,7 +11356,7 @@
         <v>374</v>
       </c>
       <c r="B369" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C369">
         <v>770124</v>
@@ -11820,7 +11373,7 @@
         <v>374</v>
       </c>
       <c r="B370" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C370">
         <v>770135</v>
@@ -11837,7 +11390,7 @@
         <v>374</v>
       </c>
       <c r="B371" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C371">
         <v>770136</v>
@@ -11854,7 +11407,7 @@
         <v>374</v>
       </c>
       <c r="B372" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C372">
         <v>770171</v>
@@ -11871,7 +11424,7 @@
         <v>374</v>
       </c>
       <c r="B373" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C373">
         <v>770172</v>
@@ -11888,7 +11441,7 @@
         <v>374</v>
       </c>
       <c r="B374" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C374">
         <v>770231</v>
@@ -11905,7 +11458,7 @@
         <v>374</v>
       </c>
       <c r="B375" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C375">
         <v>770232</v>
@@ -11922,7 +11475,7 @@
         <v>374</v>
       </c>
       <c r="B376" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C376">
         <v>770233</v>
@@ -11939,7 +11492,7 @@
         <v>374</v>
       </c>
       <c r="B377" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C377">
         <v>770234</v>
@@ -11956,7 +11509,7 @@
         <v>374</v>
       </c>
       <c r="B378" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C378">
         <v>770239</v>
@@ -11973,7 +11526,7 @@
         <v>374</v>
       </c>
       <c r="B379" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C379">
         <v>770240</v>
@@ -11990,7 +11543,7 @@
         <v>374</v>
       </c>
       <c r="B380" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C380">
         <v>770241</v>
@@ -12007,7 +11560,7 @@
         <v>374</v>
       </c>
       <c r="B381" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C381">
         <v>770242</v>
@@ -12024,7 +11577,7 @@
         <v>374</v>
       </c>
       <c r="B382" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C382">
         <v>770243</v>
@@ -12041,7 +11594,7 @@
         <v>374</v>
       </c>
       <c r="B383" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C383">
         <v>770244</v>
@@ -12058,7 +11611,7 @@
         <v>374</v>
       </c>
       <c r="B384" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C384">
         <v>770245</v>
@@ -12075,7 +11628,7 @@
         <v>374</v>
       </c>
       <c r="B385" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C385">
         <v>770246</v>
@@ -12092,7 +11645,7 @@
         <v>374</v>
       </c>
       <c r="B386" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C386">
         <v>770281</v>
@@ -12109,7 +11662,7 @@
         <v>374</v>
       </c>
       <c r="B387" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C387">
         <v>770282</v>
@@ -12126,7 +11679,7 @@
         <v>374</v>
       </c>
       <c r="B388" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C388">
         <v>770283</v>
@@ -12143,7 +11696,7 @@
         <v>374</v>
       </c>
       <c r="B389" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C389">
         <v>770284</v>
@@ -12160,7 +11713,7 @@
         <v>374</v>
       </c>
       <c r="B390" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C390">
         <v>770285</v>
@@ -12177,7 +11730,7 @@
         <v>374</v>
       </c>
       <c r="B391" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C391">
         <v>770286</v>
@@ -12194,7 +11747,7 @@
         <v>374</v>
       </c>
       <c r="B392" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C392">
         <v>770287</v>
@@ -12211,7 +11764,7 @@
         <v>374</v>
       </c>
       <c r="B393" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C393">
         <v>770288</v>
@@ -12228,7 +11781,7 @@
         <v>374</v>
       </c>
       <c r="B394" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C394">
         <v>770289</v>
@@ -12245,7 +11798,7 @@
         <v>374</v>
       </c>
       <c r="B395" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C395">
         <v>770290</v>
@@ -12262,7 +11815,7 @@
         <v>374</v>
       </c>
       <c r="B396" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C396">
         <v>770381</v>
@@ -12279,7 +11832,7 @@
         <v>374</v>
       </c>
       <c r="B397" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C397">
         <v>770382</v>
@@ -12296,7 +11849,7 @@
         <v>374</v>
       </c>
       <c r="B398" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C398">
         <v>770401</v>
@@ -12313,7 +11866,7 @@
         <v>374</v>
       </c>
       <c r="B399" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C399">
         <v>770402</v>
@@ -12330,7 +11883,7 @@
         <v>374</v>
       </c>
       <c r="B400" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C400">
         <v>770403</v>
@@ -12347,7 +11900,7 @@
         <v>374</v>
       </c>
       <c r="B401" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C401">
         <v>770404</v>
@@ -12364,7 +11917,7 @@
         <v>374</v>
       </c>
       <c r="B402" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C402">
         <v>770407</v>
@@ -12381,7 +11934,7 @@
         <v>374</v>
       </c>
       <c r="B403" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C403">
         <v>770408</v>
@@ -12398,7 +11951,7 @@
         <v>374</v>
       </c>
       <c r="B404" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C404">
         <v>770581</v>
@@ -12415,7 +11968,7 @@
         <v>374</v>
       </c>
       <c r="B405" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C405">
         <v>770582</v>
@@ -12432,7 +11985,7 @@
         <v>374</v>
       </c>
       <c r="B406" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C406">
         <v>770583</v>
@@ -12449,7 +12002,7 @@
         <v>374</v>
       </c>
       <c r="B407" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C407">
         <v>770584</v>
@@ -12466,7 +12019,7 @@
         <v>374</v>
       </c>
       <c r="B408" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C408">
         <v>770585</v>
@@ -12483,7 +12036,7 @@
         <v>374</v>
       </c>
       <c r="B409" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C409">
         <v>770586</v>
@@ -12500,7 +12053,7 @@
         <v>374</v>
       </c>
       <c r="B410" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C410">
         <v>770587</v>
@@ -12517,7 +12070,7 @@
         <v>374</v>
       </c>
       <c r="B411" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C411">
         <v>770588</v>
@@ -12534,7 +12087,7 @@
         <v>374</v>
       </c>
       <c r="B412" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C412">
         <v>770589</v>
@@ -12551,7 +12104,7 @@
         <v>374</v>
       </c>
       <c r="B413" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C413">
         <v>770590</v>
@@ -12568,7 +12121,7 @@
         <v>374</v>
       </c>
       <c r="B414" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C414">
         <v>770683</v>
@@ -12585,7 +12138,7 @@
         <v>374</v>
       </c>
       <c r="B415" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C415">
         <v>770684</v>
@@ -12602,7 +12155,7 @@
         <v>374</v>
       </c>
       <c r="B416" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C416">
         <v>770689</v>
@@ -12619,7 +12172,7 @@
         <v>374</v>
       </c>
       <c r="B417" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C417">
         <v>770690</v>
@@ -12636,7 +12189,7 @@
         <v>374</v>
       </c>
       <c r="B418" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C418">
         <v>770691</v>
@@ -12653,7 +12206,7 @@
         <v>374</v>
       </c>
       <c r="B419" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C419">
         <v>770692</v>
@@ -12670,7 +12223,7 @@
         <v>374</v>
       </c>
       <c r="B420" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C420">
         <v>770853</v>
@@ -12687,7 +12240,7 @@
         <v>374</v>
       </c>
       <c r="B421" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C421">
         <v>770854</v>
@@ -12704,7 +12257,7 @@
         <v>374</v>
       </c>
       <c r="B422" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C422">
         <v>770855</v>
@@ -12721,7 +12274,7 @@
         <v>374</v>
       </c>
       <c r="B423" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C423">
         <v>770856</v>
@@ -12738,7 +12291,7 @@
         <v>374</v>
       </c>
       <c r="B424" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C424">
         <v>770871</v>
@@ -12755,7 +12308,7 @@
         <v>374</v>
       </c>
       <c r="B425" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C425">
         <v>770872</v>
@@ -12772,7 +12325,7 @@
         <v>374</v>
       </c>
       <c r="B426" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C426">
         <v>770879</v>
@@ -12789,7 +12342,7 @@
         <v>374</v>
       </c>
       <c r="B427" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C427">
         <v>770880</v>
@@ -12806,7 +12359,7 @@
         <v>374</v>
       </c>
       <c r="B428" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C428">
         <v>770881</v>
@@ -12823,7 +12376,7 @@
         <v>374</v>
       </c>
       <c r="B429" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C429">
         <v>770882</v>
@@ -12840,7 +12393,7 @@
         <v>374</v>
       </c>
       <c r="B430" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C430">
         <v>770883</v>
@@ -12857,7 +12410,7 @@
         <v>374</v>
       </c>
       <c r="B431" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C431">
         <v>770884</v>
@@ -12874,7 +12427,7 @@
         <v>374</v>
       </c>
       <c r="B432" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C432">
         <v>770885</v>
@@ -12891,7 +12444,7 @@
         <v>374</v>
       </c>
       <c r="B433" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C433">
         <v>770886</v>
@@ -12908,7 +12461,7 @@
         <v>374</v>
       </c>
       <c r="B434" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C434">
         <v>770887</v>
@@ -12925,7 +12478,7 @@
         <v>374</v>
       </c>
       <c r="B435" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C435">
         <v>770888</v>
@@ -12942,7 +12495,7 @@
         <v>374</v>
       </c>
       <c r="B436" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C436">
         <v>770889</v>
@@ -12959,7 +12512,7 @@
         <v>374</v>
       </c>
       <c r="B437" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C437">
         <v>770890</v>
@@ -12976,7 +12529,7 @@
         <v>374</v>
       </c>
       <c r="B438" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C438">
         <v>770891</v>
@@ -12993,7 +12546,7 @@
         <v>374</v>
       </c>
       <c r="B439" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C439">
         <v>770892</v>
@@ -13010,7 +12563,7 @@
         <v>374</v>
       </c>
       <c r="B440" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C440">
         <v>770923</v>
@@ -13027,7 +12580,7 @@
         <v>374</v>
       </c>
       <c r="B441" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C441">
         <v>770924</v>
@@ -13044,7 +12597,7 @@
         <v>374</v>
       </c>
       <c r="B442" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C442">
         <v>770981</v>
@@ -13061,7 +12614,7 @@
         <v>374</v>
       </c>
       <c r="B443" t="s">
-        <v>590</v>
+        <v>441</v>
       </c>
       <c r="C443">
         <v>770982</v>
@@ -13099,10 +12652,10 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>591</v>
+        <v>442</v>
       </c>
       <c r="B1" t="s">
-        <v>592</v>
+        <v>443</v>
       </c>
       <c r="C1" t="s">
         <v>337</v>
@@ -13114,7 +12667,7 @@
         <v>152</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>592</v>
+        <v>443</v>
       </c>
       <c r="K1" t="s">
         <v>337</v>

</xml_diff>

<commit_message>
committing missing major and minor groups for tollclass 990138 990137 (SF_PM and SF_AM)
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/TOLLCLASS_Designations.xlsx
+++ b/utilities/NextGenFwys/TOLLCLASS_Designations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B104BE57-586E-48A3-B9CA-66963048B983}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F43881E-3FEF-44FC-B1DE-4A5B108D7BFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{0F0A9957-56E7-4C48-967B-2AB2A1965C2F}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1550" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1554" uniqueCount="417">
   <si>
     <t>SR92 SM - I-280 Interchange to US101 Interchange - WB</t>
   </si>
@@ -1689,8 +1689,8 @@
   <dimension ref="A1:I443"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A432" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B445" sqref="B445"/>
+      <pane ySplit="1" topLeftCell="A210" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I215" sqref="I215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7573,11 +7573,11 @@
       <c r="G214">
         <v>1E-3</v>
       </c>
-      <c r="H214" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I214" t="e">
-        <v>#N/A</v>
+      <c r="H214" t="s">
+        <v>384</v>
+      </c>
+      <c r="I214" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="215" spans="1:9" x14ac:dyDescent="0.35">
@@ -7599,11 +7599,11 @@
       <c r="G215">
         <v>1E-3</v>
       </c>
-      <c r="H215" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I215" t="e">
-        <v>#N/A</v>
+      <c r="H215" t="s">
+        <v>385</v>
+      </c>
+      <c r="I215" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="216" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Switch the direction of AM/PM for the SFOSanMateo_101 and SFOSanMateo_280380 corridors
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/TOLLCLASS_Designations.xlsx
+++ b/utilities/NextGenFwys/TOLLCLASS_Designations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F43881E-3FEF-44FC-B1DE-4A5B108D7BFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF47810B-3436-41A5-95D4-A2049B4927EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{0F0A9957-56E7-4C48-967B-2AB2A1965C2F}"/>
   </bookViews>
@@ -1688,9 +1688,9 @@
   </sheetPr>
   <dimension ref="A1:I443"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A210" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I215" sqref="I215"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A426" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J1" sqref="J1:N1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1700,7 +1700,7 @@
     <col min="4" max="4" width="15.81640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21.1796875" customWidth="1"/>
-    <col min="9" max="9" width="15.81640625" customWidth="1"/>
+    <col min="9" max="9" width="24.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
@@ -8874,10 +8874,10 @@
         <v>1E-3</v>
       </c>
       <c r="H264" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="I264" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
     </row>
     <row r="265" spans="1:9" x14ac:dyDescent="0.35">
@@ -8952,10 +8952,10 @@
         <v>1E-3</v>
       </c>
       <c r="H267" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="I267" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="268" spans="1:9" x14ac:dyDescent="0.35">
@@ -9030,10 +9030,10 @@
         <v>1E-3</v>
       </c>
       <c r="H270" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="I270" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="271" spans="1:9" x14ac:dyDescent="0.35">
@@ -9056,10 +9056,10 @@
         <v>1E-3</v>
       </c>
       <c r="H271" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="I271" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
     </row>
     <row r="272" spans="1:9" x14ac:dyDescent="0.35">
@@ -10905,10 +10905,10 @@
         <v>770103</v>
       </c>
       <c r="H348" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="I348" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
     </row>
     <row r="349" spans="1:9" x14ac:dyDescent="0.35">
@@ -10922,10 +10922,10 @@
         <v>770104</v>
       </c>
       <c r="H349" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="I349" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="350" spans="1:9" x14ac:dyDescent="0.35">
@@ -10939,10 +10939,10 @@
         <v>770105</v>
       </c>
       <c r="H350" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="I350" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
     </row>
     <row r="351" spans="1:9" x14ac:dyDescent="0.35">
@@ -10956,10 +10956,10 @@
         <v>770106</v>
       </c>
       <c r="H351" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="I351" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="352" spans="1:9" x14ac:dyDescent="0.35">
@@ -11653,10 +11653,10 @@
         <v>770287</v>
       </c>
       <c r="H392" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="I392" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="393" spans="1:9" x14ac:dyDescent="0.35">
@@ -11670,10 +11670,10 @@
         <v>770288</v>
       </c>
       <c r="H393" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="I393" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="394" spans="1:9" x14ac:dyDescent="0.35">
@@ -11721,10 +11721,10 @@
         <v>770381</v>
       </c>
       <c r="H396" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="I396" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="397" spans="1:9" x14ac:dyDescent="0.35">
@@ -11738,10 +11738,10 @@
         <v>770382</v>
       </c>
       <c r="H397" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="I397" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="398" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Add El tolls from EXP_ObservedPrices_2023
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/TOLLCLASS_Designations.xlsx
+++ b/utilities/NextGenFwys/TOLLCLASS_Designations.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jalatorre\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\llin\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{208215CC-2805-4D97-9FF3-5D3E511750C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0AE22AB-21B1-46A1-A89C-447EFA49D088}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="10690" windowWidth="22780" windowHeight="14660" xr2:uid="{0F0A9957-56E7-4C48-967B-2AB2A1965C2F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="15600" xr2:uid="{0F0A9957-56E7-4C48-967B-2AB2A1965C2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs_for_tollcalib" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1584" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1617" uniqueCount="447">
   <si>
     <t>SR92 SM - I-280 Interchange to US101 Interchange - WB</t>
   </si>
@@ -1341,6 +1341,45 @@
   </si>
   <si>
     <t>SM-019</t>
+  </si>
+  <si>
+    <t>US101 SM - 2740 San Mateo SB - SB</t>
+  </si>
+  <si>
+    <t>US101 SM - 2770 Redwood City SB - SB</t>
+  </si>
+  <si>
+    <t>US101 SM - 2830 San Mateo NB - NB</t>
+  </si>
+  <si>
+    <t>US101 SM - 2810 Redwood City NB - NB</t>
+  </si>
+  <si>
+    <t>I-880 - 2340 Union City SB - SB</t>
+  </si>
+  <si>
+    <t>I-880 - 2320 San Leandro SB - SB</t>
+  </si>
+  <si>
+    <t>I-880 - 2370 Fremont SB - SB</t>
+  </si>
+  <si>
+    <t>I-880 - 2450 Union City NB - NB</t>
+  </si>
+  <si>
+    <t>I-880 - 2420 Fremont NB - NB</t>
+  </si>
+  <si>
+    <t>I-680 - 2120 Walnut Creek SB - SB</t>
+  </si>
+  <si>
+    <t>I-680 - 2130 San Ramon SB - SB</t>
+  </si>
+  <si>
+    <t>I-680 - 2230 San Ramon NB - NB</t>
+  </si>
+  <si>
+    <t>RTP2025</t>
   </si>
 </sst>
 </file>
@@ -1737,25 +1776,25 @@
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
-  <dimension ref="A1:J443"/>
+  <dimension ref="A1:J455"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A427" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E455" sqref="E455"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.453125" customWidth="1"/>
-    <col min="2" max="2" width="79.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="79.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.1796875" customWidth="1"/>
-    <col min="10" max="10" width="24.453125" customWidth="1"/>
+    <col min="9" max="9" width="21.140625" customWidth="1"/>
+    <col min="10" max="10" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>336</v>
       </c>
@@ -1787,7 +1826,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>360</v>
       </c>
@@ -1804,7 +1843,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>360</v>
       </c>
@@ -1821,7 +1860,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>360</v>
       </c>
@@ -1838,7 +1877,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>360</v>
       </c>
@@ -1855,7 +1894,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>360</v>
       </c>
@@ -1872,7 +1911,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>360</v>
       </c>
@@ -1889,7 +1928,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>360</v>
       </c>
@@ -1906,7 +1945,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>360</v>
       </c>
@@ -1923,7 +1962,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>361</v>
       </c>
@@ -1940,7 +1979,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>361</v>
       </c>
@@ -1966,7 +2005,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>362</v>
       </c>
@@ -1992,7 +2031,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>362</v>
       </c>
@@ -2018,7 +2057,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>362</v>
       </c>
@@ -2045,7 +2084,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>361</v>
       </c>
@@ -2074,7 +2113,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>361</v>
       </c>
@@ -2103,7 +2142,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>361</v>
       </c>
@@ -2132,7 +2171,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>361</v>
       </c>
@@ -2161,7 +2200,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>361</v>
       </c>
@@ -2190,7 +2229,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>361</v>
       </c>
@@ -2219,7 +2258,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>361</v>
       </c>
@@ -2248,7 +2287,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>361</v>
       </c>
@@ -2277,7 +2316,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>361</v>
       </c>
@@ -2306,7 +2345,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>361</v>
       </c>
@@ -2335,7 +2374,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>361</v>
       </c>
@@ -2364,7 +2403,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>361</v>
       </c>
@@ -2393,7 +2432,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>361</v>
       </c>
@@ -2425,7 +2464,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>361</v>
       </c>
@@ -2457,7 +2496,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>361</v>
       </c>
@@ -2489,7 +2528,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>361</v>
       </c>
@@ -2521,7 +2560,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>361</v>
       </c>
@@ -2553,7 +2592,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>361</v>
       </c>
@@ -2585,7 +2624,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>361</v>
       </c>
@@ -2614,7 +2653,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>361</v>
       </c>
@@ -2643,7 +2682,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>361</v>
       </c>
@@ -2672,7 +2711,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>361</v>
       </c>
@@ -2701,7 +2740,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>361</v>
       </c>
@@ -2730,7 +2769,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>361</v>
       </c>
@@ -2759,7 +2798,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>361</v>
       </c>
@@ -2791,7 +2830,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>361</v>
       </c>
@@ -2823,7 +2862,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>361</v>
       </c>
@@ -2852,7 +2891,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>361</v>
       </c>
@@ -2881,7 +2920,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>361</v>
       </c>
@@ -2910,7 +2949,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>361</v>
       </c>
@@ -2939,7 +2978,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>361</v>
       </c>
@@ -2968,7 +3007,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>361</v>
       </c>
@@ -2997,7 +3036,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>361</v>
       </c>
@@ -3026,7 +3065,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>361</v>
       </c>
@@ -3055,7 +3094,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>361</v>
       </c>
@@ -3084,7 +3123,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>361</v>
       </c>
@@ -3113,7 +3152,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>361</v>
       </c>
@@ -3145,7 +3184,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>361</v>
       </c>
@@ -3177,7 +3216,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>361</v>
       </c>
@@ -3206,7 +3245,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>361</v>
       </c>
@@ -3235,7 +3274,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>361</v>
       </c>
@@ -3264,7 +3303,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>361</v>
       </c>
@@ -3293,7 +3332,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>361</v>
       </c>
@@ -3322,7 +3361,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>361</v>
       </c>
@@ -3351,7 +3390,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>361</v>
       </c>
@@ -3380,7 +3419,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>361</v>
       </c>
@@ -3409,7 +3448,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>361</v>
       </c>
@@ -3438,7 +3477,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="62" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>361</v>
       </c>
@@ -3467,7 +3506,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>361</v>
       </c>
@@ -3496,7 +3535,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>361</v>
       </c>
@@ -3525,7 +3564,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>361</v>
       </c>
@@ -3554,7 +3593,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>361</v>
       </c>
@@ -3583,7 +3622,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="67" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>361</v>
       </c>
@@ -3612,7 +3651,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>361</v>
       </c>
@@ -3641,7 +3680,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>361</v>
       </c>
@@ -3670,7 +3709,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>361</v>
       </c>
@@ -3699,7 +3738,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="71" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>361</v>
       </c>
@@ -3728,7 +3767,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="72" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>361</v>
       </c>
@@ -3757,7 +3796,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="73" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>361</v>
       </c>
@@ -3786,7 +3825,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>361</v>
       </c>
@@ -3815,7 +3854,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="75" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>361</v>
       </c>
@@ -3844,7 +3883,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="76" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>361</v>
       </c>
@@ -3873,7 +3912,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="77" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>361</v>
       </c>
@@ -3902,7 +3941,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="78" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>361</v>
       </c>
@@ -3931,7 +3970,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="79" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>361</v>
       </c>
@@ -3960,7 +3999,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="80" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>361</v>
       </c>
@@ -3989,7 +4028,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>361</v>
       </c>
@@ -4018,7 +4057,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="82" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>361</v>
       </c>
@@ -4047,7 +4086,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="83" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>361</v>
       </c>
@@ -4076,7 +4115,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="84" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>361</v>
       </c>
@@ -4105,7 +4144,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="85" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>361</v>
       </c>
@@ -4134,7 +4173,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="86" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>361</v>
       </c>
@@ -4163,7 +4202,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="87" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>361</v>
       </c>
@@ -4189,7 +4228,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="88" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>361</v>
       </c>
@@ -4215,7 +4254,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="89" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>361</v>
       </c>
@@ -4241,7 +4280,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="90" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>361</v>
       </c>
@@ -4267,7 +4306,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="91" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>361</v>
       </c>
@@ -4296,7 +4335,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>361</v>
       </c>
@@ -4325,7 +4364,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>361</v>
       </c>
@@ -4354,7 +4393,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>361</v>
       </c>
@@ -4383,7 +4422,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>361</v>
       </c>
@@ -4415,7 +4454,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>361</v>
       </c>
@@ -4447,7 +4486,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>361</v>
       </c>
@@ -4476,7 +4515,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>361</v>
       </c>
@@ -4505,7 +4544,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="99" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>361</v>
       </c>
@@ -4537,7 +4576,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="100" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>361</v>
       </c>
@@ -4569,7 +4608,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="101" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>361</v>
       </c>
@@ -4598,7 +4637,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="102" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>361</v>
       </c>
@@ -4627,7 +4666,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>361</v>
       </c>
@@ -4656,7 +4695,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>361</v>
       </c>
@@ -4685,7 +4724,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>361</v>
       </c>
@@ -4714,7 +4753,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>361</v>
       </c>
@@ -4743,7 +4782,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="107" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>361</v>
       </c>
@@ -4772,7 +4811,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="108" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>361</v>
       </c>
@@ -4801,7 +4840,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="109" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>361</v>
       </c>
@@ -4833,7 +4872,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="110" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>361</v>
       </c>
@@ -4862,7 +4901,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="111" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>361</v>
       </c>
@@ -4891,7 +4930,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="112" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>361</v>
       </c>
@@ -4920,7 +4959,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="113" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>361</v>
       </c>
@@ -4952,7 +4991,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="114" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>361</v>
       </c>
@@ -4984,7 +5023,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="115" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>361</v>
       </c>
@@ -5013,7 +5052,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="116" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>361</v>
       </c>
@@ -5042,7 +5081,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>361</v>
       </c>
@@ -5071,7 +5110,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>361</v>
       </c>
@@ -5100,7 +5139,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="119" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>361</v>
       </c>
@@ -5132,7 +5171,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="120" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>361</v>
       </c>
@@ -5164,7 +5203,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="121" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>361</v>
       </c>
@@ -5193,7 +5232,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="122" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>361</v>
       </c>
@@ -5222,7 +5261,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="123" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>361</v>
       </c>
@@ -5251,7 +5290,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="124" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>361</v>
       </c>
@@ -5280,7 +5319,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>361</v>
       </c>
@@ -5309,7 +5348,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>361</v>
       </c>
@@ -5338,7 +5377,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>361</v>
       </c>
@@ -5370,7 +5409,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>361</v>
       </c>
@@ -5402,7 +5441,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>361</v>
       </c>
@@ -5434,7 +5473,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>361</v>
       </c>
@@ -5466,7 +5505,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>361</v>
       </c>
@@ -5495,7 +5534,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>361</v>
       </c>
@@ -5524,7 +5563,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>361</v>
       </c>
@@ -5553,7 +5592,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>361</v>
       </c>
@@ -5582,7 +5621,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>361</v>
       </c>
@@ -5611,7 +5650,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>361</v>
       </c>
@@ -5640,7 +5679,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>361</v>
       </c>
@@ -5669,7 +5708,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>361</v>
       </c>
@@ -5698,7 +5737,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>361</v>
       </c>
@@ -5730,7 +5769,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>361</v>
       </c>
@@ -5762,7 +5801,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>361</v>
       </c>
@@ -5791,7 +5830,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>361</v>
       </c>
@@ -5820,7 +5859,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>361</v>
       </c>
@@ -5849,7 +5888,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>361</v>
       </c>
@@ -5878,7 +5917,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>361</v>
       </c>
@@ -5910,7 +5949,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>361</v>
       </c>
@@ -5942,7 +5981,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>361</v>
       </c>
@@ -5971,7 +6010,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>361</v>
       </c>
@@ -6000,7 +6039,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>361</v>
       </c>
@@ -6026,7 +6065,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>361</v>
       </c>
@@ -6052,7 +6091,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>361</v>
       </c>
@@ -6081,7 +6120,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>361</v>
       </c>
@@ -6110,7 +6149,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>361</v>
       </c>
@@ -6136,7 +6175,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>361</v>
       </c>
@@ -6162,7 +6201,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>361</v>
       </c>
@@ -6188,7 +6227,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>361</v>
       </c>
@@ -6214,7 +6253,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>361</v>
       </c>
@@ -6240,7 +6279,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>361</v>
       </c>
@@ -6266,7 +6305,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>361</v>
       </c>
@@ -6292,7 +6331,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>361</v>
       </c>
@@ -6318,7 +6357,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>361</v>
       </c>
@@ -6344,7 +6383,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>361</v>
       </c>
@@ -6370,7 +6409,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>361</v>
       </c>
@@ -6396,7 +6435,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>361</v>
       </c>
@@ -6422,7 +6461,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>362</v>
       </c>
@@ -6448,7 +6487,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>362</v>
       </c>
@@ -6474,7 +6513,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>362</v>
       </c>
@@ -6500,7 +6539,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>362</v>
       </c>
@@ -6526,7 +6565,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>362</v>
       </c>
@@ -6552,7 +6591,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>362</v>
       </c>
@@ -6578,7 +6617,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>362</v>
       </c>
@@ -6604,7 +6643,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>362</v>
       </c>
@@ -6630,7 +6669,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>362</v>
       </c>
@@ -6656,7 +6695,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>362</v>
       </c>
@@ -6682,7 +6721,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>362</v>
       </c>
@@ -6708,7 +6747,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>362</v>
       </c>
@@ -6734,7 +6773,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>362</v>
       </c>
@@ -6760,7 +6799,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>362</v>
       </c>
@@ -6786,7 +6825,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>362</v>
       </c>
@@ -6812,7 +6851,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>362</v>
       </c>
@@ -6838,7 +6877,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>362</v>
       </c>
@@ -6864,7 +6903,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>362</v>
       </c>
@@ -6890,7 +6929,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>362</v>
       </c>
@@ -6916,7 +6955,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>362</v>
       </c>
@@ -6942,7 +6981,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>362</v>
       </c>
@@ -6968,7 +7007,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>362</v>
       </c>
@@ -6994,7 +7033,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>362</v>
       </c>
@@ -7020,7 +7059,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>362</v>
       </c>
@@ -7046,7 +7085,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>362</v>
       </c>
@@ -7072,7 +7111,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>362</v>
       </c>
@@ -7098,7 +7137,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>362</v>
       </c>
@@ -7124,7 +7163,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>362</v>
       </c>
@@ -7150,7 +7189,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>362</v>
       </c>
@@ -7176,7 +7215,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>362</v>
       </c>
@@ -7202,7 +7241,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>362</v>
       </c>
@@ -7228,7 +7267,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>362</v>
       </c>
@@ -7254,7 +7293,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>362</v>
       </c>
@@ -7280,7 +7319,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>362</v>
       </c>
@@ -7306,7 +7345,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>362</v>
       </c>
@@ -7332,7 +7371,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>362</v>
       </c>
@@ -7358,7 +7397,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>362</v>
       </c>
@@ -7384,7 +7423,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>362</v>
       </c>
@@ -7410,7 +7449,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>362</v>
       </c>
@@ -7436,7 +7475,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>362</v>
       </c>
@@ -7462,7 +7501,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>362</v>
       </c>
@@ -7488,7 +7527,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>362</v>
       </c>
@@ -7514,7 +7553,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>362</v>
       </c>
@@ -7540,7 +7579,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>362</v>
       </c>
@@ -7566,7 +7605,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>362</v>
       </c>
@@ -7592,7 +7631,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>362</v>
       </c>
@@ -7618,7 +7657,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>362</v>
       </c>
@@ -7644,7 +7683,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>362</v>
       </c>
@@ -7670,7 +7709,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>362</v>
       </c>
@@ -7696,7 +7735,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>362</v>
       </c>
@@ -7722,7 +7761,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>362</v>
       </c>
@@ -7748,7 +7787,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>362</v>
       </c>
@@ -7774,7 +7813,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>362</v>
       </c>
@@ -7800,7 +7839,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>362</v>
       </c>
@@ -7826,7 +7865,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>362</v>
       </c>
@@ -7852,7 +7891,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>362</v>
       </c>
@@ -7878,7 +7917,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>362</v>
       </c>
@@ -7904,7 +7943,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>362</v>
       </c>
@@ -7930,7 +7969,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>362</v>
       </c>
@@ -7956,7 +7995,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>362</v>
       </c>
@@ -7982,7 +8021,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>362</v>
       </c>
@@ -8008,7 +8047,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>362</v>
       </c>
@@ -8034,7 +8073,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>362</v>
       </c>
@@ -8060,7 +8099,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>362</v>
       </c>
@@ -8086,7 +8125,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>362</v>
       </c>
@@ -8112,7 +8151,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>362</v>
       </c>
@@ -8138,7 +8177,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>362</v>
       </c>
@@ -8164,7 +8203,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>362</v>
       </c>
@@ -8190,7 +8229,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>362</v>
       </c>
@@ -8216,7 +8255,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>362</v>
       </c>
@@ -8242,7 +8281,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>362</v>
       </c>
@@ -8268,7 +8307,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="236" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>362</v>
       </c>
@@ -8294,7 +8333,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>362</v>
       </c>
@@ -8320,7 +8359,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="238" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>362</v>
       </c>
@@ -8346,7 +8385,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="239" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>362</v>
       </c>
@@ -8372,7 +8411,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="240" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>362</v>
       </c>
@@ -8398,7 +8437,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="241" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>362</v>
       </c>
@@ -8424,7 +8463,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="242" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>362</v>
       </c>
@@ -8450,7 +8489,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="243" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>362</v>
       </c>
@@ -8476,7 +8515,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="244" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>362</v>
       </c>
@@ -8502,7 +8541,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="245" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>362</v>
       </c>
@@ -8528,7 +8567,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="246" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>362</v>
       </c>
@@ -8554,7 +8593,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="247" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>362</v>
       </c>
@@ -8580,7 +8619,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="248" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>362</v>
       </c>
@@ -8606,7 +8645,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="249" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>362</v>
       </c>
@@ -8632,7 +8671,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="250" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>362</v>
       </c>
@@ -8658,7 +8697,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="251" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>362</v>
       </c>
@@ -8684,7 +8723,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="252" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>362</v>
       </c>
@@ -8710,7 +8749,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="253" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>362</v>
       </c>
@@ -8736,7 +8775,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="254" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>362</v>
       </c>
@@ -8762,7 +8801,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="255" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>362</v>
       </c>
@@ -8788,7 +8827,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="256" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>362</v>
       </c>
@@ -8814,7 +8853,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="257" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>362</v>
       </c>
@@ -8840,7 +8879,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="258" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>362</v>
       </c>
@@ -8866,7 +8905,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="259" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>362</v>
       </c>
@@ -8892,7 +8931,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="260" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>362</v>
       </c>
@@ -8918,7 +8957,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="261" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>362</v>
       </c>
@@ -8944,7 +8983,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="262" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>362</v>
       </c>
@@ -8970,7 +9009,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="263" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>362</v>
       </c>
@@ -8996,7 +9035,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="264" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>362</v>
       </c>
@@ -9022,7 +9061,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="265" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>362</v>
       </c>
@@ -9048,7 +9087,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="266" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>362</v>
       </c>
@@ -9074,7 +9113,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="267" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>362</v>
       </c>
@@ -9100,7 +9139,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="268" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>362</v>
       </c>
@@ -9126,7 +9165,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="269" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>362</v>
       </c>
@@ -9152,7 +9191,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="270" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>362</v>
       </c>
@@ -9178,7 +9217,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="271" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>362</v>
       </c>
@@ -9204,7 +9243,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="272" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>362</v>
       </c>
@@ -9230,7 +9269,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="273" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>362</v>
       </c>
@@ -9256,7 +9295,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="274" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>362</v>
       </c>
@@ -9282,7 +9321,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="275" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>362</v>
       </c>
@@ -9308,7 +9347,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="276" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>362</v>
       </c>
@@ -9334,7 +9373,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="277" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>362</v>
       </c>
@@ -9360,7 +9399,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="278" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>362</v>
       </c>
@@ -9386,7 +9425,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="279" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>362</v>
       </c>
@@ -9412,7 +9451,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="280" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>362</v>
       </c>
@@ -9438,7 +9477,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="281" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>362</v>
       </c>
@@ -9464,7 +9503,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="282" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>362</v>
       </c>
@@ -9490,7 +9529,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="283" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>362</v>
       </c>
@@ -9516,7 +9555,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="284" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>362</v>
       </c>
@@ -9542,7 +9581,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="285" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>362</v>
       </c>
@@ -9568,7 +9607,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="286" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>362</v>
       </c>
@@ -9594,7 +9633,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="287" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>362</v>
       </c>
@@ -9620,7 +9659,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="288" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>362</v>
       </c>
@@ -9646,7 +9685,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="289" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>362</v>
       </c>
@@ -9672,7 +9711,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="290" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>362</v>
       </c>
@@ -9698,7 +9737,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="291" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>362</v>
       </c>
@@ -9724,7 +9763,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="292" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>362</v>
       </c>
@@ -9750,7 +9789,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="293" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>362</v>
       </c>
@@ -9776,7 +9815,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="294" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>362</v>
       </c>
@@ -9802,7 +9841,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="295" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>362</v>
       </c>
@@ -9828,7 +9867,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="296" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>362</v>
       </c>
@@ -9854,7 +9893,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="297" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>362</v>
       </c>
@@ -9880,7 +9919,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="298" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>362</v>
       </c>
@@ -9906,7 +9945,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="299" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>362</v>
       </c>
@@ -9932,7 +9971,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="300" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>362</v>
       </c>
@@ -9958,7 +9997,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="301" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>362</v>
       </c>
@@ -9984,7 +10023,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="302" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>362</v>
       </c>
@@ -10010,7 +10049,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="303" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>362</v>
       </c>
@@ -10036,7 +10075,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="304" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>362</v>
       </c>
@@ -10062,7 +10101,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="305" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>362</v>
       </c>
@@ -10088,7 +10127,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="306" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>362</v>
       </c>
@@ -10114,7 +10153,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="307" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>362</v>
       </c>
@@ -10140,7 +10179,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="308" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>362</v>
       </c>
@@ -10166,7 +10205,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="309" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>362</v>
       </c>
@@ -10192,7 +10231,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="310" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>362</v>
       </c>
@@ -10218,7 +10257,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="311" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>362</v>
       </c>
@@ -10244,7 +10283,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="312" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>362</v>
       </c>
@@ -10270,7 +10309,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="313" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>362</v>
       </c>
@@ -10296,7 +10335,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="314" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>362</v>
       </c>
@@ -10322,7 +10361,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="315" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>362</v>
       </c>
@@ -10348,7 +10387,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="316" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>362</v>
       </c>
@@ -10374,7 +10413,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="317" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>362</v>
       </c>
@@ -10400,7 +10439,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="318" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>362</v>
       </c>
@@ -10426,7 +10465,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="319" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>362</v>
       </c>
@@ -10452,7 +10491,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="320" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>362</v>
       </c>
@@ -10478,7 +10517,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="321" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>362</v>
       </c>
@@ -10504,7 +10543,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="322" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>362</v>
       </c>
@@ -10530,7 +10569,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="323" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>362</v>
       </c>
@@ -10556,7 +10595,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="324" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
         <v>362</v>
       </c>
@@ -10582,7 +10621,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="325" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
         <v>362</v>
       </c>
@@ -10608,7 +10647,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="326" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
         <v>362</v>
       </c>
@@ -10634,7 +10673,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="327" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>362</v>
       </c>
@@ -10660,7 +10699,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="328" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>362</v>
       </c>
@@ -10686,7 +10725,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="329" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="329" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>362</v>
       </c>
@@ -10712,7 +10751,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="330" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>362</v>
       </c>
@@ -10738,7 +10777,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="331" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="331" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>362</v>
       </c>
@@ -10764,7 +10803,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="332" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="332" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
         <v>362</v>
       </c>
@@ -10781,7 +10820,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="333" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="333" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>362</v>
       </c>
@@ -10798,7 +10837,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="334" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="334" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
         <v>362</v>
       </c>
@@ -10815,7 +10854,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="335" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="335" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
         <v>362</v>
       </c>
@@ -10832,7 +10871,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="336" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="336" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
         <v>362</v>
       </c>
@@ -10849,7 +10888,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="337" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="337" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
         <v>362</v>
       </c>
@@ -10866,7 +10905,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="338" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="338" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>362</v>
       </c>
@@ -10883,7 +10922,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="339" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="339" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>362</v>
       </c>
@@ -10900,7 +10939,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="340" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="340" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
         <v>362</v>
       </c>
@@ -10917,7 +10956,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="341" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="341" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
         <v>362</v>
       </c>
@@ -10934,7 +10973,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="342" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="342" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
         <v>362</v>
       </c>
@@ -10951,7 +10990,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="343" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="343" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
         <v>362</v>
       </c>
@@ -10968,7 +11007,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="344" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="344" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
         <v>362</v>
       </c>
@@ -10985,7 +11024,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="345" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="345" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
         <v>362</v>
       </c>
@@ -11002,7 +11041,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="346" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="346" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>362</v>
       </c>
@@ -11019,7 +11058,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="347" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="347" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
         <v>362</v>
       </c>
@@ -11036,7 +11075,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="348" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="348" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
         <v>362</v>
       </c>
@@ -11053,7 +11092,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="349" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="349" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
         <v>362</v>
       </c>
@@ -11070,7 +11109,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="350" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="350" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>362</v>
       </c>
@@ -11087,7 +11126,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="351" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="351" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
         <v>362</v>
       </c>
@@ -11104,7 +11143,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="352" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="352" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
         <v>362</v>
       </c>
@@ -11121,7 +11160,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="353" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="353" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
         <v>362</v>
       </c>
@@ -11138,7 +11177,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="354" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="354" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
         <v>362</v>
       </c>
@@ -11155,7 +11194,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="355" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="355" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
         <v>362</v>
       </c>
@@ -11172,7 +11211,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="356" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="356" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
         <v>362</v>
       </c>
@@ -11189,7 +11228,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="357" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="357" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
         <v>362</v>
       </c>
@@ -11206,7 +11245,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="358" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="358" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
         <v>362</v>
       </c>
@@ -11223,7 +11262,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="359" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="359" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
         <v>362</v>
       </c>
@@ -11240,7 +11279,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="360" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="360" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
         <v>362</v>
       </c>
@@ -11257,7 +11296,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="361" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="361" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
         <v>362</v>
       </c>
@@ -11274,7 +11313,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="362" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="362" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
         <v>362</v>
       </c>
@@ -11291,7 +11330,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="363" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="363" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
         <v>362</v>
       </c>
@@ -11308,7 +11347,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="364" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="364" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
         <v>362</v>
       </c>
@@ -11325,7 +11364,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="365" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="365" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
         <v>362</v>
       </c>
@@ -11342,7 +11381,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="366" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="366" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
         <v>362</v>
       </c>
@@ -11359,7 +11398,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="367" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="367" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
         <v>362</v>
       </c>
@@ -11376,7 +11415,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="368" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="368" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
         <v>362</v>
       </c>
@@ -11393,7 +11432,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="369" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="369" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
         <v>362</v>
       </c>
@@ -11410,7 +11449,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="370" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="370" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
         <v>362</v>
       </c>
@@ -11427,7 +11466,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="371" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="371" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
         <v>362</v>
       </c>
@@ -11444,7 +11483,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="372" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="372" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
         <v>362</v>
       </c>
@@ -11461,7 +11500,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="373" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="373" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
         <v>362</v>
       </c>
@@ -11478,7 +11517,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="374" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="374" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
         <v>362</v>
       </c>
@@ -11495,7 +11534,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="375" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="375" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
         <v>362</v>
       </c>
@@ -11512,7 +11551,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="376" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="376" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
         <v>362</v>
       </c>
@@ -11529,7 +11568,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="377" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="377" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
         <v>362</v>
       </c>
@@ -11546,7 +11585,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="378" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="378" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
         <v>362</v>
       </c>
@@ -11563,7 +11602,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="379" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="379" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
         <v>362</v>
       </c>
@@ -11580,7 +11619,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="380" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="380" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
         <v>362</v>
       </c>
@@ -11597,7 +11636,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="381" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="381" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
         <v>362</v>
       </c>
@@ -11614,7 +11653,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="382" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="382" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
         <v>362</v>
       </c>
@@ -11631,7 +11670,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="383" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="383" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
         <v>362</v>
       </c>
@@ -11648,7 +11687,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="384" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="384" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
         <v>362</v>
       </c>
@@ -11665,7 +11704,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="385" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="385" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
         <v>362</v>
       </c>
@@ -11682,7 +11721,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="386" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="386" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
         <v>362</v>
       </c>
@@ -11699,7 +11738,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="387" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="387" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
         <v>362</v>
       </c>
@@ -11716,7 +11755,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="388" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="388" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
         <v>362</v>
       </c>
@@ -11733,7 +11772,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="389" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="389" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
         <v>362</v>
       </c>
@@ -11750,7 +11789,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="390" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="390" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
         <v>362</v>
       </c>
@@ -11767,7 +11806,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="391" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="391" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
         <v>362</v>
       </c>
@@ -11784,7 +11823,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="392" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="392" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
         <v>362</v>
       </c>
@@ -11801,7 +11840,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="393" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="393" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
         <v>362</v>
       </c>
@@ -11818,7 +11857,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="394" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="394" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
         <v>362</v>
       </c>
@@ -11835,7 +11874,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="395" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="395" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
         <v>362</v>
       </c>
@@ -11852,7 +11891,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="396" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="396" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
         <v>362</v>
       </c>
@@ -11869,7 +11908,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="397" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="397" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
         <v>362</v>
       </c>
@@ -11886,7 +11925,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="398" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="398" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
         <v>362</v>
       </c>
@@ -11903,7 +11942,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="399" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="399" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
         <v>362</v>
       </c>
@@ -11920,7 +11959,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="400" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="400" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
         <v>362</v>
       </c>
@@ -11937,7 +11976,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="401" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="401" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
         <v>362</v>
       </c>
@@ -11954,7 +11993,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="402" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="402" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
         <v>362</v>
       </c>
@@ -11971,7 +12010,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="403" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="403" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
         <v>362</v>
       </c>
@@ -11988,7 +12027,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="404" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="404" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
         <v>362</v>
       </c>
@@ -12005,7 +12044,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="405" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="405" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
         <v>362</v>
       </c>
@@ -12022,7 +12061,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="406" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="406" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
         <v>362</v>
       </c>
@@ -12039,7 +12078,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="407" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="407" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
         <v>362</v>
       </c>
@@ -12056,7 +12095,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="408" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="408" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
         <v>362</v>
       </c>
@@ -12073,7 +12112,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="409" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="409" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
         <v>362</v>
       </c>
@@ -12090,7 +12129,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="410" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="410" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
         <v>362</v>
       </c>
@@ -12107,7 +12146,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="411" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="411" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
         <v>362</v>
       </c>
@@ -12124,7 +12163,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="412" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="412" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
         <v>362</v>
       </c>
@@ -12141,7 +12180,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="413" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="413" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
         <v>362</v>
       </c>
@@ -12158,7 +12197,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="414" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="414" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
         <v>362</v>
       </c>
@@ -12175,7 +12214,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="415" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="415" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
         <v>362</v>
       </c>
@@ -12192,7 +12231,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="416" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="416" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
         <v>362</v>
       </c>
@@ -12209,7 +12248,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="417" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="417" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
         <v>362</v>
       </c>
@@ -12226,7 +12265,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="418" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="418" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
         <v>362</v>
       </c>
@@ -12243,7 +12282,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="419" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="419" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
         <v>362</v>
       </c>
@@ -12260,7 +12299,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="420" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="420" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
         <v>362</v>
       </c>
@@ -12277,7 +12316,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="421" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="421" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
         <v>362</v>
       </c>
@@ -12294,7 +12333,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="422" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="422" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
         <v>362</v>
       </c>
@@ -12311,7 +12350,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="423" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="423" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
         <v>362</v>
       </c>
@@ -12328,7 +12367,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="424" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="424" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
         <v>362</v>
       </c>
@@ -12345,7 +12384,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="425" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="425" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
         <v>362</v>
       </c>
@@ -12362,7 +12401,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="426" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="426" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
         <v>362</v>
       </c>
@@ -12379,7 +12418,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="427" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="427" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
         <v>362</v>
       </c>
@@ -12396,7 +12435,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="428" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="428" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
         <v>362</v>
       </c>
@@ -12413,7 +12452,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="429" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="429" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
         <v>362</v>
       </c>
@@ -12430,7 +12469,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="430" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="430" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
         <v>362</v>
       </c>
@@ -12447,7 +12486,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="431" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="431" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A431" t="s">
         <v>362</v>
       </c>
@@ -12464,7 +12503,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="432" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="432" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A432" t="s">
         <v>362</v>
       </c>
@@ -12481,7 +12520,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="433" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="433" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
         <v>362</v>
       </c>
@@ -12498,7 +12537,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="434" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="434" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A434" t="s">
         <v>362</v>
       </c>
@@ -12515,7 +12554,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="435" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="435" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
         <v>362</v>
       </c>
@@ -12532,7 +12571,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="436" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="436" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
         <v>362</v>
       </c>
@@ -12549,7 +12588,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="437" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="437" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A437" t="s">
         <v>362</v>
       </c>
@@ -12566,7 +12605,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="438" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="438" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A438" t="s">
         <v>362</v>
       </c>
@@ -12583,7 +12622,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="439" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="439" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A439" t="s">
         <v>362</v>
       </c>
@@ -12600,7 +12639,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="440" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="440" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A440" t="s">
         <v>362</v>
       </c>
@@ -12617,7 +12656,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="441" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="441" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A441" t="s">
         <v>362</v>
       </c>
@@ -12634,7 +12673,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="442" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="442" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A442" t="s">
         <v>362</v>
       </c>
@@ -12651,7 +12690,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="443" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="443" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A443" t="s">
         <v>362</v>
       </c>
@@ -12666,6 +12705,345 @@
       </c>
       <c r="J443" t="s">
         <v>404</v>
+      </c>
+    </row>
+    <row r="444" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A444" t="s">
+        <v>446</v>
+      </c>
+      <c r="B444" t="s">
+        <v>434</v>
+      </c>
+      <c r="C444">
+        <v>2740</v>
+      </c>
+      <c r="E444" t="s">
+        <v>16</v>
+      </c>
+      <c r="F444">
+        <v>45</v>
+      </c>
+      <c r="G444">
+        <v>5</v>
+      </c>
+      <c r="H444">
+        <v>0.03</v>
+      </c>
+      <c r="I444" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J444" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="445" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A445" t="s">
+        <v>446</v>
+      </c>
+      <c r="B445" t="s">
+        <v>435</v>
+      </c>
+      <c r="C445">
+        <v>2770</v>
+      </c>
+      <c r="E445" t="s">
+        <v>16</v>
+      </c>
+      <c r="F445">
+        <v>45</v>
+      </c>
+      <c r="G445">
+        <v>5</v>
+      </c>
+      <c r="H445">
+        <v>0.03</v>
+      </c>
+      <c r="I445" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J445" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="446" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A446" t="s">
+        <v>446</v>
+      </c>
+      <c r="B446" t="s">
+        <v>436</v>
+      </c>
+      <c r="C446">
+        <v>2830</v>
+      </c>
+      <c r="E446" t="s">
+        <v>16</v>
+      </c>
+      <c r="F446">
+        <v>45</v>
+      </c>
+      <c r="G446">
+        <v>5</v>
+      </c>
+      <c r="H446">
+        <v>0.03</v>
+      </c>
+      <c r="I446" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J446" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="447" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A447" t="s">
+        <v>446</v>
+      </c>
+      <c r="B447" t="s">
+        <v>437</v>
+      </c>
+      <c r="C447">
+        <v>2810</v>
+      </c>
+      <c r="E447" t="s">
+        <v>16</v>
+      </c>
+      <c r="F447">
+        <v>45</v>
+      </c>
+      <c r="G447">
+        <v>5</v>
+      </c>
+      <c r="H447">
+        <v>0.03</v>
+      </c>
+      <c r="I447" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J447" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="448" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A448" t="s">
+        <v>446</v>
+      </c>
+      <c r="B448" t="s">
+        <v>438</v>
+      </c>
+      <c r="C448">
+        <v>2340</v>
+      </c>
+      <c r="E448" t="s">
+        <v>16</v>
+      </c>
+      <c r="F448">
+        <v>45</v>
+      </c>
+      <c r="G448">
+        <v>5</v>
+      </c>
+      <c r="H448">
+        <v>0.03</v>
+      </c>
+      <c r="I448" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J448" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="449" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A449" t="s">
+        <v>446</v>
+      </c>
+      <c r="B449" t="s">
+        <v>439</v>
+      </c>
+      <c r="C449">
+        <v>2320</v>
+      </c>
+      <c r="E449" t="s">
+        <v>16</v>
+      </c>
+      <c r="F449">
+        <v>45</v>
+      </c>
+      <c r="G449">
+        <v>5</v>
+      </c>
+      <c r="H449">
+        <v>0.03</v>
+      </c>
+      <c r="I449" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J449" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="450" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A450" t="s">
+        <v>446</v>
+      </c>
+      <c r="B450" t="s">
+        <v>440</v>
+      </c>
+      <c r="C450">
+        <v>2370</v>
+      </c>
+      <c r="E450" t="s">
+        <v>16</v>
+      </c>
+      <c r="F450">
+        <v>45</v>
+      </c>
+      <c r="G450">
+        <v>5</v>
+      </c>
+      <c r="H450">
+        <v>0.03</v>
+      </c>
+      <c r="I450" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J450" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="451" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A451" t="s">
+        <v>446</v>
+      </c>
+      <c r="B451" t="s">
+        <v>441</v>
+      </c>
+      <c r="C451">
+        <v>2450</v>
+      </c>
+      <c r="E451" t="s">
+        <v>16</v>
+      </c>
+      <c r="F451">
+        <v>45</v>
+      </c>
+      <c r="G451">
+        <v>5</v>
+      </c>
+      <c r="H451">
+        <v>0.03</v>
+      </c>
+      <c r="I451" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J451" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="452" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A452" t="s">
+        <v>446</v>
+      </c>
+      <c r="B452" t="s">
+        <v>442</v>
+      </c>
+      <c r="C452">
+        <v>2420</v>
+      </c>
+      <c r="E452" t="s">
+        <v>16</v>
+      </c>
+      <c r="F452">
+        <v>45</v>
+      </c>
+      <c r="G452">
+        <v>5</v>
+      </c>
+      <c r="H452">
+        <v>0.03</v>
+      </c>
+      <c r="I452" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J452" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="453" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A453" t="s">
+        <v>446</v>
+      </c>
+      <c r="B453" t="s">
+        <v>443</v>
+      </c>
+      <c r="C453">
+        <v>2120</v>
+      </c>
+      <c r="F453">
+        <v>45</v>
+      </c>
+      <c r="G453">
+        <v>5</v>
+      </c>
+      <c r="H453">
+        <v>0.03</v>
+      </c>
+      <c r="I453" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J453" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="454" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A454" t="s">
+        <v>446</v>
+      </c>
+      <c r="B454" t="s">
+        <v>444</v>
+      </c>
+      <c r="C454">
+        <v>2130</v>
+      </c>
+      <c r="F454">
+        <v>45</v>
+      </c>
+      <c r="G454">
+        <v>5</v>
+      </c>
+      <c r="H454">
+        <v>0.03</v>
+      </c>
+      <c r="I454" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J454" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="455" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A455" t="s">
+        <v>446</v>
+      </c>
+      <c r="B455" t="s">
+        <v>445</v>
+      </c>
+      <c r="C455">
+        <v>2230</v>
+      </c>
+      <c r="F455">
+        <v>45</v>
+      </c>
+      <c r="G455">
+        <v>5</v>
+      </c>
+      <c r="H455">
+        <v>0.03</v>
+      </c>
+      <c r="I455" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J455" t="e">
+        <v>#N/A</v>
       </c>
     </row>
   </sheetData>
@@ -12686,18 +13064,18 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>324</v>
       </c>
@@ -12705,7 +13083,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>328</v>
       </c>
@@ -12713,7 +13091,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>323</v>
       </c>

</xml_diff>

<commit_message>
Added tollclass values for projects EXP_SC_101_Dunne_to_SR25 and EXP_SL_I80_I505_to_Yolo
Added values and project names.
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/TOLLCLASS_Designations.xlsx
+++ b/utilities/NextGenFwys/TOLLCLASS_Designations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\llin\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sisrael\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17D6660E-2628-4896-A935-7F084BAF6E6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{846F2A70-62FB-4BB4-A26F-0AA9CA49CD09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9180" yWindow="0" windowWidth="16725" windowHeight="15600" xr2:uid="{0F0A9957-56E7-4C48-967B-2AB2A1965C2F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{0F0A9957-56E7-4C48-967B-2AB2A1965C2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs_for_tollcalib" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1674" uniqueCount="473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1687" uniqueCount="479">
   <si>
     <t>SR92 SM - I-280 Interchange to US101 Interchange - WB</t>
   </si>
@@ -1458,6 +1458,24 @@
   </si>
   <si>
     <t>SCL_85_SB</t>
+  </si>
+  <si>
+    <t>US101 - SR25 to Dunne - NB</t>
+  </si>
+  <si>
+    <t>US101 - SR25 to Dunne - SB</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>EXP_SC_101_Dunne_to_SR25</t>
+  </si>
+  <si>
+    <t>I-80 - I-505 to Yolo County Line - EB</t>
+  </si>
+  <si>
+    <t>EXP_SL_I80_I505_to_Yolo</t>
   </si>
 </sst>
 </file>
@@ -1562,9 +1580,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1602,7 +1620,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1708,7 +1726,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1850,7 +1868,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1861,26 +1879,26 @@
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
-  <dimension ref="A1:J461"/>
+  <dimension ref="A1:K465"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A407" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D427" sqref="D427"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A440" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J466" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
-    <col min="2" max="2" width="79.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" customWidth="1"/>
+    <col min="2" max="2" width="79.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.81640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.140625" customWidth="1"/>
-    <col min="10" max="10" width="24.42578125" customWidth="1"/>
-    <col min="11" max="11" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.1796875" customWidth="1"/>
+    <col min="10" max="10" width="24.453125" customWidth="1"/>
+    <col min="11" max="11" width="23.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>336</v>
       </c>
@@ -1911,8 +1929,11 @@
       <c r="J1" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" s="2" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>360</v>
       </c>
@@ -1929,7 +1950,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>360</v>
       </c>
@@ -1946,7 +1967,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>360</v>
       </c>
@@ -1963,7 +1984,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>360</v>
       </c>
@@ -1980,7 +2001,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>360</v>
       </c>
@@ -1997,7 +2018,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>360</v>
       </c>
@@ -2014,7 +2035,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>360</v>
       </c>
@@ -2031,7 +2052,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>360</v>
       </c>
@@ -2048,7 +2069,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>361</v>
       </c>
@@ -2065,7 +2086,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>361</v>
       </c>
@@ -2091,7 +2112,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>362</v>
       </c>
@@ -2117,7 +2138,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>362</v>
       </c>
@@ -2143,7 +2164,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>362</v>
       </c>
@@ -2170,7 +2191,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>361</v>
       </c>
@@ -2199,7 +2220,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>361</v>
       </c>
@@ -2228,7 +2249,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>361</v>
       </c>
@@ -2257,7 +2278,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>361</v>
       </c>
@@ -2286,7 +2307,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>361</v>
       </c>
@@ -2315,7 +2336,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>361</v>
       </c>
@@ -2344,7 +2365,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>361</v>
       </c>
@@ -2376,7 +2397,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>361</v>
       </c>
@@ -2408,7 +2429,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>361</v>
       </c>
@@ -2440,7 +2461,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>361</v>
       </c>
@@ -2472,7 +2493,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>361</v>
       </c>
@@ -2504,7 +2525,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>361</v>
       </c>
@@ -2536,7 +2557,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>361</v>
       </c>
@@ -2568,7 +2589,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>361</v>
       </c>
@@ -2600,7 +2621,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>361</v>
       </c>
@@ -2632,7 +2653,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>361</v>
       </c>
@@ -2664,7 +2685,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>361</v>
       </c>
@@ -2696,7 +2717,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>361</v>
       </c>
@@ -2728,7 +2749,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>361</v>
       </c>
@@ -2757,7 +2778,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>361</v>
       </c>
@@ -2786,7 +2807,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>361</v>
       </c>
@@ -2818,7 +2839,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>361</v>
       </c>
@@ -2850,7 +2871,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>361</v>
       </c>
@@ -2882,7 +2903,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>361</v>
       </c>
@@ -2914,7 +2935,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>361</v>
       </c>
@@ -2946,7 +2967,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>361</v>
       </c>
@@ -2978,7 +2999,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>361</v>
       </c>
@@ -3007,7 +3028,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>361</v>
       </c>
@@ -3036,7 +3057,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>361</v>
       </c>
@@ -3065,7 +3086,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>361</v>
       </c>
@@ -3094,7 +3115,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>361</v>
       </c>
@@ -3123,7 +3144,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>361</v>
       </c>
@@ -3152,7 +3173,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>361</v>
       </c>
@@ -3181,7 +3202,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>361</v>
       </c>
@@ -3210,7 +3231,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>361</v>
       </c>
@@ -3239,7 +3260,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>361</v>
       </c>
@@ -3268,7 +3289,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>361</v>
       </c>
@@ -3300,7 +3321,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>361</v>
       </c>
@@ -3332,7 +3353,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>361</v>
       </c>
@@ -3364,7 +3385,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>361</v>
       </c>
@@ -3396,7 +3417,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>361</v>
       </c>
@@ -3428,7 +3449,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>361</v>
       </c>
@@ -3460,7 +3481,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>361</v>
       </c>
@@ -3489,7 +3510,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>361</v>
       </c>
@@ -3518,7 +3539,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>361</v>
       </c>
@@ -3547,7 +3568,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>361</v>
       </c>
@@ -3576,7 +3597,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>361</v>
       </c>
@@ -3605,7 +3626,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="62" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>361</v>
       </c>
@@ -3634,7 +3655,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>361</v>
       </c>
@@ -3660,7 +3681,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>361</v>
       </c>
@@ -3686,7 +3707,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>361</v>
       </c>
@@ -3712,7 +3733,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>361</v>
       </c>
@@ -3738,7 +3759,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="67" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>361</v>
       </c>
@@ -3767,7 +3788,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>361</v>
       </c>
@@ -3796,7 +3817,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>361</v>
       </c>
@@ -3825,7 +3846,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>361</v>
       </c>
@@ -3854,7 +3875,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="71" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>361</v>
       </c>
@@ -3883,7 +3904,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="72" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>361</v>
       </c>
@@ -3912,7 +3933,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="73" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>361</v>
       </c>
@@ -3941,7 +3962,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>361</v>
       </c>
@@ -3970,7 +3991,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="75" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>361</v>
       </c>
@@ -3999,7 +4020,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="76" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>361</v>
       </c>
@@ -4028,7 +4049,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="77" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>361</v>
       </c>
@@ -4057,7 +4078,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="78" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>361</v>
       </c>
@@ -4086,7 +4107,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="79" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>361</v>
       </c>
@@ -4112,7 +4133,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="80" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>361</v>
       </c>
@@ -4138,7 +4159,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>361</v>
       </c>
@@ -4170,7 +4191,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="82" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>361</v>
       </c>
@@ -4202,7 +4223,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="83" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>361</v>
       </c>
@@ -4231,7 +4252,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="84" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>361</v>
       </c>
@@ -4260,7 +4281,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="85" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>361</v>
       </c>
@@ -4292,7 +4313,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="86" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>361</v>
       </c>
@@ -4324,7 +4345,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="87" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>361</v>
       </c>
@@ -4356,7 +4377,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="88" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>361</v>
       </c>
@@ -4388,7 +4409,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="89" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>361</v>
       </c>
@@ -4414,7 +4435,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="90" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>361</v>
       </c>
@@ -4440,7 +4461,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="91" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>361</v>
       </c>
@@ -4469,7 +4490,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>361</v>
       </c>
@@ -4498,7 +4519,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>361</v>
       </c>
@@ -4530,7 +4551,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>361</v>
       </c>
@@ -4562,7 +4583,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>361</v>
       </c>
@@ -4591,7 +4612,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>361</v>
       </c>
@@ -4620,7 +4641,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>361</v>
       </c>
@@ -4646,7 +4667,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>361</v>
       </c>
@@ -4672,7 +4693,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="99" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>361</v>
       </c>
@@ -4698,7 +4719,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="100" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>361</v>
       </c>
@@ -4724,7 +4745,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="101" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>361</v>
       </c>
@@ -4756,7 +4777,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="102" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>361</v>
       </c>
@@ -4788,7 +4809,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>361</v>
       </c>
@@ -4820,7 +4841,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>361</v>
       </c>
@@ -4852,7 +4873,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>361</v>
       </c>
@@ -4884,7 +4905,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>361</v>
       </c>
@@ -4916,7 +4937,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="107" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>361</v>
       </c>
@@ -4945,7 +4966,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="108" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>361</v>
       </c>
@@ -4974,7 +4995,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="109" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>361</v>
       </c>
@@ -5006,7 +5027,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="110" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>361</v>
       </c>
@@ -5038,7 +5059,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="111" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>361</v>
       </c>
@@ -5067,7 +5088,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="112" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>361</v>
       </c>
@@ -5096,7 +5117,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="113" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>361</v>
       </c>
@@ -5125,7 +5146,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="114" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>361</v>
       </c>
@@ -5154,7 +5175,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="115" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>361</v>
       </c>
@@ -5183,7 +5204,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="116" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>361</v>
       </c>
@@ -5212,7 +5233,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>361</v>
       </c>
@@ -5244,7 +5265,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>361</v>
       </c>
@@ -5273,7 +5294,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="119" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>361</v>
       </c>
@@ -5305,7 +5326,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="120" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>361</v>
       </c>
@@ -5334,7 +5355,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="121" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>361</v>
       </c>
@@ -5363,7 +5384,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="122" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>361</v>
       </c>
@@ -5392,7 +5413,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="123" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>361</v>
       </c>
@@ -5424,7 +5445,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="124" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>361</v>
       </c>
@@ -5456,7 +5477,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>361</v>
       </c>
@@ -5485,7 +5506,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>361</v>
       </c>
@@ -5514,7 +5535,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>361</v>
       </c>
@@ -5546,7 +5567,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>361</v>
       </c>
@@ -5575,7 +5596,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>361</v>
       </c>
@@ -5604,7 +5625,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>361</v>
       </c>
@@ -5636,7 +5657,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>361</v>
       </c>
@@ -5665,7 +5686,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>361</v>
       </c>
@@ -5694,7 +5715,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>361</v>
       </c>
@@ -5726,7 +5747,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>361</v>
       </c>
@@ -5758,7 +5779,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>361</v>
       </c>
@@ -5790,7 +5811,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>361</v>
       </c>
@@ -5822,7 +5843,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>361</v>
       </c>
@@ -5854,7 +5875,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>361</v>
       </c>
@@ -5886,7 +5907,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>361</v>
       </c>
@@ -5918,7 +5939,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>361</v>
       </c>
@@ -5950,7 +5971,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>361</v>
       </c>
@@ -5979,7 +6000,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>361</v>
       </c>
@@ -6008,7 +6029,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>361</v>
       </c>
@@ -6040,7 +6061,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>361</v>
       </c>
@@ -6069,7 +6090,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>361</v>
       </c>
@@ -6098,7 +6119,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>361</v>
       </c>
@@ -6127,7 +6148,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>361</v>
       </c>
@@ -6156,7 +6177,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>361</v>
       </c>
@@ -6185,7 +6206,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>361</v>
       </c>
@@ -6214,7 +6235,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>361</v>
       </c>
@@ -6243,7 +6264,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>361</v>
       </c>
@@ -6275,7 +6296,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>361</v>
       </c>
@@ -6307,7 +6328,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>361</v>
       </c>
@@ -6336,7 +6357,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>361</v>
       </c>
@@ -6365,7 +6386,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>361</v>
       </c>
@@ -6394,7 +6415,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>361</v>
       </c>
@@ -6426,7 +6447,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>361</v>
       </c>
@@ -6455,7 +6476,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>361</v>
       </c>
@@ -6484,7 +6505,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>361</v>
       </c>
@@ -6513,7 +6534,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>361</v>
       </c>
@@ -6542,7 +6563,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>361</v>
       </c>
@@ -6568,7 +6589,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>361</v>
       </c>
@@ -6594,7 +6615,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>361</v>
       </c>
@@ -6620,7 +6641,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>361</v>
       </c>
@@ -6646,7 +6667,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>362</v>
       </c>
@@ -6672,7 +6693,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>362</v>
       </c>
@@ -6698,7 +6719,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>362</v>
       </c>
@@ -6724,7 +6745,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>362</v>
       </c>
@@ -6750,7 +6771,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>362</v>
       </c>
@@ -6776,7 +6797,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>362</v>
       </c>
@@ -6802,7 +6823,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>362</v>
       </c>
@@ -6828,7 +6849,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>362</v>
       </c>
@@ -6854,7 +6875,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>362</v>
       </c>
@@ -6880,7 +6901,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>362</v>
       </c>
@@ -6906,7 +6927,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>362</v>
       </c>
@@ -6932,7 +6953,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>362</v>
       </c>
@@ -6958,7 +6979,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>362</v>
       </c>
@@ -6984,7 +7005,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>362</v>
       </c>
@@ -7010,7 +7031,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>362</v>
       </c>
@@ -7036,7 +7057,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>362</v>
       </c>
@@ -7062,7 +7083,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>362</v>
       </c>
@@ -7088,7 +7109,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>362</v>
       </c>
@@ -7114,7 +7135,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>362</v>
       </c>
@@ -7140,7 +7161,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>362</v>
       </c>
@@ -7166,7 +7187,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>362</v>
       </c>
@@ -7183,7 +7204,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>362</v>
       </c>
@@ -7200,7 +7221,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>362</v>
       </c>
@@ -7217,7 +7238,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>362</v>
       </c>
@@ -7234,7 +7255,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>362</v>
       </c>
@@ -7251,7 +7272,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>362</v>
       </c>
@@ -7268,7 +7289,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>362</v>
       </c>
@@ -7285,7 +7306,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>362</v>
       </c>
@@ -7302,7 +7323,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
         <v>362</v>
       </c>
@@ -7319,7 +7340,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>362</v>
       </c>
@@ -7336,7 +7357,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
         <v>362</v>
       </c>
@@ -7353,7 +7374,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>362</v>
       </c>
@@ -7370,7 +7391,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
         <v>362</v>
       </c>
@@ -7387,7 +7408,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
         <v>362</v>
       </c>
@@ -7404,7 +7425,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
         <v>362</v>
       </c>
@@ -7421,7 +7442,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
         <v>362</v>
       </c>
@@ -7438,7 +7459,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
         <v>362</v>
       </c>
@@ -7455,7 +7476,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
         <v>362</v>
       </c>
@@ -7472,7 +7493,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
         <v>362</v>
       </c>
@@ -7489,7 +7510,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
         <v>362</v>
       </c>
@@ -7506,7 +7527,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
         <v>362</v>
       </c>
@@ -7523,7 +7544,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
         <v>362</v>
       </c>
@@ -7540,7 +7561,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
         <v>362</v>
       </c>
@@ -7557,7 +7578,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
         <v>362</v>
       </c>
@@ -7574,7 +7595,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
         <v>362</v>
       </c>
@@ -7591,7 +7612,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
         <v>362</v>
       </c>
@@ -7608,7 +7629,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
         <v>362</v>
       </c>
@@ -7625,7 +7646,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
         <v>362</v>
       </c>
@@ -7642,7 +7663,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
         <v>362</v>
       </c>
@@ -7659,7 +7680,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
         <v>362</v>
       </c>
@@ -7676,7 +7697,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
         <v>362</v>
       </c>
@@ -7693,7 +7714,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
         <v>362</v>
       </c>
@@ -7710,7 +7731,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
         <v>362</v>
       </c>
@@ -7727,7 +7748,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
         <v>362</v>
       </c>
@@ -7744,7 +7765,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
         <v>362</v>
       </c>
@@ -7761,7 +7782,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
         <v>362</v>
       </c>
@@ -7778,7 +7799,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
         <v>362</v>
       </c>
@@ -7795,7 +7816,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
         <v>362</v>
       </c>
@@ -7812,7 +7833,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
         <v>362</v>
       </c>
@@ -7829,7 +7850,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
         <v>362</v>
       </c>
@@ -7846,7 +7867,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
         <v>362</v>
       </c>
@@ -7863,7 +7884,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
         <v>362</v>
       </c>
@@ -7880,7 +7901,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
         <v>362</v>
       </c>
@@ -7897,7 +7918,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
         <v>362</v>
       </c>
@@ -7914,7 +7935,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
         <v>362</v>
       </c>
@@ -7931,7 +7952,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
         <v>362</v>
       </c>
@@ -7948,7 +7969,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
         <v>362</v>
       </c>
@@ -7965,7 +7986,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
         <v>362</v>
       </c>
@@ -7982,7 +8003,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
         <v>362</v>
       </c>
@@ -7999,7 +8020,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
         <v>362</v>
       </c>
@@ -8016,7 +8037,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
         <v>362</v>
       </c>
@@ -8033,7 +8054,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
         <v>362</v>
       </c>
@@ -8050,7 +8071,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
         <v>362</v>
       </c>
@@ -8067,7 +8088,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
         <v>362</v>
       </c>
@@ -8084,7 +8105,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
         <v>362</v>
       </c>
@@ -8101,7 +8122,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
         <v>362</v>
       </c>
@@ -8118,7 +8139,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
         <v>362</v>
       </c>
@@ -8135,7 +8156,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
         <v>362</v>
       </c>
@@ -8152,7 +8173,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
         <v>362</v>
       </c>
@@ -8169,7 +8190,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
         <v>362</v>
       </c>
@@ -8186,7 +8207,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
         <v>362</v>
       </c>
@@ -8203,7 +8224,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
         <v>362</v>
       </c>
@@ -8220,7 +8241,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
         <v>362</v>
       </c>
@@ -8237,7 +8258,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
         <v>362</v>
       </c>
@@ -8254,7 +8275,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
         <v>362</v>
       </c>
@@ -8271,7 +8292,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A250" t="s">
         <v>362</v>
       </c>
@@ -8288,7 +8309,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
         <v>362</v>
       </c>
@@ -8305,7 +8326,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A252" t="s">
         <v>362</v>
       </c>
@@ -8322,7 +8343,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A253" t="s">
         <v>362</v>
       </c>
@@ -8339,7 +8360,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A254" t="s">
         <v>362</v>
       </c>
@@ -8356,7 +8377,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
         <v>362</v>
       </c>
@@ -8373,7 +8394,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A256" t="s">
         <v>362</v>
       </c>
@@ -8390,7 +8411,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A257" t="s">
         <v>362</v>
       </c>
@@ -8407,7 +8428,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A258" t="s">
         <v>362</v>
       </c>
@@ -8424,7 +8445,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A259" t="s">
         <v>362</v>
       </c>
@@ -8441,7 +8462,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A260" t="s">
         <v>362</v>
       </c>
@@ -8458,7 +8479,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A261" t="s">
         <v>362</v>
       </c>
@@ -8475,7 +8496,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A262" t="s">
         <v>362</v>
       </c>
@@ -8492,7 +8513,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A263" t="s">
         <v>362</v>
       </c>
@@ -8509,7 +8530,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A264" t="s">
         <v>362</v>
       </c>
@@ -8526,7 +8547,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A265" t="s">
         <v>362</v>
       </c>
@@ -8543,7 +8564,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="266" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A266" t="s">
         <v>362</v>
       </c>
@@ -8560,7 +8581,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A267" t="s">
         <v>362</v>
       </c>
@@ -8577,7 +8598,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="268" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A268" t="s">
         <v>362</v>
       </c>
@@ -8594,7 +8615,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="269" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A269" t="s">
         <v>362</v>
       </c>
@@ -8611,7 +8632,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="270" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A270" t="s">
         <v>362</v>
       </c>
@@ -8628,7 +8649,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="271" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A271" t="s">
         <v>362</v>
       </c>
@@ -8645,7 +8666,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="272" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A272" t="s">
         <v>362</v>
       </c>
@@ -8662,7 +8683,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="273" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A273" t="s">
         <v>362</v>
       </c>
@@ -8679,7 +8700,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="274" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A274" t="s">
         <v>362</v>
       </c>
@@ -8696,7 +8717,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="275" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A275" t="s">
         <v>362</v>
       </c>
@@ -8713,7 +8734,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="276" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A276" t="s">
         <v>362</v>
       </c>
@@ -8730,7 +8751,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="277" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A277" t="s">
         <v>362</v>
       </c>
@@ -8747,7 +8768,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="278" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A278" t="s">
         <v>362</v>
       </c>
@@ -8764,7 +8785,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="279" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A279" t="s">
         <v>362</v>
       </c>
@@ -8781,7 +8802,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="280" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A280" t="s">
         <v>362</v>
       </c>
@@ -8798,7 +8819,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="281" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A281" t="s">
         <v>362</v>
       </c>
@@ -8815,7 +8836,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="282" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A282" t="s">
         <v>362</v>
       </c>
@@ -8832,7 +8853,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="283" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A283" t="s">
         <v>362</v>
       </c>
@@ -8849,7 +8870,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="284" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A284" t="s">
         <v>362</v>
       </c>
@@ -8866,7 +8887,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="285" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A285" t="s">
         <v>362</v>
       </c>
@@ -8883,7 +8904,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="286" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A286" t="s">
         <v>362</v>
       </c>
@@ -8900,7 +8921,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="287" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A287" t="s">
         <v>362</v>
       </c>
@@ -8917,7 +8938,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="288" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A288" t="s">
         <v>362</v>
       </c>
@@ -8934,7 +8955,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="289" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A289" t="s">
         <v>362</v>
       </c>
@@ -8951,7 +8972,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="290" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A290" t="s">
         <v>362</v>
       </c>
@@ -8968,7 +8989,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="291" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A291" t="s">
         <v>362</v>
       </c>
@@ -8985,7 +9006,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="292" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A292" t="s">
         <v>362</v>
       </c>
@@ -9002,7 +9023,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="293" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A293" t="s">
         <v>362</v>
       </c>
@@ -9019,7 +9040,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="294" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A294" t="s">
         <v>362</v>
       </c>
@@ -9036,7 +9057,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="295" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A295" t="s">
         <v>362</v>
       </c>
@@ -9053,7 +9074,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="296" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A296" t="s">
         <v>362</v>
       </c>
@@ -9070,7 +9091,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="297" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A297" t="s">
         <v>362</v>
       </c>
@@ -9096,7 +9117,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="298" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A298" t="s">
         <v>362</v>
       </c>
@@ -9122,7 +9143,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="299" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A299" t="s">
         <v>362</v>
       </c>
@@ -9148,7 +9169,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="300" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A300" t="s">
         <v>362</v>
       </c>
@@ -9174,7 +9195,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="301" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A301" t="s">
         <v>362</v>
       </c>
@@ -9200,7 +9221,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="302" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A302" t="s">
         <v>362</v>
       </c>
@@ -9226,7 +9247,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="303" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A303" t="s">
         <v>362</v>
       </c>
@@ -9252,7 +9273,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="304" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A304" t="s">
         <v>362</v>
       </c>
@@ -9278,7 +9299,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="305" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A305" t="s">
         <v>362</v>
       </c>
@@ -9304,7 +9325,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="306" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A306" t="s">
         <v>362</v>
       </c>
@@ -9330,7 +9351,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="307" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A307" t="s">
         <v>362</v>
       </c>
@@ -9356,7 +9377,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="308" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A308" t="s">
         <v>362</v>
       </c>
@@ -9382,7 +9403,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="309" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A309" t="s">
         <v>362</v>
       </c>
@@ -9408,7 +9429,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="310" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A310" t="s">
         <v>362</v>
       </c>
@@ -9434,7 +9455,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="311" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A311" t="s">
         <v>362</v>
       </c>
@@ -9460,7 +9481,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="312" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A312" t="s">
         <v>362</v>
       </c>
@@ -9486,7 +9507,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="313" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A313" t="s">
         <v>362</v>
       </c>
@@ -9512,7 +9533,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="314" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A314" t="s">
         <v>362</v>
       </c>
@@ -9538,7 +9559,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="315" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A315" t="s">
         <v>362</v>
       </c>
@@ -9564,7 +9585,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="316" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A316" t="s">
         <v>362</v>
       </c>
@@ -9590,7 +9611,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="317" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A317" t="s">
         <v>362</v>
       </c>
@@ -9616,7 +9637,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="318" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A318" t="s">
         <v>362</v>
       </c>
@@ -9642,7 +9663,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="319" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A319" t="s">
         <v>362</v>
       </c>
@@ -9668,7 +9689,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="320" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A320" t="s">
         <v>362</v>
       </c>
@@ -9694,7 +9715,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="321" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A321" t="s">
         <v>362</v>
       </c>
@@ -9720,7 +9741,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="322" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A322" t="s">
         <v>362</v>
       </c>
@@ -9746,7 +9767,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="323" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A323" t="s">
         <v>362</v>
       </c>
@@ -9772,7 +9793,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="324" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A324" t="s">
         <v>362</v>
       </c>
@@ -9798,7 +9819,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="325" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A325" t="s">
         <v>362</v>
       </c>
@@ -9824,7 +9845,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="326" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A326" t="s">
         <v>362</v>
       </c>
@@ -9850,7 +9871,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="327" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A327" t="s">
         <v>362</v>
       </c>
@@ -9876,7 +9897,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="328" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A328" t="s">
         <v>362</v>
       </c>
@@ -9902,7 +9923,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="329" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A329" t="s">
         <v>362</v>
       </c>
@@ -9928,7 +9949,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="330" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A330" t="s">
         <v>362</v>
       </c>
@@ -9954,7 +9975,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="331" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A331" t="s">
         <v>362</v>
       </c>
@@ -9980,7 +10001,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="332" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A332" t="s">
         <v>362</v>
       </c>
@@ -10006,7 +10027,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="333" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A333" t="s">
         <v>362</v>
       </c>
@@ -10032,7 +10053,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="334" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A334" t="s">
         <v>362</v>
       </c>
@@ -10058,7 +10079,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="335" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A335" t="s">
         <v>362</v>
       </c>
@@ -10084,7 +10105,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="336" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A336" t="s">
         <v>362</v>
       </c>
@@ -10110,7 +10131,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="337" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A337" t="s">
         <v>362</v>
       </c>
@@ -10136,7 +10157,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="338" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A338" t="s">
         <v>362</v>
       </c>
@@ -10162,7 +10183,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="339" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A339" t="s">
         <v>362</v>
       </c>
@@ -10188,7 +10209,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="340" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A340" t="s">
         <v>362</v>
       </c>
@@ -10214,7 +10235,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="341" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A341" t="s">
         <v>362</v>
       </c>
@@ -10240,7 +10261,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="342" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A342" t="s">
         <v>362</v>
       </c>
@@ -10266,7 +10287,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="343" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A343" t="s">
         <v>362</v>
       </c>
@@ -10292,7 +10313,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="344" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A344" t="s">
         <v>362</v>
       </c>
@@ -10318,7 +10339,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="345" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A345" t="s">
         <v>362</v>
       </c>
@@ -10344,7 +10365,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="346" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A346" t="s">
         <v>362</v>
       </c>
@@ -10370,7 +10391,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="347" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A347" t="s">
         <v>362</v>
       </c>
@@ -10396,7 +10417,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="348" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A348" t="s">
         <v>362</v>
       </c>
@@ -10422,7 +10443,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="349" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A349" t="s">
         <v>362</v>
       </c>
@@ -10448,7 +10469,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="350" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A350" t="s">
         <v>362</v>
       </c>
@@ -10474,7 +10495,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="351" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A351" t="s">
         <v>362</v>
       </c>
@@ -10500,7 +10521,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="352" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A352" t="s">
         <v>362</v>
       </c>
@@ -10526,7 +10547,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="353" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A353" t="s">
         <v>362</v>
       </c>
@@ -10552,7 +10573,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="354" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A354" t="s">
         <v>362</v>
       </c>
@@ -10578,7 +10599,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="355" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A355" t="s">
         <v>362</v>
       </c>
@@ -10604,7 +10625,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="356" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A356" t="s">
         <v>362</v>
       </c>
@@ -10630,7 +10651,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="357" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A357" t="s">
         <v>362</v>
       </c>
@@ -10656,7 +10677,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="358" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A358" t="s">
         <v>362</v>
       </c>
@@ -10682,7 +10703,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="359" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A359" t="s">
         <v>362</v>
       </c>
@@ -10708,7 +10729,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="360" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A360" t="s">
         <v>362</v>
       </c>
@@ -10734,7 +10755,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="361" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A361" t="s">
         <v>362</v>
       </c>
@@ -10760,7 +10781,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="362" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A362" t="s">
         <v>362</v>
       </c>
@@ -10786,7 +10807,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="363" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A363" t="s">
         <v>362</v>
       </c>
@@ -10812,7 +10833,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="364" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A364" t="s">
         <v>362</v>
       </c>
@@ -10838,7 +10859,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="365" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A365" t="s">
         <v>362</v>
       </c>
@@ -10864,7 +10885,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="366" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A366" t="s">
         <v>362</v>
       </c>
@@ -10890,7 +10911,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="367" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A367" t="s">
         <v>362</v>
       </c>
@@ -10916,7 +10937,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="368" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A368" t="s">
         <v>362</v>
       </c>
@@ -10942,7 +10963,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="369" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A369" t="s">
         <v>362</v>
       </c>
@@ -10968,7 +10989,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="370" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A370" t="s">
         <v>362</v>
       </c>
@@ -10994,7 +11015,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="371" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A371" t="s">
         <v>362</v>
       </c>
@@ -11020,7 +11041,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="372" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A372" t="s">
         <v>362</v>
       </c>
@@ -11046,7 +11067,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="373" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A373" t="s">
         <v>362</v>
       </c>
@@ -11072,7 +11093,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="374" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A374" t="s">
         <v>362</v>
       </c>
@@ -11098,7 +11119,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="375" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A375" t="s">
         <v>362</v>
       </c>
@@ -11124,7 +11145,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="376" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A376" t="s">
         <v>362</v>
       </c>
@@ -11150,7 +11171,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="377" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A377" t="s">
         <v>362</v>
       </c>
@@ -11176,7 +11197,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="378" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A378" t="s">
         <v>362</v>
       </c>
@@ -11202,7 +11223,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="379" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A379" t="s">
         <v>362</v>
       </c>
@@ -11228,7 +11249,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="380" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A380" t="s">
         <v>362</v>
       </c>
@@ -11254,7 +11275,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="381" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A381" t="s">
         <v>362</v>
       </c>
@@ -11280,7 +11301,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="382" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A382" t="s">
         <v>362</v>
       </c>
@@ -11306,7 +11327,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="383" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A383" t="s">
         <v>362</v>
       </c>
@@ -11332,7 +11353,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="384" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A384" t="s">
         <v>362</v>
       </c>
@@ -11358,7 +11379,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="385" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A385" t="s">
         <v>362</v>
       </c>
@@ -11384,7 +11405,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="386" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A386" t="s">
         <v>362</v>
       </c>
@@ -11410,7 +11431,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="387" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A387" t="s">
         <v>362</v>
       </c>
@@ -11436,7 +11457,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="388" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A388" t="s">
         <v>362</v>
       </c>
@@ -11462,7 +11483,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="389" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A389" t="s">
         <v>362</v>
       </c>
@@ -11488,7 +11509,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="390" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A390" t="s">
         <v>362</v>
       </c>
@@ -11514,7 +11535,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="391" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A391" t="s">
         <v>362</v>
       </c>
@@ -11540,7 +11561,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="392" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A392" t="s">
         <v>362</v>
       </c>
@@ -11566,7 +11587,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="393" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A393" t="s">
         <v>362</v>
       </c>
@@ -11592,7 +11613,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="394" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A394" t="s">
         <v>362</v>
       </c>
@@ -11618,7 +11639,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="395" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A395" t="s">
         <v>362</v>
       </c>
@@ -11644,7 +11665,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="396" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A396" t="s">
         <v>362</v>
       </c>
@@ -11670,7 +11691,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="397" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A397" t="s">
         <v>362</v>
       </c>
@@ -11696,7 +11717,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="398" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A398" t="s">
         <v>362</v>
       </c>
@@ -11722,7 +11743,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="399" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A399" t="s">
         <v>362</v>
       </c>
@@ -11748,7 +11769,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="400" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A400" t="s">
         <v>362</v>
       </c>
@@ -11774,7 +11795,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="401" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A401" t="s">
         <v>362</v>
       </c>
@@ -11800,7 +11821,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="402" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A402" t="s">
         <v>362</v>
       </c>
@@ -11826,7 +11847,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="403" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A403" t="s">
         <v>362</v>
       </c>
@@ -11852,7 +11873,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="404" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A404" t="s">
         <v>362</v>
       </c>
@@ -11878,7 +11899,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="405" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A405" t="s">
         <v>362</v>
       </c>
@@ -11904,7 +11925,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="406" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A406" t="s">
         <v>362</v>
       </c>
@@ -11930,7 +11951,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="407" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A407" t="s">
         <v>362</v>
       </c>
@@ -11956,7 +11977,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="408" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A408" t="s">
         <v>362</v>
       </c>
@@ -11982,7 +12003,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="409" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A409" t="s">
         <v>362</v>
       </c>
@@ -12008,7 +12029,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="410" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A410" t="s">
         <v>362</v>
       </c>
@@ -12034,7 +12055,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="411" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A411" t="s">
         <v>362</v>
       </c>
@@ -12060,7 +12081,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="412" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A412" t="s">
         <v>362</v>
       </c>
@@ -12086,7 +12107,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="413" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A413" t="s">
         <v>362</v>
       </c>
@@ -12112,7 +12133,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="414" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A414" t="s">
         <v>362</v>
       </c>
@@ -12138,7 +12159,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="415" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A415" t="s">
         <v>362</v>
       </c>
@@ -12164,7 +12185,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="416" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A416" t="s">
         <v>362</v>
       </c>
@@ -12190,7 +12211,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="417" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A417" t="s">
         <v>362</v>
       </c>
@@ -12216,7 +12237,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="418" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A418" s="4" t="s">
         <v>362</v>
       </c>
@@ -12244,7 +12265,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="419" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A419" s="4" t="s">
         <v>362</v>
       </c>
@@ -12272,7 +12293,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="420" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A420" s="4" t="s">
         <v>362</v>
       </c>
@@ -12300,7 +12321,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="421" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A421" s="4" t="s">
         <v>362</v>
       </c>
@@ -12328,7 +12349,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="422" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A422" t="s">
         <v>362</v>
       </c>
@@ -12354,7 +12375,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="423" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A423" t="s">
         <v>362</v>
       </c>
@@ -12380,7 +12401,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="424" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A424" t="s">
         <v>362</v>
       </c>
@@ -12406,7 +12427,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="425" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A425" t="s">
         <v>362</v>
       </c>
@@ -12432,7 +12453,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="426" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A426" t="s">
         <v>362</v>
       </c>
@@ -12458,7 +12479,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="427" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A427" t="s">
         <v>362</v>
       </c>
@@ -12484,7 +12505,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="428" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A428" t="s">
         <v>362</v>
       </c>
@@ -12510,7 +12531,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="429" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A429" t="s">
         <v>362</v>
       </c>
@@ -12536,7 +12557,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="430" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A430" t="s">
         <v>362</v>
       </c>
@@ -12562,7 +12583,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="431" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A431" t="s">
         <v>362</v>
       </c>
@@ -12588,7 +12609,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="432" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A432" t="s">
         <v>362</v>
       </c>
@@ -12614,7 +12635,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="433" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A433" t="s">
         <v>362</v>
       </c>
@@ -12640,7 +12661,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="434" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A434" t="s">
         <v>362</v>
       </c>
@@ -12666,7 +12687,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="435" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A435" t="s">
         <v>362</v>
       </c>
@@ -12692,7 +12713,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="436" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A436" t="s">
         <v>362</v>
       </c>
@@ -12718,7 +12739,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="437" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A437" t="s">
         <v>362</v>
       </c>
@@ -12744,7 +12765,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="438" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A438" t="s">
         <v>362</v>
       </c>
@@ -12770,7 +12791,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="439" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A439" t="s">
         <v>362</v>
       </c>
@@ -12796,7 +12817,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="440" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A440" t="s">
         <v>362</v>
       </c>
@@ -12822,7 +12843,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="441" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A441" t="s">
         <v>362</v>
       </c>
@@ -12848,7 +12869,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="442" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A442" t="s">
         <v>362</v>
       </c>
@@ -12874,7 +12895,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="443" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A443" t="s">
         <v>362</v>
       </c>
@@ -12900,7 +12921,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="444" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A444" t="s">
         <v>362</v>
       </c>
@@ -12926,7 +12947,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="445" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A445" t="s">
         <v>362</v>
       </c>
@@ -12952,7 +12973,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="446" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A446" t="s">
         <v>362</v>
       </c>
@@ -12978,7 +12999,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="447" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A447" t="s">
         <v>362</v>
       </c>
@@ -13004,7 +13025,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="448" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A448" t="s">
         <v>362</v>
       </c>
@@ -13030,7 +13051,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="449" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A449" t="s">
         <v>362</v>
       </c>
@@ -13056,7 +13077,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="450" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A450" t="s">
         <v>455</v>
       </c>
@@ -13085,7 +13106,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="451" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A451" t="s">
         <v>455</v>
       </c>
@@ -13114,7 +13135,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="452" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A452" t="s">
         <v>455</v>
       </c>
@@ -13143,7 +13164,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="453" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A453" t="s">
         <v>455</v>
       </c>
@@ -13172,7 +13193,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="454" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A454" t="s">
         <v>455</v>
       </c>
@@ -13201,7 +13222,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="455" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A455" t="s">
         <v>455</v>
       </c>
@@ -13230,7 +13251,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="456" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A456" t="s">
         <v>455</v>
       </c>
@@ -13259,7 +13280,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="457" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A457" t="s">
         <v>455</v>
       </c>
@@ -13288,7 +13309,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="458" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A458" t="s">
         <v>455</v>
       </c>
@@ -13317,7 +13338,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="459" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A459" t="s">
         <v>455</v>
       </c>
@@ -13343,7 +13364,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="460" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A460" t="s">
         <v>455</v>
       </c>
@@ -13369,7 +13390,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="461" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A461" t="s">
         <v>455</v>
       </c>
@@ -13393,6 +13414,122 @@
       </c>
       <c r="J461" t="e">
         <v>#N/A</v>
+      </c>
+    </row>
+    <row r="462" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A462" t="s">
+        <v>455</v>
+      </c>
+      <c r="B462" t="s">
+        <v>473</v>
+      </c>
+      <c r="C462">
+        <v>1010309</v>
+      </c>
+      <c r="F462">
+        <v>45</v>
+      </c>
+      <c r="G462">
+        <v>5</v>
+      </c>
+      <c r="H462">
+        <v>0.03</v>
+      </c>
+      <c r="I462" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J462" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K462" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="463" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A463" t="s">
+        <v>455</v>
+      </c>
+      <c r="B463" t="s">
+        <v>474</v>
+      </c>
+      <c r="C463">
+        <v>1010310</v>
+      </c>
+      <c r="F463">
+        <v>45</v>
+      </c>
+      <c r="G463">
+        <v>5</v>
+      </c>
+      <c r="H463">
+        <v>0.03</v>
+      </c>
+      <c r="I463" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J463" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K463" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="464" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A464" t="s">
+        <v>455</v>
+      </c>
+      <c r="B464" t="s">
+        <v>477</v>
+      </c>
+      <c r="C464">
+        <v>800601</v>
+      </c>
+      <c r="F464">
+        <v>45</v>
+      </c>
+      <c r="G464">
+        <v>5</v>
+      </c>
+      <c r="H464">
+        <v>0.03</v>
+      </c>
+      <c r="I464" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J464" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K464" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="465" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A465" t="s">
+        <v>455</v>
+      </c>
+      <c r="B465" t="s">
+        <v>477</v>
+      </c>
+      <c r="C465">
+        <v>800602</v>
+      </c>
+      <c r="F465">
+        <v>45</v>
+      </c>
+      <c r="G465">
+        <v>5</v>
+      </c>
+      <c r="H465">
+        <v>0.03</v>
+      </c>
+      <c r="I465" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J465" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K465" t="s">
+        <v>478</v>
       </c>
     </row>
   </sheetData>
@@ -13414,18 +13551,18 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>324</v>
       </c>
@@ -13433,7 +13570,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>328</v>
       </c>
@@ -13441,7 +13578,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>323</v>
       </c>

</xml_diff>

<commit_message>
changed suffixes of new NGF corridors from NB/SB to AM/PM
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/TOLLCLASS_Designations.xlsx
+++ b/utilities/NextGenFwys/TOLLCLASS_Designations.xlsx
@@ -5,19 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sisrael\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{846F2A70-62FB-4BB4-A26F-0AA9CA49CD09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A790124D-1702-40E4-AAA3-1622DDC8AE46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{0F0A9957-56E7-4C48-967B-2AB2A1965C2F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0F0A9957-56E7-4C48-967B-2AB2A1965C2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs_for_tollcalib" sheetId="1" r:id="rId1"/>
     <sheet name="Readme - numbering convention" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Inputs_for_tollcalib!$A$1:$J$461</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Inputs_for_tollcalib!$A$1:$J$465</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1421,18 +1421,6 @@
     <t>CC_Southern_680</t>
   </si>
   <si>
-    <t>AL_680_SB</t>
-  </si>
-  <si>
-    <t>AL_680_NB</t>
-  </si>
-  <si>
-    <t>CC_Southern_680_SB</t>
-  </si>
-  <si>
-    <t>CC_Southern_680_NB</t>
-  </si>
-  <si>
     <t>I-680 AL - I-580 interchange to SCL county line (Per Mile Tolling) - SB</t>
   </si>
   <si>
@@ -1454,12 +1442,6 @@
     <t>SCL_85</t>
   </si>
   <si>
-    <t>SCL_85_NB</t>
-  </si>
-  <si>
-    <t>SCL_85_SB</t>
-  </si>
-  <si>
     <t>US101 - SR25 to Dunne - NB</t>
   </si>
   <si>
@@ -1476,6 +1458,24 @@
   </si>
   <si>
     <t>EXP_SL_I80_I505_to_Yolo</t>
+  </si>
+  <si>
+    <t>SCL_85_AM</t>
+  </si>
+  <si>
+    <t>CC_Southern_680_PM</t>
+  </si>
+  <si>
+    <t>AL_680_PM</t>
+  </si>
+  <si>
+    <t>SCL_85_PM</t>
+  </si>
+  <si>
+    <t>CC_Southern_680_AM</t>
+  </si>
+  <si>
+    <t>AL_680_AM</t>
   </si>
 </sst>
 </file>
@@ -1881,24 +1881,24 @@
   </sheetPr>
   <dimension ref="A1:K465"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A440" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J466" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A418" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B474" sqref="B474"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.453125" customWidth="1"/>
-    <col min="2" max="2" width="79.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="79.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.1796875" customWidth="1"/>
-    <col min="10" max="10" width="24.453125" customWidth="1"/>
-    <col min="11" max="11" width="23.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.140625" customWidth="1"/>
+    <col min="10" max="10" width="24.42578125" customWidth="1"/>
+    <col min="11" max="11" width="23.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>336</v>
       </c>
@@ -1930,10 +1930,10 @@
         <v>338</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>360</v>
       </c>
@@ -1950,7 +1950,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>360</v>
       </c>
@@ -1967,7 +1967,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>360</v>
       </c>
@@ -1984,7 +1984,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>360</v>
       </c>
@@ -2001,7 +2001,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>360</v>
       </c>
@@ -2018,7 +2018,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>360</v>
       </c>
@@ -2035,7 +2035,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>360</v>
       </c>
@@ -2052,7 +2052,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>360</v>
       </c>
@@ -2069,7 +2069,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>361</v>
       </c>
@@ -2086,7 +2086,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>361</v>
       </c>
@@ -2112,7 +2112,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>362</v>
       </c>
@@ -2138,7 +2138,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>362</v>
       </c>
@@ -2164,7 +2164,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>362</v>
       </c>
@@ -2191,7 +2191,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>361</v>
       </c>
@@ -2220,7 +2220,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>361</v>
       </c>
@@ -2249,7 +2249,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>361</v>
       </c>
@@ -2278,7 +2278,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>361</v>
       </c>
@@ -2307,7 +2307,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>361</v>
       </c>
@@ -2336,7 +2336,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>361</v>
       </c>
@@ -2365,7 +2365,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>361</v>
       </c>
@@ -2397,7 +2397,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>361</v>
       </c>
@@ -2429,7 +2429,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>361</v>
       </c>
@@ -2461,7 +2461,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>361</v>
       </c>
@@ -2493,7 +2493,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>361</v>
       </c>
@@ -2525,7 +2525,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>361</v>
       </c>
@@ -2557,7 +2557,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>361</v>
       </c>
@@ -2589,7 +2589,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>361</v>
       </c>
@@ -2621,7 +2621,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>361</v>
       </c>
@@ -2653,7 +2653,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>361</v>
       </c>
@@ -2685,7 +2685,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>361</v>
       </c>
@@ -2717,7 +2717,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>361</v>
       </c>
@@ -2749,7 +2749,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>361</v>
       </c>
@@ -2778,7 +2778,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>361</v>
       </c>
@@ -2807,7 +2807,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>361</v>
       </c>
@@ -2839,7 +2839,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>361</v>
       </c>
@@ -2871,7 +2871,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>361</v>
       </c>
@@ -2903,7 +2903,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>361</v>
       </c>
@@ -2935,7 +2935,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>361</v>
       </c>
@@ -2967,7 +2967,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>361</v>
       </c>
@@ -2999,7 +2999,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>361</v>
       </c>
@@ -3028,7 +3028,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>361</v>
       </c>
@@ -3057,7 +3057,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>361</v>
       </c>
@@ -3086,7 +3086,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>361</v>
       </c>
@@ -3115,7 +3115,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>361</v>
       </c>
@@ -3144,7 +3144,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>361</v>
       </c>
@@ -3173,7 +3173,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>361</v>
       </c>
@@ -3202,7 +3202,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>361</v>
       </c>
@@ -3231,7 +3231,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>361</v>
       </c>
@@ -3260,7 +3260,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>361</v>
       </c>
@@ -3289,7 +3289,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>361</v>
       </c>
@@ -3321,7 +3321,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>361</v>
       </c>
@@ -3353,7 +3353,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>361</v>
       </c>
@@ -3385,7 +3385,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>361</v>
       </c>
@@ -3417,7 +3417,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>361</v>
       </c>
@@ -3449,7 +3449,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>361</v>
       </c>
@@ -3481,7 +3481,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>361</v>
       </c>
@@ -3510,7 +3510,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>361</v>
       </c>
@@ -3539,7 +3539,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>361</v>
       </c>
@@ -3568,7 +3568,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>361</v>
       </c>
@@ -3597,7 +3597,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>361</v>
       </c>
@@ -3626,7 +3626,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="62" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>361</v>
       </c>
@@ -3655,7 +3655,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>361</v>
       </c>
@@ -3681,7 +3681,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>361</v>
       </c>
@@ -3707,7 +3707,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>361</v>
       </c>
@@ -3733,7 +3733,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>361</v>
       </c>
@@ -3759,7 +3759,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="67" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>361</v>
       </c>
@@ -3788,7 +3788,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>361</v>
       </c>
@@ -3817,7 +3817,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>361</v>
       </c>
@@ -3846,7 +3846,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>361</v>
       </c>
@@ -3875,7 +3875,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="71" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>361</v>
       </c>
@@ -3904,7 +3904,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="72" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>361</v>
       </c>
@@ -3933,7 +3933,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="73" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>361</v>
       </c>
@@ -3962,7 +3962,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>361</v>
       </c>
@@ -3991,7 +3991,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="75" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>361</v>
       </c>
@@ -4020,7 +4020,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="76" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>361</v>
       </c>
@@ -4049,7 +4049,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="77" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>361</v>
       </c>
@@ -4078,7 +4078,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="78" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>361</v>
       </c>
@@ -4107,7 +4107,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="79" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>361</v>
       </c>
@@ -4133,7 +4133,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="80" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>361</v>
       </c>
@@ -4159,7 +4159,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>361</v>
       </c>
@@ -4191,7 +4191,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="82" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>361</v>
       </c>
@@ -4223,7 +4223,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="83" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>361</v>
       </c>
@@ -4252,7 +4252,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="84" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>361</v>
       </c>
@@ -4281,7 +4281,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="85" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>361</v>
       </c>
@@ -4313,7 +4313,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="86" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>361</v>
       </c>
@@ -4345,7 +4345,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="87" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>361</v>
       </c>
@@ -4377,7 +4377,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="88" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>361</v>
       </c>
@@ -4409,7 +4409,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="89" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>361</v>
       </c>
@@ -4435,7 +4435,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="90" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>361</v>
       </c>
@@ -4461,7 +4461,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="91" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>361</v>
       </c>
@@ -4490,7 +4490,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>361</v>
       </c>
@@ -4519,7 +4519,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>361</v>
       </c>
@@ -4551,7 +4551,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>361</v>
       </c>
@@ -4583,7 +4583,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>361</v>
       </c>
@@ -4612,7 +4612,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>361</v>
       </c>
@@ -4641,7 +4641,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>361</v>
       </c>
@@ -4667,7 +4667,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>361</v>
       </c>
@@ -4693,7 +4693,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="99" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>361</v>
       </c>
@@ -4719,7 +4719,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="100" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>361</v>
       </c>
@@ -4745,7 +4745,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="101" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>361</v>
       </c>
@@ -4777,7 +4777,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="102" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>361</v>
       </c>
@@ -4809,7 +4809,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>361</v>
       </c>
@@ -4841,7 +4841,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>361</v>
       </c>
@@ -4873,7 +4873,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>361</v>
       </c>
@@ -4905,7 +4905,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>361</v>
       </c>
@@ -4937,7 +4937,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="107" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>361</v>
       </c>
@@ -4966,7 +4966,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="108" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>361</v>
       </c>
@@ -4995,7 +4995,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="109" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>361</v>
       </c>
@@ -5027,7 +5027,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="110" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>361</v>
       </c>
@@ -5059,7 +5059,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="111" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>361</v>
       </c>
@@ -5088,7 +5088,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="112" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>361</v>
       </c>
@@ -5117,7 +5117,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="113" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>361</v>
       </c>
@@ -5146,7 +5146,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="114" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>361</v>
       </c>
@@ -5175,7 +5175,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="115" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>361</v>
       </c>
@@ -5204,7 +5204,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="116" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>361</v>
       </c>
@@ -5233,7 +5233,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>361</v>
       </c>
@@ -5265,7 +5265,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>361</v>
       </c>
@@ -5294,7 +5294,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="119" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>361</v>
       </c>
@@ -5326,7 +5326,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="120" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>361</v>
       </c>
@@ -5355,7 +5355,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="121" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>361</v>
       </c>
@@ -5384,7 +5384,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="122" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>361</v>
       </c>
@@ -5413,7 +5413,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="123" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>361</v>
       </c>
@@ -5445,7 +5445,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="124" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>361</v>
       </c>
@@ -5477,7 +5477,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>361</v>
       </c>
@@ -5506,7 +5506,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>361</v>
       </c>
@@ -5535,7 +5535,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>361</v>
       </c>
@@ -5567,7 +5567,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>361</v>
       </c>
@@ -5596,7 +5596,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>361</v>
       </c>
@@ -5625,7 +5625,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>361</v>
       </c>
@@ -5657,7 +5657,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>361</v>
       </c>
@@ -5686,7 +5686,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>361</v>
       </c>
@@ -5715,7 +5715,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>361</v>
       </c>
@@ -5747,7 +5747,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>361</v>
       </c>
@@ -5779,7 +5779,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>361</v>
       </c>
@@ -5811,7 +5811,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>361</v>
       </c>
@@ -5843,7 +5843,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>361</v>
       </c>
@@ -5875,7 +5875,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>361</v>
       </c>
@@ -5907,7 +5907,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>361</v>
       </c>
@@ -5939,7 +5939,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>361</v>
       </c>
@@ -5971,7 +5971,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>361</v>
       </c>
@@ -6000,7 +6000,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>361</v>
       </c>
@@ -6029,7 +6029,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>361</v>
       </c>
@@ -6061,7 +6061,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>361</v>
       </c>
@@ -6090,7 +6090,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>361</v>
       </c>
@@ -6119,7 +6119,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>361</v>
       </c>
@@ -6148,7 +6148,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>361</v>
       </c>
@@ -6177,7 +6177,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>361</v>
       </c>
@@ -6206,7 +6206,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>361</v>
       </c>
@@ -6235,7 +6235,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>361</v>
       </c>
@@ -6264,7 +6264,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>361</v>
       </c>
@@ -6296,7 +6296,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>361</v>
       </c>
@@ -6328,7 +6328,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>361</v>
       </c>
@@ -6357,7 +6357,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>361</v>
       </c>
@@ -6386,7 +6386,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>361</v>
       </c>
@@ -6415,7 +6415,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>361</v>
       </c>
@@ -6447,7 +6447,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>361</v>
       </c>
@@ -6476,7 +6476,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>361</v>
       </c>
@@ -6505,7 +6505,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>361</v>
       </c>
@@ -6534,7 +6534,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>361</v>
       </c>
@@ -6563,7 +6563,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>361</v>
       </c>
@@ -6589,7 +6589,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>361</v>
       </c>
@@ -6615,7 +6615,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>361</v>
       </c>
@@ -6641,7 +6641,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>361</v>
       </c>
@@ -6667,7 +6667,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>362</v>
       </c>
@@ -6693,7 +6693,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>362</v>
       </c>
@@ -6719,7 +6719,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>362</v>
       </c>
@@ -6745,7 +6745,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>362</v>
       </c>
@@ -6771,7 +6771,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>362</v>
       </c>
@@ -6797,7 +6797,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>362</v>
       </c>
@@ -6823,7 +6823,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>362</v>
       </c>
@@ -6849,7 +6849,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>362</v>
       </c>
@@ -6875,7 +6875,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>362</v>
       </c>
@@ -6901,7 +6901,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>362</v>
       </c>
@@ -6927,7 +6927,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>362</v>
       </c>
@@ -6953,7 +6953,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>362</v>
       </c>
@@ -6979,7 +6979,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>362</v>
       </c>
@@ -7005,7 +7005,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>362</v>
       </c>
@@ -7031,7 +7031,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>362</v>
       </c>
@@ -7057,7 +7057,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>362</v>
       </c>
@@ -7083,7 +7083,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>362</v>
       </c>
@@ -7109,7 +7109,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>362</v>
       </c>
@@ -7135,7 +7135,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>362</v>
       </c>
@@ -7161,7 +7161,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>362</v>
       </c>
@@ -7187,7 +7187,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>362</v>
       </c>
@@ -7204,7 +7204,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>362</v>
       </c>
@@ -7221,7 +7221,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>362</v>
       </c>
@@ -7238,7 +7238,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>362</v>
       </c>
@@ -7255,7 +7255,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>362</v>
       </c>
@@ -7272,7 +7272,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>362</v>
       </c>
@@ -7289,7 +7289,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>362</v>
       </c>
@@ -7306,7 +7306,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>362</v>
       </c>
@@ -7323,7 +7323,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>362</v>
       </c>
@@ -7340,7 +7340,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>362</v>
       </c>
@@ -7357,7 +7357,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>362</v>
       </c>
@@ -7374,7 +7374,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>362</v>
       </c>
@@ -7391,7 +7391,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>362</v>
       </c>
@@ -7408,7 +7408,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>362</v>
       </c>
@@ -7425,7 +7425,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>362</v>
       </c>
@@ -7442,7 +7442,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>362</v>
       </c>
@@ -7459,7 +7459,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>362</v>
       </c>
@@ -7476,7 +7476,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>362</v>
       </c>
@@ -7493,7 +7493,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>362</v>
       </c>
@@ -7510,7 +7510,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>362</v>
       </c>
@@ -7527,7 +7527,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>362</v>
       </c>
@@ -7544,7 +7544,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>362</v>
       </c>
@@ -7561,7 +7561,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>362</v>
       </c>
@@ -7578,7 +7578,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>362</v>
       </c>
@@ -7595,7 +7595,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>362</v>
       </c>
@@ -7612,7 +7612,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>362</v>
       </c>
@@ -7629,7 +7629,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>362</v>
       </c>
@@ -7646,7 +7646,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>362</v>
       </c>
@@ -7663,7 +7663,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>362</v>
       </c>
@@ -7680,7 +7680,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>362</v>
       </c>
@@ -7697,7 +7697,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>362</v>
       </c>
@@ -7714,7 +7714,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>362</v>
       </c>
@@ -7731,7 +7731,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>362</v>
       </c>
@@ -7748,7 +7748,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>362</v>
       </c>
@@ -7765,7 +7765,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>362</v>
       </c>
@@ -7782,7 +7782,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>362</v>
       </c>
@@ -7799,7 +7799,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>362</v>
       </c>
@@ -7816,7 +7816,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>362</v>
       </c>
@@ -7833,7 +7833,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>362</v>
       </c>
@@ -7850,7 +7850,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>362</v>
       </c>
@@ -7867,7 +7867,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>362</v>
       </c>
@@ -7884,7 +7884,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>362</v>
       </c>
@@ -7901,7 +7901,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>362</v>
       </c>
@@ -7918,7 +7918,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>362</v>
       </c>
@@ -7935,7 +7935,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>362</v>
       </c>
@@ -7952,7 +7952,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>362</v>
       </c>
@@ -7969,7 +7969,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>362</v>
       </c>
@@ -7986,7 +7986,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>362</v>
       </c>
@@ -8003,7 +8003,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>362</v>
       </c>
@@ -8020,7 +8020,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>362</v>
       </c>
@@ -8037,7 +8037,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>362</v>
       </c>
@@ -8054,7 +8054,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="236" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>362</v>
       </c>
@@ -8071,7 +8071,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>362</v>
       </c>
@@ -8088,7 +8088,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="238" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>362</v>
       </c>
@@ -8105,7 +8105,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="239" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>362</v>
       </c>
@@ -8122,7 +8122,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="240" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>362</v>
       </c>
@@ -8139,7 +8139,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="241" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>362</v>
       </c>
@@ -8156,7 +8156,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="242" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>362</v>
       </c>
@@ -8173,7 +8173,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="243" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>362</v>
       </c>
@@ -8190,7 +8190,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="244" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>362</v>
       </c>
@@ -8207,7 +8207,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="245" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>362</v>
       </c>
@@ -8224,7 +8224,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="246" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>362</v>
       </c>
@@ -8241,7 +8241,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="247" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>362</v>
       </c>
@@ -8258,7 +8258,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="248" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>362</v>
       </c>
@@ -8275,7 +8275,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="249" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>362</v>
       </c>
@@ -8292,7 +8292,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="250" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>362</v>
       </c>
@@ -8309,7 +8309,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="251" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>362</v>
       </c>
@@ -8326,7 +8326,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="252" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>362</v>
       </c>
@@ -8343,7 +8343,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="253" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>362</v>
       </c>
@@ -8360,7 +8360,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="254" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>362</v>
       </c>
@@ -8377,7 +8377,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="255" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>362</v>
       </c>
@@ -8394,7 +8394,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="256" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>362</v>
       </c>
@@ -8411,7 +8411,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="257" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>362</v>
       </c>
@@ -8428,7 +8428,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="258" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>362</v>
       </c>
@@ -8445,7 +8445,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="259" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>362</v>
       </c>
@@ -8462,7 +8462,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="260" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>362</v>
       </c>
@@ -8479,7 +8479,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="261" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>362</v>
       </c>
@@ -8496,7 +8496,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="262" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>362</v>
       </c>
@@ -8513,7 +8513,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="263" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>362</v>
       </c>
@@ -8530,7 +8530,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="264" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>362</v>
       </c>
@@ -8547,7 +8547,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="265" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>362</v>
       </c>
@@ -8564,7 +8564,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="266" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>362</v>
       </c>
@@ -8581,7 +8581,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="267" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>362</v>
       </c>
@@ -8598,7 +8598,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="268" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>362</v>
       </c>
@@ -8615,7 +8615,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="269" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>362</v>
       </c>
@@ -8632,7 +8632,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="270" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>362</v>
       </c>
@@ -8649,7 +8649,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="271" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>362</v>
       </c>
@@ -8666,7 +8666,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="272" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>362</v>
       </c>
@@ -8683,7 +8683,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="273" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>362</v>
       </c>
@@ -8700,7 +8700,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="274" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>362</v>
       </c>
@@ -8717,7 +8717,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="275" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>362</v>
       </c>
@@ -8734,7 +8734,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="276" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>362</v>
       </c>
@@ -8751,7 +8751,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="277" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>362</v>
       </c>
@@ -8768,7 +8768,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="278" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>362</v>
       </c>
@@ -8785,7 +8785,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="279" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>362</v>
       </c>
@@ -8802,7 +8802,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="280" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>362</v>
       </c>
@@ -8819,7 +8819,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="281" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>362</v>
       </c>
@@ -8836,7 +8836,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="282" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>362</v>
       </c>
@@ -8853,7 +8853,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="283" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>362</v>
       </c>
@@ -8870,7 +8870,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="284" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>362</v>
       </c>
@@ -8887,7 +8887,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="285" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>362</v>
       </c>
@@ -8904,7 +8904,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="286" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>362</v>
       </c>
@@ -8921,7 +8921,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="287" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>362</v>
       </c>
@@ -8938,7 +8938,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="288" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>362</v>
       </c>
@@ -8955,7 +8955,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="289" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>362</v>
       </c>
@@ -8972,7 +8972,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="290" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>362</v>
       </c>
@@ -8989,7 +8989,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="291" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>362</v>
       </c>
@@ -9006,7 +9006,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="292" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>362</v>
       </c>
@@ -9023,7 +9023,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="293" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>362</v>
       </c>
@@ -9040,7 +9040,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="294" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>362</v>
       </c>
@@ -9057,7 +9057,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="295" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>362</v>
       </c>
@@ -9074,7 +9074,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="296" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>362</v>
       </c>
@@ -9091,7 +9091,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="297" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>362</v>
       </c>
@@ -9117,7 +9117,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="298" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>362</v>
       </c>
@@ -9143,7 +9143,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="299" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>362</v>
       </c>
@@ -9169,7 +9169,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="300" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>362</v>
       </c>
@@ -9195,7 +9195,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="301" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>362</v>
       </c>
@@ -9221,7 +9221,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="302" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>362</v>
       </c>
@@ -9247,7 +9247,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="303" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>362</v>
       </c>
@@ -9273,7 +9273,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="304" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>362</v>
       </c>
@@ -9299,7 +9299,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="305" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>362</v>
       </c>
@@ -9325,7 +9325,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="306" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>362</v>
       </c>
@@ -9351,7 +9351,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="307" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>362</v>
       </c>
@@ -9377,7 +9377,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="308" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>362</v>
       </c>
@@ -9403,7 +9403,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="309" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>362</v>
       </c>
@@ -9429,7 +9429,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="310" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>362</v>
       </c>
@@ -9455,7 +9455,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="311" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>362</v>
       </c>
@@ -9481,7 +9481,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="312" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>362</v>
       </c>
@@ -9507,7 +9507,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="313" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>362</v>
       </c>
@@ -9533,7 +9533,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="314" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>362</v>
       </c>
@@ -9559,7 +9559,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="315" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>362</v>
       </c>
@@ -9585,7 +9585,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="316" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>362</v>
       </c>
@@ -9611,7 +9611,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="317" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>362</v>
       </c>
@@ -9637,7 +9637,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="318" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>362</v>
       </c>
@@ -9663,7 +9663,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="319" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>362</v>
       </c>
@@ -9689,7 +9689,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="320" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>362</v>
       </c>
@@ -9715,7 +9715,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="321" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>362</v>
       </c>
@@ -9741,7 +9741,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="322" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>362</v>
       </c>
@@ -9767,7 +9767,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="323" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>362</v>
       </c>
@@ -9793,7 +9793,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="324" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
         <v>362</v>
       </c>
@@ -9819,7 +9819,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="325" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
         <v>362</v>
       </c>
@@ -9845,7 +9845,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="326" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
         <v>362</v>
       </c>
@@ -9871,7 +9871,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="327" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>362</v>
       </c>
@@ -9897,7 +9897,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="328" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>362</v>
       </c>
@@ -9923,7 +9923,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="329" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="329" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>362</v>
       </c>
@@ -9949,7 +9949,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="330" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>362</v>
       </c>
@@ -9975,7 +9975,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="331" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="331" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>362</v>
       </c>
@@ -10001,7 +10001,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="332" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="332" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
         <v>362</v>
       </c>
@@ -10027,7 +10027,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="333" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="333" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>362</v>
       </c>
@@ -10053,7 +10053,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="334" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="334" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
         <v>362</v>
       </c>
@@ -10079,7 +10079,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="335" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="335" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
         <v>362</v>
       </c>
@@ -10105,7 +10105,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="336" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="336" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
         <v>362</v>
       </c>
@@ -10131,7 +10131,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="337" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="337" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
         <v>362</v>
       </c>
@@ -10157,7 +10157,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="338" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="338" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>362</v>
       </c>
@@ -10183,7 +10183,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="339" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="339" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>362</v>
       </c>
@@ -10209,7 +10209,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="340" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="340" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
         <v>362</v>
       </c>
@@ -10235,7 +10235,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="341" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="341" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
         <v>362</v>
       </c>
@@ -10261,7 +10261,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="342" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="342" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
         <v>362</v>
       </c>
@@ -10287,7 +10287,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="343" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="343" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
         <v>362</v>
       </c>
@@ -10313,7 +10313,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="344" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="344" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
         <v>362</v>
       </c>
@@ -10339,7 +10339,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="345" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="345" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
         <v>362</v>
       </c>
@@ -10365,7 +10365,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="346" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="346" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>362</v>
       </c>
@@ -10391,7 +10391,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="347" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="347" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
         <v>362</v>
       </c>
@@ -10417,7 +10417,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="348" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="348" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
         <v>362</v>
       </c>
@@ -10443,7 +10443,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="349" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="349" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
         <v>362</v>
       </c>
@@ -10469,7 +10469,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="350" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="350" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>362</v>
       </c>
@@ -10495,7 +10495,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="351" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="351" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
         <v>362</v>
       </c>
@@ -10521,7 +10521,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="352" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="352" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
         <v>362</v>
       </c>
@@ -10547,7 +10547,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="353" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="353" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
         <v>362</v>
       </c>
@@ -10573,7 +10573,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="354" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="354" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
         <v>362</v>
       </c>
@@ -10599,7 +10599,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="355" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="355" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
         <v>362</v>
       </c>
@@ -10625,7 +10625,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="356" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="356" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
         <v>362</v>
       </c>
@@ -10651,7 +10651,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="357" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="357" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
         <v>362</v>
       </c>
@@ -10677,7 +10677,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="358" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="358" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
         <v>362</v>
       </c>
@@ -10703,7 +10703,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="359" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="359" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
         <v>362</v>
       </c>
@@ -10729,7 +10729,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="360" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="360" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
         <v>362</v>
       </c>
@@ -10755,7 +10755,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="361" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="361" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
         <v>362</v>
       </c>
@@ -10781,7 +10781,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="362" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="362" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
         <v>362</v>
       </c>
@@ -10807,7 +10807,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="363" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="363" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
         <v>362</v>
       </c>
@@ -10833,7 +10833,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="364" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="364" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
         <v>362</v>
       </c>
@@ -10859,7 +10859,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="365" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="365" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
         <v>362</v>
       </c>
@@ -10885,7 +10885,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="366" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="366" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
         <v>362</v>
       </c>
@@ -10911,7 +10911,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="367" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="367" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
         <v>362</v>
       </c>
@@ -10937,7 +10937,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="368" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="368" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
         <v>362</v>
       </c>
@@ -10963,7 +10963,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="369" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="369" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
         <v>362</v>
       </c>
@@ -10989,7 +10989,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="370" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="370" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
         <v>362</v>
       </c>
@@ -11015,7 +11015,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="371" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="371" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
         <v>362</v>
       </c>
@@ -11041,7 +11041,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="372" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="372" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
         <v>362</v>
       </c>
@@ -11067,7 +11067,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="373" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="373" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
         <v>362</v>
       </c>
@@ -11093,7 +11093,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="374" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="374" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
         <v>362</v>
       </c>
@@ -11119,7 +11119,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="375" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="375" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
         <v>362</v>
       </c>
@@ -11145,7 +11145,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="376" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="376" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
         <v>362</v>
       </c>
@@ -11171,7 +11171,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="377" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="377" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
         <v>362</v>
       </c>
@@ -11197,7 +11197,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="378" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="378" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
         <v>362</v>
       </c>
@@ -11223,7 +11223,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="379" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="379" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
         <v>362</v>
       </c>
@@ -11249,7 +11249,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="380" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="380" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
         <v>362</v>
       </c>
@@ -11275,7 +11275,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="381" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="381" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
         <v>362</v>
       </c>
@@ -11301,7 +11301,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="382" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="382" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
         <v>362</v>
       </c>
@@ -11327,7 +11327,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="383" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="383" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
         <v>362</v>
       </c>
@@ -11353,7 +11353,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="384" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="384" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
         <v>362</v>
       </c>
@@ -11379,7 +11379,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="385" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="385" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
         <v>362</v>
       </c>
@@ -11405,7 +11405,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="386" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="386" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
         <v>362</v>
       </c>
@@ -11431,7 +11431,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="387" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="387" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
         <v>362</v>
       </c>
@@ -11457,7 +11457,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="388" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="388" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
         <v>362</v>
       </c>
@@ -11483,7 +11483,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="389" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="389" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
         <v>362</v>
       </c>
@@ -11509,7 +11509,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="390" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="390" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
         <v>362</v>
       </c>
@@ -11535,7 +11535,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="391" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="391" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
         <v>362</v>
       </c>
@@ -11561,7 +11561,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="392" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="392" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
         <v>362</v>
       </c>
@@ -11587,7 +11587,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="393" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="393" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
         <v>362</v>
       </c>
@@ -11613,7 +11613,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="394" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="394" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
         <v>362</v>
       </c>
@@ -11639,7 +11639,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="395" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="395" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
         <v>362</v>
       </c>
@@ -11665,7 +11665,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="396" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="396" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
         <v>362</v>
       </c>
@@ -11691,7 +11691,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="397" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="397" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
         <v>362</v>
       </c>
@@ -11717,7 +11717,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="398" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="398" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
         <v>362</v>
       </c>
@@ -11743,7 +11743,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="399" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="399" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
         <v>362</v>
       </c>
@@ -11769,7 +11769,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="400" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="400" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
         <v>362</v>
       </c>
@@ -11795,7 +11795,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="401" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="401" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
         <v>362</v>
       </c>
@@ -11821,7 +11821,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="402" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="402" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
         <v>362</v>
       </c>
@@ -11847,7 +11847,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="403" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="403" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
         <v>362</v>
       </c>
@@ -11873,7 +11873,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="404" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="404" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
         <v>362</v>
       </c>
@@ -11899,7 +11899,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="405" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="405" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
         <v>362</v>
       </c>
@@ -11925,7 +11925,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="406" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="406" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
         <v>362</v>
       </c>
@@ -11951,7 +11951,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="407" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="407" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
         <v>362</v>
       </c>
@@ -11977,7 +11977,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="408" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="408" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
         <v>362</v>
       </c>
@@ -12003,7 +12003,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="409" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="409" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
         <v>362</v>
       </c>
@@ -12029,7 +12029,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="410" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="410" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
         <v>362</v>
       </c>
@@ -12055,7 +12055,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="411" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="411" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
         <v>362</v>
       </c>
@@ -12081,7 +12081,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="412" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="412" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
         <v>362</v>
       </c>
@@ -12107,7 +12107,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="413" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="413" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
         <v>362</v>
       </c>
@@ -12133,7 +12133,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="414" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="414" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
         <v>362</v>
       </c>
@@ -12159,7 +12159,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="415" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="415" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
         <v>362</v>
       </c>
@@ -12185,7 +12185,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="416" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="416" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
         <v>362</v>
       </c>
@@ -12211,7 +12211,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="417" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="417" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
         <v>362</v>
       </c>
@@ -12237,12 +12237,12 @@
         <v>394</v>
       </c>
     </row>
-    <row r="418" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="418" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A418" s="4" t="s">
         <v>362</v>
       </c>
       <c r="B418" s="4" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="C418" s="4">
         <v>990693</v>
@@ -12262,15 +12262,15 @@
         <v>458</v>
       </c>
       <c r="J418" s="4" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="419" spans="1:10" x14ac:dyDescent="0.35">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="419" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A419" s="4" t="s">
         <v>362</v>
       </c>
       <c r="B419" s="4" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="C419" s="4">
         <v>990694</v>
@@ -12290,15 +12290,15 @@
         <v>458</v>
       </c>
       <c r="J419" s="4" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="420" spans="1:10" x14ac:dyDescent="0.35">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="420" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A420" s="4" t="s">
         <v>362</v>
       </c>
       <c r="B420" s="4" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="C420" s="4">
         <v>990695</v>
@@ -12318,15 +12318,15 @@
         <v>459</v>
       </c>
       <c r="J420" s="4" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="421" spans="1:10" x14ac:dyDescent="0.35">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="421" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A421" s="4" t="s">
         <v>362</v>
       </c>
       <c r="B421" s="4" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="C421" s="4">
         <v>990696</v>
@@ -12346,10 +12346,10 @@
         <v>459</v>
       </c>
       <c r="J421" s="4" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="422" spans="1:10" x14ac:dyDescent="0.35">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="422" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
         <v>362</v>
       </c>
@@ -12375,7 +12375,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="423" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="423" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
         <v>362</v>
       </c>
@@ -12401,7 +12401,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="424" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="424" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
         <v>362</v>
       </c>
@@ -12427,7 +12427,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="425" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="425" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
         <v>362</v>
       </c>
@@ -12453,12 +12453,12 @@
         <v>393</v>
       </c>
     </row>
-    <row r="426" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="426" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
         <v>362</v>
       </c>
       <c r="B426" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="C426">
         <v>990857</v>
@@ -12473,18 +12473,18 @@
         <v>1E-3</v>
       </c>
       <c r="I426" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="J426" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="427" spans="1:10" x14ac:dyDescent="0.35">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="427" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
         <v>362</v>
       </c>
       <c r="B427" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="C427">
         <v>990858</v>
@@ -12499,13 +12499,13 @@
         <v>1E-3</v>
       </c>
       <c r="I427" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="J427" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="428" spans="1:10" x14ac:dyDescent="0.35">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="428" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
         <v>362</v>
       </c>
@@ -12531,7 +12531,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="429" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="429" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
         <v>362</v>
       </c>
@@ -12557,7 +12557,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="430" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="430" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
         <v>362</v>
       </c>
@@ -12583,7 +12583,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="431" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="431" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A431" t="s">
         <v>362</v>
       </c>
@@ -12609,7 +12609,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="432" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="432" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A432" t="s">
         <v>362</v>
       </c>
@@ -12635,7 +12635,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="433" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="433" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
         <v>362</v>
       </c>
@@ -12661,7 +12661,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="434" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="434" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A434" t="s">
         <v>362</v>
       </c>
@@ -12687,7 +12687,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="435" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="435" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
         <v>362</v>
       </c>
@@ -12713,7 +12713,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="436" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="436" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
         <v>362</v>
       </c>
@@ -12739,7 +12739,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="437" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="437" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A437" t="s">
         <v>362</v>
       </c>
@@ -12765,7 +12765,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="438" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="438" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A438" t="s">
         <v>362</v>
       </c>
@@ -12791,7 +12791,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="439" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="439" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A439" t="s">
         <v>362</v>
       </c>
@@ -12817,7 +12817,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="440" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="440" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A440" t="s">
         <v>362</v>
       </c>
@@ -12843,7 +12843,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="441" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="441" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A441" t="s">
         <v>362</v>
       </c>
@@ -12869,7 +12869,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="442" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="442" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A442" t="s">
         <v>362</v>
       </c>
@@ -12895,7 +12895,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="443" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="443" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A443" t="s">
         <v>362</v>
       </c>
@@ -12921,7 +12921,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="444" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="444" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A444" t="s">
         <v>362</v>
       </c>
@@ -12947,7 +12947,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="445" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="445" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A445" t="s">
         <v>362</v>
       </c>
@@ -12973,7 +12973,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="446" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="446" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A446" t="s">
         <v>362</v>
       </c>
@@ -12999,7 +12999,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="447" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="447" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A447" t="s">
         <v>362</v>
       </c>
@@ -13025,7 +13025,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="448" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="448" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A448" t="s">
         <v>362</v>
       </c>
@@ -13051,7 +13051,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="449" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="449" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A449" t="s">
         <v>362</v>
       </c>
@@ -13077,7 +13077,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="450" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="450" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A450" t="s">
         <v>455</v>
       </c>
@@ -13106,7 +13106,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="451" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="451" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A451" t="s">
         <v>455</v>
       </c>
@@ -13135,7 +13135,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="452" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="452" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A452" t="s">
         <v>455</v>
       </c>
@@ -13164,7 +13164,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="453" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="453" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A453" t="s">
         <v>455</v>
       </c>
@@ -13193,7 +13193,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="454" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="454" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A454" t="s">
         <v>455</v>
       </c>
@@ -13222,7 +13222,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="455" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="455" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A455" t="s">
         <v>455</v>
       </c>
@@ -13251,7 +13251,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="456" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="456" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A456" t="s">
         <v>455</v>
       </c>
@@ -13280,7 +13280,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="457" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="457" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A457" t="s">
         <v>455</v>
       </c>
@@ -13309,7 +13309,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="458" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="458" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A458" t="s">
         <v>455</v>
       </c>
@@ -13338,7 +13338,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="459" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="459" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A459" t="s">
         <v>455</v>
       </c>
@@ -13364,7 +13364,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="460" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="460" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A460" t="s">
         <v>455</v>
       </c>
@@ -13390,7 +13390,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="461" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="461" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A461" t="s">
         <v>455</v>
       </c>
@@ -13416,12 +13416,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="462" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="462" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A462" t="s">
         <v>455</v>
       </c>
       <c r="B462" t="s">
-        <v>473</v>
+        <v>467</v>
       </c>
       <c r="C462">
         <v>1010309</v>
@@ -13442,15 +13442,15 @@
         <v>#N/A</v>
       </c>
       <c r="K462" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="463" spans="1:11" x14ac:dyDescent="0.35">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="463" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A463" t="s">
         <v>455</v>
       </c>
       <c r="B463" t="s">
-        <v>474</v>
+        <v>468</v>
       </c>
       <c r="C463">
         <v>1010310</v>
@@ -13471,15 +13471,15 @@
         <v>#N/A</v>
       </c>
       <c r="K463" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="464" spans="1:11" x14ac:dyDescent="0.35">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="464" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A464" t="s">
         <v>455</v>
       </c>
       <c r="B464" t="s">
-        <v>477</v>
+        <v>471</v>
       </c>
       <c r="C464">
         <v>800601</v>
@@ -13500,15 +13500,15 @@
         <v>#N/A</v>
       </c>
       <c r="K464" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="465" spans="1:11" x14ac:dyDescent="0.35">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="465" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A465" t="s">
         <v>455</v>
       </c>
       <c r="B465" t="s">
-        <v>477</v>
+        <v>471</v>
       </c>
       <c r="C465">
         <v>800602</v>
@@ -13529,11 +13529,11 @@
         <v>#N/A</v>
       </c>
       <c r="K465" t="s">
-        <v>478</v>
+        <v>472</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J461" xr:uid="{11CF1E80-DA68-4CB3-BCA6-87A36AC41371}"/>
+  <autoFilter ref="A1:J465" xr:uid="{11CF1E80-DA68-4CB3-BCA6-87A36AC41371}"/>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -13551,18 +13551,18 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>324</v>
       </c>
@@ -13570,7 +13570,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>328</v>
       </c>
@@ -13578,7 +13578,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>323</v>
       </c>

</xml_diff>

<commit_message>
Added 2800308 for northbound (westbound in South Bay) 280
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/TOLLCLASS_Designations.xlsx
+++ b/utilities/NextGenFwys/TOLLCLASS_Designations.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one-master\utilities\NextGenFwys\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sisrael\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D697986-AB5B-4AD7-84C3-4528E6992431}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7218028F-4202-42D1-928E-E03B63052863}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{0F0A9957-56E7-4C48-967B-2AB2A1965C2F}"/>
+    <workbookView xWindow="33720" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{0F0A9957-56E7-4C48-967B-2AB2A1965C2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs_for_tollcalib" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1817" uniqueCount="481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1819" uniqueCount="481">
   <si>
     <t>SR92 SM - I-280 Interchange to US101 Interchange - WB</t>
   </si>
@@ -1885,11 +1885,11 @@
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
-  <dimension ref="A1:K530"/>
+  <dimension ref="A1:K531"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A453" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B466" sqref="B466"/>
+      <selection pane="bottomLeft" activeCell="B468" sqref="B468"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13656,7 +13656,7 @@
         <v>480</v>
       </c>
       <c r="C476">
-        <v>2800309</v>
+        <v>2800308</v>
       </c>
     </row>
     <row r="477" spans="1:11" x14ac:dyDescent="0.35">
@@ -13667,7 +13667,7 @@
         <v>480</v>
       </c>
       <c r="C477">
-        <v>2800310</v>
+        <v>2800309</v>
       </c>
     </row>
     <row r="478" spans="1:11" x14ac:dyDescent="0.35">
@@ -13678,7 +13678,7 @@
         <v>480</v>
       </c>
       <c r="C478">
-        <v>2800311</v>
+        <v>2800310</v>
       </c>
     </row>
     <row r="479" spans="1:11" x14ac:dyDescent="0.35">
@@ -13689,7 +13689,7 @@
         <v>480</v>
       </c>
       <c r="C479">
-        <v>2800312</v>
+        <v>2800311</v>
       </c>
     </row>
     <row r="480" spans="1:11" x14ac:dyDescent="0.35">
@@ -13700,7 +13700,7 @@
         <v>480</v>
       </c>
       <c r="C480">
-        <v>2800313</v>
+        <v>2800312</v>
       </c>
     </row>
     <row r="481" spans="1:3" x14ac:dyDescent="0.35">
@@ -13711,7 +13711,7 @@
         <v>480</v>
       </c>
       <c r="C481">
-        <v>2800314</v>
+        <v>2800313</v>
       </c>
     </row>
     <row r="482" spans="1:3" x14ac:dyDescent="0.35">
@@ -13722,7 +13722,7 @@
         <v>480</v>
       </c>
       <c r="C482">
-        <v>2800315</v>
+        <v>2800314</v>
       </c>
     </row>
     <row r="483" spans="1:3" x14ac:dyDescent="0.35">
@@ -13733,7 +13733,7 @@
         <v>480</v>
       </c>
       <c r="C483">
-        <v>40516</v>
+        <v>2800315</v>
       </c>
     </row>
     <row r="484" spans="1:3" x14ac:dyDescent="0.35">
@@ -13744,7 +13744,7 @@
         <v>480</v>
       </c>
       <c r="C484">
-        <v>40517</v>
+        <v>40516</v>
       </c>
     </row>
     <row r="485" spans="1:3" x14ac:dyDescent="0.35">
@@ -13755,7 +13755,7 @@
         <v>480</v>
       </c>
       <c r="C485">
-        <v>40518</v>
+        <v>40517</v>
       </c>
     </row>
     <row r="486" spans="1:3" x14ac:dyDescent="0.35">
@@ -13766,7 +13766,7 @@
         <v>480</v>
       </c>
       <c r="C486">
-        <v>40519</v>
+        <v>40518</v>
       </c>
     </row>
     <row r="487" spans="1:3" x14ac:dyDescent="0.35">
@@ -13777,7 +13777,7 @@
         <v>480</v>
       </c>
       <c r="C487">
-        <v>5800420</v>
+        <v>40519</v>
       </c>
     </row>
     <row r="488" spans="1:3" x14ac:dyDescent="0.35">
@@ -13788,7 +13788,7 @@
         <v>480</v>
       </c>
       <c r="C488">
-        <v>5800421</v>
+        <v>5800420</v>
       </c>
     </row>
     <row r="489" spans="1:3" x14ac:dyDescent="0.35">
@@ -13799,7 +13799,7 @@
         <v>480</v>
       </c>
       <c r="C489">
-        <v>5800422</v>
+        <v>5800421</v>
       </c>
     </row>
     <row r="490" spans="1:3" x14ac:dyDescent="0.35">
@@ -13810,7 +13810,7 @@
         <v>480</v>
       </c>
       <c r="C490">
-        <v>5800423</v>
+        <v>5800422</v>
       </c>
     </row>
     <row r="491" spans="1:3" x14ac:dyDescent="0.35">
@@ -13821,7 +13821,7 @@
         <v>480</v>
       </c>
       <c r="C491">
-        <v>5800424</v>
+        <v>5800423</v>
       </c>
     </row>
     <row r="492" spans="1:3" x14ac:dyDescent="0.35">
@@ -13832,7 +13832,7 @@
         <v>480</v>
       </c>
       <c r="C492">
-        <v>5800425</v>
+        <v>5800424</v>
       </c>
     </row>
     <row r="493" spans="1:3" x14ac:dyDescent="0.35">
@@ -13843,7 +13843,7 @@
         <v>480</v>
       </c>
       <c r="C493">
-        <v>5800426</v>
+        <v>5800425</v>
       </c>
     </row>
     <row r="494" spans="1:3" x14ac:dyDescent="0.35">
@@ -13854,7 +13854,7 @@
         <v>480</v>
       </c>
       <c r="C494">
-        <v>5800427</v>
+        <v>5800426</v>
       </c>
     </row>
     <row r="495" spans="1:3" x14ac:dyDescent="0.35">
@@ -13865,7 +13865,7 @@
         <v>480</v>
       </c>
       <c r="C495">
-        <v>6800528</v>
+        <v>5800427</v>
       </c>
     </row>
     <row r="496" spans="1:3" x14ac:dyDescent="0.35">
@@ -13876,7 +13876,7 @@
         <v>480</v>
       </c>
       <c r="C496">
-        <v>6800529</v>
+        <v>6800528</v>
       </c>
     </row>
     <row r="497" spans="1:3" x14ac:dyDescent="0.35">
@@ -13887,7 +13887,7 @@
         <v>480</v>
       </c>
       <c r="C497">
-        <v>6800330</v>
+        <v>6800529</v>
       </c>
     </row>
     <row r="498" spans="1:3" x14ac:dyDescent="0.35">
@@ -13898,7 +13898,7 @@
         <v>480</v>
       </c>
       <c r="C498">
-        <v>850331</v>
+        <v>6800330</v>
       </c>
     </row>
     <row r="499" spans="1:3" x14ac:dyDescent="0.35">
@@ -13909,7 +13909,7 @@
         <v>480</v>
       </c>
       <c r="C499">
-        <v>850332</v>
+        <v>850331</v>
       </c>
     </row>
     <row r="500" spans="1:3" x14ac:dyDescent="0.35">
@@ -13920,7 +13920,7 @@
         <v>480</v>
       </c>
       <c r="C500">
-        <v>850333</v>
+        <v>850332</v>
       </c>
     </row>
     <row r="501" spans="1:3" x14ac:dyDescent="0.35">
@@ -13931,7 +13931,7 @@
         <v>480</v>
       </c>
       <c r="C501">
-        <v>850334</v>
+        <v>850333</v>
       </c>
     </row>
     <row r="502" spans="1:3" x14ac:dyDescent="0.35">
@@ -13942,7 +13942,7 @@
         <v>480</v>
       </c>
       <c r="C502">
-        <v>870335</v>
+        <v>850334</v>
       </c>
     </row>
     <row r="503" spans="1:3" x14ac:dyDescent="0.35">
@@ -13953,7 +13953,7 @@
         <v>480</v>
       </c>
       <c r="C503">
-        <v>870336</v>
+        <v>870335</v>
       </c>
     </row>
     <row r="504" spans="1:3" x14ac:dyDescent="0.35">
@@ -13964,7 +13964,7 @@
         <v>480</v>
       </c>
       <c r="C504">
-        <v>870337</v>
+        <v>870336</v>
       </c>
     </row>
     <row r="505" spans="1:3" x14ac:dyDescent="0.35">
@@ -13975,7 +13975,7 @@
         <v>480</v>
       </c>
       <c r="C505">
-        <v>870338</v>
+        <v>870337</v>
       </c>
     </row>
     <row r="506" spans="1:3" x14ac:dyDescent="0.35">
@@ -13986,7 +13986,7 @@
         <v>480</v>
       </c>
       <c r="C506">
-        <v>8800439</v>
+        <v>870338</v>
       </c>
     </row>
     <row r="507" spans="1:3" x14ac:dyDescent="0.35">
@@ -13997,7 +13997,7 @@
         <v>480</v>
       </c>
       <c r="C507">
-        <v>8800440</v>
+        <v>8800439</v>
       </c>
     </row>
     <row r="508" spans="1:3" x14ac:dyDescent="0.35">
@@ -14008,7 +14008,7 @@
         <v>480</v>
       </c>
       <c r="C508">
-        <v>8800441</v>
+        <v>8800440</v>
       </c>
     </row>
     <row r="509" spans="1:3" x14ac:dyDescent="0.35">
@@ -14019,7 +14019,7 @@
         <v>480</v>
       </c>
       <c r="C509">
-        <v>8800442</v>
+        <v>8800441</v>
       </c>
     </row>
     <row r="510" spans="1:3" x14ac:dyDescent="0.35">
@@ -14030,7 +14030,7 @@
         <v>480</v>
       </c>
       <c r="C510">
-        <v>8800443</v>
+        <v>8800442</v>
       </c>
     </row>
     <row r="511" spans="1:3" x14ac:dyDescent="0.35">
@@ -14041,7 +14041,7 @@
         <v>480</v>
       </c>
       <c r="C511">
-        <v>6800544</v>
+        <v>8800443</v>
       </c>
     </row>
     <row r="512" spans="1:3" x14ac:dyDescent="0.35">
@@ -14052,7 +14052,7 @@
         <v>480</v>
       </c>
       <c r="C512">
-        <v>6800545</v>
+        <v>6800544</v>
       </c>
     </row>
     <row r="513" spans="1:3" x14ac:dyDescent="0.35">
@@ -14063,7 +14063,7 @@
         <v>480</v>
       </c>
       <c r="C513">
-        <v>8800446</v>
+        <v>6800545</v>
       </c>
     </row>
     <row r="514" spans="1:3" x14ac:dyDescent="0.35">
@@ -14074,7 +14074,7 @@
         <v>480</v>
       </c>
       <c r="C514">
-        <v>8800447</v>
+        <v>8800446</v>
       </c>
     </row>
     <row r="515" spans="1:3" x14ac:dyDescent="0.35">
@@ -14085,7 +14085,7 @@
         <v>480</v>
       </c>
       <c r="C515">
-        <v>8800448</v>
+        <v>8800447</v>
       </c>
     </row>
     <row r="516" spans="1:3" x14ac:dyDescent="0.35">
@@ -14096,7 +14096,7 @@
         <v>480</v>
       </c>
       <c r="C516">
-        <v>8800349</v>
+        <v>8800448</v>
       </c>
     </row>
     <row r="517" spans="1:3" x14ac:dyDescent="0.35">
@@ -14107,7 +14107,7 @@
         <v>480</v>
       </c>
       <c r="C517">
-        <v>8800449</v>
+        <v>8800349</v>
       </c>
     </row>
     <row r="518" spans="1:3" x14ac:dyDescent="0.35">
@@ -14118,7 +14118,7 @@
         <v>480</v>
       </c>
       <c r="C518">
-        <v>8800450</v>
+        <v>8800449</v>
       </c>
     </row>
     <row r="519" spans="1:3" x14ac:dyDescent="0.35">
@@ -14129,7 +14129,7 @@
         <v>480</v>
       </c>
       <c r="C519">
-        <v>8800351</v>
+        <v>8800450</v>
       </c>
     </row>
     <row r="520" spans="1:3" x14ac:dyDescent="0.35">
@@ -14140,7 +14140,7 @@
         <v>480</v>
       </c>
       <c r="C520">
-        <v>8800451</v>
+        <v>8800351</v>
       </c>
     </row>
     <row r="521" spans="1:3" x14ac:dyDescent="0.35">
@@ -14151,7 +14151,7 @@
         <v>480</v>
       </c>
       <c r="C521">
-        <v>8800452</v>
+        <v>8800451</v>
       </c>
     </row>
     <row r="522" spans="1:3" x14ac:dyDescent="0.35">
@@ -14162,7 +14162,7 @@
         <v>480</v>
       </c>
       <c r="C522">
-        <v>1010253</v>
+        <v>8800452</v>
       </c>
     </row>
     <row r="523" spans="1:3" x14ac:dyDescent="0.35">
@@ -14173,7 +14173,7 @@
         <v>480</v>
       </c>
       <c r="C523">
-        <v>1010254</v>
+        <v>1010253</v>
       </c>
     </row>
     <row r="524" spans="1:3" x14ac:dyDescent="0.35">
@@ -14184,7 +14184,7 @@
         <v>480</v>
       </c>
       <c r="C524">
-        <v>1010255</v>
+        <v>1010254</v>
       </c>
     </row>
     <row r="525" spans="1:3" x14ac:dyDescent="0.35">
@@ -14195,7 +14195,7 @@
         <v>480</v>
       </c>
       <c r="C525">
-        <v>1010256</v>
+        <v>1010255</v>
       </c>
     </row>
     <row r="526" spans="1:3" x14ac:dyDescent="0.35">
@@ -14206,7 +14206,7 @@
         <v>480</v>
       </c>
       <c r="C526">
-        <v>1010356</v>
+        <v>1010256</v>
       </c>
     </row>
     <row r="527" spans="1:3" x14ac:dyDescent="0.35">
@@ -14217,7 +14217,7 @@
         <v>480</v>
       </c>
       <c r="C527">
-        <v>1010257</v>
+        <v>1010356</v>
       </c>
     </row>
     <row r="528" spans="1:3" x14ac:dyDescent="0.35">
@@ -14228,7 +14228,7 @@
         <v>480</v>
       </c>
       <c r="C528">
-        <v>1010258</v>
+        <v>1010257</v>
       </c>
     </row>
     <row r="529" spans="1:3" x14ac:dyDescent="0.35">
@@ -14239,7 +14239,7 @@
         <v>480</v>
       </c>
       <c r="C529">
-        <v>1010259</v>
+        <v>1010258</v>
       </c>
     </row>
     <row r="530" spans="1:3" x14ac:dyDescent="0.35">
@@ -14250,6 +14250,17 @@
         <v>480</v>
       </c>
       <c r="C530">
+        <v>1010259</v>
+      </c>
+    </row>
+    <row r="531" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A531" t="s">
+        <v>479</v>
+      </c>
+      <c r="B531" t="s">
+        <v>480</v>
+      </c>
+      <c r="C531">
         <v>1010260</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added tollclasses 6800530, 531, 532, 533
https://app.asana.com/0/0/1207386873764342/f
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/TOLLCLASS_Designations.xlsx
+++ b/utilities/NextGenFwys/TOLLCLASS_Designations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sisrael\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7218028F-4202-42D1-928E-E03B63052863}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DD309B9-1CAA-4DA9-8FCD-8283D08A442C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33720" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{0F0A9957-56E7-4C48-967B-2AB2A1965C2F}"/>
+    <workbookView xWindow="33720" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0F0A9957-56E7-4C48-967B-2AB2A1965C2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs_for_tollcalib" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1819" uniqueCount="481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1823" uniqueCount="483">
   <si>
     <t>SR92 SM - I-280 Interchange to US101 Interchange - WB</t>
   </si>
@@ -1482,6 +1482,12 @@
   </si>
   <si>
     <t>RouteNum*10000 + CountyNum*100 + SegmentNum</t>
+  </si>
+  <si>
+    <t>NextGenFwyR3</t>
+  </si>
+  <si>
+    <t>NextGenFwyR4</t>
   </si>
 </sst>
 </file>
@@ -1885,11 +1891,11 @@
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
-  <dimension ref="A1:K531"/>
+  <dimension ref="A1:K533"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A453" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B468" sqref="B468"/>
+      <pane ySplit="1" topLeftCell="A472" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B498" sqref="B498"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13876,7 +13882,7 @@
         <v>480</v>
       </c>
       <c r="C496">
-        <v>6800528</v>
+        <v>6800530</v>
       </c>
     </row>
     <row r="497" spans="1:3" x14ac:dyDescent="0.35">
@@ -13887,29 +13893,29 @@
         <v>480</v>
       </c>
       <c r="C497">
-        <v>6800529</v>
+        <v>6800531</v>
       </c>
     </row>
     <row r="498" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A498" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="B498" t="s">
         <v>480</v>
       </c>
       <c r="C498">
-        <v>6800330</v>
+        <v>6800532</v>
       </c>
     </row>
     <row r="499" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A499" t="s">
-        <v>479</v>
+        <v>482</v>
       </c>
       <c r="B499" t="s">
         <v>480</v>
       </c>
       <c r="C499">
-        <v>850331</v>
+        <v>6800533</v>
       </c>
     </row>
     <row r="500" spans="1:3" x14ac:dyDescent="0.35">
@@ -13920,7 +13926,7 @@
         <v>480</v>
       </c>
       <c r="C500">
-        <v>850332</v>
+        <v>6800330</v>
       </c>
     </row>
     <row r="501" spans="1:3" x14ac:dyDescent="0.35">
@@ -13931,7 +13937,7 @@
         <v>480</v>
       </c>
       <c r="C501">
-        <v>850333</v>
+        <v>850331</v>
       </c>
     </row>
     <row r="502" spans="1:3" x14ac:dyDescent="0.35">
@@ -13942,7 +13948,7 @@
         <v>480</v>
       </c>
       <c r="C502">
-        <v>850334</v>
+        <v>850332</v>
       </c>
     </row>
     <row r="503" spans="1:3" x14ac:dyDescent="0.35">
@@ -13953,7 +13959,7 @@
         <v>480</v>
       </c>
       <c r="C503">
-        <v>870335</v>
+        <v>850333</v>
       </c>
     </row>
     <row r="504" spans="1:3" x14ac:dyDescent="0.35">
@@ -13964,7 +13970,7 @@
         <v>480</v>
       </c>
       <c r="C504">
-        <v>870336</v>
+        <v>850334</v>
       </c>
     </row>
     <row r="505" spans="1:3" x14ac:dyDescent="0.35">
@@ -13975,7 +13981,7 @@
         <v>480</v>
       </c>
       <c r="C505">
-        <v>870337</v>
+        <v>870335</v>
       </c>
     </row>
     <row r="506" spans="1:3" x14ac:dyDescent="0.35">
@@ -13986,7 +13992,7 @@
         <v>480</v>
       </c>
       <c r="C506">
-        <v>870338</v>
+        <v>870336</v>
       </c>
     </row>
     <row r="507" spans="1:3" x14ac:dyDescent="0.35">
@@ -13997,7 +14003,7 @@
         <v>480</v>
       </c>
       <c r="C507">
-        <v>8800439</v>
+        <v>870337</v>
       </c>
     </row>
     <row r="508" spans="1:3" x14ac:dyDescent="0.35">
@@ -14008,7 +14014,7 @@
         <v>480</v>
       </c>
       <c r="C508">
-        <v>8800440</v>
+        <v>870338</v>
       </c>
     </row>
     <row r="509" spans="1:3" x14ac:dyDescent="0.35">
@@ -14019,7 +14025,7 @@
         <v>480</v>
       </c>
       <c r="C509">
-        <v>8800441</v>
+        <v>8800439</v>
       </c>
     </row>
     <row r="510" spans="1:3" x14ac:dyDescent="0.35">
@@ -14030,7 +14036,7 @@
         <v>480</v>
       </c>
       <c r="C510">
-        <v>8800442</v>
+        <v>8800440</v>
       </c>
     </row>
     <row r="511" spans="1:3" x14ac:dyDescent="0.35">
@@ -14041,7 +14047,7 @@
         <v>480</v>
       </c>
       <c r="C511">
-        <v>8800443</v>
+        <v>8800441</v>
       </c>
     </row>
     <row r="512" spans="1:3" x14ac:dyDescent="0.35">
@@ -14052,7 +14058,7 @@
         <v>480</v>
       </c>
       <c r="C512">
-        <v>6800544</v>
+        <v>8800442</v>
       </c>
     </row>
     <row r="513" spans="1:3" x14ac:dyDescent="0.35">
@@ -14063,7 +14069,7 @@
         <v>480</v>
       </c>
       <c r="C513">
-        <v>6800545</v>
+        <v>8800443</v>
       </c>
     </row>
     <row r="514" spans="1:3" x14ac:dyDescent="0.35">
@@ -14074,7 +14080,7 @@
         <v>480</v>
       </c>
       <c r="C514">
-        <v>8800446</v>
+        <v>6800544</v>
       </c>
     </row>
     <row r="515" spans="1:3" x14ac:dyDescent="0.35">
@@ -14085,7 +14091,7 @@
         <v>480</v>
       </c>
       <c r="C515">
-        <v>8800447</v>
+        <v>6800545</v>
       </c>
     </row>
     <row r="516" spans="1:3" x14ac:dyDescent="0.35">
@@ -14096,7 +14102,7 @@
         <v>480</v>
       </c>
       <c r="C516">
-        <v>8800448</v>
+        <v>8800446</v>
       </c>
     </row>
     <row r="517" spans="1:3" x14ac:dyDescent="0.35">
@@ -14107,7 +14113,7 @@
         <v>480</v>
       </c>
       <c r="C517">
-        <v>8800349</v>
+        <v>8800447</v>
       </c>
     </row>
     <row r="518" spans="1:3" x14ac:dyDescent="0.35">
@@ -14118,7 +14124,7 @@
         <v>480</v>
       </c>
       <c r="C518">
-        <v>8800449</v>
+        <v>8800448</v>
       </c>
     </row>
     <row r="519" spans="1:3" x14ac:dyDescent="0.35">
@@ -14129,7 +14135,7 @@
         <v>480</v>
       </c>
       <c r="C519">
-        <v>8800450</v>
+        <v>8800349</v>
       </c>
     </row>
     <row r="520" spans="1:3" x14ac:dyDescent="0.35">
@@ -14140,7 +14146,7 @@
         <v>480</v>
       </c>
       <c r="C520">
-        <v>8800351</v>
+        <v>8800449</v>
       </c>
     </row>
     <row r="521" spans="1:3" x14ac:dyDescent="0.35">
@@ -14151,7 +14157,7 @@
         <v>480</v>
       </c>
       <c r="C521">
-        <v>8800451</v>
+        <v>8800450</v>
       </c>
     </row>
     <row r="522" spans="1:3" x14ac:dyDescent="0.35">
@@ -14162,7 +14168,7 @@
         <v>480</v>
       </c>
       <c r="C522">
-        <v>8800452</v>
+        <v>8800351</v>
       </c>
     </row>
     <row r="523" spans="1:3" x14ac:dyDescent="0.35">
@@ -14173,7 +14179,7 @@
         <v>480</v>
       </c>
       <c r="C523">
-        <v>1010253</v>
+        <v>8800451</v>
       </c>
     </row>
     <row r="524" spans="1:3" x14ac:dyDescent="0.35">
@@ -14184,7 +14190,7 @@
         <v>480</v>
       </c>
       <c r="C524">
-        <v>1010254</v>
+        <v>8800452</v>
       </c>
     </row>
     <row r="525" spans="1:3" x14ac:dyDescent="0.35">
@@ -14195,7 +14201,7 @@
         <v>480</v>
       </c>
       <c r="C525">
-        <v>1010255</v>
+        <v>1010253</v>
       </c>
     </row>
     <row r="526" spans="1:3" x14ac:dyDescent="0.35">
@@ -14206,7 +14212,7 @@
         <v>480</v>
       </c>
       <c r="C526">
-        <v>1010256</v>
+        <v>1010254</v>
       </c>
     </row>
     <row r="527" spans="1:3" x14ac:dyDescent="0.35">
@@ -14217,7 +14223,7 @@
         <v>480</v>
       </c>
       <c r="C527">
-        <v>1010356</v>
+        <v>1010255</v>
       </c>
     </row>
     <row r="528" spans="1:3" x14ac:dyDescent="0.35">
@@ -14228,7 +14234,7 @@
         <v>480</v>
       </c>
       <c r="C528">
-        <v>1010257</v>
+        <v>1010256</v>
       </c>
     </row>
     <row r="529" spans="1:3" x14ac:dyDescent="0.35">
@@ -14239,7 +14245,7 @@
         <v>480</v>
       </c>
       <c r="C529">
-        <v>1010258</v>
+        <v>1010356</v>
       </c>
     </row>
     <row r="530" spans="1:3" x14ac:dyDescent="0.35">
@@ -14250,7 +14256,7 @@
         <v>480</v>
       </c>
       <c r="C530">
-        <v>1010259</v>
+        <v>1010257</v>
       </c>
     </row>
     <row r="531" spans="1:3" x14ac:dyDescent="0.35">
@@ -14261,6 +14267,28 @@
         <v>480</v>
       </c>
       <c r="C531">
+        <v>1010258</v>
+      </c>
+    </row>
+    <row r="532" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A532" t="s">
+        <v>479</v>
+      </c>
+      <c r="B532" t="s">
+        <v>480</v>
+      </c>
+      <c r="C532">
+        <v>1010259</v>
+      </c>
+    </row>
+    <row r="533" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A533" t="s">
+        <v>479</v>
+      </c>
+      <c r="B533" t="s">
+        <v>480</v>
+      </c>
+      <c r="C533">
         <v>1010260</v>
       </c>
     </row>

</xml_diff>

<commit_message>
filled in THRESHOLD_SPEED, MAX_TOLL and MIN_TOLL; replace the space with _ in PBA2050_RTP_ID
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/TOLLCLASS_Designations.xlsx
+++ b/utilities/NextGenFwys/TOLLCLASS_Designations.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sisrael\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DD309B9-1CAA-4DA9-8FCD-8283D08A442C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89FBC2BD-9447-45CF-8455-5FF28E51FF04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33720" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0F0A9957-56E7-4C48-967B-2AB2A1965C2F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{0F0A9957-56E7-4C48-967B-2AB2A1965C2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs_for_tollcalib" sheetId="1" r:id="rId1"/>
@@ -1292,9 +1292,6 @@
     <t>EastBay_Inner580_AM</t>
   </si>
   <si>
-    <t>PBA2050 RTP ID</t>
-  </si>
-  <si>
     <t>AL-031</t>
   </si>
   <si>
@@ -1488,6 +1485,9 @@
   </si>
   <si>
     <t>NextGenFwyR4</t>
+  </si>
+  <si>
+    <t>PBA2050_RTP_ID</t>
   </si>
 </sst>
 </file>
@@ -1894,8 +1894,8 @@
   <dimension ref="A1:K533"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A472" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B498" sqref="B498"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1921,7 +1921,7 @@
         <v>152</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>417</v>
+        <v>482</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>151</v>
@@ -1942,7 +1942,7 @@
         <v>338</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
@@ -2388,7 +2388,7 @@
         <v>81</v>
       </c>
       <c r="D21" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="E21" t="s">
         <v>16</v>
@@ -2420,7 +2420,7 @@
         <v>82</v>
       </c>
       <c r="D22" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="E22" t="s">
         <v>16</v>
@@ -2452,7 +2452,7 @@
         <v>83</v>
       </c>
       <c r="D23" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="E23" t="s">
         <v>16</v>
@@ -2484,7 +2484,7 @@
         <v>84</v>
       </c>
       <c r="D24" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="E24" t="s">
         <v>16</v>
@@ -2516,7 +2516,7 @@
         <v>85</v>
       </c>
       <c r="D25" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="E25" t="s">
         <v>16</v>
@@ -2548,7 +2548,7 @@
         <v>86</v>
       </c>
       <c r="D26" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="E26" t="s">
         <v>16</v>
@@ -2580,7 +2580,7 @@
         <v>87</v>
       </c>
       <c r="D27" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E27" t="s">
         <v>274</v>
@@ -2612,7 +2612,7 @@
         <v>88</v>
       </c>
       <c r="D28" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E28" t="s">
         <v>274</v>
@@ -2644,7 +2644,7 @@
         <v>89</v>
       </c>
       <c r="D29" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E29" t="s">
         <v>274</v>
@@ -2676,7 +2676,7 @@
         <v>90</v>
       </c>
       <c r="D30" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E30" t="s">
         <v>274</v>
@@ -2708,7 +2708,7 @@
         <v>91</v>
       </c>
       <c r="D31" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="E31" t="s">
         <v>274</v>
@@ -2740,7 +2740,7 @@
         <v>92</v>
       </c>
       <c r="D32" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="E32" t="s">
         <v>274</v>
@@ -2830,7 +2830,7 @@
         <v>101</v>
       </c>
       <c r="D35" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="E35" t="s">
         <v>16</v>
@@ -2862,7 +2862,7 @@
         <v>102</v>
       </c>
       <c r="D36" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="E36" t="s">
         <v>16</v>
@@ -2894,7 +2894,7 @@
         <v>103</v>
       </c>
       <c r="D37" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="E37" t="s">
         <v>16</v>
@@ -2926,7 +2926,7 @@
         <v>104</v>
       </c>
       <c r="D38" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="E38" t="s">
         <v>16</v>
@@ -2958,7 +2958,7 @@
         <v>105</v>
       </c>
       <c r="D39" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E39" t="s">
         <v>16</v>
@@ -2990,7 +2990,7 @@
         <v>106</v>
       </c>
       <c r="D40" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E40" t="s">
         <v>16</v>
@@ -3312,7 +3312,7 @@
         <v>117</v>
       </c>
       <c r="D51" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="E51" t="s">
         <v>16</v>
@@ -3344,7 +3344,7 @@
         <v>118</v>
       </c>
       <c r="D52" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="E52" t="s">
         <v>16</v>
@@ -3376,7 +3376,7 @@
         <v>119</v>
       </c>
       <c r="D53" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="E53" t="s">
         <v>274</v>
@@ -3408,7 +3408,7 @@
         <v>120</v>
       </c>
       <c r="D54" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="E54" t="s">
         <v>274</v>
@@ -3440,7 +3440,7 @@
         <v>121</v>
       </c>
       <c r="D55" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="E55" t="s">
         <v>274</v>
@@ -3472,7 +3472,7 @@
         <v>122</v>
       </c>
       <c r="D56" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="E56" t="s">
         <v>274</v>
@@ -4182,7 +4182,7 @@
         <v>281</v>
       </c>
       <c r="D81" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="E81" t="s">
         <v>16</v>
@@ -4214,7 +4214,7 @@
         <v>282</v>
       </c>
       <c r="D82" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="E82" t="s">
         <v>16</v>
@@ -4304,7 +4304,7 @@
         <v>285</v>
       </c>
       <c r="D85" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E85" t="s">
         <v>274</v>
@@ -4336,7 +4336,7 @@
         <v>286</v>
       </c>
       <c r="D86" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E86" t="s">
         <v>274</v>
@@ -4368,7 +4368,7 @@
         <v>287</v>
       </c>
       <c r="D87" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="E87" t="s">
         <v>16</v>
@@ -4400,7 +4400,7 @@
         <v>288</v>
       </c>
       <c r="D88" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="E88" t="s">
         <v>16</v>
@@ -4542,7 +4542,7 @@
         <v>401</v>
       </c>
       <c r="D93" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="E93" t="s">
         <v>274</v>
@@ -4574,7 +4574,7 @@
         <v>402</v>
       </c>
       <c r="D94" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="E94" t="s">
         <v>274</v>
@@ -4606,7 +4606,7 @@
         <v>403</v>
       </c>
       <c r="D95" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F95">
         <v>45</v>
@@ -4635,7 +4635,7 @@
         <v>404</v>
       </c>
       <c r="D96" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F96">
         <v>45</v>
@@ -4768,7 +4768,7 @@
         <v>581</v>
       </c>
       <c r="D101" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E101" t="s">
         <v>16</v>
@@ -4800,7 +4800,7 @@
         <v>582</v>
       </c>
       <c r="D102" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E102" t="s">
         <v>16</v>
@@ -4832,7 +4832,7 @@
         <v>583</v>
       </c>
       <c r="D103" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E103" t="s">
         <v>16</v>
@@ -4864,7 +4864,7 @@
         <v>584</v>
       </c>
       <c r="D104" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E104" t="s">
         <v>16</v>
@@ -4896,7 +4896,7 @@
         <v>585</v>
       </c>
       <c r="D105" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E105" t="s">
         <v>274</v>
@@ -4928,7 +4928,7 @@
         <v>586</v>
       </c>
       <c r="D106" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E106" t="s">
         <v>274</v>
@@ -5018,7 +5018,7 @@
         <v>589</v>
       </c>
       <c r="D109" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="E109" t="s">
         <v>274</v>
@@ -5050,7 +5050,7 @@
         <v>590</v>
       </c>
       <c r="D110" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="E110" t="s">
         <v>274</v>
@@ -5256,7 +5256,7 @@
         <v>681</v>
       </c>
       <c r="D117" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="E117" t="s">
         <v>274</v>
@@ -5317,7 +5317,7 @@
         <v>683</v>
       </c>
       <c r="D119" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="E119" t="s">
         <v>274</v>
@@ -5436,7 +5436,7 @@
         <v>687</v>
       </c>
       <c r="D123" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E123" t="s">
         <v>274</v>
@@ -5468,7 +5468,7 @@
         <v>688</v>
       </c>
       <c r="D124" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E124" t="s">
         <v>274</v>
@@ -5558,7 +5558,7 @@
         <v>691</v>
       </c>
       <c r="D127" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E127" t="s">
         <v>274</v>
@@ -5648,7 +5648,7 @@
         <v>842</v>
       </c>
       <c r="D130" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E130" t="s">
         <v>16</v>
@@ -5738,7 +5738,7 @@
         <v>851</v>
       </c>
       <c r="D133" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E133" t="s">
         <v>274</v>
@@ -5770,7 +5770,7 @@
         <v>852</v>
       </c>
       <c r="D134" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E134" t="s">
         <v>274</v>
@@ -5802,7 +5802,7 @@
         <v>853</v>
       </c>
       <c r="D135" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E135" t="s">
         <v>274</v>
@@ -5834,7 +5834,7 @@
         <v>854</v>
       </c>
       <c r="D136" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E136" t="s">
         <v>274</v>
@@ -5866,7 +5866,7 @@
         <v>855</v>
       </c>
       <c r="D137" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E137" t="s">
         <v>274</v>
@@ -5898,7 +5898,7 @@
         <v>856</v>
       </c>
       <c r="D138" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E138" t="s">
         <v>274</v>
@@ -5930,7 +5930,7 @@
         <v>871</v>
       </c>
       <c r="D139" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E139" t="s">
         <v>274</v>
@@ -5962,7 +5962,7 @@
         <v>872</v>
       </c>
       <c r="D140" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E140" t="s">
         <v>274</v>
@@ -5994,7 +5994,7 @@
         <v>879</v>
       </c>
       <c r="D141" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="F141">
         <v>45</v>
@@ -6023,7 +6023,7 @@
         <v>880</v>
       </c>
       <c r="D142" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="F142">
         <v>45</v>
@@ -6052,7 +6052,7 @@
         <v>881</v>
       </c>
       <c r="D143" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="E143" t="s">
         <v>16</v>
@@ -6287,7 +6287,7 @@
         <v>889</v>
       </c>
       <c r="D151" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E151" t="s">
         <v>16</v>
@@ -6319,7 +6319,7 @@
         <v>890</v>
       </c>
       <c r="D152" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E152" t="s">
         <v>16</v>
@@ -6438,7 +6438,7 @@
         <v>922</v>
       </c>
       <c r="D156" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E156" t="s">
         <v>16</v>
@@ -7209,6 +7209,9 @@
       <c r="C185">
         <v>770075</v>
       </c>
+      <c r="G185">
+        <v>5</v>
+      </c>
       <c r="I185" t="s">
         <v>384</v>
       </c>
@@ -7226,6 +7229,9 @@
       <c r="C186">
         <v>770076</v>
       </c>
+      <c r="G186">
+        <v>5</v>
+      </c>
       <c r="I186" t="s">
         <v>385</v>
       </c>
@@ -7243,6 +7249,9 @@
       <c r="C187">
         <v>770077</v>
       </c>
+      <c r="G187">
+        <v>5</v>
+      </c>
       <c r="I187" t="s">
         <v>385</v>
       </c>
@@ -7260,6 +7269,9 @@
       <c r="C188">
         <v>770078</v>
       </c>
+      <c r="G188">
+        <v>5</v>
+      </c>
       <c r="I188" t="s">
         <v>384</v>
       </c>
@@ -7277,6 +7289,9 @@
       <c r="C189">
         <v>770081</v>
       </c>
+      <c r="G189">
+        <v>5</v>
+      </c>
       <c r="I189" t="s">
         <v>364</v>
       </c>
@@ -7294,6 +7309,9 @@
       <c r="C190">
         <v>770082</v>
       </c>
+      <c r="G190">
+        <v>5</v>
+      </c>
       <c r="I190" t="s">
         <v>363</v>
       </c>
@@ -7311,6 +7329,9 @@
       <c r="C191">
         <v>770083</v>
       </c>
+      <c r="G191">
+        <v>5</v>
+      </c>
       <c r="I191" t="s">
         <v>365</v>
       </c>
@@ -7328,6 +7349,9 @@
       <c r="C192">
         <v>770084</v>
       </c>
+      <c r="G192">
+        <v>5</v>
+      </c>
       <c r="I192" t="s">
         <v>403</v>
       </c>
@@ -7345,6 +7369,9 @@
       <c r="C193">
         <v>770085</v>
       </c>
+      <c r="G193">
+        <v>5</v>
+      </c>
       <c r="I193" t="s">
         <v>365</v>
       </c>
@@ -7362,6 +7389,9 @@
       <c r="C194">
         <v>770086</v>
       </c>
+      <c r="G194">
+        <v>5</v>
+      </c>
       <c r="I194" t="s">
         <v>403</v>
       </c>
@@ -7379,6 +7409,9 @@
       <c r="C195">
         <v>770087</v>
       </c>
+      <c r="G195">
+        <v>5</v>
+      </c>
       <c r="I195" t="s">
         <v>372</v>
       </c>
@@ -7396,6 +7429,9 @@
       <c r="C196">
         <v>770088</v>
       </c>
+      <c r="G196">
+        <v>5</v>
+      </c>
       <c r="I196" t="s">
         <v>366</v>
       </c>
@@ -7413,6 +7449,9 @@
       <c r="C197">
         <v>770091</v>
       </c>
+      <c r="G197">
+        <v>5</v>
+      </c>
       <c r="I197" t="s">
         <v>372</v>
       </c>
@@ -7430,6 +7469,9 @@
       <c r="C198">
         <v>770092</v>
       </c>
+      <c r="G198">
+        <v>5</v>
+      </c>
       <c r="I198" t="s">
         <v>366</v>
       </c>
@@ -7447,6 +7489,9 @@
       <c r="C199">
         <v>770101</v>
       </c>
+      <c r="G199">
+        <v>5</v>
+      </c>
       <c r="I199" t="s">
         <v>384</v>
       </c>
@@ -7464,6 +7509,9 @@
       <c r="C200">
         <v>770102</v>
       </c>
+      <c r="G200">
+        <v>5</v>
+      </c>
       <c r="I200" t="s">
         <v>385</v>
       </c>
@@ -7481,6 +7529,9 @@
       <c r="C201">
         <v>770103</v>
       </c>
+      <c r="G201">
+        <v>5</v>
+      </c>
       <c r="I201" t="s">
         <v>388</v>
       </c>
@@ -7498,6 +7549,9 @@
       <c r="C202">
         <v>770104</v>
       </c>
+      <c r="G202">
+        <v>5</v>
+      </c>
       <c r="I202" t="s">
         <v>386</v>
       </c>
@@ -7515,6 +7569,9 @@
       <c r="C203">
         <v>770105</v>
       </c>
+      <c r="G203">
+        <v>5</v>
+      </c>
       <c r="I203" t="s">
         <v>388</v>
       </c>
@@ -7532,6 +7589,9 @@
       <c r="C204">
         <v>770106</v>
       </c>
+      <c r="G204">
+        <v>5</v>
+      </c>
       <c r="I204" t="s">
         <v>386</v>
       </c>
@@ -7549,6 +7609,9 @@
       <c r="C205">
         <v>770107</v>
       </c>
+      <c r="G205">
+        <v>5</v>
+      </c>
       <c r="I205" t="s">
         <v>381</v>
       </c>
@@ -7566,6 +7629,9 @@
       <c r="C206">
         <v>770108</v>
       </c>
+      <c r="G206">
+        <v>5</v>
+      </c>
       <c r="I206" t="s">
         <v>378</v>
       </c>
@@ -7583,6 +7649,9 @@
       <c r="C207">
         <v>770109</v>
       </c>
+      <c r="G207">
+        <v>5</v>
+      </c>
       <c r="I207" t="s">
         <v>381</v>
       </c>
@@ -7600,6 +7669,9 @@
       <c r="C208">
         <v>770110</v>
       </c>
+      <c r="G208">
+        <v>5</v>
+      </c>
       <c r="I208" t="s">
         <v>378</v>
       </c>
@@ -7617,6 +7689,9 @@
       <c r="C209">
         <v>770111</v>
       </c>
+      <c r="G209">
+        <v>5</v>
+      </c>
       <c r="I209" t="s">
         <v>381</v>
       </c>
@@ -7634,6 +7709,9 @@
       <c r="C210">
         <v>770112</v>
       </c>
+      <c r="G210">
+        <v>5</v>
+      </c>
       <c r="I210" t="s">
         <v>378</v>
       </c>
@@ -7651,6 +7729,9 @@
       <c r="C211">
         <v>770113</v>
       </c>
+      <c r="G211">
+        <v>5</v>
+      </c>
       <c r="I211" t="s">
         <v>381</v>
       </c>
@@ -7668,6 +7749,9 @@
       <c r="C212">
         <v>770114</v>
       </c>
+      <c r="G212">
+        <v>5</v>
+      </c>
       <c r="I212" t="s">
         <v>378</v>
       </c>
@@ -7685,6 +7769,9 @@
       <c r="C213">
         <v>770115</v>
       </c>
+      <c r="G213">
+        <v>5</v>
+      </c>
       <c r="I213" t="s">
         <v>390</v>
       </c>
@@ -7702,6 +7789,9 @@
       <c r="C214">
         <v>770116</v>
       </c>
+      <c r="G214">
+        <v>5</v>
+      </c>
       <c r="I214" t="s">
         <v>391</v>
       </c>
@@ -7719,6 +7809,9 @@
       <c r="C215">
         <v>770117</v>
       </c>
+      <c r="G215">
+        <v>5</v>
+      </c>
       <c r="I215" t="s">
         <v>390</v>
       </c>
@@ -7736,6 +7829,9 @@
       <c r="C216">
         <v>770118</v>
       </c>
+      <c r="G216">
+        <v>5</v>
+      </c>
       <c r="I216" t="s">
         <v>391</v>
       </c>
@@ -7753,6 +7849,9 @@
       <c r="C217">
         <v>770119</v>
       </c>
+      <c r="G217">
+        <v>5</v>
+      </c>
       <c r="I217" t="s">
         <v>392</v>
       </c>
@@ -7770,6 +7869,9 @@
       <c r="C218">
         <v>770120</v>
       </c>
+      <c r="G218">
+        <v>5</v>
+      </c>
       <c r="I218" t="s">
         <v>395</v>
       </c>
@@ -7787,6 +7889,9 @@
       <c r="C219">
         <v>770121</v>
       </c>
+      <c r="G219">
+        <v>5</v>
+      </c>
       <c r="I219" t="s">
         <v>366</v>
       </c>
@@ -7804,6 +7909,9 @@
       <c r="C220">
         <v>770122</v>
       </c>
+      <c r="G220">
+        <v>5</v>
+      </c>
       <c r="I220" t="s">
         <v>372</v>
       </c>
@@ -7821,6 +7929,9 @@
       <c r="C221">
         <v>770123</v>
       </c>
+      <c r="G221">
+        <v>5</v>
+      </c>
       <c r="I221" t="s">
         <v>366</v>
       </c>
@@ -7838,6 +7949,9 @@
       <c r="C222">
         <v>770124</v>
       </c>
+      <c r="G222">
+        <v>5</v>
+      </c>
       <c r="I222" t="s">
         <v>372</v>
       </c>
@@ -7855,6 +7969,9 @@
       <c r="C223">
         <v>770135</v>
       </c>
+      <c r="G223">
+        <v>5</v>
+      </c>
       <c r="I223" t="s">
         <v>372</v>
       </c>
@@ -7872,6 +7989,9 @@
       <c r="C224">
         <v>770136</v>
       </c>
+      <c r="G224">
+        <v>5</v>
+      </c>
       <c r="I224" t="s">
         <v>366</v>
       </c>
@@ -7889,6 +8009,9 @@
       <c r="C225">
         <v>770171</v>
       </c>
+      <c r="G225">
+        <v>5</v>
+      </c>
       <c r="I225" t="s">
         <v>392</v>
       </c>
@@ -7906,6 +8029,9 @@
       <c r="C226">
         <v>770172</v>
       </c>
+      <c r="G226">
+        <v>5</v>
+      </c>
       <c r="I226" t="s">
         <v>395</v>
       </c>
@@ -7923,6 +8049,9 @@
       <c r="C227">
         <v>770231</v>
       </c>
+      <c r="G227">
+        <v>5</v>
+      </c>
       <c r="I227" t="s">
         <v>391</v>
       </c>
@@ -7940,6 +8069,9 @@
       <c r="C228">
         <v>770232</v>
       </c>
+      <c r="G228">
+        <v>5</v>
+      </c>
       <c r="I228" t="s">
         <v>390</v>
       </c>
@@ -7957,6 +8089,9 @@
       <c r="C229">
         <v>770233</v>
       </c>
+      <c r="G229">
+        <v>5</v>
+      </c>
       <c r="I229" t="s">
         <v>391</v>
       </c>
@@ -7974,6 +8109,9 @@
       <c r="C230">
         <v>770234</v>
       </c>
+      <c r="G230">
+        <v>5</v>
+      </c>
       <c r="I230" t="s">
         <v>390</v>
       </c>
@@ -7991,6 +8129,9 @@
       <c r="C231">
         <v>770239</v>
       </c>
+      <c r="G231">
+        <v>5</v>
+      </c>
       <c r="I231" t="s">
         <v>365</v>
       </c>
@@ -8008,6 +8149,9 @@
       <c r="C232">
         <v>770240</v>
       </c>
+      <c r="G232">
+        <v>5</v>
+      </c>
       <c r="I232" t="s">
         <v>403</v>
       </c>
@@ -8025,6 +8169,9 @@
       <c r="C233">
         <v>770241</v>
       </c>
+      <c r="G233">
+        <v>5</v>
+      </c>
       <c r="I233" t="s">
         <v>365</v>
       </c>
@@ -8042,6 +8189,9 @@
       <c r="C234">
         <v>770242</v>
       </c>
+      <c r="G234">
+        <v>5</v>
+      </c>
       <c r="I234" t="s">
         <v>403</v>
       </c>
@@ -8059,6 +8209,9 @@
       <c r="C235">
         <v>770243</v>
       </c>
+      <c r="G235">
+        <v>5</v>
+      </c>
       <c r="I235" t="s">
         <v>365</v>
       </c>
@@ -8076,6 +8229,9 @@
       <c r="C236">
         <v>770244</v>
       </c>
+      <c r="G236">
+        <v>5</v>
+      </c>
       <c r="I236" t="s">
         <v>403</v>
       </c>
@@ -8093,6 +8249,9 @@
       <c r="C237">
         <v>770245</v>
       </c>
+      <c r="G237">
+        <v>5</v>
+      </c>
       <c r="I237" t="s">
         <v>365</v>
       </c>
@@ -8110,6 +8269,9 @@
       <c r="C238">
         <v>770246</v>
       </c>
+      <c r="G238">
+        <v>5</v>
+      </c>
       <c r="I238" t="s">
         <v>403</v>
       </c>
@@ -8127,6 +8289,9 @@
       <c r="C239">
         <v>770281</v>
       </c>
+      <c r="G239">
+        <v>5</v>
+      </c>
       <c r="I239" t="s">
         <v>384</v>
       </c>
@@ -8144,6 +8309,9 @@
       <c r="C240">
         <v>770282</v>
       </c>
+      <c r="G240">
+        <v>5</v>
+      </c>
       <c r="I240" t="s">
         <v>385</v>
       </c>
@@ -8161,6 +8329,9 @@
       <c r="C241">
         <v>770283</v>
       </c>
+      <c r="G241">
+        <v>5</v>
+      </c>
       <c r="I241" t="s">
         <v>392</v>
       </c>
@@ -8178,6 +8349,9 @@
       <c r="C242">
         <v>770284</v>
       </c>
+      <c r="G242">
+        <v>5</v>
+      </c>
       <c r="I242" t="s">
         <v>395</v>
       </c>
@@ -8195,6 +8369,9 @@
       <c r="C243">
         <v>770285</v>
       </c>
+      <c r="G243">
+        <v>5</v>
+      </c>
       <c r="I243" t="s">
         <v>392</v>
       </c>
@@ -8212,6 +8389,9 @@
       <c r="C244">
         <v>770286</v>
       </c>
+      <c r="G244">
+        <v>5</v>
+      </c>
       <c r="I244" t="s">
         <v>395</v>
       </c>
@@ -8229,6 +8409,9 @@
       <c r="C245">
         <v>770287</v>
       </c>
+      <c r="G245">
+        <v>5</v>
+      </c>
       <c r="I245" t="s">
         <v>388</v>
       </c>
@@ -8246,6 +8429,9 @@
       <c r="C246">
         <v>770288</v>
       </c>
+      <c r="G246">
+        <v>5</v>
+      </c>
       <c r="I246" t="s">
         <v>386</v>
       </c>
@@ -8263,6 +8449,9 @@
       <c r="C247">
         <v>770289</v>
       </c>
+      <c r="G247">
+        <v>5</v>
+      </c>
       <c r="I247" t="s">
         <v>378</v>
       </c>
@@ -8280,6 +8469,9 @@
       <c r="C248">
         <v>770290</v>
       </c>
+      <c r="G248">
+        <v>5</v>
+      </c>
       <c r="I248" t="s">
         <v>381</v>
       </c>
@@ -8297,6 +8489,9 @@
       <c r="C249">
         <v>770381</v>
       </c>
+      <c r="G249">
+        <v>5</v>
+      </c>
       <c r="I249" t="s">
         <v>388</v>
       </c>
@@ -8314,6 +8509,9 @@
       <c r="C250">
         <v>770382</v>
       </c>
+      <c r="G250">
+        <v>5</v>
+      </c>
       <c r="I250" t="s">
         <v>386</v>
       </c>
@@ -8331,6 +8529,9 @@
       <c r="C251">
         <v>770401</v>
       </c>
+      <c r="G251">
+        <v>5</v>
+      </c>
       <c r="I251" t="s">
         <v>372</v>
       </c>
@@ -8348,6 +8549,9 @@
       <c r="C252">
         <v>770402</v>
       </c>
+      <c r="G252">
+        <v>5</v>
+      </c>
       <c r="I252" t="s">
         <v>366</v>
       </c>
@@ -8365,6 +8569,9 @@
       <c r="C253">
         <v>770403</v>
       </c>
+      <c r="G253">
+        <v>5</v>
+      </c>
       <c r="I253" t="s">
         <v>372</v>
       </c>
@@ -8382,6 +8589,9 @@
       <c r="C254">
         <v>770404</v>
       </c>
+      <c r="G254">
+        <v>5</v>
+      </c>
       <c r="I254" t="s">
         <v>366</v>
       </c>
@@ -8399,6 +8609,9 @@
       <c r="C255">
         <v>770407</v>
       </c>
+      <c r="G255">
+        <v>5</v>
+      </c>
       <c r="I255" t="s">
         <v>372</v>
       </c>
@@ -8416,6 +8629,9 @@
       <c r="C256">
         <v>770408</v>
       </c>
+      <c r="G256">
+        <v>5</v>
+      </c>
       <c r="I256" t="s">
         <v>366</v>
       </c>
@@ -8433,6 +8649,9 @@
       <c r="C257">
         <v>770581</v>
       </c>
+      <c r="G257">
+        <v>5</v>
+      </c>
       <c r="I257" t="s">
         <v>364</v>
       </c>
@@ -8450,6 +8669,9 @@
       <c r="C258">
         <v>770582</v>
       </c>
+      <c r="G258">
+        <v>5</v>
+      </c>
       <c r="I258" t="s">
         <v>363</v>
       </c>
@@ -8467,6 +8689,9 @@
       <c r="C259">
         <v>770583</v>
       </c>
+      <c r="G259">
+        <v>5</v>
+      </c>
       <c r="I259" t="s">
         <v>364</v>
       </c>
@@ -8484,6 +8709,9 @@
       <c r="C260">
         <v>770584</v>
       </c>
+      <c r="G260">
+        <v>5</v>
+      </c>
       <c r="I260" t="s">
         <v>363</v>
       </c>
@@ -8501,6 +8729,9 @@
       <c r="C261">
         <v>770585</v>
       </c>
+      <c r="G261">
+        <v>5</v>
+      </c>
       <c r="I261" t="s">
         <v>365</v>
       </c>
@@ -8518,6 +8749,9 @@
       <c r="C262">
         <v>770586</v>
       </c>
+      <c r="G262">
+        <v>5</v>
+      </c>
       <c r="I262" t="s">
         <v>403</v>
       </c>
@@ -8535,6 +8769,9 @@
       <c r="C263">
         <v>770587</v>
       </c>
+      <c r="G263">
+        <v>5</v>
+      </c>
       <c r="I263" t="s">
         <v>372</v>
       </c>
@@ -8552,6 +8789,9 @@
       <c r="C264">
         <v>770588</v>
       </c>
+      <c r="G264">
+        <v>5</v>
+      </c>
       <c r="I264" t="s">
         <v>366</v>
       </c>
@@ -8569,6 +8809,9 @@
       <c r="C265">
         <v>770589</v>
       </c>
+      <c r="G265">
+        <v>5</v>
+      </c>
       <c r="I265" t="s">
         <v>372</v>
       </c>
@@ -8586,6 +8829,9 @@
       <c r="C266">
         <v>770590</v>
       </c>
+      <c r="G266">
+        <v>5</v>
+      </c>
       <c r="I266" t="s">
         <v>366</v>
       </c>
@@ -8603,6 +8849,9 @@
       <c r="C267">
         <v>770683</v>
       </c>
+      <c r="G267">
+        <v>5</v>
+      </c>
       <c r="I267" t="s">
         <v>365</v>
       </c>
@@ -8620,6 +8869,9 @@
       <c r="C268">
         <v>770684</v>
       </c>
+      <c r="G268">
+        <v>5</v>
+      </c>
       <c r="I268" t="s">
         <v>403</v>
       </c>
@@ -8637,6 +8889,9 @@
       <c r="C269">
         <v>770689</v>
       </c>
+      <c r="G269">
+        <v>5</v>
+      </c>
       <c r="I269" t="s">
         <v>365</v>
       </c>
@@ -8654,6 +8909,9 @@
       <c r="C270">
         <v>770690</v>
       </c>
+      <c r="G270">
+        <v>5</v>
+      </c>
       <c r="I270" t="s">
         <v>403</v>
       </c>
@@ -8671,6 +8929,9 @@
       <c r="C271">
         <v>770691</v>
       </c>
+      <c r="G271">
+        <v>5</v>
+      </c>
       <c r="I271" t="s">
         <v>395</v>
       </c>
@@ -8688,6 +8949,9 @@
       <c r="C272">
         <v>770692</v>
       </c>
+      <c r="G272">
+        <v>5</v>
+      </c>
       <c r="I272" t="s">
         <v>392</v>
       </c>
@@ -8705,6 +8969,9 @@
       <c r="C273">
         <v>770853</v>
       </c>
+      <c r="G273">
+        <v>5</v>
+      </c>
       <c r="I273" t="s">
         <v>395</v>
       </c>
@@ -8722,6 +8989,9 @@
       <c r="C274">
         <v>770854</v>
       </c>
+      <c r="G274">
+        <v>5</v>
+      </c>
       <c r="I274" t="s">
         <v>395</v>
       </c>
@@ -8739,6 +9009,9 @@
       <c r="C275">
         <v>770855</v>
       </c>
+      <c r="G275">
+        <v>5</v>
+      </c>
       <c r="I275" t="s">
         <v>395</v>
       </c>
@@ -8756,6 +9029,9 @@
       <c r="C276">
         <v>770856</v>
       </c>
+      <c r="G276">
+        <v>5</v>
+      </c>
       <c r="I276" t="s">
         <v>392</v>
       </c>
@@ -8773,6 +9049,9 @@
       <c r="C277">
         <v>770871</v>
       </c>
+      <c r="G277">
+        <v>5</v>
+      </c>
       <c r="I277" t="s">
         <v>392</v>
       </c>
@@ -8790,6 +9069,9 @@
       <c r="C278">
         <v>770872</v>
       </c>
+      <c r="G278">
+        <v>5</v>
+      </c>
       <c r="I278" t="s">
         <v>395</v>
       </c>
@@ -8807,6 +9089,9 @@
       <c r="C279">
         <v>770879</v>
       </c>
+      <c r="G279">
+        <v>5</v>
+      </c>
       <c r="I279" t="s">
         <v>363</v>
       </c>
@@ -8824,6 +9109,9 @@
       <c r="C280">
         <v>770880</v>
       </c>
+      <c r="G280">
+        <v>5</v>
+      </c>
       <c r="I280" t="s">
         <v>364</v>
       </c>
@@ -8841,6 +9129,9 @@
       <c r="C281">
         <v>770881</v>
       </c>
+      <c r="G281">
+        <v>5</v>
+      </c>
       <c r="I281" t="s">
         <v>365</v>
       </c>
@@ -8858,6 +9149,9 @@
       <c r="C282">
         <v>770882</v>
       </c>
+      <c r="G282">
+        <v>5</v>
+      </c>
       <c r="I282" t="s">
         <v>403</v>
       </c>
@@ -8875,6 +9169,9 @@
       <c r="C283">
         <v>770883</v>
       </c>
+      <c r="G283">
+        <v>5</v>
+      </c>
       <c r="I283" t="s">
         <v>365</v>
       </c>
@@ -8892,6 +9189,9 @@
       <c r="C284">
         <v>770884</v>
       </c>
+      <c r="G284">
+        <v>5</v>
+      </c>
       <c r="I284" t="s">
         <v>403</v>
       </c>
@@ -8909,6 +9209,9 @@
       <c r="C285">
         <v>770885</v>
       </c>
+      <c r="G285">
+        <v>5</v>
+      </c>
       <c r="I285" t="s">
         <v>365</v>
       </c>
@@ -8926,6 +9229,9 @@
       <c r="C286">
         <v>770886</v>
       </c>
+      <c r="G286">
+        <v>5</v>
+      </c>
       <c r="I286" t="s">
         <v>403</v>
       </c>
@@ -8943,6 +9249,9 @@
       <c r="C287">
         <v>770887</v>
       </c>
+      <c r="G287">
+        <v>5</v>
+      </c>
       <c r="I287" t="s">
         <v>391</v>
       </c>
@@ -8960,6 +9269,9 @@
       <c r="C288">
         <v>770888</v>
       </c>
+      <c r="G288">
+        <v>5</v>
+      </c>
       <c r="I288" t="s">
         <v>390</v>
       </c>
@@ -8977,6 +9289,9 @@
       <c r="C289">
         <v>770889</v>
       </c>
+      <c r="G289">
+        <v>5</v>
+      </c>
       <c r="I289" t="s">
         <v>391</v>
       </c>
@@ -8994,6 +9309,9 @@
       <c r="C290">
         <v>770890</v>
       </c>
+      <c r="G290">
+        <v>5</v>
+      </c>
       <c r="I290" t="s">
         <v>390</v>
       </c>
@@ -9011,6 +9329,9 @@
       <c r="C291">
         <v>770891</v>
       </c>
+      <c r="G291">
+        <v>5</v>
+      </c>
       <c r="I291" t="s">
         <v>392</v>
       </c>
@@ -9028,6 +9349,9 @@
       <c r="C292">
         <v>770892</v>
       </c>
+      <c r="G292">
+        <v>5</v>
+      </c>
       <c r="I292" t="s">
         <v>395</v>
       </c>
@@ -9045,6 +9369,9 @@
       <c r="C293">
         <v>770923</v>
       </c>
+      <c r="G293">
+        <v>5</v>
+      </c>
       <c r="I293" t="s">
         <v>378</v>
       </c>
@@ -9062,6 +9389,9 @@
       <c r="C294">
         <v>770924</v>
       </c>
+      <c r="G294">
+        <v>5</v>
+      </c>
       <c r="I294" t="s">
         <v>381</v>
       </c>
@@ -9079,6 +9409,9 @@
       <c r="C295">
         <v>770981</v>
       </c>
+      <c r="G295">
+        <v>5</v>
+      </c>
       <c r="I295" t="s">
         <v>365</v>
       </c>
@@ -9096,6 +9429,9 @@
       <c r="C296">
         <v>770982</v>
       </c>
+      <c r="G296">
+        <v>5</v>
+      </c>
       <c r="I296" t="s">
         <v>403</v>
       </c>
@@ -12254,7 +12590,7 @@
         <v>362</v>
       </c>
       <c r="B418" s="4" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C418" s="4">
         <v>990693</v>
@@ -12264,17 +12600,17 @@
       <c r="F418" s="4">
         <v>45</v>
       </c>
-      <c r="G418" s="4">
+      <c r="G418">
         <v>5</v>
       </c>
       <c r="H418" s="4">
         <v>1E-3</v>
       </c>
       <c r="I418" s="4" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="J418" s="4" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="419" spans="1:10" x14ac:dyDescent="0.35">
@@ -12282,7 +12618,7 @@
         <v>362</v>
       </c>
       <c r="B419" s="4" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C419" s="4">
         <v>990694</v>
@@ -12292,17 +12628,17 @@
       <c r="F419" s="4">
         <v>45</v>
       </c>
-      <c r="G419" s="4">
+      <c r="G419">
         <v>5</v>
       </c>
       <c r="H419" s="4">
         <v>1E-3</v>
       </c>
       <c r="I419" s="4" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="J419" s="4" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="420" spans="1:10" x14ac:dyDescent="0.35">
@@ -12310,7 +12646,7 @@
         <v>362</v>
       </c>
       <c r="B420" s="4" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C420" s="4">
         <v>990695</v>
@@ -12320,17 +12656,17 @@
       <c r="F420" s="4">
         <v>45</v>
       </c>
-      <c r="G420" s="4">
+      <c r="G420">
         <v>5</v>
       </c>
       <c r="H420" s="4">
         <v>1E-3</v>
       </c>
       <c r="I420" s="4" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="J420" s="4" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="421" spans="1:10" x14ac:dyDescent="0.35">
@@ -12338,7 +12674,7 @@
         <v>362</v>
       </c>
       <c r="B421" s="4" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C421" s="4">
         <v>990696</v>
@@ -12348,17 +12684,17 @@
       <c r="F421" s="4">
         <v>45</v>
       </c>
-      <c r="G421" s="4">
+      <c r="G421">
         <v>5</v>
       </c>
       <c r="H421" s="4">
         <v>1E-3</v>
       </c>
       <c r="I421" s="4" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="J421" s="4" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="422" spans="1:10" x14ac:dyDescent="0.35">
@@ -12470,7 +12806,7 @@
         <v>362</v>
       </c>
       <c r="B426" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C426">
         <v>990857</v>
@@ -12485,10 +12821,10 @@
         <v>1E-3</v>
       </c>
       <c r="I426" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="J426" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="427" spans="1:10" x14ac:dyDescent="0.35">
@@ -12496,7 +12832,7 @@
         <v>362</v>
       </c>
       <c r="B427" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C427">
         <v>990858</v>
@@ -12511,10 +12847,10 @@
         <v>1E-3</v>
       </c>
       <c r="I427" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="J427" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="428" spans="1:10" x14ac:dyDescent="0.35">
@@ -13091,10 +13427,10 @@
     </row>
     <row r="450" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A450" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B450" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C450">
         <v>2740</v>
@@ -13120,10 +13456,10 @@
     </row>
     <row r="451" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A451" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B451" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C451">
         <v>2770</v>
@@ -13149,10 +13485,10 @@
     </row>
     <row r="452" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A452" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B452" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C452">
         <v>2830</v>
@@ -13178,10 +13514,10 @@
     </row>
     <row r="453" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A453" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B453" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C453">
         <v>2810</v>
@@ -13207,10 +13543,10 @@
     </row>
     <row r="454" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A454" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B454" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C454">
         <v>2340</v>
@@ -13236,10 +13572,10 @@
     </row>
     <row r="455" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A455" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B455" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C455">
         <v>2320</v>
@@ -13265,10 +13601,10 @@
     </row>
     <row r="456" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A456" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B456" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C456">
         <v>2370</v>
@@ -13294,10 +13630,10 @@
     </row>
     <row r="457" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A457" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B457" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C457">
         <v>2450</v>
@@ -13323,10 +13659,10 @@
     </row>
     <row r="458" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A458" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B458" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C458">
         <v>2420</v>
@@ -13352,10 +13688,10 @@
     </row>
     <row r="459" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A459" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B459" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C459">
         <v>2120</v>
@@ -13378,10 +13714,10 @@
     </row>
     <row r="460" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A460" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B460" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C460">
         <v>2130</v>
@@ -13404,10 +13740,10 @@
     </row>
     <row r="461" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A461" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B461" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C461">
         <v>2230</v>
@@ -13430,10 +13766,10 @@
     </row>
     <row r="462" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A462" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B462" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C462">
         <v>1010309</v>
@@ -13454,15 +13790,15 @@
         <v>#N/A</v>
       </c>
       <c r="K462" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="463" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A463" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B463" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C463">
         <v>1010310</v>
@@ -13483,15 +13819,15 @@
         <v>#N/A</v>
       </c>
       <c r="K463" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="464" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A464" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B464" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C464">
         <v>800601</v>
@@ -13512,15 +13848,15 @@
         <v>#N/A</v>
       </c>
       <c r="K464" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="465" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A465" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B465" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C465">
         <v>800602</v>
@@ -13541,755 +13877,1367 @@
         <v>#N/A</v>
       </c>
       <c r="K465" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="466" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A466" t="s">
+        <v>478</v>
+      </c>
+      <c r="B466" t="s">
         <v>479</v>
-      </c>
-      <c r="B466" t="s">
-        <v>480</v>
       </c>
       <c r="C466">
         <v>800501</v>
       </c>
+      <c r="F466">
+        <v>45</v>
+      </c>
+      <c r="G466">
+        <v>5</v>
+      </c>
+      <c r="H466">
+        <v>0.03</v>
+      </c>
     </row>
     <row r="467" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A467" t="s">
+        <v>478</v>
+      </c>
+      <c r="B467" t="s">
         <v>479</v>
-      </c>
-      <c r="B467" t="s">
-        <v>480</v>
       </c>
       <c r="C467">
         <v>800502</v>
       </c>
+      <c r="F467">
+        <v>45</v>
+      </c>
+      <c r="G467">
+        <v>5</v>
+      </c>
+      <c r="H467">
+        <v>0.03</v>
+      </c>
     </row>
     <row r="468" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A468" t="s">
+        <v>478</v>
+      </c>
+      <c r="B468" t="s">
         <v>479</v>
-      </c>
-      <c r="B468" t="s">
-        <v>480</v>
       </c>
       <c r="C468">
         <v>800503</v>
       </c>
+      <c r="F468">
+        <v>45</v>
+      </c>
+      <c r="G468">
+        <v>5</v>
+      </c>
+      <c r="H468">
+        <v>0.03</v>
+      </c>
     </row>
     <row r="469" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A469" t="s">
+        <v>478</v>
+      </c>
+      <c r="B469" t="s">
         <v>479</v>
-      </c>
-      <c r="B469" t="s">
-        <v>480</v>
       </c>
       <c r="C469">
         <v>800603</v>
       </c>
+      <c r="F469">
+        <v>45</v>
+      </c>
+      <c r="G469">
+        <v>5</v>
+      </c>
+      <c r="H469">
+        <v>0.03</v>
+      </c>
     </row>
     <row r="470" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A470" t="s">
+        <v>478</v>
+      </c>
+      <c r="B470" t="s">
         <v>479</v>
-      </c>
-      <c r="B470" t="s">
-        <v>480</v>
       </c>
       <c r="C470">
         <v>800504</v>
       </c>
+      <c r="F470">
+        <v>45</v>
+      </c>
+      <c r="G470">
+        <v>5</v>
+      </c>
+      <c r="H470">
+        <v>0.03</v>
+      </c>
     </row>
     <row r="471" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A471" t="s">
+        <v>478</v>
+      </c>
+      <c r="B471" t="s">
         <v>479</v>
-      </c>
-      <c r="B471" t="s">
-        <v>480</v>
       </c>
       <c r="C471">
         <v>800604</v>
       </c>
+      <c r="F471">
+        <v>45</v>
+      </c>
+      <c r="G471">
+        <v>5</v>
+      </c>
+      <c r="H471">
+        <v>0.03</v>
+      </c>
     </row>
     <row r="472" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A472" t="s">
+        <v>478</v>
+      </c>
+      <c r="B472" t="s">
         <v>479</v>
-      </c>
-      <c r="B472" t="s">
-        <v>480</v>
       </c>
       <c r="C472">
         <v>1010305</v>
       </c>
+      <c r="F472">
+        <v>45</v>
+      </c>
+      <c r="G472">
+        <v>5</v>
+      </c>
+      <c r="H472">
+        <v>0.03</v>
+      </c>
     </row>
     <row r="473" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A473" t="s">
+        <v>478</v>
+      </c>
+      <c r="B473" t="s">
         <v>479</v>
-      </c>
-      <c r="B473" t="s">
-        <v>480</v>
       </c>
       <c r="C473">
         <v>1010306</v>
       </c>
+      <c r="F473">
+        <v>45</v>
+      </c>
+      <c r="G473">
+        <v>5</v>
+      </c>
+      <c r="H473">
+        <v>0.03</v>
+      </c>
     </row>
     <row r="474" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A474" t="s">
+        <v>478</v>
+      </c>
+      <c r="B474" t="s">
         <v>479</v>
-      </c>
-      <c r="B474" t="s">
-        <v>480</v>
       </c>
       <c r="C474">
         <v>1010307</v>
       </c>
+      <c r="F474">
+        <v>45</v>
+      </c>
+      <c r="G474">
+        <v>5</v>
+      </c>
+      <c r="H474">
+        <v>0.03</v>
+      </c>
     </row>
     <row r="475" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A475" t="s">
+        <v>478</v>
+      </c>
+      <c r="B475" t="s">
         <v>479</v>
-      </c>
-      <c r="B475" t="s">
-        <v>480</v>
       </c>
       <c r="C475">
         <v>1010308</v>
       </c>
+      <c r="F475">
+        <v>45</v>
+      </c>
+      <c r="G475">
+        <v>5</v>
+      </c>
+      <c r="H475">
+        <v>0.03</v>
+      </c>
     </row>
     <row r="476" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A476" t="s">
+        <v>478</v>
+      </c>
+      <c r="B476" t="s">
         <v>479</v>
-      </c>
-      <c r="B476" t="s">
-        <v>480</v>
       </c>
       <c r="C476">
         <v>2800308</v>
       </c>
+      <c r="F476">
+        <v>45</v>
+      </c>
+      <c r="G476">
+        <v>5</v>
+      </c>
+      <c r="H476">
+        <v>0.03</v>
+      </c>
     </row>
     <row r="477" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A477" t="s">
+        <v>478</v>
+      </c>
+      <c r="B477" t="s">
         <v>479</v>
-      </c>
-      <c r="B477" t="s">
-        <v>480</v>
       </c>
       <c r="C477">
         <v>2800309</v>
       </c>
+      <c r="F477">
+        <v>45</v>
+      </c>
+      <c r="G477">
+        <v>5</v>
+      </c>
+      <c r="H477">
+        <v>0.03</v>
+      </c>
     </row>
     <row r="478" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A478" t="s">
+        <v>478</v>
+      </c>
+      <c r="B478" t="s">
         <v>479</v>
-      </c>
-      <c r="B478" t="s">
-        <v>480</v>
       </c>
       <c r="C478">
         <v>2800310</v>
       </c>
+      <c r="F478">
+        <v>45</v>
+      </c>
+      <c r="G478">
+        <v>5</v>
+      </c>
+      <c r="H478">
+        <v>0.03</v>
+      </c>
     </row>
     <row r="479" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A479" t="s">
+        <v>478</v>
+      </c>
+      <c r="B479" t="s">
         <v>479</v>
-      </c>
-      <c r="B479" t="s">
-        <v>480</v>
       </c>
       <c r="C479">
         <v>2800311</v>
       </c>
+      <c r="F479">
+        <v>45</v>
+      </c>
+      <c r="G479">
+        <v>5</v>
+      </c>
+      <c r="H479">
+        <v>0.03</v>
+      </c>
     </row>
     <row r="480" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A480" t="s">
+        <v>478</v>
+      </c>
+      <c r="B480" t="s">
         <v>479</v>
-      </c>
-      <c r="B480" t="s">
-        <v>480</v>
       </c>
       <c r="C480">
         <v>2800312</v>
       </c>
-    </row>
-    <row r="481" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F480">
+        <v>45</v>
+      </c>
+      <c r="G480">
+        <v>5</v>
+      </c>
+      <c r="H480">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="481" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A481" t="s">
+        <v>478</v>
+      </c>
+      <c r="B481" t="s">
         <v>479</v>
-      </c>
-      <c r="B481" t="s">
-        <v>480</v>
       </c>
       <c r="C481">
         <v>2800313</v>
       </c>
-    </row>
-    <row r="482" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F481">
+        <v>45</v>
+      </c>
+      <c r="G481">
+        <v>5</v>
+      </c>
+      <c r="H481">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="482" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A482" t="s">
+        <v>478</v>
+      </c>
+      <c r="B482" t="s">
         <v>479</v>
-      </c>
-      <c r="B482" t="s">
-        <v>480</v>
       </c>
       <c r="C482">
         <v>2800314</v>
       </c>
-    </row>
-    <row r="483" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F482">
+        <v>45</v>
+      </c>
+      <c r="G482">
+        <v>5</v>
+      </c>
+      <c r="H482">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="483" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A483" t="s">
+        <v>478</v>
+      </c>
+      <c r="B483" t="s">
         <v>479</v>
-      </c>
-      <c r="B483" t="s">
-        <v>480</v>
       </c>
       <c r="C483">
         <v>2800315</v>
       </c>
-    </row>
-    <row r="484" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F483">
+        <v>45</v>
+      </c>
+      <c r="G483">
+        <v>5</v>
+      </c>
+      <c r="H483">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="484" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A484" t="s">
+        <v>478</v>
+      </c>
+      <c r="B484" t="s">
         <v>479</v>
-      </c>
-      <c r="B484" t="s">
-        <v>480</v>
       </c>
       <c r="C484">
         <v>40516</v>
       </c>
-    </row>
-    <row r="485" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F484">
+        <v>45</v>
+      </c>
+      <c r="G484">
+        <v>5</v>
+      </c>
+      <c r="H484">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="485" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A485" t="s">
+        <v>478</v>
+      </c>
+      <c r="B485" t="s">
         <v>479</v>
-      </c>
-      <c r="B485" t="s">
-        <v>480</v>
       </c>
       <c r="C485">
         <v>40517</v>
       </c>
-    </row>
-    <row r="486" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F485">
+        <v>45</v>
+      </c>
+      <c r="G485">
+        <v>5</v>
+      </c>
+      <c r="H485">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="486" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A486" t="s">
+        <v>478</v>
+      </c>
+      <c r="B486" t="s">
         <v>479</v>
-      </c>
-      <c r="B486" t="s">
-        <v>480</v>
       </c>
       <c r="C486">
         <v>40518</v>
       </c>
-    </row>
-    <row r="487" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F486">
+        <v>45</v>
+      </c>
+      <c r="G486">
+        <v>5</v>
+      </c>
+      <c r="H486">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="487" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A487" t="s">
+        <v>478</v>
+      </c>
+      <c r="B487" t="s">
         <v>479</v>
-      </c>
-      <c r="B487" t="s">
-        <v>480</v>
       </c>
       <c r="C487">
         <v>40519</v>
       </c>
-    </row>
-    <row r="488" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F487">
+        <v>45</v>
+      </c>
+      <c r="G487">
+        <v>5</v>
+      </c>
+      <c r="H487">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="488" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A488" t="s">
+        <v>478</v>
+      </c>
+      <c r="B488" t="s">
         <v>479</v>
-      </c>
-      <c r="B488" t="s">
-        <v>480</v>
       </c>
       <c r="C488">
         <v>5800420</v>
       </c>
-    </row>
-    <row r="489" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F488">
+        <v>45</v>
+      </c>
+      <c r="G488">
+        <v>5</v>
+      </c>
+      <c r="H488">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="489" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A489" t="s">
+        <v>478</v>
+      </c>
+      <c r="B489" t="s">
         <v>479</v>
-      </c>
-      <c r="B489" t="s">
-        <v>480</v>
       </c>
       <c r="C489">
         <v>5800421</v>
       </c>
-    </row>
-    <row r="490" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F489">
+        <v>45</v>
+      </c>
+      <c r="G489">
+        <v>5</v>
+      </c>
+      <c r="H489">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="490" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A490" t="s">
+        <v>478</v>
+      </c>
+      <c r="B490" t="s">
         <v>479</v>
-      </c>
-      <c r="B490" t="s">
-        <v>480</v>
       </c>
       <c r="C490">
         <v>5800422</v>
       </c>
-    </row>
-    <row r="491" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F490">
+        <v>45</v>
+      </c>
+      <c r="G490">
+        <v>5</v>
+      </c>
+      <c r="H490">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="491" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A491" t="s">
+        <v>478</v>
+      </c>
+      <c r="B491" t="s">
         <v>479</v>
-      </c>
-      <c r="B491" t="s">
-        <v>480</v>
       </c>
       <c r="C491">
         <v>5800423</v>
       </c>
-    </row>
-    <row r="492" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F491">
+        <v>45</v>
+      </c>
+      <c r="G491">
+        <v>5</v>
+      </c>
+      <c r="H491">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="492" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A492" t="s">
+        <v>478</v>
+      </c>
+      <c r="B492" t="s">
         <v>479</v>
-      </c>
-      <c r="B492" t="s">
-        <v>480</v>
       </c>
       <c r="C492">
         <v>5800424</v>
       </c>
-    </row>
-    <row r="493" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F492">
+        <v>45</v>
+      </c>
+      <c r="G492">
+        <v>5</v>
+      </c>
+      <c r="H492">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="493" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A493" t="s">
+        <v>478</v>
+      </c>
+      <c r="B493" t="s">
         <v>479</v>
-      </c>
-      <c r="B493" t="s">
-        <v>480</v>
       </c>
       <c r="C493">
         <v>5800425</v>
       </c>
-    </row>
-    <row r="494" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F493">
+        <v>45</v>
+      </c>
+      <c r="G493">
+        <v>5</v>
+      </c>
+      <c r="H493">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="494" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A494" t="s">
+        <v>478</v>
+      </c>
+      <c r="B494" t="s">
         <v>479</v>
-      </c>
-      <c r="B494" t="s">
-        <v>480</v>
       </c>
       <c r="C494">
         <v>5800426</v>
       </c>
-    </row>
-    <row r="495" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F494">
+        <v>45</v>
+      </c>
+      <c r="G494">
+        <v>5</v>
+      </c>
+      <c r="H494">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="495" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A495" t="s">
+        <v>478</v>
+      </c>
+      <c r="B495" t="s">
         <v>479</v>
-      </c>
-      <c r="B495" t="s">
-        <v>480</v>
       </c>
       <c r="C495">
         <v>5800427</v>
       </c>
-    </row>
-    <row r="496" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F495">
+        <v>45</v>
+      </c>
+      <c r="G495">
+        <v>5</v>
+      </c>
+      <c r="H495">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="496" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A496" t="s">
+        <v>478</v>
+      </c>
+      <c r="B496" t="s">
         <v>479</v>
-      </c>
-      <c r="B496" t="s">
-        <v>480</v>
       </c>
       <c r="C496">
         <v>6800530</v>
       </c>
-    </row>
-    <row r="497" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F496">
+        <v>45</v>
+      </c>
+      <c r="G496">
+        <v>5</v>
+      </c>
+      <c r="H496">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="497" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A497" t="s">
+        <v>478</v>
+      </c>
+      <c r="B497" t="s">
         <v>479</v>
-      </c>
-      <c r="B497" t="s">
-        <v>480</v>
       </c>
       <c r="C497">
         <v>6800531</v>
       </c>
-    </row>
-    <row r="498" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F497">
+        <v>45</v>
+      </c>
+      <c r="G497">
+        <v>5</v>
+      </c>
+      <c r="H497">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="498" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A498" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B498" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C498">
         <v>6800532</v>
       </c>
-    </row>
-    <row r="499" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F498">
+        <v>45</v>
+      </c>
+      <c r="G498">
+        <v>5</v>
+      </c>
+      <c r="H498">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="499" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A499" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B499" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C499">
         <v>6800533</v>
       </c>
-    </row>
-    <row r="500" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F499">
+        <v>45</v>
+      </c>
+      <c r="G499">
+        <v>5</v>
+      </c>
+      <c r="H499">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="500" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A500" t="s">
+        <v>478</v>
+      </c>
+      <c r="B500" t="s">
         <v>479</v>
-      </c>
-      <c r="B500" t="s">
-        <v>480</v>
       </c>
       <c r="C500">
         <v>6800330</v>
       </c>
-    </row>
-    <row r="501" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F500">
+        <v>45</v>
+      </c>
+      <c r="G500">
+        <v>5</v>
+      </c>
+      <c r="H500">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="501" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A501" t="s">
+        <v>478</v>
+      </c>
+      <c r="B501" t="s">
         <v>479</v>
-      </c>
-      <c r="B501" t="s">
-        <v>480</v>
       </c>
       <c r="C501">
         <v>850331</v>
       </c>
-    </row>
-    <row r="502" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F501">
+        <v>45</v>
+      </c>
+      <c r="G501">
+        <v>5</v>
+      </c>
+      <c r="H501">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="502" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A502" t="s">
+        <v>478</v>
+      </c>
+      <c r="B502" t="s">
         <v>479</v>
-      </c>
-      <c r="B502" t="s">
-        <v>480</v>
       </c>
       <c r="C502">
         <v>850332</v>
       </c>
-    </row>
-    <row r="503" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F502">
+        <v>45</v>
+      </c>
+      <c r="G502">
+        <v>5</v>
+      </c>
+      <c r="H502">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="503" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A503" t="s">
+        <v>478</v>
+      </c>
+      <c r="B503" t="s">
         <v>479</v>
-      </c>
-      <c r="B503" t="s">
-        <v>480</v>
       </c>
       <c r="C503">
         <v>850333</v>
       </c>
-    </row>
-    <row r="504" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F503">
+        <v>45</v>
+      </c>
+      <c r="G503">
+        <v>5</v>
+      </c>
+      <c r="H503">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="504" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A504" t="s">
+        <v>478</v>
+      </c>
+      <c r="B504" t="s">
         <v>479</v>
-      </c>
-      <c r="B504" t="s">
-        <v>480</v>
       </c>
       <c r="C504">
         <v>850334</v>
       </c>
-    </row>
-    <row r="505" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F504">
+        <v>45</v>
+      </c>
+      <c r="G504">
+        <v>5</v>
+      </c>
+      <c r="H504">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="505" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A505" t="s">
+        <v>478</v>
+      </c>
+      <c r="B505" t="s">
         <v>479</v>
-      </c>
-      <c r="B505" t="s">
-        <v>480</v>
       </c>
       <c r="C505">
         <v>870335</v>
       </c>
-    </row>
-    <row r="506" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F505">
+        <v>45</v>
+      </c>
+      <c r="G505">
+        <v>5</v>
+      </c>
+      <c r="H505">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="506" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A506" t="s">
+        <v>478</v>
+      </c>
+      <c r="B506" t="s">
         <v>479</v>
-      </c>
-      <c r="B506" t="s">
-        <v>480</v>
       </c>
       <c r="C506">
         <v>870336</v>
       </c>
-    </row>
-    <row r="507" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F506">
+        <v>45</v>
+      </c>
+      <c r="G506">
+        <v>5</v>
+      </c>
+      <c r="H506">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="507" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A507" t="s">
+        <v>478</v>
+      </c>
+      <c r="B507" t="s">
         <v>479</v>
-      </c>
-      <c r="B507" t="s">
-        <v>480</v>
       </c>
       <c r="C507">
         <v>870337</v>
       </c>
-    </row>
-    <row r="508" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F507">
+        <v>45</v>
+      </c>
+      <c r="G507">
+        <v>5</v>
+      </c>
+      <c r="H507">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="508" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A508" t="s">
+        <v>478</v>
+      </c>
+      <c r="B508" t="s">
         <v>479</v>
-      </c>
-      <c r="B508" t="s">
-        <v>480</v>
       </c>
       <c r="C508">
         <v>870338</v>
       </c>
-    </row>
-    <row r="509" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F508">
+        <v>45</v>
+      </c>
+      <c r="G508">
+        <v>5</v>
+      </c>
+      <c r="H508">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="509" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A509" t="s">
+        <v>478</v>
+      </c>
+      <c r="B509" t="s">
         <v>479</v>
-      </c>
-      <c r="B509" t="s">
-        <v>480</v>
       </c>
       <c r="C509">
         <v>8800439</v>
       </c>
-    </row>
-    <row r="510" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F509">
+        <v>45</v>
+      </c>
+      <c r="G509">
+        <v>5</v>
+      </c>
+      <c r="H509">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="510" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A510" t="s">
+        <v>478</v>
+      </c>
+      <c r="B510" t="s">
         <v>479</v>
-      </c>
-      <c r="B510" t="s">
-        <v>480</v>
       </c>
       <c r="C510">
         <v>8800440</v>
       </c>
-    </row>
-    <row r="511" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F510">
+        <v>45</v>
+      </c>
+      <c r="G510">
+        <v>5</v>
+      </c>
+      <c r="H510">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="511" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A511" t="s">
+        <v>478</v>
+      </c>
+      <c r="B511" t="s">
         <v>479</v>
-      </c>
-      <c r="B511" t="s">
-        <v>480</v>
       </c>
       <c r="C511">
         <v>8800441</v>
       </c>
-    </row>
-    <row r="512" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F511">
+        <v>45</v>
+      </c>
+      <c r="G511">
+        <v>5</v>
+      </c>
+      <c r="H511">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="512" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A512" t="s">
+        <v>478</v>
+      </c>
+      <c r="B512" t="s">
         <v>479</v>
-      </c>
-      <c r="B512" t="s">
-        <v>480</v>
       </c>
       <c r="C512">
         <v>8800442</v>
       </c>
-    </row>
-    <row r="513" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F512">
+        <v>45</v>
+      </c>
+      <c r="G512">
+        <v>5</v>
+      </c>
+      <c r="H512">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="513" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A513" t="s">
+        <v>478</v>
+      </c>
+      <c r="B513" t="s">
         <v>479</v>
-      </c>
-      <c r="B513" t="s">
-        <v>480</v>
       </c>
       <c r="C513">
         <v>8800443</v>
       </c>
-    </row>
-    <row r="514" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F513">
+        <v>45</v>
+      </c>
+      <c r="G513">
+        <v>5</v>
+      </c>
+      <c r="H513">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="514" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A514" t="s">
+        <v>478</v>
+      </c>
+      <c r="B514" t="s">
         <v>479</v>
-      </c>
-      <c r="B514" t="s">
-        <v>480</v>
       </c>
       <c r="C514">
         <v>6800544</v>
       </c>
-    </row>
-    <row r="515" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F514">
+        <v>45</v>
+      </c>
+      <c r="G514">
+        <v>5</v>
+      </c>
+      <c r="H514">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="515" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A515" t="s">
+        <v>478</v>
+      </c>
+      <c r="B515" t="s">
         <v>479</v>
-      </c>
-      <c r="B515" t="s">
-        <v>480</v>
       </c>
       <c r="C515">
         <v>6800545</v>
       </c>
-    </row>
-    <row r="516" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F515">
+        <v>45</v>
+      </c>
+      <c r="G515">
+        <v>5</v>
+      </c>
+      <c r="H515">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="516" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A516" t="s">
+        <v>478</v>
+      </c>
+      <c r="B516" t="s">
         <v>479</v>
-      </c>
-      <c r="B516" t="s">
-        <v>480</v>
       </c>
       <c r="C516">
         <v>8800446</v>
       </c>
-    </row>
-    <row r="517" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F516">
+        <v>45</v>
+      </c>
+      <c r="G516">
+        <v>5</v>
+      </c>
+      <c r="H516">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="517" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A517" t="s">
+        <v>478</v>
+      </c>
+      <c r="B517" t="s">
         <v>479</v>
-      </c>
-      <c r="B517" t="s">
-        <v>480</v>
       </c>
       <c r="C517">
         <v>8800447</v>
       </c>
-    </row>
-    <row r="518" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F517">
+        <v>45</v>
+      </c>
+      <c r="G517">
+        <v>5</v>
+      </c>
+      <c r="H517">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="518" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A518" t="s">
+        <v>478</v>
+      </c>
+      <c r="B518" t="s">
         <v>479</v>
-      </c>
-      <c r="B518" t="s">
-        <v>480</v>
       </c>
       <c r="C518">
         <v>8800448</v>
       </c>
-    </row>
-    <row r="519" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F518">
+        <v>45</v>
+      </c>
+      <c r="G518">
+        <v>5</v>
+      </c>
+      <c r="H518">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="519" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A519" t="s">
+        <v>478</v>
+      </c>
+      <c r="B519" t="s">
         <v>479</v>
-      </c>
-      <c r="B519" t="s">
-        <v>480</v>
       </c>
       <c r="C519">
         <v>8800349</v>
       </c>
-    </row>
-    <row r="520" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F519">
+        <v>45</v>
+      </c>
+      <c r="G519">
+        <v>5</v>
+      </c>
+      <c r="H519">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="520" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A520" t="s">
+        <v>478</v>
+      </c>
+      <c r="B520" t="s">
         <v>479</v>
-      </c>
-      <c r="B520" t="s">
-        <v>480</v>
       </c>
       <c r="C520">
         <v>8800449</v>
       </c>
-    </row>
-    <row r="521" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F520">
+        <v>45</v>
+      </c>
+      <c r="G520">
+        <v>5</v>
+      </c>
+      <c r="H520">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="521" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A521" t="s">
+        <v>478</v>
+      </c>
+      <c r="B521" t="s">
         <v>479</v>
-      </c>
-      <c r="B521" t="s">
-        <v>480</v>
       </c>
       <c r="C521">
         <v>8800450</v>
       </c>
-    </row>
-    <row r="522" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F521">
+        <v>45</v>
+      </c>
+      <c r="G521">
+        <v>5</v>
+      </c>
+      <c r="H521">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="522" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A522" t="s">
+        <v>478</v>
+      </c>
+      <c r="B522" t="s">
         <v>479</v>
-      </c>
-      <c r="B522" t="s">
-        <v>480</v>
       </c>
       <c r="C522">
         <v>8800351</v>
       </c>
-    </row>
-    <row r="523" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F522">
+        <v>45</v>
+      </c>
+      <c r="G522">
+        <v>5</v>
+      </c>
+      <c r="H522">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="523" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A523" t="s">
+        <v>478</v>
+      </c>
+      <c r="B523" t="s">
         <v>479</v>
-      </c>
-      <c r="B523" t="s">
-        <v>480</v>
       </c>
       <c r="C523">
         <v>8800451</v>
       </c>
-    </row>
-    <row r="524" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F523">
+        <v>45</v>
+      </c>
+      <c r="G523">
+        <v>5</v>
+      </c>
+      <c r="H523">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="524" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A524" t="s">
+        <v>478</v>
+      </c>
+      <c r="B524" t="s">
         <v>479</v>
-      </c>
-      <c r="B524" t="s">
-        <v>480</v>
       </c>
       <c r="C524">
         <v>8800452</v>
       </c>
-    </row>
-    <row r="525" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F524">
+        <v>45</v>
+      </c>
+      <c r="G524">
+        <v>5</v>
+      </c>
+      <c r="H524">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="525" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A525" t="s">
+        <v>478</v>
+      </c>
+      <c r="B525" t="s">
         <v>479</v>
-      </c>
-      <c r="B525" t="s">
-        <v>480</v>
       </c>
       <c r="C525">
         <v>1010253</v>
       </c>
-    </row>
-    <row r="526" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F525">
+        <v>45</v>
+      </c>
+      <c r="G525">
+        <v>5</v>
+      </c>
+      <c r="H525">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="526" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A526" t="s">
+        <v>478</v>
+      </c>
+      <c r="B526" t="s">
         <v>479</v>
-      </c>
-      <c r="B526" t="s">
-        <v>480</v>
       </c>
       <c r="C526">
         <v>1010254</v>
       </c>
-    </row>
-    <row r="527" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F526">
+        <v>45</v>
+      </c>
+      <c r="G526">
+        <v>5</v>
+      </c>
+      <c r="H526">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="527" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A527" t="s">
+        <v>478</v>
+      </c>
+      <c r="B527" t="s">
         <v>479</v>
-      </c>
-      <c r="B527" t="s">
-        <v>480</v>
       </c>
       <c r="C527">
         <v>1010255</v>
       </c>
-    </row>
-    <row r="528" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F527">
+        <v>45</v>
+      </c>
+      <c r="G527">
+        <v>5</v>
+      </c>
+      <c r="H527">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="528" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A528" t="s">
+        <v>478</v>
+      </c>
+      <c r="B528" t="s">
         <v>479</v>
-      </c>
-      <c r="B528" t="s">
-        <v>480</v>
       </c>
       <c r="C528">
         <v>1010256</v>
       </c>
-    </row>
-    <row r="529" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F528">
+        <v>45</v>
+      </c>
+      <c r="G528">
+        <v>5</v>
+      </c>
+      <c r="H528">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="529" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A529" t="s">
+        <v>478</v>
+      </c>
+      <c r="B529" t="s">
         <v>479</v>
-      </c>
-      <c r="B529" t="s">
-        <v>480</v>
       </c>
       <c r="C529">
         <v>1010356</v>
       </c>
-    </row>
-    <row r="530" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F529">
+        <v>45</v>
+      </c>
+      <c r="G529">
+        <v>5</v>
+      </c>
+      <c r="H529">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="530" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A530" t="s">
+        <v>478</v>
+      </c>
+      <c r="B530" t="s">
         <v>479</v>
-      </c>
-      <c r="B530" t="s">
-        <v>480</v>
       </c>
       <c r="C530">
         <v>1010257</v>
       </c>
-    </row>
-    <row r="531" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F530">
+        <v>45</v>
+      </c>
+      <c r="G530">
+        <v>5</v>
+      </c>
+      <c r="H530">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="531" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A531" t="s">
+        <v>478</v>
+      </c>
+      <c r="B531" t="s">
         <v>479</v>
-      </c>
-      <c r="B531" t="s">
-        <v>480</v>
       </c>
       <c r="C531">
         <v>1010258</v>
       </c>
-    </row>
-    <row r="532" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F531">
+        <v>45</v>
+      </c>
+      <c r="G531">
+        <v>5</v>
+      </c>
+      <c r="H531">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="532" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A532" t="s">
+        <v>478</v>
+      </c>
+      <c r="B532" t="s">
         <v>479</v>
-      </c>
-      <c r="B532" t="s">
-        <v>480</v>
       </c>
       <c r="C532">
         <v>1010259</v>
       </c>
-    </row>
-    <row r="533" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F532">
+        <v>45</v>
+      </c>
+      <c r="G532">
+        <v>5</v>
+      </c>
+      <c r="H532">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="533" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A533" t="s">
+        <v>478</v>
+      </c>
+      <c r="B533" t="s">
         <v>479</v>
-      </c>
-      <c r="B533" t="s">
-        <v>480</v>
       </c>
       <c r="C533">
         <v>1010260</v>
+      </c>
+      <c r="F533">
+        <v>45</v>
+      </c>
+      <c r="G533">
+        <v>5</v>
+      </c>
+      <c r="H533">
+        <v>0.03</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes to TOLLCLASS_Designations.xlsx in a previous commit got overwritten
https://github.com/BayAreaMetro/travel-model-one/commit/94f16d2d71aa6f5993f3637c7905bc457a5a4a32
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/TOLLCLASS_Designations.xlsx
+++ b/utilities/NextGenFwys/TOLLCLASS_Designations.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jalatorre\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7118B422-45A2-4E2F-8DD4-CA8874220BCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF79082-C686-4F1A-8071-EBF5DE118E8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1875" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{0F0A9957-56E7-4C48-967B-2AB2A1965C2F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{0F0A9957-56E7-4C48-967B-2AB2A1965C2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs_for_tollcalib" sheetId="1" r:id="rId1"/>
@@ -1229,9 +1229,6 @@
     <t>EastBay_Inner580_AM</t>
   </si>
   <si>
-    <t>PBA2050 RTP ID</t>
-  </si>
-  <si>
     <t>AL-031</t>
   </si>
   <si>
@@ -1479,6 +1476,9 @@
   </si>
   <si>
     <t>SR92 SM - I-280 Interchange to El Camino Real (Per Mile Tolling) - WB</t>
+  </si>
+  <si>
+    <t>PBA2050_RTP_ID</t>
   </si>
 </sst>
 </file>
@@ -1885,8 +1885,8 @@
   <dimension ref="A1:K533"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A498" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F516" sqref="F516"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1912,7 +1912,7 @@
         <v>152</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>396</v>
+        <v>479</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>151</v>
@@ -1933,7 +1933,7 @@
         <v>317</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
@@ -2379,7 +2379,7 @@
         <v>81</v>
       </c>
       <c r="D21" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E21" t="s">
         <v>16</v>
@@ -2411,7 +2411,7 @@
         <v>82</v>
       </c>
       <c r="D22" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="E22" t="s">
         <v>16</v>
@@ -2443,7 +2443,7 @@
         <v>83</v>
       </c>
       <c r="D23" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E23" t="s">
         <v>16</v>
@@ -2475,7 +2475,7 @@
         <v>84</v>
       </c>
       <c r="D24" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E24" t="s">
         <v>16</v>
@@ -2507,7 +2507,7 @@
         <v>85</v>
       </c>
       <c r="D25" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E25" t="s">
         <v>16</v>
@@ -2539,7 +2539,7 @@
         <v>86</v>
       </c>
       <c r="D26" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E26" t="s">
         <v>16</v>
@@ -2571,7 +2571,7 @@
         <v>87</v>
       </c>
       <c r="D27" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E27" t="s">
         <v>253</v>
@@ -2603,7 +2603,7 @@
         <v>88</v>
       </c>
       <c r="D28" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E28" t="s">
         <v>253</v>
@@ -2635,7 +2635,7 @@
         <v>89</v>
       </c>
       <c r="D29" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E29" t="s">
         <v>253</v>
@@ -2667,7 +2667,7 @@
         <v>90</v>
       </c>
       <c r="D30" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E30" t="s">
         <v>253</v>
@@ -2699,7 +2699,7 @@
         <v>91</v>
       </c>
       <c r="D31" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="E31" t="s">
         <v>253</v>
@@ -2731,7 +2731,7 @@
         <v>92</v>
       </c>
       <c r="D32" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="E32" t="s">
         <v>253</v>
@@ -2821,7 +2821,7 @@
         <v>101</v>
       </c>
       <c r="D35" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E35" t="s">
         <v>16</v>
@@ -2853,7 +2853,7 @@
         <v>102</v>
       </c>
       <c r="D36" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E36" t="s">
         <v>16</v>
@@ -2885,7 +2885,7 @@
         <v>103</v>
       </c>
       <c r="D37" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E37" t="s">
         <v>16</v>
@@ -2917,7 +2917,7 @@
         <v>104</v>
       </c>
       <c r="D38" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E38" t="s">
         <v>16</v>
@@ -2949,7 +2949,7 @@
         <v>105</v>
       </c>
       <c r="D39" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="E39" t="s">
         <v>16</v>
@@ -2981,7 +2981,7 @@
         <v>106</v>
       </c>
       <c r="D40" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="E40" t="s">
         <v>16</v>
@@ -3303,7 +3303,7 @@
         <v>117</v>
       </c>
       <c r="D51" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E51" t="s">
         <v>16</v>
@@ -3335,7 +3335,7 @@
         <v>118</v>
       </c>
       <c r="D52" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E52" t="s">
         <v>16</v>
@@ -3367,7 +3367,7 @@
         <v>119</v>
       </c>
       <c r="D53" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E53" t="s">
         <v>253</v>
@@ -3399,7 +3399,7 @@
         <v>120</v>
       </c>
       <c r="D54" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E54" t="s">
         <v>253</v>
@@ -3431,7 +3431,7 @@
         <v>121</v>
       </c>
       <c r="D55" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E55" t="s">
         <v>253</v>
@@ -3463,7 +3463,7 @@
         <v>122</v>
       </c>
       <c r="D56" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E56" t="s">
         <v>253</v>
@@ -4173,7 +4173,7 @@
         <v>281</v>
       </c>
       <c r="D81" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E81" t="s">
         <v>16</v>
@@ -4205,7 +4205,7 @@
         <v>282</v>
       </c>
       <c r="D82" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E82" t="s">
         <v>16</v>
@@ -4295,7 +4295,7 @@
         <v>285</v>
       </c>
       <c r="D85" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E85" t="s">
         <v>253</v>
@@ -4327,7 +4327,7 @@
         <v>286</v>
       </c>
       <c r="D86" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E86" t="s">
         <v>253</v>
@@ -4359,7 +4359,7 @@
         <v>287</v>
       </c>
       <c r="D87" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E87" t="s">
         <v>16</v>
@@ -4391,7 +4391,7 @@
         <v>288</v>
       </c>
       <c r="D88" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E88" t="s">
         <v>16</v>
@@ -4533,7 +4533,7 @@
         <v>401</v>
       </c>
       <c r="D93" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E93" t="s">
         <v>253</v>
@@ -4565,7 +4565,7 @@
         <v>402</v>
       </c>
       <c r="D94" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E94" t="s">
         <v>253</v>
@@ -4597,7 +4597,7 @@
         <v>403</v>
       </c>
       <c r="D95" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="F95">
         <v>45</v>
@@ -4626,7 +4626,7 @@
         <v>404</v>
       </c>
       <c r="D96" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="F96">
         <v>45</v>
@@ -4759,7 +4759,7 @@
         <v>581</v>
       </c>
       <c r="D101" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E101" t="s">
         <v>16</v>
@@ -4791,7 +4791,7 @@
         <v>582</v>
       </c>
       <c r="D102" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E102" t="s">
         <v>16</v>
@@ -4823,7 +4823,7 @@
         <v>583</v>
       </c>
       <c r="D103" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E103" t="s">
         <v>16</v>
@@ -4855,7 +4855,7 @@
         <v>584</v>
       </c>
       <c r="D104" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E104" t="s">
         <v>16</v>
@@ -4887,7 +4887,7 @@
         <v>585</v>
       </c>
       <c r="D105" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E105" t="s">
         <v>253</v>
@@ -4919,7 +4919,7 @@
         <v>586</v>
       </c>
       <c r="D106" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E106" t="s">
         <v>253</v>
@@ -5009,7 +5009,7 @@
         <v>589</v>
       </c>
       <c r="D109" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E109" t="s">
         <v>253</v>
@@ -5041,7 +5041,7 @@
         <v>590</v>
       </c>
       <c r="D110" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E110" t="s">
         <v>253</v>
@@ -5247,7 +5247,7 @@
         <v>681</v>
       </c>
       <c r="D117" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="E117" t="s">
         <v>253</v>
@@ -5308,7 +5308,7 @@
         <v>683</v>
       </c>
       <c r="D119" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E119" t="s">
         <v>253</v>
@@ -5427,7 +5427,7 @@
         <v>687</v>
       </c>
       <c r="D123" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E123" t="s">
         <v>253</v>
@@ -5459,7 +5459,7 @@
         <v>688</v>
       </c>
       <c r="D124" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E124" t="s">
         <v>253</v>
@@ -5549,7 +5549,7 @@
         <v>691</v>
       </c>
       <c r="D127" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="E127" t="s">
         <v>253</v>
@@ -5639,7 +5639,7 @@
         <v>842</v>
       </c>
       <c r="D130" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E130" t="s">
         <v>16</v>
@@ -5729,7 +5729,7 @@
         <v>851</v>
       </c>
       <c r="D133" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E133" t="s">
         <v>253</v>
@@ -5761,7 +5761,7 @@
         <v>852</v>
       </c>
       <c r="D134" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E134" t="s">
         <v>253</v>
@@ -5793,7 +5793,7 @@
         <v>853</v>
       </c>
       <c r="D135" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E135" t="s">
         <v>253</v>
@@ -5825,7 +5825,7 @@
         <v>854</v>
       </c>
       <c r="D136" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E136" t="s">
         <v>253</v>
@@ -5857,7 +5857,7 @@
         <v>855</v>
       </c>
       <c r="D137" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E137" t="s">
         <v>253</v>
@@ -5889,7 +5889,7 @@
         <v>856</v>
       </c>
       <c r="D138" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E138" t="s">
         <v>253</v>
@@ -5921,7 +5921,7 @@
         <v>871</v>
       </c>
       <c r="D139" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E139" t="s">
         <v>253</v>
@@ -5953,7 +5953,7 @@
         <v>872</v>
       </c>
       <c r="D140" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E140" t="s">
         <v>253</v>
@@ -5985,7 +5985,7 @@
         <v>879</v>
       </c>
       <c r="D141" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F141">
         <v>45</v>
@@ -6014,7 +6014,7 @@
         <v>880</v>
       </c>
       <c r="D142" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F142">
         <v>45</v>
@@ -6043,7 +6043,7 @@
         <v>881</v>
       </c>
       <c r="D143" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E143" t="s">
         <v>16</v>
@@ -6278,7 +6278,7 @@
         <v>889</v>
       </c>
       <c r="D151" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E151" t="s">
         <v>16</v>
@@ -6310,7 +6310,7 @@
         <v>890</v>
       </c>
       <c r="D152" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E152" t="s">
         <v>16</v>
@@ -6429,7 +6429,7 @@
         <v>922</v>
       </c>
       <c r="D156" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E156" t="s">
         <v>16</v>
@@ -9879,7 +9879,7 @@
         <v>341</v>
       </c>
       <c r="B327" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C327">
         <v>990079</v>
@@ -11569,7 +11569,7 @@
         <v>341</v>
       </c>
       <c r="B392" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C392">
         <v>990289</v>
@@ -11595,7 +11595,7 @@
         <v>341</v>
       </c>
       <c r="B393" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C393">
         <v>990290</v>
@@ -12089,7 +12089,7 @@
         <v>341</v>
       </c>
       <c r="B412" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C412">
         <v>990683</v>
@@ -12115,7 +12115,7 @@
         <v>341</v>
       </c>
       <c r="B413" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C413">
         <v>990684</v>
@@ -12141,7 +12141,7 @@
         <v>341</v>
       </c>
       <c r="B414" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C414">
         <v>990689</v>
@@ -12167,7 +12167,7 @@
         <v>341</v>
       </c>
       <c r="B415" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C415">
         <v>990690</v>
@@ -12193,7 +12193,7 @@
         <v>341</v>
       </c>
       <c r="B416" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C416">
         <v>990691</v>
@@ -12219,7 +12219,7 @@
         <v>341</v>
       </c>
       <c r="B417" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C417">
         <v>990692</v>
@@ -12245,7 +12245,7 @@
         <v>341</v>
       </c>
       <c r="B418" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C418">
         <v>990693</v>
@@ -12260,10 +12260,10 @@
         <v>1E-3</v>
       </c>
       <c r="I418" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="J418" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="419" spans="1:10" x14ac:dyDescent="0.35">
@@ -12271,7 +12271,7 @@
         <v>341</v>
       </c>
       <c r="B419" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C419">
         <v>990694</v>
@@ -12286,10 +12286,10 @@
         <v>1E-3</v>
       </c>
       <c r="I419" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="J419" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="420" spans="1:10" x14ac:dyDescent="0.35">
@@ -12297,7 +12297,7 @@
         <v>341</v>
       </c>
       <c r="B420" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C420">
         <v>990695</v>
@@ -12312,10 +12312,10 @@
         <v>1E-3</v>
       </c>
       <c r="I420" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="J420" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="421" spans="1:10" x14ac:dyDescent="0.35">
@@ -12323,7 +12323,7 @@
         <v>341</v>
       </c>
       <c r="B421" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C421">
         <v>990696</v>
@@ -12338,10 +12338,10 @@
         <v>1E-3</v>
       </c>
       <c r="I421" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="J421" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="422" spans="1:10" x14ac:dyDescent="0.35">
@@ -12349,7 +12349,7 @@
         <v>341</v>
       </c>
       <c r="B422" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C422">
         <v>990857</v>
@@ -12364,10 +12364,10 @@
         <v>1E-3</v>
       </c>
       <c r="I422" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="J422" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="423" spans="1:10" x14ac:dyDescent="0.35">
@@ -12375,7 +12375,7 @@
         <v>341</v>
       </c>
       <c r="B423" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C423">
         <v>990858</v>
@@ -12390,10 +12390,10 @@
         <v>1E-3</v>
       </c>
       <c r="I423" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="J423" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="424" spans="1:10" x14ac:dyDescent="0.35">
@@ -12401,7 +12401,7 @@
         <v>341</v>
       </c>
       <c r="B424" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C424">
         <v>990853</v>
@@ -12416,10 +12416,10 @@
         <v>1E-3</v>
       </c>
       <c r="I424" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="J424" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="425" spans="1:10" x14ac:dyDescent="0.35">
@@ -12427,7 +12427,7 @@
         <v>341</v>
       </c>
       <c r="B425" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C425">
         <v>990854</v>
@@ -12442,10 +12442,10 @@
         <v>1E-3</v>
       </c>
       <c r="I425" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="J425" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="426" spans="1:10" x14ac:dyDescent="0.35">
@@ -12453,7 +12453,7 @@
         <v>341</v>
       </c>
       <c r="B426" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C426">
         <v>990855</v>
@@ -12468,10 +12468,10 @@
         <v>1E-3</v>
       </c>
       <c r="I426" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="J426" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="427" spans="1:10" x14ac:dyDescent="0.35">
@@ -12479,7 +12479,7 @@
         <v>341</v>
       </c>
       <c r="B427" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C427">
         <v>990856</v>
@@ -12494,10 +12494,10 @@
         <v>1E-3</v>
       </c>
       <c r="I427" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="J427" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="428" spans="1:10" x14ac:dyDescent="0.35">
@@ -12713,7 +12713,7 @@
         <v>341</v>
       </c>
       <c r="B436" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="C436">
         <v>990885</v>
@@ -12739,7 +12739,7 @@
         <v>341</v>
       </c>
       <c r="B437" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C437">
         <v>990886</v>
@@ -12765,7 +12765,7 @@
         <v>341</v>
       </c>
       <c r="B438" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C438">
         <v>990887</v>
@@ -12791,7 +12791,7 @@
         <v>341</v>
       </c>
       <c r="B439" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C439">
         <v>990888</v>
@@ -12921,7 +12921,7 @@
         <v>341</v>
       </c>
       <c r="B444" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C444">
         <v>990923</v>
@@ -12947,7 +12947,7 @@
         <v>341</v>
       </c>
       <c r="B445" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C445">
         <v>990924</v>
@@ -12973,7 +12973,7 @@
         <v>341</v>
       </c>
       <c r="B446" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C446">
         <v>990927</v>
@@ -12999,7 +12999,7 @@
         <v>341</v>
       </c>
       <c r="B447" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C447">
         <v>990928</v>
@@ -13074,10 +13074,10 @@
     </row>
     <row r="450" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A450" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B450" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C450">
         <v>2740</v>
@@ -13103,10 +13103,10 @@
     </row>
     <row r="451" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A451" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B451" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C451">
         <v>2770</v>
@@ -13132,10 +13132,10 @@
     </row>
     <row r="452" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A452" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B452" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C452">
         <v>2830</v>
@@ -13161,10 +13161,10 @@
     </row>
     <row r="453" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A453" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B453" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C453">
         <v>2810</v>
@@ -13190,10 +13190,10 @@
     </row>
     <row r="454" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A454" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B454" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C454">
         <v>2340</v>
@@ -13219,10 +13219,10 @@
     </row>
     <row r="455" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A455" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B455" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C455">
         <v>2320</v>
@@ -13248,10 +13248,10 @@
     </row>
     <row r="456" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A456" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B456" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C456">
         <v>2370</v>
@@ -13277,10 +13277,10 @@
     </row>
     <row r="457" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A457" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B457" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C457">
         <v>2450</v>
@@ -13306,10 +13306,10 @@
     </row>
     <row r="458" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A458" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B458" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C458">
         <v>2420</v>
@@ -13335,10 +13335,10 @@
     </row>
     <row r="459" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A459" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B459" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C459">
         <v>2120</v>
@@ -13361,10 +13361,10 @@
     </row>
     <row r="460" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A460" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B460" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C460">
         <v>2130</v>
@@ -13387,10 +13387,10 @@
     </row>
     <row r="461" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A461" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B461" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C461">
         <v>2230</v>
@@ -13413,10 +13413,10 @@
     </row>
     <row r="462" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A462" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B462" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C462">
         <v>1010309</v>
@@ -13437,15 +13437,15 @@
         <v>#N/A</v>
       </c>
       <c r="K462" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="463" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A463" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B463" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C463">
         <v>1010310</v>
@@ -13466,15 +13466,15 @@
         <v>#N/A</v>
       </c>
       <c r="K463" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="464" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A464" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B464" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C464">
         <v>800601</v>
@@ -13495,15 +13495,15 @@
         <v>#N/A</v>
       </c>
       <c r="K464" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="465" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A465" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B465" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C465">
         <v>800602</v>
@@ -13524,755 +13524,1367 @@
         <v>#N/A</v>
       </c>
       <c r="K465" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="466" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A466" t="s">
+        <v>454</v>
+      </c>
+      <c r="B466" t="s">
         <v>455</v>
-      </c>
-      <c r="B466" t="s">
-        <v>456</v>
       </c>
       <c r="C466">
         <v>800501</v>
       </c>
+      <c r="F466">
+        <v>45</v>
+      </c>
+      <c r="G466">
+        <v>5</v>
+      </c>
+      <c r="H466">
+        <v>0.03</v>
+      </c>
     </row>
     <row r="467" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A467" t="s">
+        <v>454</v>
+      </c>
+      <c r="B467" t="s">
         <v>455</v>
-      </c>
-      <c r="B467" t="s">
-        <v>456</v>
       </c>
       <c r="C467">
         <v>800502</v>
       </c>
+      <c r="F467">
+        <v>45</v>
+      </c>
+      <c r="G467">
+        <v>5</v>
+      </c>
+      <c r="H467">
+        <v>0.03</v>
+      </c>
     </row>
     <row r="468" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A468" t="s">
+        <v>454</v>
+      </c>
+      <c r="B468" t="s">
         <v>455</v>
-      </c>
-      <c r="B468" t="s">
-        <v>456</v>
       </c>
       <c r="C468">
         <v>800503</v>
       </c>
+      <c r="F468">
+        <v>45</v>
+      </c>
+      <c r="G468">
+        <v>5</v>
+      </c>
+      <c r="H468">
+        <v>0.03</v>
+      </c>
     </row>
     <row r="469" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A469" t="s">
+        <v>454</v>
+      </c>
+      <c r="B469" t="s">
         <v>455</v>
-      </c>
-      <c r="B469" t="s">
-        <v>456</v>
       </c>
       <c r="C469">
         <v>800603</v>
       </c>
+      <c r="F469">
+        <v>45</v>
+      </c>
+      <c r="G469">
+        <v>5</v>
+      </c>
+      <c r="H469">
+        <v>0.03</v>
+      </c>
     </row>
     <row r="470" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A470" t="s">
+        <v>454</v>
+      </c>
+      <c r="B470" t="s">
         <v>455</v>
-      </c>
-      <c r="B470" t="s">
-        <v>456</v>
       </c>
       <c r="C470">
         <v>800504</v>
       </c>
+      <c r="F470">
+        <v>45</v>
+      </c>
+      <c r="G470">
+        <v>5</v>
+      </c>
+      <c r="H470">
+        <v>0.03</v>
+      </c>
     </row>
     <row r="471" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A471" t="s">
+        <v>454</v>
+      </c>
+      <c r="B471" t="s">
         <v>455</v>
-      </c>
-      <c r="B471" t="s">
-        <v>456</v>
       </c>
       <c r="C471">
         <v>800604</v>
       </c>
+      <c r="F471">
+        <v>45</v>
+      </c>
+      <c r="G471">
+        <v>5</v>
+      </c>
+      <c r="H471">
+        <v>0.03</v>
+      </c>
     </row>
     <row r="472" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A472" t="s">
+        <v>454</v>
+      </c>
+      <c r="B472" t="s">
         <v>455</v>
-      </c>
-      <c r="B472" t="s">
-        <v>456</v>
       </c>
       <c r="C472">
         <v>1010305</v>
       </c>
+      <c r="F472">
+        <v>45</v>
+      </c>
+      <c r="G472">
+        <v>5</v>
+      </c>
+      <c r="H472">
+        <v>0.03</v>
+      </c>
     </row>
     <row r="473" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A473" t="s">
+        <v>454</v>
+      </c>
+      <c r="B473" t="s">
         <v>455</v>
-      </c>
-      <c r="B473" t="s">
-        <v>456</v>
       </c>
       <c r="C473">
         <v>1010306</v>
       </c>
+      <c r="F473">
+        <v>45</v>
+      </c>
+      <c r="G473">
+        <v>5</v>
+      </c>
+      <c r="H473">
+        <v>0.03</v>
+      </c>
     </row>
     <row r="474" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A474" t="s">
+        <v>454</v>
+      </c>
+      <c r="B474" t="s">
         <v>455</v>
-      </c>
-      <c r="B474" t="s">
-        <v>456</v>
       </c>
       <c r="C474">
         <v>1010307</v>
       </c>
+      <c r="F474">
+        <v>45</v>
+      </c>
+      <c r="G474">
+        <v>5</v>
+      </c>
+      <c r="H474">
+        <v>0.03</v>
+      </c>
     </row>
     <row r="475" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A475" t="s">
+        <v>454</v>
+      </c>
+      <c r="B475" t="s">
         <v>455</v>
-      </c>
-      <c r="B475" t="s">
-        <v>456</v>
       </c>
       <c r="C475">
         <v>1010308</v>
       </c>
+      <c r="F475">
+        <v>45</v>
+      </c>
+      <c r="G475">
+        <v>5</v>
+      </c>
+      <c r="H475">
+        <v>0.03</v>
+      </c>
     </row>
     <row r="476" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A476" t="s">
+        <v>454</v>
+      </c>
+      <c r="B476" t="s">
         <v>455</v>
-      </c>
-      <c r="B476" t="s">
-        <v>456</v>
       </c>
       <c r="C476">
         <v>2800308</v>
       </c>
+      <c r="F476">
+        <v>45</v>
+      </c>
+      <c r="G476">
+        <v>5</v>
+      </c>
+      <c r="H476">
+        <v>0.03</v>
+      </c>
     </row>
     <row r="477" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A477" t="s">
+        <v>454</v>
+      </c>
+      <c r="B477" t="s">
         <v>455</v>
-      </c>
-      <c r="B477" t="s">
-        <v>456</v>
       </c>
       <c r="C477">
         <v>2800309</v>
       </c>
+      <c r="F477">
+        <v>45</v>
+      </c>
+      <c r="G477">
+        <v>5</v>
+      </c>
+      <c r="H477">
+        <v>0.03</v>
+      </c>
     </row>
     <row r="478" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A478" t="s">
+        <v>454</v>
+      </c>
+      <c r="B478" t="s">
         <v>455</v>
-      </c>
-      <c r="B478" t="s">
-        <v>456</v>
       </c>
       <c r="C478">
         <v>2800310</v>
       </c>
+      <c r="F478">
+        <v>45</v>
+      </c>
+      <c r="G478">
+        <v>5</v>
+      </c>
+      <c r="H478">
+        <v>0.03</v>
+      </c>
     </row>
     <row r="479" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A479" t="s">
+        <v>454</v>
+      </c>
+      <c r="B479" t="s">
         <v>455</v>
-      </c>
-      <c r="B479" t="s">
-        <v>456</v>
       </c>
       <c r="C479">
         <v>2800311</v>
       </c>
+      <c r="F479">
+        <v>45</v>
+      </c>
+      <c r="G479">
+        <v>5</v>
+      </c>
+      <c r="H479">
+        <v>0.03</v>
+      </c>
     </row>
     <row r="480" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A480" t="s">
+        <v>454</v>
+      </c>
+      <c r="B480" t="s">
         <v>455</v>
-      </c>
-      <c r="B480" t="s">
-        <v>456</v>
       </c>
       <c r="C480">
         <v>2800312</v>
       </c>
-    </row>
-    <row r="481" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F480">
+        <v>45</v>
+      </c>
+      <c r="G480">
+        <v>5</v>
+      </c>
+      <c r="H480">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="481" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A481" t="s">
+        <v>454</v>
+      </c>
+      <c r="B481" t="s">
         <v>455</v>
-      </c>
-      <c r="B481" t="s">
-        <v>456</v>
       </c>
       <c r="C481">
         <v>2800313</v>
       </c>
-    </row>
-    <row r="482" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F481">
+        <v>45</v>
+      </c>
+      <c r="G481">
+        <v>5</v>
+      </c>
+      <c r="H481">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="482" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A482" t="s">
+        <v>454</v>
+      </c>
+      <c r="B482" t="s">
         <v>455</v>
-      </c>
-      <c r="B482" t="s">
-        <v>456</v>
       </c>
       <c r="C482">
         <v>2800314</v>
       </c>
-    </row>
-    <row r="483" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F482">
+        <v>45</v>
+      </c>
+      <c r="G482">
+        <v>5</v>
+      </c>
+      <c r="H482">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="483" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A483" t="s">
+        <v>454</v>
+      </c>
+      <c r="B483" t="s">
         <v>455</v>
-      </c>
-      <c r="B483" t="s">
-        <v>456</v>
       </c>
       <c r="C483">
         <v>2800315</v>
       </c>
-    </row>
-    <row r="484" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F483">
+        <v>45</v>
+      </c>
+      <c r="G483">
+        <v>5</v>
+      </c>
+      <c r="H483">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="484" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A484" t="s">
+        <v>454</v>
+      </c>
+      <c r="B484" t="s">
         <v>455</v>
-      </c>
-      <c r="B484" t="s">
-        <v>456</v>
       </c>
       <c r="C484">
         <v>40516</v>
       </c>
-    </row>
-    <row r="485" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F484">
+        <v>45</v>
+      </c>
+      <c r="G484">
+        <v>5</v>
+      </c>
+      <c r="H484">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="485" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A485" t="s">
+        <v>454</v>
+      </c>
+      <c r="B485" t="s">
         <v>455</v>
-      </c>
-      <c r="B485" t="s">
-        <v>456</v>
       </c>
       <c r="C485">
         <v>40517</v>
       </c>
-    </row>
-    <row r="486" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F485">
+        <v>45</v>
+      </c>
+      <c r="G485">
+        <v>5</v>
+      </c>
+      <c r="H485">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="486" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A486" t="s">
+        <v>454</v>
+      </c>
+      <c r="B486" t="s">
         <v>455</v>
-      </c>
-      <c r="B486" t="s">
-        <v>456</v>
       </c>
       <c r="C486">
         <v>40518</v>
       </c>
-    </row>
-    <row r="487" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F486">
+        <v>45</v>
+      </c>
+      <c r="G486">
+        <v>5</v>
+      </c>
+      <c r="H486">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="487" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A487" t="s">
+        <v>454</v>
+      </c>
+      <c r="B487" t="s">
         <v>455</v>
-      </c>
-      <c r="B487" t="s">
-        <v>456</v>
       </c>
       <c r="C487">
         <v>40519</v>
       </c>
-    </row>
-    <row r="488" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F487">
+        <v>45</v>
+      </c>
+      <c r="G487">
+        <v>5</v>
+      </c>
+      <c r="H487">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="488" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A488" t="s">
+        <v>454</v>
+      </c>
+      <c r="B488" t="s">
         <v>455</v>
-      </c>
-      <c r="B488" t="s">
-        <v>456</v>
       </c>
       <c r="C488">
         <v>5800420</v>
       </c>
-    </row>
-    <row r="489" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F488">
+        <v>45</v>
+      </c>
+      <c r="G488">
+        <v>5</v>
+      </c>
+      <c r="H488">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="489" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A489" t="s">
+        <v>454</v>
+      </c>
+      <c r="B489" t="s">
         <v>455</v>
-      </c>
-      <c r="B489" t="s">
-        <v>456</v>
       </c>
       <c r="C489">
         <v>5800421</v>
       </c>
-    </row>
-    <row r="490" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F489">
+        <v>45</v>
+      </c>
+      <c r="G489">
+        <v>5</v>
+      </c>
+      <c r="H489">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="490" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A490" t="s">
+        <v>454</v>
+      </c>
+      <c r="B490" t="s">
         <v>455</v>
-      </c>
-      <c r="B490" t="s">
-        <v>456</v>
       </c>
       <c r="C490">
         <v>5800422</v>
       </c>
-    </row>
-    <row r="491" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F490">
+        <v>45</v>
+      </c>
+      <c r="G490">
+        <v>5</v>
+      </c>
+      <c r="H490">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="491" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A491" t="s">
+        <v>454</v>
+      </c>
+      <c r="B491" t="s">
         <v>455</v>
-      </c>
-      <c r="B491" t="s">
-        <v>456</v>
       </c>
       <c r="C491">
         <v>5800423</v>
       </c>
-    </row>
-    <row r="492" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F491">
+        <v>45</v>
+      </c>
+      <c r="G491">
+        <v>5</v>
+      </c>
+      <c r="H491">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="492" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A492" t="s">
+        <v>454</v>
+      </c>
+      <c r="B492" t="s">
         <v>455</v>
-      </c>
-      <c r="B492" t="s">
-        <v>456</v>
       </c>
       <c r="C492">
         <v>5800424</v>
       </c>
-    </row>
-    <row r="493" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F492">
+        <v>45</v>
+      </c>
+      <c r="G492">
+        <v>5</v>
+      </c>
+      <c r="H492">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="493" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A493" t="s">
+        <v>454</v>
+      </c>
+      <c r="B493" t="s">
         <v>455</v>
-      </c>
-      <c r="B493" t="s">
-        <v>456</v>
       </c>
       <c r="C493">
         <v>5800425</v>
       </c>
-    </row>
-    <row r="494" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F493">
+        <v>45</v>
+      </c>
+      <c r="G493">
+        <v>5</v>
+      </c>
+      <c r="H493">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="494" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A494" t="s">
+        <v>454</v>
+      </c>
+      <c r="B494" t="s">
         <v>455</v>
-      </c>
-      <c r="B494" t="s">
-        <v>456</v>
       </c>
       <c r="C494">
         <v>5800426</v>
       </c>
-    </row>
-    <row r="495" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F494">
+        <v>45</v>
+      </c>
+      <c r="G494">
+        <v>5</v>
+      </c>
+      <c r="H494">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="495" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A495" t="s">
+        <v>454</v>
+      </c>
+      <c r="B495" t="s">
         <v>455</v>
-      </c>
-      <c r="B495" t="s">
-        <v>456</v>
       </c>
       <c r="C495">
         <v>5800427</v>
       </c>
-    </row>
-    <row r="496" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F495">
+        <v>45</v>
+      </c>
+      <c r="G495">
+        <v>5</v>
+      </c>
+      <c r="H495">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="496" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A496" t="s">
+        <v>454</v>
+      </c>
+      <c r="B496" t="s">
         <v>455</v>
-      </c>
-      <c r="B496" t="s">
-        <v>456</v>
       </c>
       <c r="C496">
         <v>6800530</v>
       </c>
-    </row>
-    <row r="497" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F496">
+        <v>45</v>
+      </c>
+      <c r="G496">
+        <v>5</v>
+      </c>
+      <c r="H496">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="497" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A497" t="s">
+        <v>454</v>
+      </c>
+      <c r="B497" t="s">
         <v>455</v>
-      </c>
-      <c r="B497" t="s">
-        <v>456</v>
       </c>
       <c r="C497">
         <v>6800531</v>
       </c>
-    </row>
-    <row r="498" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F497">
+        <v>45</v>
+      </c>
+      <c r="G497">
+        <v>5</v>
+      </c>
+      <c r="H497">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="498" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A498" t="s">
+        <v>454</v>
+      </c>
+      <c r="B498" t="s">
         <v>455</v>
-      </c>
-      <c r="B498" t="s">
-        <v>456</v>
       </c>
       <c r="C498">
         <v>6800532</v>
       </c>
-    </row>
-    <row r="499" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F498">
+        <v>45</v>
+      </c>
+      <c r="G498">
+        <v>5</v>
+      </c>
+      <c r="H498">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="499" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A499" t="s">
+        <v>454</v>
+      </c>
+      <c r="B499" t="s">
         <v>455</v>
-      </c>
-      <c r="B499" t="s">
-        <v>456</v>
       </c>
       <c r="C499">
         <v>6800533</v>
       </c>
-    </row>
-    <row r="500" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F499">
+        <v>45</v>
+      </c>
+      <c r="G499">
+        <v>5</v>
+      </c>
+      <c r="H499">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="500" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A500" t="s">
+        <v>454</v>
+      </c>
+      <c r="B500" t="s">
         <v>455</v>
-      </c>
-      <c r="B500" t="s">
-        <v>456</v>
       </c>
       <c r="C500">
         <v>6800330</v>
       </c>
-    </row>
-    <row r="501" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F500">
+        <v>45</v>
+      </c>
+      <c r="G500">
+        <v>5</v>
+      </c>
+      <c r="H500">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="501" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A501" t="s">
+        <v>454</v>
+      </c>
+      <c r="B501" t="s">
         <v>455</v>
-      </c>
-      <c r="B501" t="s">
-        <v>456</v>
       </c>
       <c r="C501">
         <v>850331</v>
       </c>
-    </row>
-    <row r="502" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F501">
+        <v>45</v>
+      </c>
+      <c r="G501">
+        <v>5</v>
+      </c>
+      <c r="H501">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="502" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A502" t="s">
+        <v>454</v>
+      </c>
+      <c r="B502" t="s">
         <v>455</v>
-      </c>
-      <c r="B502" t="s">
-        <v>456</v>
       </c>
       <c r="C502">
         <v>850332</v>
       </c>
-    </row>
-    <row r="503" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F502">
+        <v>45</v>
+      </c>
+      <c r="G502">
+        <v>5</v>
+      </c>
+      <c r="H502">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="503" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A503" t="s">
+        <v>454</v>
+      </c>
+      <c r="B503" t="s">
         <v>455</v>
-      </c>
-      <c r="B503" t="s">
-        <v>456</v>
       </c>
       <c r="C503">
         <v>850333</v>
       </c>
-    </row>
-    <row r="504" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F503">
+        <v>45</v>
+      </c>
+      <c r="G503">
+        <v>5</v>
+      </c>
+      <c r="H503">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="504" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A504" t="s">
+        <v>454</v>
+      </c>
+      <c r="B504" t="s">
         <v>455</v>
-      </c>
-      <c r="B504" t="s">
-        <v>456</v>
       </c>
       <c r="C504">
         <v>850334</v>
       </c>
-    </row>
-    <row r="505" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F504">
+        <v>45</v>
+      </c>
+      <c r="G504">
+        <v>5</v>
+      </c>
+      <c r="H504">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="505" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A505" t="s">
+        <v>454</v>
+      </c>
+      <c r="B505" t="s">
         <v>455</v>
-      </c>
-      <c r="B505" t="s">
-        <v>456</v>
       </c>
       <c r="C505">
         <v>870335</v>
       </c>
-    </row>
-    <row r="506" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F505">
+        <v>45</v>
+      </c>
+      <c r="G505">
+        <v>5</v>
+      </c>
+      <c r="H505">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="506" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A506" t="s">
+        <v>454</v>
+      </c>
+      <c r="B506" t="s">
         <v>455</v>
-      </c>
-      <c r="B506" t="s">
-        <v>456</v>
       </c>
       <c r="C506">
         <v>870336</v>
       </c>
-    </row>
-    <row r="507" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F506">
+        <v>45</v>
+      </c>
+      <c r="G506">
+        <v>5</v>
+      </c>
+      <c r="H506">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="507" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A507" t="s">
+        <v>454</v>
+      </c>
+      <c r="B507" t="s">
         <v>455</v>
-      </c>
-      <c r="B507" t="s">
-        <v>456</v>
       </c>
       <c r="C507">
         <v>870337</v>
       </c>
-    </row>
-    <row r="508" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F507">
+        <v>45</v>
+      </c>
+      <c r="G507">
+        <v>5</v>
+      </c>
+      <c r="H507">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="508" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A508" t="s">
+        <v>454</v>
+      </c>
+      <c r="B508" t="s">
         <v>455</v>
-      </c>
-      <c r="B508" t="s">
-        <v>456</v>
       </c>
       <c r="C508">
         <v>870338</v>
       </c>
-    </row>
-    <row r="509" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F508">
+        <v>45</v>
+      </c>
+      <c r="G508">
+        <v>5</v>
+      </c>
+      <c r="H508">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="509" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A509" t="s">
+        <v>454</v>
+      </c>
+      <c r="B509" t="s">
         <v>455</v>
-      </c>
-      <c r="B509" t="s">
-        <v>456</v>
       </c>
       <c r="C509">
         <v>8800439</v>
       </c>
-    </row>
-    <row r="510" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F509">
+        <v>45</v>
+      </c>
+      <c r="G509">
+        <v>5</v>
+      </c>
+      <c r="H509">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="510" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A510" t="s">
+        <v>454</v>
+      </c>
+      <c r="B510" t="s">
         <v>455</v>
-      </c>
-      <c r="B510" t="s">
-        <v>456</v>
       </c>
       <c r="C510">
         <v>8800440</v>
       </c>
-    </row>
-    <row r="511" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F510">
+        <v>45</v>
+      </c>
+      <c r="G510">
+        <v>5</v>
+      </c>
+      <c r="H510">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="511" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A511" t="s">
+        <v>454</v>
+      </c>
+      <c r="B511" t="s">
         <v>455</v>
-      </c>
-      <c r="B511" t="s">
-        <v>456</v>
       </c>
       <c r="C511">
         <v>8800441</v>
       </c>
-    </row>
-    <row r="512" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F511">
+        <v>45</v>
+      </c>
+      <c r="G511">
+        <v>5</v>
+      </c>
+      <c r="H511">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="512" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A512" t="s">
+        <v>454</v>
+      </c>
+      <c r="B512" t="s">
         <v>455</v>
-      </c>
-      <c r="B512" t="s">
-        <v>456</v>
       </c>
       <c r="C512">
         <v>8800442</v>
       </c>
-    </row>
-    <row r="513" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F512">
+        <v>45</v>
+      </c>
+      <c r="G512">
+        <v>5</v>
+      </c>
+      <c r="H512">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="513" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A513" t="s">
+        <v>454</v>
+      </c>
+      <c r="B513" t="s">
         <v>455</v>
-      </c>
-      <c r="B513" t="s">
-        <v>456</v>
       </c>
       <c r="C513">
         <v>8800443</v>
       </c>
-    </row>
-    <row r="514" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F513">
+        <v>45</v>
+      </c>
+      <c r="G513">
+        <v>5</v>
+      </c>
+      <c r="H513">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="514" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A514" t="s">
+        <v>454</v>
+      </c>
+      <c r="B514" t="s">
         <v>455</v>
-      </c>
-      <c r="B514" t="s">
-        <v>456</v>
       </c>
       <c r="C514">
         <v>6800544</v>
       </c>
-    </row>
-    <row r="515" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F514">
+        <v>45</v>
+      </c>
+      <c r="G514">
+        <v>5</v>
+      </c>
+      <c r="H514">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="515" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A515" t="s">
+        <v>454</v>
+      </c>
+      <c r="B515" t="s">
         <v>455</v>
-      </c>
-      <c r="B515" t="s">
-        <v>456</v>
       </c>
       <c r="C515">
         <v>6800545</v>
       </c>
-    </row>
-    <row r="516" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F515">
+        <v>45</v>
+      </c>
+      <c r="G515">
+        <v>5</v>
+      </c>
+      <c r="H515">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="516" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A516" t="s">
+        <v>454</v>
+      </c>
+      <c r="B516" t="s">
         <v>455</v>
-      </c>
-      <c r="B516" t="s">
-        <v>456</v>
       </c>
       <c r="C516">
         <v>8800446</v>
       </c>
-    </row>
-    <row r="517" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F516">
+        <v>45</v>
+      </c>
+      <c r="G516">
+        <v>5</v>
+      </c>
+      <c r="H516">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="517" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A517" t="s">
+        <v>454</v>
+      </c>
+      <c r="B517" t="s">
         <v>455</v>
-      </c>
-      <c r="B517" t="s">
-        <v>456</v>
       </c>
       <c r="C517">
         <v>8800447</v>
       </c>
-    </row>
-    <row r="518" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F517">
+        <v>45</v>
+      </c>
+      <c r="G517">
+        <v>5</v>
+      </c>
+      <c r="H517">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="518" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A518" t="s">
+        <v>454</v>
+      </c>
+      <c r="B518" t="s">
         <v>455</v>
-      </c>
-      <c r="B518" t="s">
-        <v>456</v>
       </c>
       <c r="C518">
         <v>8800448</v>
       </c>
-    </row>
-    <row r="519" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F518">
+        <v>45</v>
+      </c>
+      <c r="G518">
+        <v>5</v>
+      </c>
+      <c r="H518">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="519" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A519" t="s">
+        <v>454</v>
+      </c>
+      <c r="B519" t="s">
         <v>455</v>
-      </c>
-      <c r="B519" t="s">
-        <v>456</v>
       </c>
       <c r="C519">
         <v>8800349</v>
       </c>
-    </row>
-    <row r="520" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F519">
+        <v>45</v>
+      </c>
+      <c r="G519">
+        <v>5</v>
+      </c>
+      <c r="H519">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="520" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A520" t="s">
+        <v>454</v>
+      </c>
+      <c r="B520" t="s">
         <v>455</v>
-      </c>
-      <c r="B520" t="s">
-        <v>456</v>
       </c>
       <c r="C520">
         <v>8800449</v>
       </c>
-    </row>
-    <row r="521" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F520">
+        <v>45</v>
+      </c>
+      <c r="G520">
+        <v>5</v>
+      </c>
+      <c r="H520">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="521" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A521" t="s">
+        <v>454</v>
+      </c>
+      <c r="B521" t="s">
         <v>455</v>
-      </c>
-      <c r="B521" t="s">
-        <v>456</v>
       </c>
       <c r="C521">
         <v>8800450</v>
       </c>
-    </row>
-    <row r="522" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F521">
+        <v>45</v>
+      </c>
+      <c r="G521">
+        <v>5</v>
+      </c>
+      <c r="H521">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="522" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A522" t="s">
+        <v>454</v>
+      </c>
+      <c r="B522" t="s">
         <v>455</v>
-      </c>
-      <c r="B522" t="s">
-        <v>456</v>
       </c>
       <c r="C522">
         <v>8800351</v>
       </c>
-    </row>
-    <row r="523" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F522">
+        <v>45</v>
+      </c>
+      <c r="G522">
+        <v>5</v>
+      </c>
+      <c r="H522">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="523" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A523" t="s">
+        <v>454</v>
+      </c>
+      <c r="B523" t="s">
         <v>455</v>
-      </c>
-      <c r="B523" t="s">
-        <v>456</v>
       </c>
       <c r="C523">
         <v>8800451</v>
       </c>
-    </row>
-    <row r="524" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F523">
+        <v>45</v>
+      </c>
+      <c r="G523">
+        <v>5</v>
+      </c>
+      <c r="H523">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="524" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A524" t="s">
+        <v>454</v>
+      </c>
+      <c r="B524" t="s">
         <v>455</v>
-      </c>
-      <c r="B524" t="s">
-        <v>456</v>
       </c>
       <c r="C524">
         <v>8800452</v>
       </c>
-    </row>
-    <row r="525" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F524">
+        <v>45</v>
+      </c>
+      <c r="G524">
+        <v>5</v>
+      </c>
+      <c r="H524">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="525" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A525" t="s">
+        <v>454</v>
+      </c>
+      <c r="B525" t="s">
         <v>455</v>
-      </c>
-      <c r="B525" t="s">
-        <v>456</v>
       </c>
       <c r="C525">
         <v>1010253</v>
       </c>
-    </row>
-    <row r="526" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F525">
+        <v>45</v>
+      </c>
+      <c r="G525">
+        <v>5</v>
+      </c>
+      <c r="H525">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="526" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A526" t="s">
+        <v>454</v>
+      </c>
+      <c r="B526" t="s">
         <v>455</v>
-      </c>
-      <c r="B526" t="s">
-        <v>456</v>
       </c>
       <c r="C526">
         <v>1010254</v>
       </c>
-    </row>
-    <row r="527" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F526">
+        <v>45</v>
+      </c>
+      <c r="G526">
+        <v>5</v>
+      </c>
+      <c r="H526">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="527" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A527" t="s">
+        <v>454</v>
+      </c>
+      <c r="B527" t="s">
         <v>455</v>
-      </c>
-      <c r="B527" t="s">
-        <v>456</v>
       </c>
       <c r="C527">
         <v>1010255</v>
       </c>
-    </row>
-    <row r="528" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F527">
+        <v>45</v>
+      </c>
+      <c r="G527">
+        <v>5</v>
+      </c>
+      <c r="H527">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="528" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A528" t="s">
+        <v>454</v>
+      </c>
+      <c r="B528" t="s">
         <v>455</v>
-      </c>
-      <c r="B528" t="s">
-        <v>456</v>
       </c>
       <c r="C528">
         <v>1010256</v>
       </c>
-    </row>
-    <row r="529" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F528">
+        <v>45</v>
+      </c>
+      <c r="G528">
+        <v>5</v>
+      </c>
+      <c r="H528">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="529" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A529" t="s">
+        <v>454</v>
+      </c>
+      <c r="B529" t="s">
         <v>455</v>
-      </c>
-      <c r="B529" t="s">
-        <v>456</v>
       </c>
       <c r="C529">
         <v>1010356</v>
       </c>
-    </row>
-    <row r="530" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F529">
+        <v>45</v>
+      </c>
+      <c r="G529">
+        <v>5</v>
+      </c>
+      <c r="H529">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="530" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A530" t="s">
+        <v>454</v>
+      </c>
+      <c r="B530" t="s">
         <v>455</v>
-      </c>
-      <c r="B530" t="s">
-        <v>456</v>
       </c>
       <c r="C530">
         <v>1010257</v>
       </c>
-    </row>
-    <row r="531" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F530">
+        <v>45</v>
+      </c>
+      <c r="G530">
+        <v>5</v>
+      </c>
+      <c r="H530">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="531" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A531" t="s">
+        <v>454</v>
+      </c>
+      <c r="B531" t="s">
         <v>455</v>
-      </c>
-      <c r="B531" t="s">
-        <v>456</v>
       </c>
       <c r="C531">
         <v>1010258</v>
       </c>
-    </row>
-    <row r="532" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F531">
+        <v>45</v>
+      </c>
+      <c r="G531">
+        <v>5</v>
+      </c>
+      <c r="H531">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="532" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A532" t="s">
+        <v>454</v>
+      </c>
+      <c r="B532" t="s">
         <v>455</v>
-      </c>
-      <c r="B532" t="s">
-        <v>456</v>
       </c>
       <c r="C532">
         <v>1010259</v>
       </c>
-    </row>
-    <row r="533" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F532">
+        <v>45</v>
+      </c>
+      <c r="G532">
+        <v>5</v>
+      </c>
+      <c r="H532">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="533" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A533" t="s">
+        <v>454</v>
+      </c>
+      <c r="B533" t="s">
         <v>455</v>
-      </c>
-      <c r="B533" t="s">
-        <v>456</v>
       </c>
       <c r="C533">
         <v>1010260</v>
+      </c>
+      <c r="F533">
+        <v>45</v>
+      </c>
+      <c r="G533">
+        <v>5</v>
+      </c>
+      <c r="H533">
+        <v>0.03</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add the generic all-lane-tolling code 999999 to the tollclass designation file
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/TOLLCLASS_Designations.xlsx
+++ b/utilities/NextGenFwys/TOLLCLASS_Designations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sisrael\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C0BBCD-7138-4206-BDE7-D68D395DC354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB3DD0AB-1D3F-4DC7-A195-574FF4A39985}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33720" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{0F0A9957-56E7-4C48-967B-2AB2A1965C2F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{0F0A9957-56E7-4C48-967B-2AB2A1965C2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs_for_tollcalib" sheetId="1" r:id="rId1"/>
@@ -97,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1831" uniqueCount="482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1833" uniqueCount="483">
   <si>
     <t>SR92 SM - I-280 Interchange to US101 Interchange - WB</t>
   </si>
@@ -1543,6 +1543,9 @@
   </si>
   <si>
     <t>I-280 SF - SF/SM County Line to US101 Interchange  (Per Mile Tolling) - SB</t>
+  </si>
+  <si>
+    <t>Generic all-lane-tolling</t>
   </si>
 </sst>
 </file>
@@ -1657,10 +1660,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1963,11 +1962,11 @@
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
-  <dimension ref="A1:K535"/>
+  <dimension ref="A1:K536"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A376" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B395" sqref="B395"/>
+      <pane ySplit="1" topLeftCell="A504" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B536" sqref="B536"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15018,6 +15017,17 @@
       </c>
       <c r="H535">
         <v>0.03</v>
+      </c>
+    </row>
+    <row r="536" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A536" t="s">
+        <v>452</v>
+      </c>
+      <c r="B536" t="s">
+        <v>482</v>
+      </c>
+      <c r="C536">
+        <v>999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit missing tollclass 1010001
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/TOLLCLASS_Designations.xlsx
+++ b/utilities/NextGenFwys/TOLLCLASS_Designations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0502B6C1-66FF-4120-88D3-ACCDDFCB142A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93DD6CD1-608E-4EE8-A21E-84113B1D34A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{0F0A9957-56E7-4C48-967B-2AB2A1965C2F}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Readme - numbering convention" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Inputs_for_tollcalib!$A$1:$J$535</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Inputs_for_tollcalib!$A$1:$K$547</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1942" uniqueCount="491">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1942" uniqueCount="501">
   <si>
     <t>SR92 SM - I-280 Interchange to US101 Interchange - WB</t>
   </si>
@@ -1512,6 +1512,36 @@
   </si>
   <si>
     <t xml:space="preserve">SR92 in San Mateo </t>
+  </si>
+  <si>
+    <t>NextGenFwyR2 - P8</t>
+  </si>
+  <si>
+    <t>NextGenFwyR2 - P9</t>
+  </si>
+  <si>
+    <t>NextGenFwyR2 - P10</t>
+  </si>
+  <si>
+    <t>NextGenFwyR2 - P11</t>
+  </si>
+  <si>
+    <t>NextGenFwyR2 - P13</t>
+  </si>
+  <si>
+    <t>NextGenFwyR2 - P14</t>
+  </si>
+  <si>
+    <t>NextGenFwyR2 - P15</t>
+  </si>
+  <si>
+    <t>NextGenFwyR2 - P16</t>
+  </si>
+  <si>
+    <t>NextGenFwyR2 - P17</t>
+  </si>
+  <si>
+    <t>NextGenFwyR2 - P18</t>
   </si>
 </sst>
 </file>
@@ -1918,8 +1948,8 @@
   <dimension ref="A1:K547"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A522" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B550" sqref="B550"/>
+      <pane ySplit="1" topLeftCell="A525" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A541" sqref="A541:XFD541"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7233,6 +7263,9 @@
       <c r="C185">
         <v>770075</v>
       </c>
+      <c r="G185">
+        <v>5</v>
+      </c>
       <c r="I185" t="s">
         <v>361</v>
       </c>
@@ -7250,6 +7283,9 @@
       <c r="C186">
         <v>770076</v>
       </c>
+      <c r="G186">
+        <v>5</v>
+      </c>
       <c r="I186" t="s">
         <v>362</v>
       </c>
@@ -7267,6 +7303,9 @@
       <c r="C187">
         <v>770077</v>
       </c>
+      <c r="G187">
+        <v>5</v>
+      </c>
       <c r="I187" t="s">
         <v>362</v>
       </c>
@@ -7284,6 +7323,9 @@
       <c r="C188">
         <v>770078</v>
       </c>
+      <c r="G188">
+        <v>5</v>
+      </c>
       <c r="I188" t="s">
         <v>361</v>
       </c>
@@ -7301,6 +7343,9 @@
       <c r="C189">
         <v>770081</v>
       </c>
+      <c r="G189">
+        <v>5</v>
+      </c>
       <c r="I189" t="s">
         <v>341</v>
       </c>
@@ -7318,6 +7363,9 @@
       <c r="C190">
         <v>770082</v>
       </c>
+      <c r="G190">
+        <v>5</v>
+      </c>
       <c r="I190" t="s">
         <v>340</v>
       </c>
@@ -7335,6 +7383,9 @@
       <c r="C191">
         <v>770083</v>
       </c>
+      <c r="G191">
+        <v>5</v>
+      </c>
       <c r="I191" t="s">
         <v>342</v>
       </c>
@@ -7352,6 +7403,9 @@
       <c r="C192">
         <v>770084</v>
       </c>
+      <c r="G192">
+        <v>5</v>
+      </c>
       <c r="I192" t="s">
         <v>380</v>
       </c>
@@ -7369,6 +7423,9 @@
       <c r="C193">
         <v>770085</v>
       </c>
+      <c r="G193">
+        <v>5</v>
+      </c>
       <c r="I193" t="s">
         <v>342</v>
       </c>
@@ -7386,6 +7443,9 @@
       <c r="C194">
         <v>770086</v>
       </c>
+      <c r="G194">
+        <v>5</v>
+      </c>
       <c r="I194" t="s">
         <v>380</v>
       </c>
@@ -7403,6 +7463,9 @@
       <c r="C195">
         <v>770087</v>
       </c>
+      <c r="G195">
+        <v>5</v>
+      </c>
       <c r="I195" t="s">
         <v>349</v>
       </c>
@@ -7420,6 +7483,9 @@
       <c r="C196">
         <v>770088</v>
       </c>
+      <c r="G196">
+        <v>5</v>
+      </c>
       <c r="I196" t="s">
         <v>343</v>
       </c>
@@ -7437,6 +7503,9 @@
       <c r="C197">
         <v>770091</v>
       </c>
+      <c r="G197">
+        <v>5</v>
+      </c>
       <c r="I197" t="s">
         <v>349</v>
       </c>
@@ -7454,6 +7523,9 @@
       <c r="C198">
         <v>770092</v>
       </c>
+      <c r="G198">
+        <v>5</v>
+      </c>
       <c r="I198" t="s">
         <v>343</v>
       </c>
@@ -7471,6 +7543,9 @@
       <c r="C199">
         <v>770101</v>
       </c>
+      <c r="G199">
+        <v>5</v>
+      </c>
       <c r="I199" t="s">
         <v>361</v>
       </c>
@@ -7488,6 +7563,9 @@
       <c r="C200">
         <v>770102</v>
       </c>
+      <c r="G200">
+        <v>5</v>
+      </c>
       <c r="I200" t="s">
         <v>362</v>
       </c>
@@ -7505,6 +7583,9 @@
       <c r="C201">
         <v>770103</v>
       </c>
+      <c r="G201">
+        <v>5</v>
+      </c>
       <c r="I201" t="s">
         <v>365</v>
       </c>
@@ -7522,6 +7603,9 @@
       <c r="C202">
         <v>770104</v>
       </c>
+      <c r="G202">
+        <v>5</v>
+      </c>
       <c r="I202" t="s">
         <v>363</v>
       </c>
@@ -7539,6 +7623,9 @@
       <c r="C203">
         <v>770105</v>
       </c>
+      <c r="G203">
+        <v>5</v>
+      </c>
       <c r="I203" t="s">
         <v>365</v>
       </c>
@@ -7556,6 +7643,9 @@
       <c r="C204">
         <v>770106</v>
       </c>
+      <c r="G204">
+        <v>5</v>
+      </c>
       <c r="I204" t="s">
         <v>363</v>
       </c>
@@ -7573,6 +7663,9 @@
       <c r="C205">
         <v>770107</v>
       </c>
+      <c r="G205">
+        <v>5</v>
+      </c>
       <c r="I205" t="s">
         <v>358</v>
       </c>
@@ -7590,6 +7683,9 @@
       <c r="C206">
         <v>770108</v>
       </c>
+      <c r="G206">
+        <v>5</v>
+      </c>
       <c r="I206" t="s">
         <v>355</v>
       </c>
@@ -7607,6 +7703,9 @@
       <c r="C207">
         <v>770109</v>
       </c>
+      <c r="G207">
+        <v>5</v>
+      </c>
       <c r="I207" t="s">
         <v>358</v>
       </c>
@@ -7624,6 +7723,9 @@
       <c r="C208">
         <v>770110</v>
       </c>
+      <c r="G208">
+        <v>5</v>
+      </c>
       <c r="I208" t="s">
         <v>355</v>
       </c>
@@ -7641,6 +7743,9 @@
       <c r="C209">
         <v>770111</v>
       </c>
+      <c r="G209">
+        <v>5</v>
+      </c>
       <c r="I209" t="s">
         <v>358</v>
       </c>
@@ -7658,6 +7763,9 @@
       <c r="C210">
         <v>770112</v>
       </c>
+      <c r="G210">
+        <v>5</v>
+      </c>
       <c r="I210" t="s">
         <v>355</v>
       </c>
@@ -7675,6 +7783,9 @@
       <c r="C211">
         <v>770113</v>
       </c>
+      <c r="G211">
+        <v>5</v>
+      </c>
       <c r="I211" t="s">
         <v>358</v>
       </c>
@@ -7692,6 +7803,9 @@
       <c r="C212">
         <v>770114</v>
       </c>
+      <c r="G212">
+        <v>5</v>
+      </c>
       <c r="I212" t="s">
         <v>355</v>
       </c>
@@ -7709,6 +7823,9 @@
       <c r="C213">
         <v>770115</v>
       </c>
+      <c r="G213">
+        <v>5</v>
+      </c>
       <c r="I213" t="s">
         <v>367</v>
       </c>
@@ -7726,6 +7843,9 @@
       <c r="C214">
         <v>770116</v>
       </c>
+      <c r="G214">
+        <v>5</v>
+      </c>
       <c r="I214" t="s">
         <v>368</v>
       </c>
@@ -7743,6 +7863,9 @@
       <c r="C215">
         <v>770117</v>
       </c>
+      <c r="G215">
+        <v>5</v>
+      </c>
       <c r="I215" t="s">
         <v>367</v>
       </c>
@@ -7760,6 +7883,9 @@
       <c r="C216">
         <v>770118</v>
       </c>
+      <c r="G216">
+        <v>5</v>
+      </c>
       <c r="I216" t="s">
         <v>368</v>
       </c>
@@ -7777,6 +7903,9 @@
       <c r="C217">
         <v>770119</v>
       </c>
+      <c r="G217">
+        <v>5</v>
+      </c>
       <c r="I217" t="s">
         <v>369</v>
       </c>
@@ -7794,6 +7923,9 @@
       <c r="C218">
         <v>770120</v>
       </c>
+      <c r="G218">
+        <v>5</v>
+      </c>
       <c r="I218" t="s">
         <v>372</v>
       </c>
@@ -7811,6 +7943,9 @@
       <c r="C219">
         <v>770121</v>
       </c>
+      <c r="G219">
+        <v>5</v>
+      </c>
       <c r="I219" t="s">
         <v>343</v>
       </c>
@@ -7828,6 +7963,9 @@
       <c r="C220">
         <v>770122</v>
       </c>
+      <c r="G220">
+        <v>5</v>
+      </c>
       <c r="I220" t="s">
         <v>349</v>
       </c>
@@ -7845,6 +7983,9 @@
       <c r="C221">
         <v>770123</v>
       </c>
+      <c r="G221">
+        <v>5</v>
+      </c>
       <c r="I221" t="s">
         <v>343</v>
       </c>
@@ -7862,6 +8003,9 @@
       <c r="C222">
         <v>770124</v>
       </c>
+      <c r="G222">
+        <v>5</v>
+      </c>
       <c r="I222" t="s">
         <v>349</v>
       </c>
@@ -7879,6 +8023,9 @@
       <c r="C223">
         <v>770135</v>
       </c>
+      <c r="G223">
+        <v>5</v>
+      </c>
       <c r="I223" t="s">
         <v>349</v>
       </c>
@@ -7896,6 +8043,9 @@
       <c r="C224">
         <v>770136</v>
       </c>
+      <c r="G224">
+        <v>5</v>
+      </c>
       <c r="I224" t="s">
         <v>343</v>
       </c>
@@ -7913,6 +8063,9 @@
       <c r="C225">
         <v>770171</v>
       </c>
+      <c r="G225">
+        <v>5</v>
+      </c>
       <c r="I225" t="s">
         <v>369</v>
       </c>
@@ -7930,6 +8083,9 @@
       <c r="C226">
         <v>770172</v>
       </c>
+      <c r="G226">
+        <v>5</v>
+      </c>
       <c r="I226" t="s">
         <v>372</v>
       </c>
@@ -7947,6 +8103,9 @@
       <c r="C227">
         <v>770231</v>
       </c>
+      <c r="G227">
+        <v>5</v>
+      </c>
       <c r="I227" t="s">
         <v>368</v>
       </c>
@@ -7964,6 +8123,9 @@
       <c r="C228">
         <v>770232</v>
       </c>
+      <c r="G228">
+        <v>5</v>
+      </c>
       <c r="I228" t="s">
         <v>367</v>
       </c>
@@ -7981,6 +8143,9 @@
       <c r="C229">
         <v>770233</v>
       </c>
+      <c r="G229">
+        <v>5</v>
+      </c>
       <c r="I229" t="s">
         <v>368</v>
       </c>
@@ -7998,6 +8163,9 @@
       <c r="C230">
         <v>770234</v>
       </c>
+      <c r="G230">
+        <v>5</v>
+      </c>
       <c r="I230" t="s">
         <v>367</v>
       </c>
@@ -8015,6 +8183,9 @@
       <c r="C231">
         <v>770239</v>
       </c>
+      <c r="G231">
+        <v>5</v>
+      </c>
       <c r="I231" t="s">
         <v>342</v>
       </c>
@@ -8032,6 +8203,9 @@
       <c r="C232">
         <v>770240</v>
       </c>
+      <c r="G232">
+        <v>5</v>
+      </c>
       <c r="I232" t="s">
         <v>380</v>
       </c>
@@ -8049,6 +8223,9 @@
       <c r="C233">
         <v>770241</v>
       </c>
+      <c r="G233">
+        <v>5</v>
+      </c>
       <c r="I233" t="s">
         <v>342</v>
       </c>
@@ -8066,6 +8243,9 @@
       <c r="C234">
         <v>770242</v>
       </c>
+      <c r="G234">
+        <v>5</v>
+      </c>
       <c r="I234" t="s">
         <v>380</v>
       </c>
@@ -8083,6 +8263,9 @@
       <c r="C235">
         <v>770243</v>
       </c>
+      <c r="G235">
+        <v>5</v>
+      </c>
       <c r="I235" t="s">
         <v>342</v>
       </c>
@@ -8100,6 +8283,9 @@
       <c r="C236">
         <v>770244</v>
       </c>
+      <c r="G236">
+        <v>5</v>
+      </c>
       <c r="I236" t="s">
         <v>380</v>
       </c>
@@ -8117,6 +8303,9 @@
       <c r="C237">
         <v>770245</v>
       </c>
+      <c r="G237">
+        <v>5</v>
+      </c>
       <c r="I237" t="s">
         <v>342</v>
       </c>
@@ -8134,6 +8323,9 @@
       <c r="C238">
         <v>770246</v>
       </c>
+      <c r="G238">
+        <v>5</v>
+      </c>
       <c r="I238" t="s">
         <v>380</v>
       </c>
@@ -8151,6 +8343,9 @@
       <c r="C239">
         <v>770281</v>
       </c>
+      <c r="G239">
+        <v>5</v>
+      </c>
       <c r="I239" t="s">
         <v>361</v>
       </c>
@@ -8168,6 +8363,9 @@
       <c r="C240">
         <v>770282</v>
       </c>
+      <c r="G240">
+        <v>5</v>
+      </c>
       <c r="I240" t="s">
         <v>362</v>
       </c>
@@ -8185,6 +8383,9 @@
       <c r="C241">
         <v>770283</v>
       </c>
+      <c r="G241">
+        <v>5</v>
+      </c>
       <c r="I241" t="s">
         <v>369</v>
       </c>
@@ -8202,6 +8403,9 @@
       <c r="C242">
         <v>770284</v>
       </c>
+      <c r="G242">
+        <v>5</v>
+      </c>
       <c r="I242" t="s">
         <v>372</v>
       </c>
@@ -8219,6 +8423,9 @@
       <c r="C243">
         <v>770285</v>
       </c>
+      <c r="G243">
+        <v>5</v>
+      </c>
       <c r="I243" t="s">
         <v>369</v>
       </c>
@@ -8236,6 +8443,9 @@
       <c r="C244">
         <v>770286</v>
       </c>
+      <c r="G244">
+        <v>5</v>
+      </c>
       <c r="I244" t="s">
         <v>372</v>
       </c>
@@ -8253,6 +8463,9 @@
       <c r="C245">
         <v>770287</v>
       </c>
+      <c r="G245">
+        <v>5</v>
+      </c>
       <c r="I245" t="s">
         <v>365</v>
       </c>
@@ -8270,6 +8483,9 @@
       <c r="C246">
         <v>770288</v>
       </c>
+      <c r="G246">
+        <v>5</v>
+      </c>
       <c r="I246" t="s">
         <v>363</v>
       </c>
@@ -8287,6 +8503,9 @@
       <c r="C247">
         <v>770289</v>
       </c>
+      <c r="G247">
+        <v>5</v>
+      </c>
       <c r="I247" t="s">
         <v>355</v>
       </c>
@@ -8304,6 +8523,9 @@
       <c r="C248">
         <v>770290</v>
       </c>
+      <c r="G248">
+        <v>5</v>
+      </c>
       <c r="I248" t="s">
         <v>358</v>
       </c>
@@ -8321,6 +8543,9 @@
       <c r="C249">
         <v>770381</v>
       </c>
+      <c r="G249">
+        <v>5</v>
+      </c>
       <c r="I249" t="s">
         <v>365</v>
       </c>
@@ -8338,6 +8563,9 @@
       <c r="C250">
         <v>770382</v>
       </c>
+      <c r="G250">
+        <v>5</v>
+      </c>
       <c r="I250" t="s">
         <v>363</v>
       </c>
@@ -8355,6 +8583,9 @@
       <c r="C251">
         <v>770401</v>
       </c>
+      <c r="G251">
+        <v>5</v>
+      </c>
       <c r="I251" t="s">
         <v>349</v>
       </c>
@@ -8372,6 +8603,9 @@
       <c r="C252">
         <v>770402</v>
       </c>
+      <c r="G252">
+        <v>5</v>
+      </c>
       <c r="I252" t="s">
         <v>343</v>
       </c>
@@ -8389,6 +8623,9 @@
       <c r="C253">
         <v>770403</v>
       </c>
+      <c r="G253">
+        <v>5</v>
+      </c>
       <c r="I253" t="s">
         <v>349</v>
       </c>
@@ -8406,6 +8643,9 @@
       <c r="C254">
         <v>770404</v>
       </c>
+      <c r="G254">
+        <v>5</v>
+      </c>
       <c r="I254" t="s">
         <v>343</v>
       </c>
@@ -8423,6 +8663,9 @@
       <c r="C255">
         <v>770407</v>
       </c>
+      <c r="G255">
+        <v>5</v>
+      </c>
       <c r="I255" t="s">
         <v>349</v>
       </c>
@@ -8440,6 +8683,9 @@
       <c r="C256">
         <v>770408</v>
       </c>
+      <c r="G256">
+        <v>5</v>
+      </c>
       <c r="I256" t="s">
         <v>343</v>
       </c>
@@ -8457,6 +8703,9 @@
       <c r="C257">
         <v>770581</v>
       </c>
+      <c r="G257">
+        <v>5</v>
+      </c>
       <c r="I257" t="s">
         <v>341</v>
       </c>
@@ -8474,6 +8723,9 @@
       <c r="C258">
         <v>770582</v>
       </c>
+      <c r="G258">
+        <v>5</v>
+      </c>
       <c r="I258" t="s">
         <v>340</v>
       </c>
@@ -8491,6 +8743,9 @@
       <c r="C259">
         <v>770583</v>
       </c>
+      <c r="G259">
+        <v>5</v>
+      </c>
       <c r="I259" t="s">
         <v>341</v>
       </c>
@@ -8508,6 +8763,9 @@
       <c r="C260">
         <v>770584</v>
       </c>
+      <c r="G260">
+        <v>5</v>
+      </c>
       <c r="I260" t="s">
         <v>340</v>
       </c>
@@ -8525,6 +8783,9 @@
       <c r="C261">
         <v>770585</v>
       </c>
+      <c r="G261">
+        <v>5</v>
+      </c>
       <c r="I261" t="s">
         <v>342</v>
       </c>
@@ -8542,6 +8803,9 @@
       <c r="C262">
         <v>770586</v>
       </c>
+      <c r="G262">
+        <v>5</v>
+      </c>
       <c r="I262" t="s">
         <v>380</v>
       </c>
@@ -8559,6 +8823,9 @@
       <c r="C263">
         <v>770587</v>
       </c>
+      <c r="G263">
+        <v>5</v>
+      </c>
       <c r="I263" t="s">
         <v>349</v>
       </c>
@@ -8576,6 +8843,9 @@
       <c r="C264">
         <v>770588</v>
       </c>
+      <c r="G264">
+        <v>5</v>
+      </c>
       <c r="I264" t="s">
         <v>343</v>
       </c>
@@ -8593,6 +8863,9 @@
       <c r="C265">
         <v>770589</v>
       </c>
+      <c r="G265">
+        <v>5</v>
+      </c>
       <c r="I265" t="s">
         <v>349</v>
       </c>
@@ -8610,6 +8883,9 @@
       <c r="C266">
         <v>770590</v>
       </c>
+      <c r="G266">
+        <v>5</v>
+      </c>
       <c r="I266" t="s">
         <v>343</v>
       </c>
@@ -8627,6 +8903,9 @@
       <c r="C267">
         <v>770683</v>
       </c>
+      <c r="G267">
+        <v>5</v>
+      </c>
       <c r="I267" t="s">
         <v>342</v>
       </c>
@@ -8644,6 +8923,9 @@
       <c r="C268">
         <v>770684</v>
       </c>
+      <c r="G268">
+        <v>5</v>
+      </c>
       <c r="I268" t="s">
         <v>380</v>
       </c>
@@ -8661,6 +8943,9 @@
       <c r="C269">
         <v>770689</v>
       </c>
+      <c r="G269">
+        <v>5</v>
+      </c>
       <c r="I269" t="s">
         <v>342</v>
       </c>
@@ -8678,6 +8963,9 @@
       <c r="C270">
         <v>770690</v>
       </c>
+      <c r="G270">
+        <v>5</v>
+      </c>
       <c r="I270" t="s">
         <v>380</v>
       </c>
@@ -8695,6 +8983,9 @@
       <c r="C271">
         <v>770691</v>
       </c>
+      <c r="G271">
+        <v>5</v>
+      </c>
       <c r="I271" t="s">
         <v>372</v>
       </c>
@@ -8712,6 +9003,9 @@
       <c r="C272">
         <v>770692</v>
       </c>
+      <c r="G272">
+        <v>5</v>
+      </c>
       <c r="I272" t="s">
         <v>369</v>
       </c>
@@ -8729,6 +9023,9 @@
       <c r="C273">
         <v>770853</v>
       </c>
+      <c r="G273">
+        <v>5</v>
+      </c>
       <c r="I273" t="s">
         <v>372</v>
       </c>
@@ -8746,6 +9043,9 @@
       <c r="C274">
         <v>770854</v>
       </c>
+      <c r="G274">
+        <v>5</v>
+      </c>
       <c r="I274" t="s">
         <v>372</v>
       </c>
@@ -8763,6 +9063,9 @@
       <c r="C275">
         <v>770855</v>
       </c>
+      <c r="G275">
+        <v>5</v>
+      </c>
       <c r="I275" t="s">
         <v>372</v>
       </c>
@@ -8780,6 +9083,9 @@
       <c r="C276">
         <v>770856</v>
       </c>
+      <c r="G276">
+        <v>5</v>
+      </c>
       <c r="I276" t="s">
         <v>369</v>
       </c>
@@ -8797,6 +9103,9 @@
       <c r="C277">
         <v>770871</v>
       </c>
+      <c r="G277">
+        <v>5</v>
+      </c>
       <c r="I277" t="s">
         <v>369</v>
       </c>
@@ -8814,6 +9123,9 @@
       <c r="C278">
         <v>770872</v>
       </c>
+      <c r="G278">
+        <v>5</v>
+      </c>
       <c r="I278" t="s">
         <v>372</v>
       </c>
@@ -8831,6 +9143,9 @@
       <c r="C279">
         <v>770879</v>
       </c>
+      <c r="G279">
+        <v>5</v>
+      </c>
       <c r="I279" t="s">
         <v>340</v>
       </c>
@@ -8848,6 +9163,9 @@
       <c r="C280">
         <v>770880</v>
       </c>
+      <c r="G280">
+        <v>5</v>
+      </c>
       <c r="I280" t="s">
         <v>341</v>
       </c>
@@ -8865,6 +9183,9 @@
       <c r="C281">
         <v>770881</v>
       </c>
+      <c r="G281">
+        <v>5</v>
+      </c>
       <c r="I281" t="s">
         <v>342</v>
       </c>
@@ -8882,6 +9203,9 @@
       <c r="C282">
         <v>770882</v>
       </c>
+      <c r="G282">
+        <v>5</v>
+      </c>
       <c r="I282" t="s">
         <v>380</v>
       </c>
@@ -8899,6 +9223,9 @@
       <c r="C283">
         <v>770883</v>
       </c>
+      <c r="G283">
+        <v>5</v>
+      </c>
       <c r="I283" t="s">
         <v>342</v>
       </c>
@@ -8916,6 +9243,9 @@
       <c r="C284">
         <v>770884</v>
       </c>
+      <c r="G284">
+        <v>5</v>
+      </c>
       <c r="I284" t="s">
         <v>380</v>
       </c>
@@ -8933,6 +9263,9 @@
       <c r="C285">
         <v>770885</v>
       </c>
+      <c r="G285">
+        <v>5</v>
+      </c>
       <c r="I285" t="s">
         <v>342</v>
       </c>
@@ -8950,6 +9283,9 @@
       <c r="C286">
         <v>770886</v>
       </c>
+      <c r="G286">
+        <v>5</v>
+      </c>
       <c r="I286" t="s">
         <v>380</v>
       </c>
@@ -8967,6 +9303,9 @@
       <c r="C287">
         <v>770887</v>
       </c>
+      <c r="G287">
+        <v>5</v>
+      </c>
       <c r="I287" t="s">
         <v>368</v>
       </c>
@@ -8984,6 +9323,9 @@
       <c r="C288">
         <v>770888</v>
       </c>
+      <c r="G288">
+        <v>5</v>
+      </c>
       <c r="I288" t="s">
         <v>367</v>
       </c>
@@ -9001,6 +9343,9 @@
       <c r="C289">
         <v>770889</v>
       </c>
+      <c r="G289">
+        <v>5</v>
+      </c>
       <c r="I289" t="s">
         <v>368</v>
       </c>
@@ -9018,6 +9363,9 @@
       <c r="C290">
         <v>770890</v>
       </c>
+      <c r="G290">
+        <v>5</v>
+      </c>
       <c r="I290" t="s">
         <v>367</v>
       </c>
@@ -9035,6 +9383,9 @@
       <c r="C291">
         <v>770891</v>
       </c>
+      <c r="G291">
+        <v>5</v>
+      </c>
       <c r="I291" t="s">
         <v>369</v>
       </c>
@@ -9052,6 +9403,9 @@
       <c r="C292">
         <v>770892</v>
       </c>
+      <c r="G292">
+        <v>5</v>
+      </c>
       <c r="I292" t="s">
         <v>372</v>
       </c>
@@ -9069,6 +9423,9 @@
       <c r="C293">
         <v>770923</v>
       </c>
+      <c r="G293">
+        <v>5</v>
+      </c>
       <c r="I293" t="s">
         <v>355</v>
       </c>
@@ -9086,6 +9443,9 @@
       <c r="C294">
         <v>770924</v>
       </c>
+      <c r="G294">
+        <v>5</v>
+      </c>
       <c r="I294" t="s">
         <v>358</v>
       </c>
@@ -9103,6 +9463,9 @@
       <c r="C295">
         <v>770981</v>
       </c>
+      <c r="G295">
+        <v>5</v>
+      </c>
       <c r="I295" t="s">
         <v>342</v>
       </c>
@@ -9119,6 +9482,9 @@
       </c>
       <c r="C296">
         <v>770982</v>
+      </c>
+      <c r="G296">
+        <v>5</v>
       </c>
       <c r="I296" t="s">
         <v>380</v>
@@ -15222,7 +15588,7 @@
     </row>
     <row r="537" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A537" t="s">
-        <v>452</v>
+        <v>491</v>
       </c>
       <c r="B537" t="s">
         <v>483</v>
@@ -15245,7 +15611,7 @@
     </row>
     <row r="538" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A538" t="s">
-        <v>452</v>
+        <v>492</v>
       </c>
       <c r="B538" t="s">
         <v>484</v>
@@ -15268,7 +15634,7 @@
     </row>
     <row r="539" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A539" t="s">
-        <v>452</v>
+        <v>493</v>
       </c>
       <c r="B539" t="s">
         <v>485</v>
@@ -15291,7 +15657,7 @@
     </row>
     <row r="540" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A540" t="s">
-        <v>452</v>
+        <v>494</v>
       </c>
       <c r="B540" t="s">
         <v>486</v>
@@ -15314,13 +15680,13 @@
     </row>
     <row r="541" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A541" t="s">
-        <v>452</v>
+        <v>495</v>
       </c>
       <c r="B541" t="s">
-        <v>80</v>
+        <v>487</v>
       </c>
       <c r="C541">
-        <v>401</v>
+        <v>800404</v>
       </c>
       <c r="E541" t="s">
         <v>16</v>
@@ -15337,13 +15703,13 @@
     </row>
     <row r="542" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A542" t="s">
-        <v>452</v>
+        <v>496</v>
       </c>
       <c r="B542" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="C542">
-        <v>800404</v>
+        <v>5800504</v>
       </c>
       <c r="E542" t="s">
         <v>16</v>
@@ -15360,13 +15726,13 @@
     </row>
     <row r="543" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A543" t="s">
-        <v>452</v>
+        <v>497</v>
       </c>
       <c r="B543" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="C543">
-        <v>5800504</v>
+        <v>1600501</v>
       </c>
       <c r="E543" t="s">
         <v>16</v>
@@ -15383,13 +15749,13 @@
     </row>
     <row r="544" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A544" t="s">
-        <v>452</v>
+        <v>498</v>
       </c>
       <c r="B544" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="C544">
-        <v>1600501</v>
+        <v>920202</v>
       </c>
       <c r="E544" t="s">
         <v>16</v>
@@ -15406,13 +15772,13 @@
     </row>
     <row r="545" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A545" t="s">
-        <v>452</v>
+        <v>499</v>
       </c>
       <c r="B545" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="C545">
-        <v>920202</v>
+        <v>920204</v>
       </c>
       <c r="E545" t="s">
         <v>16</v>
@@ -15429,13 +15795,13 @@
     </row>
     <row r="546" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A546" t="s">
-        <v>452</v>
+        <v>500</v>
       </c>
       <c r="B546" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="C546">
-        <v>920204</v>
+        <v>201</v>
       </c>
       <c r="E546" t="s">
         <v>16</v>
@@ -15455,10 +15821,10 @@
         <v>452</v>
       </c>
       <c r="B547" t="s">
-        <v>487</v>
+        <v>453</v>
       </c>
       <c r="C547">
-        <v>201</v>
+        <v>1010001</v>
       </c>
       <c r="E547" t="s">
         <v>16</v>

</xml_diff>